<commit_message>
complete and verified LinearVisualizer
</commit_message>
<xml_diff>
--- a/other/LinearVisualizer.xlsx
+++ b/other/LinearVisualizer.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\CCHW\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25656570-4913-41E1-B3F6-41AE48E14653}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9002FC-17E3-43D1-A96C-CC701FCE76E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9DBF0F91-83D7-4F64-B04C-B7CB81DC62EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="77">
   <si>
     <t>W</t>
   </si>
@@ -210,6 +210,84 @@
   </si>
   <si>
     <t>LEDColorCount</t>
+  </si>
+  <si>
+    <t>amplitudes</t>
+  </si>
+  <si>
+    <t>positions</t>
+  </si>
+  <si>
+    <t>0000000111101111</t>
+  </si>
+  <si>
+    <t>0000000100001100</t>
+  </si>
+  <si>
+    <t>0000001101100000</t>
+  </si>
+  <si>
+    <t>0000001111000100</t>
+  </si>
+  <si>
+    <t>0000001100011011</t>
+  </si>
+  <si>
+    <t>0000001010001110</t>
+  </si>
+  <si>
+    <t>0000000101011001</t>
+  </si>
+  <si>
+    <t>0000001000111110</t>
+  </si>
+  <si>
+    <t>0000000000101000</t>
+  </si>
+  <si>
+    <t>0000001101010101</t>
+  </si>
+  <si>
+    <t>0000000000000000</t>
+  </si>
+  <si>
+    <t>0000001001011000</t>
+  </si>
+  <si>
+    <t>0000001011001101</t>
+  </si>
+  <si>
+    <t>0000000111000010</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>amplitudeSum Multiplied</t>
+  </si>
+  <si>
+    <t>noteMult_d1</t>
+  </si>
+  <si>
+    <t>noteHue</t>
+  </si>
+  <si>
+    <t>hueDevided</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>RGB</t>
+  </si>
+  <si>
+    <t>RGBh</t>
   </si>
 </sst>
 </file>
@@ -246,12 +324,24 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -266,22 +356,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -597,10 +693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A6626A4-8C87-4B90-BEEB-AEB487ACEA9E}">
-  <dimension ref="A1:P52"/>
+  <dimension ref="A1:Y114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H22" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26:G28"/>
+    <sheetView tabSelected="1" topLeftCell="J82" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P106" sqref="P106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -610,17 +706,24 @@
     <col min="3" max="3" width="8.88671875" style="2"/>
     <col min="4" max="4" width="12.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="74.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="23.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="33.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="28.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="4" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.88671875" style="2"/>
+    <col min="14" max="14" width="18.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.33203125" style="2" customWidth="1"/>
+    <col min="21" max="22" width="5" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="3.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -661,27 +764,27 @@
       </c>
       <c r="D2" s="2" t="str">
         <f ca="1">_xlfn.CONCAT(B$16+B$17,"'b",REPT("0",B$16-LEN(E2)))</f>
-        <v>16'b0000</v>
+        <v>16'b00000</v>
       </c>
       <c r="E2" s="2" t="str">
         <f ca="1">DEC2BIN(_xlfn.FLOOR.MATH(RAND()*10))</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F2" s="2" t="str">
         <f>_xlfn.CONCAT(REPT("0",B$17),";")</f>
         <v>0000000000;</v>
       </c>
-      <c r="G2" s="5" t="str">
+      <c r="G2" s="4" t="str">
         <f ca="1">_xlfn.CONCAT(A2,B2,C2,D2,E2,F2)</f>
-        <v xml:space="preserve">            noteAmplitudes_i[ 0] = 16'b0000100000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 0] = 16'b0000000000000000;</v>
       </c>
       <c r="H2" s="2">
         <f t="shared" ref="H2:H13" ca="1" si="0">BIN2DEC(E2)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I2" s="2">
         <f t="shared" ref="I2:I13" ca="1" si="1">H2*2^B$17</f>
-        <v>2048</v>
+        <v>0</v>
       </c>
       <c r="J2" s="2">
         <f ca="1">SUM(H2:H13)</f>
@@ -689,7 +792,7 @@
       </c>
       <c r="K2" s="2">
         <f t="shared" ref="K2:K13" ca="1" si="2">I2-J$7</f>
-        <v>-2542</v>
+        <v>-4590</v>
       </c>
       <c r="L2" s="2">
         <f ca="1">IF(K2&gt;0,K2,0)</f>
@@ -712,27 +815,27 @@
       </c>
       <c r="D3" s="2" t="str">
         <f t="shared" ref="D3:D13" ca="1" si="3">_xlfn.CONCAT(B$16+B$17,"'b",REPT("0",B$16-LEN(E3)))</f>
-        <v>16'b00</v>
+        <v>16'b00000</v>
       </c>
       <c r="E3" s="2" t="str">
         <f t="shared" ref="E3:E13" ca="1" si="4">DEC2BIN(_xlfn.FLOOR.MATH(RAND()*10))</f>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F3" s="2" t="str">
         <f t="shared" ref="F3:F13" si="5">_xlfn.CONCAT(REPT("0",B$17),";")</f>
         <v>0000000000;</v>
       </c>
-      <c r="G3" s="5" t="str">
+      <c r="G3" s="4" t="str">
         <f t="shared" ref="G3:G13" ca="1" si="6">_xlfn.CONCAT(A3,B3,C3,D3,E3,F3)</f>
-        <v xml:space="preserve">            noteAmplitudes_i[ 1] = 16'b0010000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 1] = 16'b0000000000000000;</v>
       </c>
       <c r="H3" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I3" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>8192</v>
+        <v>0</v>
       </c>
       <c r="J3" s="2">
         <f ca="1">J2*2^B17</f>
@@ -740,15 +843,15 @@
       </c>
       <c r="K3" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>3602</v>
+        <v>-4590</v>
       </c>
       <c r="L3" s="2">
         <f t="shared" ref="L3:L13" ca="1" si="7">IF(K3&gt;0,K3,0)</f>
-        <v>3602</v>
+        <v>0</v>
       </c>
       <c r="M3" s="2">
         <f t="shared" ref="M3:M13" ca="1" si="8">IF(K3&gt;0,I3,0)</f>
-        <v>8192</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -773,7 +876,7 @@
         <f t="shared" si="5"/>
         <v>0000000000;</v>
       </c>
-      <c r="G4" s="5" t="str">
+      <c r="G4" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
         <v xml:space="preserve">            noteAmplitudes_i[ 2] = 16'b0000010000000000;</v>
       </c>
@@ -820,7 +923,7 @@
         <f t="shared" si="5"/>
         <v>0000000000;</v>
       </c>
-      <c r="G5" s="5" t="str">
+      <c r="G5" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
         <v xml:space="preserve">            noteAmplitudes_i[ 3] = 16'b0001100000000000;</v>
       </c>
@@ -860,35 +963,35 @@
       </c>
       <c r="D6" s="2" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>16'b00000</v>
+        <v>16'b0000</v>
       </c>
       <c r="E6" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F6" s="2" t="str">
         <f t="shared" si="5"/>
         <v>0000000000;</v>
       </c>
-      <c r="G6" s="5" t="str">
+      <c r="G6" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 4] = 16'b0000000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 4] = 16'b0000110000000000;</v>
       </c>
       <c r="H6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I6" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J6" s="4">
+        <v>3072</v>
+      </c>
+      <c r="J6" s="3">
         <f ca="1">J2*B18</f>
         <v>4.482421875</v>
       </c>
       <c r="K6" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>-4590</v>
+        <v>-1518</v>
       </c>
       <c r="L6" s="2">
         <f t="shared" ca="1" si="7"/>
@@ -915,23 +1018,23 @@
       </c>
       <c r="E7" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F7" s="2" t="str">
         <f t="shared" si="5"/>
         <v>0000000000;</v>
       </c>
-      <c r="G7" s="5" t="str">
+      <c r="G7" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 5] = 16'b0001110000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 5] = 16'b0001100000000000;</v>
       </c>
       <c r="H7" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I7" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>7168</v>
+        <v>6144</v>
       </c>
       <c r="J7" s="2">
         <f ca="1">J3 * BIN2DEC(C18) / 2^B17</f>
@@ -939,15 +1042,15 @@
       </c>
       <c r="K7" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>2578</v>
+        <v>1554</v>
       </c>
       <c r="L7" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>2578</v>
+        <v>1554</v>
       </c>
       <c r="M7" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>7168</v>
+        <v>6144</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -962,39 +1065,39 @@
       </c>
       <c r="D8" s="2" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>16'b000</v>
+        <v>16'b00</v>
       </c>
       <c r="E8" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>111</v>
+        <v>1001</v>
       </c>
       <c r="F8" s="2" t="str">
         <f t="shared" si="5"/>
         <v>0000000000;</v>
       </c>
-      <c r="G8" s="5" t="str">
+      <c r="G8" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 6] = 16'b0001110000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 6] = 16'b0010010000000000;</v>
       </c>
       <c r="H8" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I8" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>7168</v>
+        <v>9216</v>
       </c>
       <c r="K8" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>2578</v>
+        <v>4626</v>
       </c>
       <c r="L8" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>2578</v>
+        <v>4626</v>
       </c>
       <c r="M8" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>7168</v>
+        <v>9216</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -1009,42 +1112,42 @@
       </c>
       <c r="D9" s="2" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>16'b00</v>
+        <v>16'b00000</v>
       </c>
       <c r="E9" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1001</v>
+        <v>0</v>
       </c>
       <c r="F9" s="2" t="str">
         <f t="shared" si="5"/>
         <v>0000000000;</v>
       </c>
-      <c r="G9" s="5" t="str">
+      <c r="G9" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 7] = 16'b0010010000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 7] = 16'b0000000000000000;</v>
       </c>
       <c r="H9" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="I9" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>9216</v>
+        <v>0</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="K9" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>4626</v>
+        <v>-4590</v>
       </c>
       <c r="L9" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>4626</v>
+        <v>0</v>
       </c>
       <c r="M9" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>9216</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -1059,43 +1162,43 @@
       </c>
       <c r="D10" s="2" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>16'b0000</v>
+        <v>16'b00</v>
       </c>
       <c r="E10" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>1000</v>
       </c>
       <c r="F10" s="2" t="str">
         <f t="shared" si="5"/>
         <v>0000000000;</v>
       </c>
-      <c r="G10" s="5" t="str">
+      <c r="G10" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 8] = 16'b0000100000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 8] = 16'b0010000000000000;</v>
       </c>
       <c r="H10" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I10" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>2048</v>
+        <v>8192</v>
       </c>
       <c r="J10" s="2">
         <f ca="1">J11/2^B17</f>
-        <v>14.587890625</v>
+        <v>13.587890625</v>
       </c>
       <c r="K10" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>-2542</v>
+        <v>3602</v>
       </c>
       <c r="L10" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>3602</v>
       </c>
       <c r="M10" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>8192</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -1110,43 +1213,43 @@
       </c>
       <c r="D11" s="2" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>16'b00000</v>
+        <v>16'b000</v>
       </c>
       <c r="E11" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>111</v>
       </c>
       <c r="F11" s="2" t="str">
         <f t="shared" si="5"/>
         <v>0000000000;</v>
       </c>
-      <c r="G11" s="5" t="str">
+      <c r="G11" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 9] = 16'b0000000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 9] = 16'b0001110000000000;</v>
       </c>
       <c r="H11" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I11" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>7168</v>
       </c>
       <c r="J11" s="2">
         <f ca="1">SUM(L2:L13)</f>
-        <v>14938</v>
+        <v>13914</v>
       </c>
       <c r="K11" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>-4590</v>
+        <v>2578</v>
       </c>
       <c r="L11" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>2578</v>
       </c>
       <c r="M11" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>7168</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -1161,31 +1264,31 @@
       </c>
       <c r="D12" s="2" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>16'b00000</v>
+        <v>16'b0000</v>
       </c>
       <c r="E12" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F12" s="2" t="str">
         <f t="shared" si="5"/>
         <v>0000000000;</v>
       </c>
-      <c r="G12" s="5" t="str">
+      <c r="G12" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[10] = 16'b0000010000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[10] = 16'b0000100000000000;</v>
       </c>
       <c r="H12" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I12" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>1024</v>
+        <v>2048</v>
       </c>
       <c r="K12" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>-3566</v>
+        <v>-2542</v>
       </c>
       <c r="L12" s="2">
         <f t="shared" ca="1" si="7"/>
@@ -1212,27 +1315,27 @@
       </c>
       <c r="E13" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F13" s="2" t="str">
         <f t="shared" si="5"/>
         <v>0000000000;</v>
       </c>
-      <c r="G13" s="5" t="str">
+      <c r="G13" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[11] = 16'b0000100000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[11] = 16'b0000110000000000;</v>
       </c>
       <c r="H13" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I13" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>2048</v>
+        <v>3072</v>
       </c>
       <c r="K13" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>-2542</v>
+        <v>-1518</v>
       </c>
       <c r="L13" s="2">
         <f t="shared" ca="1" si="7"/>
@@ -1244,24 +1347,25 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="8">
         <v>24</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="8">
         <f>_xlfn.CEILING.MATH(IMLOG2(B15))</f>
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="2">
+      <c r="A16" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="8">
         <v>6</v>
       </c>
+      <c r="C16" s="8"/>
       <c r="J16" s="2" t="s">
         <v>15</v>
       </c>
@@ -1273,55 +1377,57 @@
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="8">
         <v>10</v>
       </c>
-      <c r="G17" s="5" t="str">
+      <c r="C17" s="8"/>
+      <c r="G17" s="4" t="str">
         <f ca="1">_xlfn.CONCAT("notePosition_i = 10'b",REPT(0,B17-LEN(_xlfn.BASE(I17,2))),_xlfn.BASE(I17,2),";" )</f>
-        <v>notePosition_i = 10'b1101100101;</v>
+        <v>notePosition_i = 10'b0111010101;</v>
       </c>
       <c r="H17" s="2">
         <f ca="1">I17/2^10</f>
-        <v>0.8486328125</v>
+        <v>0.4580078125</v>
       </c>
       <c r="I17" s="2">
         <f ca="1">RANDBETWEEN(0,1023)</f>
-        <v>869</v>
+        <v>469</v>
       </c>
       <c r="J17" s="2">
         <f ca="1">I17*24</f>
-        <v>20856</v>
+        <v>11256</v>
       </c>
       <c r="K17" s="2">
         <f ca="1">IF(J21=3,24576-J17,8192-J17)</f>
-        <v>3720</v>
+        <v>-3064</v>
       </c>
       <c r="L17" s="2">
         <f ca="1">IF(J21=3,K23+170, K23)</f>
-        <v>228</v>
+        <v>-32</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="8">
         <v>9.9609375E-2</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="10">
         <v>1100110</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="8">
         <v>50</v>
       </c>
+      <c r="C19" s="8"/>
       <c r="J19" s="2" t="s">
         <v>14</v>
       </c>
@@ -1330,14 +1436,14 @@
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="E20" s="2">
+      <c r="E20" s="8">
         <f>_xlfn.FLOOR.MATH(IMLOG2(G20))</f>
         <v>14</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="11">
         <v>21824</v>
       </c>
       <c r="H20" s="2">
@@ -1346,58 +1452,58 @@
       </c>
       <c r="J20" s="2" t="str">
         <f ca="1">_xlfn.CONCAT(REPT(0,3-LEN(DEC2BIN(2^_xlfn.FLOOR.MATH((J17+1)/8192)))),DEC2BIN(2^_xlfn.FLOOR.MATH((J17+1)/8192)))</f>
-        <v>100</v>
+        <v>010</v>
       </c>
       <c r="K20" s="2">
         <f ca="1">K17*H20*H21*H22</f>
-        <v>243555840</v>
+        <v>-133737472</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="E21" s="2">
+      <c r="E21" s="8">
         <f>_xlfn.FLOOR.MATH(IMLOG2(G21))</f>
         <v>15</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G21" s="11">
         <v>43648</v>
       </c>
       <c r="H21" s="2">
         <f ca="1">IF(J$21=2,G21,1)</f>
-        <v>1</v>
+        <v>43648</v>
       </c>
       <c r="J21" s="2">
         <f ca="1">LEN(DEC2BIN(2^_xlfn.FLOOR.MATH((J17+1)/8192)))</f>
-        <v>3</v>
-      </c>
-      <c r="K21" s="2" t="str">
+        <v>2</v>
+      </c>
+      <c r="K21" s="2" t="e">
         <f ca="1">_xlfn.BASE(K20,2,32)</f>
-        <v>00001110100001000101111000000000</v>
+        <v>#NUM!</v>
       </c>
       <c r="L21" s="2">
         <f ca="1">MOD(IF(L17&lt;0,L17+1023,L17), 1024)</f>
-        <v>228</v>
+        <v>991</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="E22" s="2">
+      <c r="E22" s="8">
         <f>_xlfn.FLOOR.MATH(IMLOG2(G22))</f>
         <v>15</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G22" s="6">
+      <c r="G22" s="11">
         <v>65472</v>
       </c>
       <c r="H22" s="2">
         <f ca="1">IF(J$21=3,G22,1)</f>
-        <v>65472</v>
+        <v>1</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>21</v>
@@ -1406,21 +1512,21 @@
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="K23" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(K20/2^(B17+B17+C15-3))</f>
-        <v>58</v>
+        <v>-32</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="G26" s="5" t="str">
+      <c r="G26" s="4" t="str">
         <f ca="1">_xlfn.CONCAT("        noteAmplitude_i = 10'b",REPT(0,B17-LEN(_xlfn.BASE(I26,2))),_xlfn.BASE(I26,2),";" )</f>
-        <v xml:space="preserve">        noteAmplitude_i = 10'b1001111010;</v>
+        <v xml:space="preserve">        noteAmplitude_i = 10'b0100011101;</v>
       </c>
       <c r="H26" s="2">
         <f ca="1">I26/2^10</f>
-        <v>0.619140625</v>
+        <v>0.2783203125</v>
       </c>
       <c r="I26" s="2">
         <f ca="1">RANDBETWEEN(0,1023)</f>
-        <v>634</v>
+        <v>285</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>28</v>
@@ -1442,37 +1548,45 @@
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="G27" s="5" t="str">
+      <c r="B27" s="2">
+        <f>LEN(C18)</f>
+        <v>7</v>
+      </c>
+      <c r="C27" s="2">
+        <f>2^B27</f>
+        <v>128</v>
+      </c>
+      <c r="G27" s="4" t="str">
         <f ca="1">_xlfn.CONCAT("        noteAmplitudeFast_i = 10'b",REPT(0,B17-LEN(_xlfn.BASE(I27,2))),_xlfn.BASE(I27,2),";" )</f>
-        <v xml:space="preserve">        noteAmplitudeFast_i = 10'b0100001110;</v>
+        <v xml:space="preserve">        noteAmplitudeFast_i = 10'b0111111000;</v>
       </c>
       <c r="H27" s="2">
         <f t="shared" ref="H27:H28" ca="1" si="9">I27/2^10</f>
-        <v>0.263671875</v>
+        <v>0.4921875</v>
       </c>
       <c r="I27" s="2">
         <f ca="1">RANDBETWEEN(0,1023)</f>
-        <v>270</v>
+        <v>504</v>
       </c>
       <c r="J27" s="2">
         <f ca="1">I28*E31</f>
-        <v>1536</v>
+        <v>5640</v>
       </c>
       <c r="K27" s="2">
         <f ca="1">IF(E33,I26,I27)</f>
-        <v>270</v>
+        <v>504</v>
       </c>
       <c r="L27" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(K33/2^(B17-8))</f>
-        <v>107</v>
+        <v>201</v>
       </c>
       <c r="M27" s="2">
         <f ca="1">$L$27</f>
-        <v>107</v>
+        <v>201</v>
       </c>
       <c r="N27" s="2">
         <f ca="1">$L$33</f>
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="O27" s="2">
         <f>0</f>
@@ -1480,21 +1594,21 @@
       </c>
       <c r="P27" s="2">
         <f ca="1">M27*2^16+N27*2^8+O27</f>
-        <v>7025920</v>
+        <v>13198848</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="G28" s="5" t="str">
+      <c r="G28" s="4" t="str">
         <f ca="1">_xlfn.CONCAT("        noteHue_i = 10'b",REPT(0,B17-LEN(_xlfn.BASE(I28,2))),_xlfn.BASE(I28,2),";" )</f>
-        <v xml:space="preserve">        noteHue_i = 10'b0100000000;</v>
+        <v xml:space="preserve">        noteHue_i = 10'b1110101100;</v>
       </c>
       <c r="H28" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>0.25</v>
+        <v>0.91796875</v>
       </c>
       <c r="I28" s="2">
         <f ca="1">RANDBETWEEN(0,1023)</f>
-        <v>256</v>
+        <v>940</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>29</v>
@@ -1507,11 +1621,11 @@
       </c>
       <c r="M28" s="2">
         <f ca="1">$L$35</f>
-        <v>53</v>
+        <v>98</v>
       </c>
       <c r="N28" s="2">
         <f ca="1">$L$27</f>
-        <v>107</v>
+        <v>201</v>
       </c>
       <c r="O28" s="2">
         <f>0</f>
@@ -1519,21 +1633,21 @@
       </c>
       <c r="P28" s="2">
         <f t="shared" ref="P28:P33" ca="1" si="10">M28*2^16+N28*2^8+O28</f>
-        <v>3500800</v>
+        <v>6473984</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="J29" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(J27/2^10)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K29" s="2">
         <f ca="1">K27*E30</f>
-        <v>442260</v>
+        <v>825552</v>
       </c>
       <c r="L29" s="2">
         <f ca="1">K33*J31</f>
-        <v>220672</v>
+        <v>419120</v>
       </c>
       <c r="M29" s="2">
         <f>0</f>
@@ -1541,22 +1655,22 @@
       </c>
       <c r="N29" s="2">
         <f ca="1">$L$27</f>
-        <v>107</v>
+        <v>201</v>
       </c>
       <c r="O29" s="2">
         <f ca="1">$L$33</f>
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="P29" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>27445</v>
+        <v>51558</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="E30" s="2">
+      <c r="E30" s="8">
         <v>1638</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F30" s="8" t="s">
         <v>26</v>
       </c>
       <c r="J30" s="2" t="s">
@@ -1574,39 +1688,39 @@
       </c>
       <c r="N30" s="2">
         <f ca="1">$L$35</f>
-        <v>53</v>
+        <v>98</v>
       </c>
       <c r="O30" s="2">
         <f ca="1">$L$27</f>
-        <v>107</v>
+        <v>201</v>
       </c>
       <c r="P30" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>13675</v>
+        <v>25289</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="E31" s="2">
+      <c r="E31" s="8">
         <v>6</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F31" s="8" t="s">
         <v>25</v>
       </c>
       <c r="J31" s="2">
         <f ca="1">MOD(J27,2^10)</f>
-        <v>512</v>
+        <v>520</v>
       </c>
       <c r="K31" s="2">
         <f ca="1">IF(_xlfn.FLOOR.MATH(K29/2^10) &gt; 1023, 1023, _xlfn.FLOOR.MATH(K29/2^10))</f>
-        <v>431</v>
+        <v>806</v>
       </c>
       <c r="L31" s="2">
         <f ca="1">K33*(1023-J31)</f>
-        <v>220241</v>
+        <v>405418</v>
       </c>
       <c r="M31" s="2">
         <f ca="1">$L$33</f>
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="N31" s="2">
         <f>0</f>
@@ -1614,18 +1728,18 @@
       </c>
       <c r="O31" s="2">
         <f ca="1">$L$27</f>
-        <v>107</v>
+        <v>201</v>
       </c>
       <c r="P31" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>3473515</v>
+        <v>6684873</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="E32" s="2">
+      <c r="E32" s="8">
         <v>1023</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="8" t="s">
         <v>27</v>
       </c>
       <c r="K32" s="2" t="s">
@@ -1636,7 +1750,7 @@
       </c>
       <c r="M32" s="2">
         <f ca="1">$L$27</f>
-        <v>107</v>
+        <v>201</v>
       </c>
       <c r="N32" s="2">
         <f>0</f>
@@ -1644,35 +1758,35 @@
       </c>
       <c r="O32" s="2">
         <f ca="1">$L$35</f>
-        <v>53</v>
+        <v>98</v>
       </c>
       <c r="P32" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>7012405</v>
+        <v>13172834</v>
       </c>
     </row>
     <row r="33" spans="5:16" x14ac:dyDescent="0.3">
-      <c r="E33" s="2">
-        <v>0</v>
-      </c>
-      <c r="F33" s="2" t="s">
+      <c r="E33" s="8">
+        <v>0</v>
+      </c>
+      <c r="F33" s="8" t="s">
         <v>38</v>
       </c>
       <c r="K33" s="2">
         <f ca="1">IF(K31&gt;E32,E32,K31)</f>
-        <v>431</v>
+        <v>806</v>
       </c>
       <c r="L33" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(L29/2^(2*B17-8))</f>
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="M33" s="2">
         <f ca="1">$L$27</f>
-        <v>107</v>
+        <v>201</v>
       </c>
       <c r="N33" s="2">
         <f ca="1">$L$33</f>
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="O33" s="2">
         <f>0</f>
@@ -1680,7 +1794,7 @@
       </c>
       <c r="P33" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>7025920</v>
+        <v>13198848</v>
       </c>
     </row>
     <row r="34" spans="5:16" x14ac:dyDescent="0.3">
@@ -1694,11 +1808,11 @@
     <row r="35" spans="5:16" x14ac:dyDescent="0.3">
       <c r="L35" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(L31/2^(2*B17-8))</f>
-        <v>53</v>
+        <v>98</v>
       </c>
       <c r="M35" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="M35" ca="1">_xlfn.BASE(_xlfn.SWITCH(J29,0,P27,1,P28,2,P29,3,P30,4,P31,5,P32,6,P33),16,6)</f>
-        <v>356B00</v>
+        <v>C90062</v>
       </c>
     </row>
     <row r="36" spans="5:16" x14ac:dyDescent="0.3">
@@ -1715,7 +1829,7 @@
       </c>
     </row>
     <row r="39" spans="5:16" x14ac:dyDescent="0.3">
-      <c r="G39" s="5" t="str">
+      <c r="G39" s="4" t="str">
         <f ca="1">_xlfn.CONCAT(A2,B2,C2,B$16+B$17,"'b",_xlfn.BASE(L2,2,$B$16+$B$17),";")</f>
         <v xml:space="preserve">            noteAmplitudes_i[ 0] = 16'b0000000000000000;</v>
       </c>
@@ -1725,7 +1839,7 @@
       </c>
       <c r="I39" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(H52/B19)</f>
-        <v>298</v>
+        <v>278</v>
       </c>
       <c r="J39" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(H39/I$39)</f>
@@ -1737,21 +1851,21 @@
       </c>
     </row>
     <row r="40" spans="5:16" x14ac:dyDescent="0.3">
-      <c r="G40" s="5" t="str">
+      <c r="G40" s="4" t="str">
         <f t="shared" ref="G40:G50" ca="1" si="11">_xlfn.CONCAT(A3,B3,C3,B$16+B$17,"'b",_xlfn.BASE(L3,2,$B$16+$B$17),";")</f>
-        <v xml:space="preserve">            noteAmplitudes_i[ 1] = 16'b0000111000010010;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 1] = 16'b0000000000000000;</v>
       </c>
       <c r="H40" s="2">
         <f t="shared" ref="H40:H50" ca="1" si="12">L3</f>
-        <v>3602</v>
+        <v>0</v>
       </c>
       <c r="J40" s="2">
         <f t="shared" ref="J40:J50" ca="1" si="13">_xlfn.FLOOR.MATH(H40/I$39)</f>
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="5:16" x14ac:dyDescent="0.3">
-      <c r="G41" s="5" t="str">
+      <c r="G41" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
         <v xml:space="preserve">            noteAmplitudes_i[ 2] = 16'b0000000000000000;</v>
       </c>
@@ -1765,7 +1879,7 @@
       </c>
     </row>
     <row r="42" spans="5:16" x14ac:dyDescent="0.3">
-      <c r="G42" s="5" t="str">
+      <c r="G42" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
         <v xml:space="preserve">            noteAmplitudes_i[ 3] = 16'b0000011000010010;</v>
       </c>
@@ -1779,7 +1893,7 @@
       </c>
     </row>
     <row r="43" spans="5:16" x14ac:dyDescent="0.3">
-      <c r="G43" s="5" t="str">
+      <c r="G43" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
         <v xml:space="preserve">            noteAmplitudes_i[ 4] = 16'b0000000000000000;</v>
       </c>
@@ -1793,77 +1907,77 @@
       </c>
     </row>
     <row r="44" spans="5:16" x14ac:dyDescent="0.3">
-      <c r="G44" s="5" t="str">
+      <c r="G44" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 5] = 16'b0000101000010010;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 5] = 16'b0000011000010010;</v>
       </c>
       <c r="H44" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>2578</v>
+        <v>1554</v>
       </c>
       <c r="J44" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="5:16" x14ac:dyDescent="0.3">
-      <c r="G45" s="5" t="str">
+      <c r="G45" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 6] = 16'b0000101000010010;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 6] = 16'b0001001000010010;</v>
       </c>
       <c r="H45" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>2578</v>
+        <v>4626</v>
       </c>
       <c r="J45" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="5:16" x14ac:dyDescent="0.3">
-      <c r="G46" s="5" t="str">
+      <c r="G46" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 7] = 16'b0001001000010010;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 7] = 16'b0000000000000000;</v>
       </c>
       <c r="H46" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>4626</v>
+        <v>0</v>
       </c>
       <c r="J46" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="5:16" x14ac:dyDescent="0.3">
-      <c r="G47" s="5" t="str">
+      <c r="G47" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 8] = 16'b0000000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 8] = 16'b0000111000010010;</v>
       </c>
       <c r="H47" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>3602</v>
       </c>
       <c r="J47" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="48" spans="5:16" x14ac:dyDescent="0.3">
-      <c r="G48" s="5" t="str">
+      <c r="G48" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 9] = 16'b0000000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 9] = 16'b0000101000010010;</v>
       </c>
       <c r="H48" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>2578</v>
       </c>
       <c r="J48" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="7:10" x14ac:dyDescent="0.3">
-      <c r="G49" s="5" t="str">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="G49" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
         <v xml:space="preserve">            noteAmplitudes_i[10] = 16'b0000000000000000;</v>
       </c>
@@ -1876,8 +1990,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="7:10" x14ac:dyDescent="0.3">
-      <c r="G50" s="5" t="str">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="G50" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
         <v xml:space="preserve">            noteAmplitudes_i[11] = 16'b0000000000000000;</v>
       </c>
@@ -1890,22 +2004,2060 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="7:10" x14ac:dyDescent="0.3">
-      <c r="G51" s="7" t="str">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="G51" s="5" t="str">
         <f ca="1">_xlfn.CONCAT("            amplitudeSumNew_i = ",B16+B17+_xlfn.CEILING.MATH(IMLOG2(B19)),"'b",_xlfn.BASE(H52,2,B16+B17+_xlfn.CEILING.MATH(IMLOG2(B19))),";")</f>
-        <v xml:space="preserve">            amplitudeSumNew_i = 22'b0000000011101001011010;</v>
-      </c>
-    </row>
-    <row r="52" spans="7:10" x14ac:dyDescent="0.3">
+        <v xml:space="preserve">            amplitudeSumNew_i = 22'b0000000011011001011010;</v>
+      </c>
+    </row>
+    <row r="52" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G52" s="2" t="s">
         <v>46</v>
       </c>
       <c r="H52" s="2">
         <f ca="1">SUM(H39:H50)</f>
-        <v>14938</v>
+        <v>13914</v>
+      </c>
+    </row>
+    <row r="54" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A54" s="7"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
+      <c r="I54" s="7"/>
+      <c r="J54" s="7"/>
+      <c r="K54" s="7"/>
+      <c r="L54" s="7"/>
+      <c r="M54" s="7"/>
+      <c r="N54" s="7"/>
+      <c r="O54" s="7"/>
+      <c r="P54" s="7"/>
+      <c r="Q54" s="7"/>
+      <c r="R54" s="7"/>
+      <c r="S54" s="7"/>
+      <c r="T54" s="7"/>
+      <c r="U54" s="7"/>
+      <c r="V54" s="7"/>
+      <c r="W54" s="7"/>
+      <c r="X54" s="7"/>
+      <c r="Y54" s="7"/>
+    </row>
+    <row r="55" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A55" s="7"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="7"/>
+      <c r="I55" s="7"/>
+      <c r="J55" s="7"/>
+      <c r="K55" s="7"/>
+      <c r="L55" s="7"/>
+      <c r="M55" s="7"/>
+      <c r="N55" s="7"/>
+      <c r="O55" s="7"/>
+      <c r="P55" s="7"/>
+      <c r="Q55" s="7"/>
+      <c r="R55" s="7"/>
+      <c r="S55" s="7"/>
+      <c r="T55" s="7"/>
+      <c r="U55" s="7"/>
+      <c r="V55" s="7"/>
+      <c r="W55" s="7"/>
+      <c r="X55" s="7"/>
+      <c r="Y55" s="7"/>
+    </row>
+    <row r="56" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A56" s="7"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="7"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="7"/>
+      <c r="I56" s="7"/>
+      <c r="J56" s="7"/>
+      <c r="K56" s="7"/>
+      <c r="L56" s="7"/>
+      <c r="M56" s="7"/>
+      <c r="N56" s="7"/>
+      <c r="O56" s="7"/>
+      <c r="P56" s="7"/>
+      <c r="Q56" s="7"/>
+      <c r="R56" s="7"/>
+      <c r="S56" s="7"/>
+      <c r="T56" s="7"/>
+      <c r="U56" s="7"/>
+      <c r="V56" s="7"/>
+      <c r="W56" s="7"/>
+      <c r="X56" s="7"/>
+      <c r="Y56" s="7"/>
+    </row>
+    <row r="58" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="G58" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J58" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K58" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L58" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="F59" s="2">
+        <f ca="1">H59/2^B$17</f>
+        <v>0.5859375</v>
+      </c>
+      <c r="G59" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H59" s="2" cm="1">
+        <f t="array" aca="1" ref="H59" ca="1">SUMPRODUCT(--MID(G59,LEN(G59)+1-ROW(INDIRECT("1:"&amp;LEN(G59))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G59)))-1)))</f>
+        <v>600</v>
+      </c>
+      <c r="I59" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J59" s="2">
+        <f ca="1">H59-I$63</f>
+        <v>423.990234375</v>
+      </c>
+      <c r="K59" s="2">
+        <f ca="1">IF(J59&lt;0, 0, J59)</f>
+        <v>423.990234375</v>
+      </c>
+      <c r="L59" s="2">
+        <f ca="1">IF(K59=0,0,H59)</f>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="60" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="F60" s="2">
+        <f t="shared" ref="F60:F84" ca="1" si="14">H60/2^B$17</f>
+        <v>0.7001953125</v>
+      </c>
+      <c r="G60" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H60" s="2" cm="1">
+        <f t="array" aca="1" ref="H60" ca="1">SUMPRODUCT(--MID(G60,LEN(G60)+1-ROW(INDIRECT("1:"&amp;LEN(G60))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G60)))-1)))</f>
+        <v>717</v>
+      </c>
+      <c r="I60" s="2">
+        <f ca="1">SUM(H59:H70)</f>
+        <v>1767</v>
+      </c>
+      <c r="J60" s="2">
+        <f t="shared" ref="J60:J70" ca="1" si="15">H60-I$63</f>
+        <v>540.990234375</v>
+      </c>
+      <c r="K60" s="2">
+        <f t="shared" ref="K60:K70" ca="1" si="16">IF(J60&lt;0, 0, J60)</f>
+        <v>540.990234375</v>
+      </c>
+      <c r="L60" s="2">
+        <f t="shared" ref="L60:L70" ca="1" si="17">IF(K60=0,0,H60)</f>
+        <v>717</v>
+      </c>
+    </row>
+    <row r="61" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="F61" s="2">
+        <f t="shared" ca="1" si="14"/>
+        <v>0.439453125</v>
+      </c>
+      <c r="G61" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H61" s="2" cm="1">
+        <f t="array" aca="1" ref="H61" ca="1">SUMPRODUCT(--MID(G61,LEN(G61)+1-ROW(INDIRECT("1:"&amp;LEN(G61))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G61)))-1)))</f>
+        <v>450</v>
+      </c>
+      <c r="I61" s="2">
+        <f ca="1">I60/2^B17</f>
+        <v>1.7255859375</v>
+      </c>
+      <c r="J61" s="2">
+        <f t="shared" ca="1" si="15"/>
+        <v>273.990234375</v>
+      </c>
+      <c r="K61" s="2">
+        <f t="shared" ca="1" si="16"/>
+        <v>273.990234375</v>
+      </c>
+      <c r="L61" s="2">
+        <f t="shared" ca="1" si="17"/>
+        <v>450</v>
+      </c>
+    </row>
+    <row r="62" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="F62" s="2">
+        <f t="shared" ca="1" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="G62" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H62" s="2" cm="1">
+        <f t="array" aca="1" ref="H62" ca="1">SUMPRODUCT(--MID(G62,LEN(G62)+1-ROW(INDIRECT("1:"&amp;LEN(G62))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G62)))-1)))</f>
+        <v>0</v>
+      </c>
+      <c r="I62" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J62" s="2">
+        <f t="shared" ca="1" si="15"/>
+        <v>-176.009765625</v>
+      </c>
+      <c r="K62" s="2">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="L62" s="2">
+        <f t="shared" ca="1" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="F63" s="2">
+        <f t="shared" ca="1" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="G63" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H63" s="2" cm="1">
+        <f t="array" aca="1" ref="H63" ca="1">SUMPRODUCT(--MID(G63,LEN(G63)+1-ROW(INDIRECT("1:"&amp;LEN(G63))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G63)))-1)))</f>
+        <v>0</v>
+      </c>
+      <c r="I63" s="2">
+        <f ca="1">I60*BIN2DEC(C18)/2^B17</f>
+        <v>176.009765625</v>
+      </c>
+      <c r="J63" s="2">
+        <f t="shared" ca="1" si="15"/>
+        <v>-176.009765625</v>
+      </c>
+      <c r="K63" s="2">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="L63" s="2">
+        <f t="shared" ca="1" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="F64" s="2">
+        <f t="shared" ca="1" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="G64" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H64" s="2" cm="1">
+        <f t="array" aca="1" ref="H64" ca="1">SUMPRODUCT(--MID(G64,LEN(G64)+1-ROW(INDIRECT("1:"&amp;LEN(G64))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G64)))-1)))</f>
+        <v>0</v>
+      </c>
+      <c r="I64" s="2">
+        <f ca="1">I61*B18</f>
+        <v>0.17188453674316406</v>
+      </c>
+      <c r="J64" s="2">
+        <f t="shared" ca="1" si="15"/>
+        <v>-176.009765625</v>
+      </c>
+      <c r="K64" s="2">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="L64" s="2">
+        <f t="shared" ca="1" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="F65" s="2">
+        <f t="shared" ca="1" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="G65" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H65" s="2" cm="1">
+        <f t="array" aca="1" ref="H65" ca="1">SUMPRODUCT(--MID(G65,LEN(G65)+1-ROW(INDIRECT("1:"&amp;LEN(G65))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G65)))-1)))</f>
+        <v>0</v>
+      </c>
+      <c r="I65" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J65" s="2">
+        <f t="shared" ca="1" si="15"/>
+        <v>-176.009765625</v>
+      </c>
+      <c r="K65" s="2">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="L65" s="2">
+        <f t="shared" ca="1" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="F66" s="2">
+        <f t="shared" ca="1" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H66" s="2" cm="1">
+        <f t="array" aca="1" ref="H66" ca="1">SUMPRODUCT(--MID(G66,LEN(G66)+1-ROW(INDIRECT("1:"&amp;LEN(G66))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G66)))-1)))</f>
+        <v>0</v>
+      </c>
+      <c r="I66" s="2">
+        <f ca="1">SUM(K59:K70)</f>
+        <v>1238.970703125</v>
+      </c>
+      <c r="J66" s="2">
+        <f t="shared" ca="1" si="15"/>
+        <v>-176.009765625</v>
+      </c>
+      <c r="K66" s="2">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="L66" s="2">
+        <f t="shared" ca="1" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="F67" s="2">
+        <f t="shared" ca="1" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="G67" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H67" s="2" cm="1">
+        <f t="array" aca="1" ref="H67" ca="1">SUMPRODUCT(--MID(G67,LEN(G67)+1-ROW(INDIRECT("1:"&amp;LEN(G67))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G67)))-1)))</f>
+        <v>0</v>
+      </c>
+      <c r="J67" s="2">
+        <f t="shared" ca="1" si="15"/>
+        <v>-176.009765625</v>
+      </c>
+      <c r="K67" s="2">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="L67" s="2">
+        <f t="shared" ca="1" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="F68" s="2">
+        <f t="shared" ca="1" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="G68" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H68" s="2" cm="1">
+        <f t="array" aca="1" ref="H68" ca="1">SUMPRODUCT(--MID(G68,LEN(G68)+1-ROW(INDIRECT("1:"&amp;LEN(G68))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G68)))-1)))</f>
+        <v>0</v>
+      </c>
+      <c r="J68" s="2">
+        <f t="shared" ca="1" si="15"/>
+        <v>-176.009765625</v>
+      </c>
+      <c r="K68" s="2">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="L68" s="2">
+        <f t="shared" ca="1" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="F69" s="2">
+        <f t="shared" ca="1" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="G69" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H69" s="2" cm="1">
+        <f t="array" aca="1" ref="H69" ca="1">SUMPRODUCT(--MID(G69,LEN(G69)+1-ROW(INDIRECT("1:"&amp;LEN(G69))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G69)))-1)))</f>
+        <v>0</v>
+      </c>
+      <c r="J69" s="2">
+        <f t="shared" ca="1" si="15"/>
+        <v>-176.009765625</v>
+      </c>
+      <c r="K69" s="2">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="L69" s="2">
+        <f t="shared" ca="1" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="F70" s="2">
+        <f t="shared" ca="1" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="G70" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H70" s="2" cm="1">
+        <f t="array" aca="1" ref="H70" ca="1">SUMPRODUCT(--MID(G70,LEN(G70)+1-ROW(INDIRECT("1:"&amp;LEN(G70))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G70)))-1)))</f>
+        <v>0</v>
+      </c>
+      <c r="J70" s="2">
+        <f t="shared" ca="1" si="15"/>
+        <v>-176.009765625</v>
+      </c>
+      <c r="K70" s="2">
+        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="L70" s="2">
+        <f t="shared" ca="1" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="G72" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I72" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J72" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K72" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L72" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M72" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="N72" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O72" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="F73" s="2">
+        <f t="shared" ca="1" si="14"/>
+        <v>0.4833984375</v>
+      </c>
+      <c r="G73" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H73" s="2" cm="1">
+        <f t="array" aca="1" ref="H73" ca="1">SUMPRODUCT(--MID(G73,LEN(G73)+1-ROW(INDIRECT("1:"&amp;LEN(G73))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G73)))-1)))</f>
+        <v>495</v>
+      </c>
+      <c r="I73" s="2">
+        <f ca="1">H73*B$15</f>
+        <v>11880</v>
+      </c>
+      <c r="J73" s="2">
+        <f ca="1">LEN(DEC2BIN(2^_xlfn.FLOOR.MATH((I73+1)/8192)))</f>
+        <v>2</v>
+      </c>
+      <c r="K73" s="2" cm="1">
+        <f t="array" aca="1" ref="K73" ca="1">_xlfn.SWITCH(J73,1,8*2^10 - I73, 2, 8*2^10 -I73, 3, 24*2^10 -I73)</f>
+        <v>-3688</v>
+      </c>
+      <c r="L73" s="2" cm="1">
+        <f t="array" aca="1" ref="L73" ca="1">_xlfn.SWITCH(J73,1,K73*G$20, 2, K73*G$21, 3, K73*G$22)</f>
+        <v>-160973824</v>
+      </c>
+      <c r="M73" s="2">
+        <f t="shared" ref="M73:M83" ca="1" si="18">_xlfn.FLOOR.MATH(L73/2^(B$17+B$17))</f>
+        <v>-154</v>
+      </c>
+      <c r="N73" s="2">
+        <f ca="1">IF(J73=3,M73+170,M73)</f>
+        <v>-154</v>
+      </c>
+      <c r="O73" s="2">
+        <f ca="1">MOD(N73,1024)</f>
+        <v>870</v>
+      </c>
+      <c r="P73" s="2">
+        <f ca="1">O73/2^B$17</f>
+        <v>0.849609375</v>
+      </c>
+      <c r="Q73" s="2">
+        <f ca="1">P73*360</f>
+        <v>305.859375</v>
+      </c>
+    </row>
+    <row r="74" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="F74" s="2">
+        <f t="shared" ca="1" si="14"/>
+        <v>0.26171875</v>
+      </c>
+      <c r="G74" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H74" s="2" cm="1">
+        <f t="array" aca="1" ref="H74" ca="1">SUMPRODUCT(--MID(G74,LEN(G74)+1-ROW(INDIRECT("1:"&amp;LEN(G74))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G74)))-1)))</f>
+        <v>268</v>
+      </c>
+      <c r="I74" s="2">
+        <f t="shared" ref="I74:I84" ca="1" si="19">H74*B$15</f>
+        <v>6432</v>
+      </c>
+      <c r="J74" s="2">
+        <f t="shared" ref="J74:J84" ca="1" si="20">LEN(DEC2BIN(2^_xlfn.FLOOR.MATH((I74+1)/8192)))</f>
+        <v>1</v>
+      </c>
+      <c r="K74" s="2" cm="1">
+        <f t="array" aca="1" ref="K74" ca="1">_xlfn.SWITCH(J74,1,8*2^10 - I74, 2, 8*2^10 -I74, 3, 24*2^10 -I74)</f>
+        <v>1760</v>
+      </c>
+      <c r="L74" s="2" cm="1">
+        <f t="array" aca="1" ref="L74" ca="1">_xlfn.SWITCH(J74,1,K74*G$20, 2, K74*G$21, 3, K74*G$22)</f>
+        <v>38410240</v>
+      </c>
+      <c r="M74" s="2">
+        <f t="shared" ca="1" si="18"/>
+        <v>36</v>
+      </c>
+      <c r="N74" s="2">
+        <f t="shared" ref="N74:N84" ca="1" si="21">IF(J74=3,M74+170,M74)</f>
+        <v>36</v>
+      </c>
+      <c r="O74" s="2">
+        <f t="shared" ref="O74:O84" ca="1" si="22">MOD(N74,1024)</f>
+        <v>36</v>
+      </c>
+      <c r="P74" s="2">
+        <f t="shared" ref="P74:P84" ca="1" si="23">O74/2^B$17</f>
+        <v>3.515625E-2</v>
+      </c>
+      <c r="Q74" s="2">
+        <f t="shared" ref="Q74:Q84" ca="1" si="24">P74*360</f>
+        <v>12.65625</v>
+      </c>
+    </row>
+    <row r="75" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="F75" s="2">
+        <f t="shared" ca="1" si="14"/>
+        <v>0.84375</v>
+      </c>
+      <c r="G75" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H75" s="2" cm="1">
+        <f t="array" aca="1" ref="H75" ca="1">SUMPRODUCT(--MID(G75,LEN(G75)+1-ROW(INDIRECT("1:"&amp;LEN(G75))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G75)))-1)))</f>
+        <v>864</v>
+      </c>
+      <c r="I75" s="2">
+        <f t="shared" ca="1" si="19"/>
+        <v>20736</v>
+      </c>
+      <c r="J75" s="2">
+        <f t="shared" ca="1" si="20"/>
+        <v>3</v>
+      </c>
+      <c r="K75" s="2" cm="1">
+        <f t="array" aca="1" ref="K75" ca="1">_xlfn.SWITCH(J75,1,8*2^10 - I75, 2, 8*2^10 -I75, 3, 24*2^10 -I75)</f>
+        <v>3840</v>
+      </c>
+      <c r="L75" s="2" cm="1">
+        <f t="array" aca="1" ref="L75" ca="1">_xlfn.SWITCH(J75,1,K75*G$20, 2, K75*G$21, 3, K75*G$22)</f>
+        <v>251412480</v>
+      </c>
+      <c r="M75" s="2">
+        <f t="shared" ca="1" si="18"/>
+        <v>239</v>
+      </c>
+      <c r="N75" s="2">
+        <f t="shared" ca="1" si="21"/>
+        <v>409</v>
+      </c>
+      <c r="O75" s="2">
+        <f t="shared" ca="1" si="22"/>
+        <v>409</v>
+      </c>
+      <c r="P75" s="2">
+        <f t="shared" ca="1" si="23"/>
+        <v>0.3994140625</v>
+      </c>
+      <c r="Q75" s="2">
+        <f t="shared" ca="1" si="24"/>
+        <v>143.7890625</v>
+      </c>
+    </row>
+    <row r="76" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="F76" s="2">
+        <f t="shared" ca="1" si="14"/>
+        <v>0.94140625</v>
+      </c>
+      <c r="G76" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H76" s="2" cm="1">
+        <f t="array" aca="1" ref="H76" ca="1">SUMPRODUCT(--MID(G76,LEN(G76)+1-ROW(INDIRECT("1:"&amp;LEN(G76))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G76)))-1)))</f>
+        <v>964</v>
+      </c>
+      <c r="I76" s="2">
+        <f t="shared" ca="1" si="19"/>
+        <v>23136</v>
+      </c>
+      <c r="J76" s="2">
+        <f t="shared" ca="1" si="20"/>
+        <v>3</v>
+      </c>
+      <c r="K76" s="2" cm="1">
+        <f t="array" aca="1" ref="K76" ca="1">_xlfn.SWITCH(J76,1,8*2^10 - I76, 2, 8*2^10 -I76, 3, 24*2^10 -I76)</f>
+        <v>1440</v>
+      </c>
+      <c r="L76" s="2" cm="1">
+        <f t="array" aca="1" ref="L76" ca="1">_xlfn.SWITCH(J76,1,K76*G$20, 2, K76*G$21, 3, K76*G$22)</f>
+        <v>94279680</v>
+      </c>
+      <c r="M76" s="2">
+        <f t="shared" ca="1" si="18"/>
+        <v>89</v>
+      </c>
+      <c r="N76" s="2">
+        <f t="shared" ca="1" si="21"/>
+        <v>259</v>
+      </c>
+      <c r="O76" s="2">
+        <f t="shared" ca="1" si="22"/>
+        <v>259</v>
+      </c>
+      <c r="P76" s="2">
+        <f t="shared" ca="1" si="23"/>
+        <v>0.2529296875</v>
+      </c>
+      <c r="Q76" s="2">
+        <f t="shared" ca="1" si="24"/>
+        <v>91.0546875</v>
+      </c>
+    </row>
+    <row r="77" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="F77" s="2">
+        <f t="shared" ca="1" si="14"/>
+        <v>0.7763671875</v>
+      </c>
+      <c r="G77" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H77" s="2" cm="1">
+        <f t="array" aca="1" ref="H77" ca="1">SUMPRODUCT(--MID(G77,LEN(G77)+1-ROW(INDIRECT("1:"&amp;LEN(G77))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G77)))-1)))</f>
+        <v>795</v>
+      </c>
+      <c r="I77" s="2">
+        <f t="shared" ca="1" si="19"/>
+        <v>19080</v>
+      </c>
+      <c r="J77" s="2">
+        <f t="shared" ca="1" si="20"/>
+        <v>3</v>
+      </c>
+      <c r="K77" s="2" cm="1">
+        <f t="array" aca="1" ref="K77" ca="1">_xlfn.SWITCH(J77,1,8*2^10 - I77, 2, 8*2^10 -I77, 3, 24*2^10 -I77)</f>
+        <v>5496</v>
+      </c>
+      <c r="L77" s="2" cm="1">
+        <f t="array" aca="1" ref="L77" ca="1">_xlfn.SWITCH(J77,1,K77*G$20, 2, K77*G$21, 3, K77*G$22)</f>
+        <v>359834112</v>
+      </c>
+      <c r="M77" s="2">
+        <f t="shared" ca="1" si="18"/>
+        <v>343</v>
+      </c>
+      <c r="N77" s="2">
+        <f t="shared" ca="1" si="21"/>
+        <v>513</v>
+      </c>
+      <c r="O77" s="2">
+        <f t="shared" ca="1" si="22"/>
+        <v>513</v>
+      </c>
+      <c r="P77" s="2">
+        <f t="shared" ca="1" si="23"/>
+        <v>0.5009765625</v>
+      </c>
+      <c r="Q77" s="2">
+        <f t="shared" ca="1" si="24"/>
+        <v>180.3515625</v>
+      </c>
+    </row>
+    <row r="78" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="F78" s="2">
+        <f t="shared" ca="1" si="14"/>
+        <v>0.638671875</v>
+      </c>
+      <c r="G78" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H78" s="2" cm="1">
+        <f t="array" aca="1" ref="H78" ca="1">SUMPRODUCT(--MID(G78,LEN(G78)+1-ROW(INDIRECT("1:"&amp;LEN(G78))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G78)))-1)))</f>
+        <v>654</v>
+      </c>
+      <c r="I78" s="2">
+        <f t="shared" ca="1" si="19"/>
+        <v>15696</v>
+      </c>
+      <c r="J78" s="2">
+        <f t="shared" ca="1" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="K78" s="2" cm="1">
+        <f t="array" aca="1" ref="K78" ca="1">_xlfn.SWITCH(J78,1,8*2^10 - I78, 2, 8*2^10 -I78, 3, 24*2^10 -I78)</f>
+        <v>-7504</v>
+      </c>
+      <c r="L78" s="2" cm="1">
+        <f t="array" aca="1" ref="L78" ca="1">_xlfn.SWITCH(J78,1,K78*G$20, 2, K78*G$21, 3, K78*G$22)</f>
+        <v>-327534592</v>
+      </c>
+      <c r="M78" s="2">
+        <f t="shared" ca="1" si="18"/>
+        <v>-313</v>
+      </c>
+      <c r="N78" s="2">
+        <f t="shared" ca="1" si="21"/>
+        <v>-313</v>
+      </c>
+      <c r="O78" s="2">
+        <f t="shared" ca="1" si="22"/>
+        <v>711</v>
+      </c>
+      <c r="P78" s="2">
+        <f t="shared" ca="1" si="23"/>
+        <v>0.6943359375</v>
+      </c>
+      <c r="Q78" s="2">
+        <f t="shared" ca="1" si="24"/>
+        <v>249.9609375</v>
+      </c>
+    </row>
+    <row r="79" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="F79" s="2">
+        <f t="shared" ca="1" si="14"/>
+        <v>0.3369140625</v>
+      </c>
+      <c r="G79" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H79" s="2" cm="1">
+        <f t="array" aca="1" ref="H79" ca="1">SUMPRODUCT(--MID(G79,LEN(G79)+1-ROW(INDIRECT("1:"&amp;LEN(G79))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G79)))-1)))</f>
+        <v>345</v>
+      </c>
+      <c r="I79" s="2">
+        <f t="shared" ca="1" si="19"/>
+        <v>8280</v>
+      </c>
+      <c r="J79" s="2">
+        <f t="shared" ca="1" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="K79" s="2" cm="1">
+        <f t="array" aca="1" ref="K79" ca="1">_xlfn.SWITCH(J79,1,8*2^10 - I79, 2, 8*2^10 -I79, 3, 24*2^10 -I79)</f>
+        <v>-88</v>
+      </c>
+      <c r="L79" s="2" cm="1">
+        <f t="array" aca="1" ref="L79" ca="1">_xlfn.SWITCH(J79,1,K79*G$20, 2, K79*G$21, 3, K79*G$22)</f>
+        <v>-3841024</v>
+      </c>
+      <c r="M79" s="2">
+        <f t="shared" ca="1" si="18"/>
+        <v>-4</v>
+      </c>
+      <c r="N79" s="2">
+        <f t="shared" ca="1" si="21"/>
+        <v>-4</v>
+      </c>
+      <c r="O79" s="2">
+        <f t="shared" ca="1" si="22"/>
+        <v>1020</v>
+      </c>
+      <c r="P79" s="2">
+        <f t="shared" ca="1" si="23"/>
+        <v>0.99609375</v>
+      </c>
+      <c r="Q79" s="2">
+        <f t="shared" ca="1" si="24"/>
+        <v>358.59375</v>
+      </c>
+    </row>
+    <row r="80" spans="6:17" x14ac:dyDescent="0.3">
+      <c r="F80" s="2">
+        <f t="shared" ca="1" si="14"/>
+        <v>0.560546875</v>
+      </c>
+      <c r="G80" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H80" s="2" cm="1">
+        <f t="array" aca="1" ref="H80" ca="1">SUMPRODUCT(--MID(G80,LEN(G80)+1-ROW(INDIRECT("1:"&amp;LEN(G80))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G80)))-1)))</f>
+        <v>574</v>
+      </c>
+      <c r="I80" s="2">
+        <f t="shared" ca="1" si="19"/>
+        <v>13776</v>
+      </c>
+      <c r="J80" s="2">
+        <f t="shared" ca="1" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="K80" s="2" cm="1">
+        <f t="array" aca="1" ref="K80" ca="1">_xlfn.SWITCH(J80,1,8*2^10 - I80, 2, 8*2^10 -I80, 3, 24*2^10 -I80)</f>
+        <v>-5584</v>
+      </c>
+      <c r="L80" s="2" cm="1">
+        <f t="array" aca="1" ref="L80" ca="1">_xlfn.SWITCH(J80,1,K80*G$20, 2, K80*G$21, 3, K80*G$22)</f>
+        <v>-243730432</v>
+      </c>
+      <c r="M80" s="2">
+        <f t="shared" ca="1" si="18"/>
+        <v>-233</v>
+      </c>
+      <c r="N80" s="2">
+        <f t="shared" ca="1" si="21"/>
+        <v>-233</v>
+      </c>
+      <c r="O80" s="2">
+        <f t="shared" ca="1" si="22"/>
+        <v>791</v>
+      </c>
+      <c r="P80" s="2">
+        <f t="shared" ca="1" si="23"/>
+        <v>0.7724609375</v>
+      </c>
+      <c r="Q80" s="2">
+        <f t="shared" ca="1" si="24"/>
+        <v>278.0859375</v>
+      </c>
+    </row>
+    <row r="81" spans="6:25" x14ac:dyDescent="0.3">
+      <c r="F81" s="2">
+        <f t="shared" ca="1" si="14"/>
+        <v>3.90625E-2</v>
+      </c>
+      <c r="G81" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="H81" s="2" cm="1">
+        <f t="array" aca="1" ref="H81" ca="1">SUMPRODUCT(--MID(G81,LEN(G81)+1-ROW(INDIRECT("1:"&amp;LEN(G81))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G81)))-1)))</f>
+        <v>40</v>
+      </c>
+      <c r="I81" s="2">
+        <f t="shared" ca="1" si="19"/>
+        <v>960</v>
+      </c>
+      <c r="J81" s="2">
+        <f t="shared" ca="1" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="K81" s="2" cm="1">
+        <f t="array" aca="1" ref="K81" ca="1">_xlfn.SWITCH(J81,1,8*2^10 - I81, 2, 8*2^10 -I81, 3, 24*2^10 -I81)</f>
+        <v>7232</v>
+      </c>
+      <c r="L81" s="2" cm="1">
+        <f t="array" aca="1" ref="L81" ca="1">_xlfn.SWITCH(J81,1,K81*G$20, 2, K81*G$21, 3, K81*G$22)</f>
+        <v>157831168</v>
+      </c>
+      <c r="M81" s="2">
+        <f t="shared" ca="1" si="18"/>
+        <v>150</v>
+      </c>
+      <c r="N81" s="2">
+        <f t="shared" ca="1" si="21"/>
+        <v>150</v>
+      </c>
+      <c r="O81" s="2">
+        <f t="shared" ca="1" si="22"/>
+        <v>150</v>
+      </c>
+      <c r="P81" s="2">
+        <f t="shared" ca="1" si="23"/>
+        <v>0.146484375</v>
+      </c>
+      <c r="Q81" s="2">
+        <f t="shared" ca="1" si="24"/>
+        <v>52.734375</v>
+      </c>
+    </row>
+    <row r="82" spans="6:25" x14ac:dyDescent="0.3">
+      <c r="F82" s="2">
+        <f t="shared" ca="1" si="14"/>
+        <v>0.8330078125</v>
+      </c>
+      <c r="G82" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H82" s="2" cm="1">
+        <f t="array" aca="1" ref="H82" ca="1">SUMPRODUCT(--MID(G82,LEN(G82)+1-ROW(INDIRECT("1:"&amp;LEN(G82))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G82)))-1)))</f>
+        <v>853</v>
+      </c>
+      <c r="I82" s="2">
+        <f t="shared" ca="1" si="19"/>
+        <v>20472</v>
+      </c>
+      <c r="J82" s="2">
+        <f t="shared" ca="1" si="20"/>
+        <v>3</v>
+      </c>
+      <c r="K82" s="2" cm="1">
+        <f t="array" aca="1" ref="K82" ca="1">_xlfn.SWITCH(J82,1,8*2^10 - I82, 2, 8*2^10 -I82, 3, 24*2^10 -I82)</f>
+        <v>4104</v>
+      </c>
+      <c r="L82" s="2" cm="1">
+        <f t="array" aca="1" ref="L82" ca="1">_xlfn.SWITCH(J82,1,K82*G$20, 2, K82*G$21, 3, K82*G$22)</f>
+        <v>268697088</v>
+      </c>
+      <c r="M82" s="2">
+        <f t="shared" ca="1" si="18"/>
+        <v>256</v>
+      </c>
+      <c r="N82" s="2">
+        <f t="shared" ca="1" si="21"/>
+        <v>426</v>
+      </c>
+      <c r="O82" s="2">
+        <f t="shared" ca="1" si="22"/>
+        <v>426</v>
+      </c>
+      <c r="P82" s="2">
+        <f t="shared" ca="1" si="23"/>
+        <v>0.416015625</v>
+      </c>
+      <c r="Q82" s="2">
+        <f t="shared" ca="1" si="24"/>
+        <v>149.765625</v>
+      </c>
+    </row>
+    <row r="83" spans="6:25" x14ac:dyDescent="0.3">
+      <c r="F83" s="2">
+        <f t="shared" ca="1" si="14"/>
+        <v>0.8330078125</v>
+      </c>
+      <c r="G83" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H83" s="2" cm="1">
+        <f t="array" aca="1" ref="H83" ca="1">SUMPRODUCT(--MID(G83,LEN(G83)+1-ROW(INDIRECT("1:"&amp;LEN(G83))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G83)))-1)))</f>
+        <v>853</v>
+      </c>
+      <c r="I83" s="2">
+        <f t="shared" ca="1" si="19"/>
+        <v>20472</v>
+      </c>
+      <c r="J83" s="2">
+        <f t="shared" ca="1" si="20"/>
+        <v>3</v>
+      </c>
+      <c r="K83" s="2" cm="1">
+        <f t="array" aca="1" ref="K83" ca="1">_xlfn.SWITCH(J83,1,8*2^10 - I83, 2, 8*2^10 -I83, 3, 24*2^10 -I83)</f>
+        <v>4104</v>
+      </c>
+      <c r="L83" s="2" cm="1">
+        <f t="array" aca="1" ref="L83" ca="1">_xlfn.SWITCH(J83,1,K83*G$20, 2, K83*G$21, 3, K83*G$22)</f>
+        <v>268697088</v>
+      </c>
+      <c r="M83" s="2">
+        <f t="shared" ca="1" si="18"/>
+        <v>256</v>
+      </c>
+      <c r="N83" s="2">
+        <f t="shared" ca="1" si="21"/>
+        <v>426</v>
+      </c>
+      <c r="O83" s="2">
+        <f t="shared" ca="1" si="22"/>
+        <v>426</v>
+      </c>
+      <c r="P83" s="2">
+        <f t="shared" ca="1" si="23"/>
+        <v>0.416015625</v>
+      </c>
+      <c r="Q83" s="2">
+        <f t="shared" ca="1" si="24"/>
+        <v>149.765625</v>
+      </c>
+    </row>
+    <row r="84" spans="6:25" x14ac:dyDescent="0.3">
+      <c r="F84" s="2">
+        <f t="shared" ca="1" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="G84" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H84" s="2" cm="1">
+        <f t="array" aca="1" ref="H84" ca="1">SUMPRODUCT(--MID(G84,LEN(G84)+1-ROW(INDIRECT("1:"&amp;LEN(G84))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G84)))-1)))</f>
+        <v>0</v>
+      </c>
+      <c r="I84" s="2">
+        <f t="shared" ca="1" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="J84" s="2">
+        <f t="shared" ca="1" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="K84" s="2" cm="1">
+        <f t="array" aca="1" ref="K84" ca="1">_xlfn.SWITCH(J84,1,8*2^10 - I84, 2, 8*2^10 -I84, 3, 24*2^10 -I84)</f>
+        <v>8192</v>
+      </c>
+      <c r="L84" s="2" cm="1">
+        <f t="array" aca="1" ref="L84" ca="1">_xlfn.SWITCH(J84,1,K84*G$20, 2, K84*G$21, 3, K84*G$22)</f>
+        <v>178782208</v>
+      </c>
+      <c r="M84" s="2">
+        <f ca="1">_xlfn.FLOOR.MATH(L84/2^(B$17+B$17))</f>
+        <v>170</v>
+      </c>
+      <c r="N84" s="2">
+        <f t="shared" ca="1" si="21"/>
+        <v>170</v>
+      </c>
+      <c r="O84" s="2">
+        <f t="shared" ca="1" si="22"/>
+        <v>170</v>
+      </c>
+      <c r="P84" s="2">
+        <f t="shared" ca="1" si="23"/>
+        <v>0.166015625</v>
+      </c>
+      <c r="Q84" s="2">
+        <f t="shared" ca="1" si="24"/>
+        <v>59.765625</v>
+      </c>
+    </row>
+    <row r="87" spans="6:25" x14ac:dyDescent="0.3">
+      <c r="I87" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J87" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K87" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L87" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M87" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N87" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O87" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="P87" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q87" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R87" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="S87" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="T87" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="U87" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="V87" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="W87" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="X87" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y87" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="88" spans="6:25" x14ac:dyDescent="0.3">
+      <c r="I88" s="2">
+        <f ca="1">O73*E$31</f>
+        <v>5220</v>
+      </c>
+      <c r="J88" s="2">
+        <f ca="1">_xlfn.FLOOR.MATH(I88/2^B$17)</f>
+        <v>5</v>
+      </c>
+      <c r="K88" s="2">
+        <f ca="1">MOD(I88, 2^B$17)</f>
+        <v>100</v>
+      </c>
+      <c r="L88" s="2">
+        <f ca="1">IF(E33,K59,L59)</f>
+        <v>600</v>
+      </c>
+      <c r="M88" s="2">
+        <f ca="1">L88*E$30</f>
+        <v>982800</v>
+      </c>
+      <c r="N88" s="2">
+        <f ca="1">IF(_xlfn.FLOOR.MATH(M88/2^B$17) &gt; 1023, 1023, _xlfn.FLOOR.MATH(M88/2^B$17))</f>
+        <v>959</v>
+      </c>
+      <c r="O88" s="2">
+        <f ca="1">IF(N88&gt;E$32,E$32,N88)</f>
+        <v>959</v>
+      </c>
+      <c r="P88" s="2">
+        <f ca="1">_xlfn.FLOOR.MATH(O88/2^(B$17-8))</f>
+        <v>239</v>
+      </c>
+      <c r="Q88" s="2">
+        <f ca="1">O88*K88</f>
+        <v>95900</v>
+      </c>
+      <c r="R88" s="2">
+        <f ca="1">O88*(2^(B$17) - 1 - K88)</f>
+        <v>885157</v>
+      </c>
+      <c r="S88" s="2">
+        <f ca="1">_xlfn.FLOOR.MATH(Q88/2^(2*B$17-8))</f>
+        <v>23</v>
+      </c>
+      <c r="T88" s="2">
+        <f ca="1">_xlfn.FLOOR.MATH(R88/2^(2*B$17-8))</f>
+        <v>216</v>
+      </c>
+      <c r="U88" s="2" cm="1">
+        <f t="array" aca="1" ref="U88" ca="1">_xlfn.SWITCH(J88,0,P88,1,T88,2,0,3,0,4,S88,5,P88)</f>
+        <v>239</v>
+      </c>
+      <c r="V88" s="2" cm="1">
+        <f t="array" aca="1" ref="V88" ca="1">_xlfn.SWITCH(J88,0,S88,1,P88,2,P88,3,T88,4,0,5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="W88" s="2" cm="1">
+        <f t="array" aca="1" ref="W88" ca="1">_xlfn.SWITCH(J88,0,0,1,0,2,S88,3,P88,4,P88,5,T88)</f>
+        <v>216</v>
+      </c>
+      <c r="X88" s="2">
+        <f ca="1">U88*2^16+V88*2^8+W88</f>
+        <v>15663320</v>
+      </c>
+      <c r="Y88" s="2" t="str">
+        <f ca="1">_xlfn.BASE(X88,16,6)</f>
+        <v>EF00D8</v>
+      </c>
+    </row>
+    <row r="89" spans="6:25" x14ac:dyDescent="0.3">
+      <c r="I89" s="2">
+        <f t="shared" ref="I89:I101" ca="1" si="25">O74*E$31</f>
+        <v>216</v>
+      </c>
+      <c r="J89" s="2">
+        <f t="shared" ref="J89:J99" ca="1" si="26">_xlfn.FLOOR.MATH(I89/2^B$17)</f>
+        <v>0</v>
+      </c>
+      <c r="K89" s="2">
+        <f t="shared" ref="K89:K99" ca="1" si="27">MOD(I89, 2^B$17)</f>
+        <v>216</v>
+      </c>
+      <c r="L89" s="2">
+        <f t="shared" ref="L89:L99" ca="1" si="28">IF(E34,K60,L60)</f>
+        <v>717</v>
+      </c>
+      <c r="M89" s="2">
+        <f t="shared" ref="M89:M99" ca="1" si="29">L89*E$30</f>
+        <v>1174446</v>
+      </c>
+      <c r="N89" s="2">
+        <f t="shared" ref="N89:N99" ca="1" si="30">IF(_xlfn.FLOOR.MATH(M89/2^B$17) &gt; 1023, 1023, _xlfn.FLOOR.MATH(M89/2^B$17))</f>
+        <v>1023</v>
+      </c>
+      <c r="O89" s="2">
+        <f t="shared" ref="O89:O99" ca="1" si="31">IF(N89&gt;E$32,E$32,N89)</f>
+        <v>1023</v>
+      </c>
+      <c r="P89" s="2">
+        <f t="shared" ref="P89:P99" ca="1" si="32">_xlfn.FLOOR.MATH(O89/2^(B$17-8))</f>
+        <v>255</v>
+      </c>
+      <c r="Q89" s="2">
+        <f t="shared" ref="Q89:Q99" ca="1" si="33">O89*K89</f>
+        <v>220968</v>
+      </c>
+      <c r="R89" s="2">
+        <f t="shared" ref="R89:R99" ca="1" si="34">O89*(2^(B$17) - 1 - K89)</f>
+        <v>825561</v>
+      </c>
+      <c r="S89" s="2">
+        <f t="shared" ref="S89:S99" ca="1" si="35">_xlfn.FLOOR.MATH(Q89/2^(2*B$17-8))</f>
+        <v>53</v>
+      </c>
+      <c r="T89" s="2">
+        <f t="shared" ref="T89:T99" ca="1" si="36">_xlfn.FLOOR.MATH(R89/2^(2*B$17-8))</f>
+        <v>201</v>
+      </c>
+      <c r="U89" s="2" cm="1">
+        <f t="array" aca="1" ref="U89" ca="1">_xlfn.SWITCH(J89,0,P89,1,T89,2,0,3,0,4,S89,5,P89)</f>
+        <v>255</v>
+      </c>
+      <c r="V89" s="2" cm="1">
+        <f t="array" aca="1" ref="V89" ca="1">_xlfn.SWITCH(J89,0,S89,1,P89,2,P89,3,T89,4,0,5,0)</f>
+        <v>53</v>
+      </c>
+      <c r="W89" s="2" cm="1">
+        <f t="array" aca="1" ref="W89" ca="1">_xlfn.SWITCH(J89,0,0,1,0,2,S89,3,P89,4,P89,5,T89)</f>
+        <v>0</v>
+      </c>
+      <c r="X89" s="2">
+        <f t="shared" ref="X89:X99" ca="1" si="37">U89*2^16+V89*2^8+W89</f>
+        <v>16725248</v>
+      </c>
+      <c r="Y89" s="2" t="str">
+        <f t="shared" ref="Y89:Y99" ca="1" si="38">_xlfn.BASE(X89,16,6)</f>
+        <v>FF3500</v>
+      </c>
+    </row>
+    <row r="90" spans="6:25" x14ac:dyDescent="0.3">
+      <c r="I90" s="2">
+        <f t="shared" ca="1" si="25"/>
+        <v>2454</v>
+      </c>
+      <c r="J90" s="2">
+        <f t="shared" ca="1" si="26"/>
+        <v>2</v>
+      </c>
+      <c r="K90" s="2">
+        <f t="shared" ca="1" si="27"/>
+        <v>406</v>
+      </c>
+      <c r="L90" s="2">
+        <f t="shared" ca="1" si="28"/>
+        <v>450</v>
+      </c>
+      <c r="M90" s="2">
+        <f t="shared" ca="1" si="29"/>
+        <v>737100</v>
+      </c>
+      <c r="N90" s="2">
+        <f t="shared" ca="1" si="30"/>
+        <v>719</v>
+      </c>
+      <c r="O90" s="2">
+        <f t="shared" ca="1" si="31"/>
+        <v>719</v>
+      </c>
+      <c r="P90" s="2">
+        <f t="shared" ca="1" si="32"/>
+        <v>179</v>
+      </c>
+      <c r="Q90" s="2">
+        <f t="shared" ca="1" si="33"/>
+        <v>291914</v>
+      </c>
+      <c r="R90" s="2">
+        <f t="shared" ca="1" si="34"/>
+        <v>443623</v>
+      </c>
+      <c r="S90" s="2">
+        <f t="shared" ca="1" si="35"/>
+        <v>71</v>
+      </c>
+      <c r="T90" s="2">
+        <f t="shared" ca="1" si="36"/>
+        <v>108</v>
+      </c>
+      <c r="U90" s="2" cm="1">
+        <f t="array" aca="1" ref="U90" ca="1">_xlfn.SWITCH(J90,0,P90,1,T90,2,0,3,0,4,S90,5,P90)</f>
+        <v>0</v>
+      </c>
+      <c r="V90" s="2" cm="1">
+        <f t="array" aca="1" ref="V90" ca="1">_xlfn.SWITCH(J90,0,S90,1,P90,2,P90,3,T90,4,0,5,0)</f>
+        <v>179</v>
+      </c>
+      <c r="W90" s="2" cm="1">
+        <f t="array" aca="1" ref="W90" ca="1">_xlfn.SWITCH(J90,0,0,1,0,2,S90,3,P90,4,P90,5,T90)</f>
+        <v>71</v>
+      </c>
+      <c r="X90" s="2">
+        <f t="shared" ca="1" si="37"/>
+        <v>45895</v>
+      </c>
+      <c r="Y90" s="2" t="str">
+        <f t="shared" ca="1" si="38"/>
+        <v>00B347</v>
+      </c>
+    </row>
+    <row r="91" spans="6:25" x14ac:dyDescent="0.3">
+      <c r="I91" s="2">
+        <f t="shared" ca="1" si="25"/>
+        <v>1554</v>
+      </c>
+      <c r="J91" s="2">
+        <f t="shared" ca="1" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="K91" s="2">
+        <f t="shared" ca="1" si="27"/>
+        <v>530</v>
+      </c>
+      <c r="L91" s="2">
+        <f t="shared" ca="1" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="M91" s="2">
+        <f t="shared" ca="1" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="N91" s="2">
+        <f t="shared" ca="1" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="O91" s="2">
+        <f t="shared" ca="1" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="P91" s="2">
+        <f t="shared" ca="1" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="Q91" s="2">
+        <f t="shared" ca="1" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="R91" s="2">
+        <f t="shared" ca="1" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="S91" s="2">
+        <f t="shared" ca="1" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="T91" s="2">
+        <f t="shared" ca="1" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="U91" s="2" cm="1">
+        <f t="array" aca="1" ref="U91" ca="1">_xlfn.SWITCH(J91,0,P91,1,T91,2,0,3,0,4,S91,5,P91)</f>
+        <v>0</v>
+      </c>
+      <c r="V91" s="2" cm="1">
+        <f t="array" aca="1" ref="V91" ca="1">_xlfn.SWITCH(J91,0,S91,1,P91,2,P91,3,T91,4,0,5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="W91" s="2" cm="1">
+        <f t="array" aca="1" ref="W91" ca="1">_xlfn.SWITCH(J91,0,0,1,0,2,S91,3,P91,4,P91,5,T91)</f>
+        <v>0</v>
+      </c>
+      <c r="X91" s="2">
+        <f t="shared" ca="1" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="Y91" s="2" t="str">
+        <f t="shared" ca="1" si="38"/>
+        <v>000000</v>
+      </c>
+    </row>
+    <row r="92" spans="6:25" x14ac:dyDescent="0.3">
+      <c r="I92" s="2">
+        <f t="shared" ca="1" si="25"/>
+        <v>3078</v>
+      </c>
+      <c r="J92" s="2">
+        <f t="shared" ca="1" si="26"/>
+        <v>3</v>
+      </c>
+      <c r="K92" s="2">
+        <f t="shared" ca="1" si="27"/>
+        <v>6</v>
+      </c>
+      <c r="L92" s="2">
+        <f t="shared" ca="1" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="M92" s="2">
+        <f t="shared" ca="1" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="N92" s="2">
+        <f t="shared" ca="1" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="O92" s="2">
+        <f t="shared" ca="1" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="P92" s="2">
+        <f t="shared" ca="1" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="Q92" s="2">
+        <f t="shared" ca="1" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="R92" s="2">
+        <f t="shared" ca="1" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="S92" s="2">
+        <f t="shared" ca="1" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="T92" s="2">
+        <f t="shared" ca="1" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="U92" s="2" cm="1">
+        <f t="array" aca="1" ref="U92" ca="1">_xlfn.SWITCH(J92,0,P92,1,T92,2,0,3,0,4,S92,5,P92)</f>
+        <v>0</v>
+      </c>
+      <c r="V92" s="2" cm="1">
+        <f t="array" aca="1" ref="V92" ca="1">_xlfn.SWITCH(J92,0,S92,1,P92,2,P92,3,T92,4,0,5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="W92" s="2" cm="1">
+        <f t="array" aca="1" ref="W92" ca="1">_xlfn.SWITCH(J92,0,0,1,0,2,S92,3,P92,4,P92,5,T92)</f>
+        <v>0</v>
+      </c>
+      <c r="X92" s="2">
+        <f t="shared" ca="1" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="Y92" s="2" t="str">
+        <f t="shared" ca="1" si="38"/>
+        <v>000000</v>
+      </c>
+    </row>
+    <row r="93" spans="6:25" x14ac:dyDescent="0.3">
+      <c r="I93" s="2">
+        <f t="shared" ca="1" si="25"/>
+        <v>4266</v>
+      </c>
+      <c r="J93" s="2">
+        <f t="shared" ca="1" si="26"/>
+        <v>4</v>
+      </c>
+      <c r="K93" s="2">
+        <f t="shared" ca="1" si="27"/>
+        <v>170</v>
+      </c>
+      <c r="L93" s="2">
+        <f t="shared" ca="1" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="M93" s="2">
+        <f t="shared" ca="1" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="N93" s="2">
+        <f t="shared" ca="1" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="O93" s="2">
+        <f t="shared" ca="1" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="P93" s="2">
+        <f t="shared" ca="1" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="Q93" s="2">
+        <f t="shared" ca="1" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="R93" s="2">
+        <f t="shared" ca="1" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="S93" s="2">
+        <f t="shared" ca="1" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="T93" s="2">
+        <f t="shared" ca="1" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="U93" s="2" cm="1">
+        <f t="array" aca="1" ref="U93" ca="1">_xlfn.SWITCH(J93,0,P93,1,T93,2,0,3,0,4,S93,5,P93)</f>
+        <v>0</v>
+      </c>
+      <c r="V93" s="2" cm="1">
+        <f t="array" aca="1" ref="V93" ca="1">_xlfn.SWITCH(J93,0,S93,1,P93,2,P93,3,T93,4,0,5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="W93" s="2" cm="1">
+        <f t="array" aca="1" ref="W93" ca="1">_xlfn.SWITCH(J93,0,0,1,0,2,S93,3,P93,4,P93,5,T93)</f>
+        <v>0</v>
+      </c>
+      <c r="X93" s="2">
+        <f t="shared" ca="1" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="Y93" s="2" t="str">
+        <f t="shared" ca="1" si="38"/>
+        <v>000000</v>
+      </c>
+    </row>
+    <row r="94" spans="6:25" x14ac:dyDescent="0.3">
+      <c r="I94" s="2">
+        <f t="shared" ca="1" si="25"/>
+        <v>6120</v>
+      </c>
+      <c r="J94" s="2">
+        <f t="shared" ca="1" si="26"/>
+        <v>5</v>
+      </c>
+      <c r="K94" s="2">
+        <f t="shared" ca="1" si="27"/>
+        <v>1000</v>
+      </c>
+      <c r="L94" s="2">
+        <f t="shared" ca="1" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="M94" s="2">
+        <f t="shared" ca="1" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="N94" s="2">
+        <f t="shared" ca="1" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="O94" s="2">
+        <f t="shared" ca="1" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="P94" s="2">
+        <f t="shared" ca="1" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="Q94" s="2">
+        <f t="shared" ca="1" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="R94" s="2">
+        <f t="shared" ca="1" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="S94" s="2">
+        <f t="shared" ca="1" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="T94" s="2">
+        <f t="shared" ca="1" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="U94" s="2" cm="1">
+        <f t="array" aca="1" ref="U94" ca="1">_xlfn.SWITCH(J94,0,P94,1,T94,2,0,3,0,4,S94,5,P94)</f>
+        <v>0</v>
+      </c>
+      <c r="V94" s="2" cm="1">
+        <f t="array" aca="1" ref="V94" ca="1">_xlfn.SWITCH(J94,0,S94,1,P94,2,P94,3,T94,4,0,5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="W94" s="2" cm="1">
+        <f t="array" aca="1" ref="W94" ca="1">_xlfn.SWITCH(J94,0,0,1,0,2,S94,3,P94,4,P94,5,T94)</f>
+        <v>0</v>
+      </c>
+      <c r="X94" s="2">
+        <f t="shared" ca="1" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="Y94" s="2" t="str">
+        <f t="shared" ca="1" si="38"/>
+        <v>000000</v>
+      </c>
+    </row>
+    <row r="95" spans="6:25" x14ac:dyDescent="0.3">
+      <c r="I95" s="2">
+        <f t="shared" ca="1" si="25"/>
+        <v>4746</v>
+      </c>
+      <c r="J95" s="2">
+        <f t="shared" ca="1" si="26"/>
+        <v>4</v>
+      </c>
+      <c r="K95" s="2">
+        <f t="shared" ca="1" si="27"/>
+        <v>650</v>
+      </c>
+      <c r="L95" s="2">
+        <f t="shared" ca="1" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="M95" s="2">
+        <f t="shared" ca="1" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="N95" s="2">
+        <f t="shared" ca="1" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="O95" s="2">
+        <f t="shared" ca="1" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="P95" s="2">
+        <f t="shared" ca="1" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="Q95" s="2">
+        <f t="shared" ca="1" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="R95" s="2">
+        <f t="shared" ca="1" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="S95" s="2">
+        <f t="shared" ca="1" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="T95" s="2">
+        <f t="shared" ca="1" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="U95" s="2" cm="1">
+        <f t="array" aca="1" ref="U95" ca="1">_xlfn.SWITCH(J95,0,P95,1,T95,2,0,3,0,4,S95,5,P95)</f>
+        <v>0</v>
+      </c>
+      <c r="V95" s="2" cm="1">
+        <f t="array" aca="1" ref="V95" ca="1">_xlfn.SWITCH(J95,0,S95,1,P95,2,P95,3,T95,4,0,5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="W95" s="2" cm="1">
+        <f t="array" aca="1" ref="W95" ca="1">_xlfn.SWITCH(J95,0,0,1,0,2,S95,3,P95,4,P95,5,T95)</f>
+        <v>0</v>
+      </c>
+      <c r="X95" s="2">
+        <f t="shared" ca="1" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="Y95" s="2" t="str">
+        <f t="shared" ca="1" si="38"/>
+        <v>000000</v>
+      </c>
+    </row>
+    <row r="96" spans="6:25" x14ac:dyDescent="0.3">
+      <c r="I96" s="2">
+        <f t="shared" ca="1" si="25"/>
+        <v>900</v>
+      </c>
+      <c r="J96" s="2">
+        <f t="shared" ca="1" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="K96" s="2">
+        <f t="shared" ca="1" si="27"/>
+        <v>900</v>
+      </c>
+      <c r="L96" s="2">
+        <f t="shared" ca="1" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="M96" s="2">
+        <f t="shared" ca="1" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="N96" s="2">
+        <f t="shared" ca="1" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="O96" s="2">
+        <f t="shared" ca="1" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="P96" s="2">
+        <f t="shared" ca="1" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="Q96" s="2">
+        <f t="shared" ca="1" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="R96" s="2">
+        <f t="shared" ca="1" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="S96" s="2">
+        <f t="shared" ca="1" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="T96" s="2">
+        <f t="shared" ca="1" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="U96" s="2" cm="1">
+        <f t="array" aca="1" ref="U96" ca="1">_xlfn.SWITCH(J96,0,P96,1,T96,2,0,3,0,4,S96,5,P96)</f>
+        <v>0</v>
+      </c>
+      <c r="V96" s="2" cm="1">
+        <f t="array" aca="1" ref="V96" ca="1">_xlfn.SWITCH(J96,0,S96,1,P96,2,P96,3,T96,4,0,5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="W96" s="2" cm="1">
+        <f t="array" aca="1" ref="W96" ca="1">_xlfn.SWITCH(J96,0,0,1,0,2,S96,3,P96,4,P96,5,T96)</f>
+        <v>0</v>
+      </c>
+      <c r="X96" s="2">
+        <f t="shared" ca="1" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="Y96" s="2" t="str">
+        <f t="shared" ca="1" si="38"/>
+        <v>000000</v>
+      </c>
+    </row>
+    <row r="97" spans="9:25" x14ac:dyDescent="0.3">
+      <c r="I97" s="2">
+        <f t="shared" ca="1" si="25"/>
+        <v>2556</v>
+      </c>
+      <c r="J97" s="2">
+        <f t="shared" ca="1" si="26"/>
+        <v>2</v>
+      </c>
+      <c r="K97" s="2">
+        <f t="shared" ca="1" si="27"/>
+        <v>508</v>
+      </c>
+      <c r="L97" s="2">
+        <f t="shared" ca="1" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="M97" s="2">
+        <f t="shared" ca="1" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="N97" s="2">
+        <f t="shared" ca="1" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="O97" s="2">
+        <f t="shared" ca="1" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="P97" s="2">
+        <f t="shared" ca="1" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="Q97" s="2">
+        <f t="shared" ca="1" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="R97" s="2">
+        <f t="shared" ca="1" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="S97" s="2">
+        <f t="shared" ca="1" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="T97" s="2">
+        <f t="shared" ca="1" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="U97" s="2" cm="1">
+        <f t="array" aca="1" ref="U97" ca="1">_xlfn.SWITCH(J97,0,P97,1,T97,2,0,3,0,4,S97,5,P97)</f>
+        <v>0</v>
+      </c>
+      <c r="V97" s="2" cm="1">
+        <f t="array" aca="1" ref="V97" ca="1">_xlfn.SWITCH(J97,0,S97,1,P97,2,P97,3,T97,4,0,5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="W97" s="2" cm="1">
+        <f t="array" aca="1" ref="W97" ca="1">_xlfn.SWITCH(J97,0,0,1,0,2,S97,3,P97,4,P97,5,T97)</f>
+        <v>0</v>
+      </c>
+      <c r="X97" s="2">
+        <f t="shared" ca="1" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="Y97" s="2" t="str">
+        <f t="shared" ca="1" si="38"/>
+        <v>000000</v>
+      </c>
+    </row>
+    <row r="98" spans="9:25" x14ac:dyDescent="0.3">
+      <c r="I98" s="2">
+        <f t="shared" ca="1" si="25"/>
+        <v>2556</v>
+      </c>
+      <c r="J98" s="2">
+        <f t="shared" ca="1" si="26"/>
+        <v>2</v>
+      </c>
+      <c r="K98" s="2">
+        <f t="shared" ca="1" si="27"/>
+        <v>508</v>
+      </c>
+      <c r="L98" s="2">
+        <f t="shared" ca="1" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="M98" s="2">
+        <f t="shared" ca="1" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="N98" s="2">
+        <f t="shared" ca="1" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="O98" s="2">
+        <f t="shared" ca="1" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="P98" s="2">
+        <f t="shared" ca="1" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="Q98" s="2">
+        <f t="shared" ca="1" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="R98" s="2">
+        <f t="shared" ca="1" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="S98" s="2">
+        <f t="shared" ca="1" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="T98" s="2">
+        <f t="shared" ca="1" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="U98" s="2" cm="1">
+        <f t="array" aca="1" ref="U98" ca="1">_xlfn.SWITCH(J98,0,P98,1,T98,2,0,3,0,4,S98,5,P98)</f>
+        <v>0</v>
+      </c>
+      <c r="V98" s="2" cm="1">
+        <f t="array" aca="1" ref="V98" ca="1">_xlfn.SWITCH(J98,0,S98,1,P98,2,P98,3,T98,4,0,5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="W98" s="2" cm="1">
+        <f t="array" aca="1" ref="W98" ca="1">_xlfn.SWITCH(J98,0,0,1,0,2,S98,3,P98,4,P98,5,T98)</f>
+        <v>0</v>
+      </c>
+      <c r="X98" s="2">
+        <f t="shared" ca="1" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="Y98" s="2" t="str">
+        <f t="shared" ca="1" si="38"/>
+        <v>000000</v>
+      </c>
+    </row>
+    <row r="99" spans="9:25" x14ac:dyDescent="0.3">
+      <c r="I99" s="2">
+        <f t="shared" ca="1" si="25"/>
+        <v>1020</v>
+      </c>
+      <c r="J99" s="2">
+        <f t="shared" ca="1" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="K99" s="2">
+        <f t="shared" ca="1" si="27"/>
+        <v>1020</v>
+      </c>
+      <c r="L99" s="2">
+        <f t="shared" ca="1" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="M99" s="2">
+        <f t="shared" ca="1" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="N99" s="2">
+        <f t="shared" ca="1" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="O99" s="2">
+        <f t="shared" ca="1" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="P99" s="2">
+        <f t="shared" ca="1" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="Q99" s="2">
+        <f t="shared" ca="1" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="R99" s="2">
+        <f t="shared" ca="1" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="S99" s="2">
+        <f t="shared" ca="1" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="T99" s="2">
+        <f t="shared" ca="1" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="U99" s="2" cm="1">
+        <f t="array" aca="1" ref="U99" ca="1">_xlfn.SWITCH(J99,0,P99,1,T99,2,0,3,0,4,S99,5,P99)</f>
+        <v>0</v>
+      </c>
+      <c r="V99" s="2" cm="1">
+        <f t="array" aca="1" ref="V99" ca="1">_xlfn.SWITCH(J99,0,S99,1,P99,2,P99,3,T99,4,0,5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="W99" s="2" cm="1">
+        <f t="array" aca="1" ref="W99" ca="1">_xlfn.SWITCH(J99,0,0,1,0,2,S99,3,P99,4,P99,5,T99)</f>
+        <v>0</v>
+      </c>
+      <c r="X99" s="2">
+        <f t="shared" ca="1" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="Y99" s="2" t="str">
+        <f t="shared" ca="1" si="38"/>
+        <v>000000</v>
+      </c>
+    </row>
+    <row r="101" spans="9:25" x14ac:dyDescent="0.3">
+      <c r="I101" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J101" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="102" spans="9:25" x14ac:dyDescent="0.3">
+      <c r="I102" s="2">
+        <f ca="1">I66/B19</f>
+        <v>24.779414062499999</v>
+      </c>
+      <c r="J102" s="2">
+        <f ca="1">K59/I$102</f>
+        <v>17.110583539448857</v>
+      </c>
+    </row>
+    <row r="103" spans="9:25" x14ac:dyDescent="0.3">
+      <c r="J103" s="2">
+        <f t="shared" ref="J103:J118" ca="1" si="39">K60/I$102</f>
+        <v>21.832244822677595</v>
+      </c>
+    </row>
+    <row r="104" spans="9:25" x14ac:dyDescent="0.3">
+      <c r="J104" s="2">
+        <f t="shared" ca="1" si="39"/>
+        <v>11.05717163787355</v>
+      </c>
+    </row>
+    <row r="105" spans="9:25" x14ac:dyDescent="0.3">
+      <c r="J105" s="2">
+        <f t="shared" ca="1" si="39"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="9:25" x14ac:dyDescent="0.3">
+      <c r="J106" s="2">
+        <f t="shared" ca="1" si="39"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="9:25" x14ac:dyDescent="0.3">
+      <c r="J107" s="2">
+        <f t="shared" ca="1" si="39"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="9:25" x14ac:dyDescent="0.3">
+      <c r="J108" s="2">
+        <f t="shared" ca="1" si="39"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="9:25" x14ac:dyDescent="0.3">
+      <c r="J109" s="2">
+        <f t="shared" ca="1" si="39"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="9:25" x14ac:dyDescent="0.3">
+      <c r="J110" s="2">
+        <f t="shared" ca="1" si="39"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="9:25" x14ac:dyDescent="0.3">
+      <c r="J111" s="2">
+        <f t="shared" ca="1" si="39"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="9:25" x14ac:dyDescent="0.3">
+      <c r="J112" s="2">
+        <f t="shared" ca="1" si="39"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J113" s="2">
+        <f t="shared" ca="1" si="39"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J114" s="2">
+        <f t="shared" ca="1" si="39"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6CFBF30-C73F-44F3-B868-D68CE6420F38}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
completed basic testing of LEDDriver2
</commit_message>
<xml_diff>
--- a/other/LinearVisualizer.xlsx
+++ b/other/LinearVisualizer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\CCHW\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9002FC-17E3-43D1-A96C-CC701FCE76E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E2924C-ACA5-4443-8016-4CF75D04D2A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9DBF0F91-83D7-4F64-B04C-B7CB81DC62EF}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{9DBF0F91-83D7-4F64-B04C-B7CB81DC62EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -695,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A6626A4-8C87-4B90-BEEB-AEB487ACEA9E}">
   <dimension ref="A1:Y114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J82" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P106" sqref="P106"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F73" sqref="F73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -764,11 +764,11 @@
       </c>
       <c r="D2" s="2" t="str">
         <f ca="1">_xlfn.CONCAT(B$16+B$17,"'b",REPT("0",B$16-LEN(E2)))</f>
-        <v>16'b00000</v>
+        <v>16'b000</v>
       </c>
       <c r="E2" s="2" t="str">
         <f ca="1">DEC2BIN(_xlfn.FLOOR.MATH(RAND()*10))</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F2" s="2" t="str">
         <f>_xlfn.CONCAT(REPT("0",B$17),";")</f>
@@ -776,23 +776,23 @@
       </c>
       <c r="G2" s="4" t="str">
         <f ca="1">_xlfn.CONCAT(A2,B2,C2,D2,E2,F2)</f>
-        <v xml:space="preserve">            noteAmplitudes_i[ 0] = 16'b0000000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 0] = 16'b0001000000000000;</v>
       </c>
       <c r="H2" s="2">
         <f t="shared" ref="H2:H13" ca="1" si="0">BIN2DEC(E2)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I2" s="2">
         <f t="shared" ref="I2:I13" ca="1" si="1">H2*2^B$17</f>
-        <v>0</v>
+        <v>4096</v>
       </c>
       <c r="J2" s="2">
         <f ca="1">SUM(H2:H13)</f>
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="K2" s="2">
         <f t="shared" ref="K2:K13" ca="1" si="2">I2-J$7</f>
-        <v>-4590</v>
+        <v>-1718</v>
       </c>
       <c r="L2" s="2">
         <f ca="1">IF(K2&gt;0,K2,0)</f>
@@ -815,11 +815,11 @@
       </c>
       <c r="D3" s="2" t="str">
         <f t="shared" ref="D3:D13" ca="1" si="3">_xlfn.CONCAT(B$16+B$17,"'b",REPT("0",B$16-LEN(E3)))</f>
-        <v>16'b00000</v>
+        <v>16'b000</v>
       </c>
       <c r="E3" s="2" t="str">
         <f t="shared" ref="E3:E13" ca="1" si="4">DEC2BIN(_xlfn.FLOOR.MATH(RAND()*10))</f>
-        <v>0</v>
+        <v>111</v>
       </c>
       <c r="F3" s="2" t="str">
         <f t="shared" ref="F3:F13" si="5">_xlfn.CONCAT(REPT("0",B$17),";")</f>
@@ -827,31 +827,31 @@
       </c>
       <c r="G3" s="4" t="str">
         <f t="shared" ref="G3:G13" ca="1" si="6">_xlfn.CONCAT(A3,B3,C3,D3,E3,F3)</f>
-        <v xml:space="preserve">            noteAmplitudes_i[ 1] = 16'b0000000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 1] = 16'b0001110000000000;</v>
       </c>
       <c r="H3" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I3" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>7168</v>
       </c>
       <c r="J3" s="2">
         <f ca="1">J2*2^B17</f>
-        <v>46080</v>
+        <v>58368</v>
       </c>
       <c r="K3" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>-4590</v>
+        <v>1354</v>
       </c>
       <c r="L3" s="2">
         <f t="shared" ref="L3:L13" ca="1" si="7">IF(K3&gt;0,K3,0)</f>
-        <v>0</v>
+        <v>1354</v>
       </c>
       <c r="M3" s="2">
         <f t="shared" ref="M3:M13" ca="1" si="8">IF(K3&gt;0,I3,0)</f>
-        <v>0</v>
+        <v>7168</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -866,11 +866,11 @@
       </c>
       <c r="D4" s="2" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>16'b00000</v>
+        <v>16'b00</v>
       </c>
       <c r="E4" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>1001</v>
       </c>
       <c r="F4" s="2" t="str">
         <f t="shared" si="5"/>
@@ -878,27 +878,27 @@
       </c>
       <c r="G4" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 2] = 16'b0000010000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 2] = 16'b0010010000000000;</v>
       </c>
       <c r="H4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="I4" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>1024</v>
+        <v>9216</v>
       </c>
       <c r="K4" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>-3566</v>
+        <v>3402</v>
       </c>
       <c r="L4" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>3402</v>
       </c>
       <c r="M4" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>9216</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -913,11 +913,11 @@
       </c>
       <c r="D5" s="2" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>16'b000</v>
+        <v>16'b00000</v>
       </c>
       <c r="E5" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>110</v>
+        <v>1</v>
       </c>
       <c r="F5" s="2" t="str">
         <f t="shared" si="5"/>
@@ -925,30 +925,30 @@
       </c>
       <c r="G5" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 3] = 16'b0001100000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 3] = 16'b0000010000000000;</v>
       </c>
       <c r="H5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I5" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>6144</v>
+        <v>1024</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="K5" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1554</v>
+        <v>-4790</v>
       </c>
       <c r="L5" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>1554</v>
+        <v>0</v>
       </c>
       <c r="M5" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>6144</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -963,11 +963,11 @@
       </c>
       <c r="D6" s="2" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>16'b0000</v>
+        <v>16'b00</v>
       </c>
       <c r="E6" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>11</v>
+        <v>1001</v>
       </c>
       <c r="F6" s="2" t="str">
         <f t="shared" si="5"/>
@@ -975,31 +975,31 @@
       </c>
       <c r="G6" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 4] = 16'b0000110000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 4] = 16'b0010010000000000;</v>
       </c>
       <c r="H6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="I6" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>3072</v>
+        <v>9216</v>
       </c>
       <c r="J6" s="3">
         <f ca="1">J2*B18</f>
-        <v>4.482421875</v>
+        <v>5.677734375</v>
       </c>
       <c r="K6" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>-1518</v>
+        <v>3402</v>
       </c>
       <c r="L6" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>3402</v>
       </c>
       <c r="M6" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>9216</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -1018,7 +1018,7 @@
       </c>
       <c r="E7" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="F7" s="2" t="str">
         <f t="shared" si="5"/>
@@ -1026,31 +1026,31 @@
       </c>
       <c r="G7" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 5] = 16'b0001100000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 5] = 16'b0001010000000000;</v>
       </c>
       <c r="H7" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I7" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>6144</v>
+        <v>5120</v>
       </c>
       <c r="J7" s="2">
         <f ca="1">J3 * BIN2DEC(C18) / 2^B17</f>
-        <v>4590</v>
+        <v>5814</v>
       </c>
       <c r="K7" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1554</v>
+        <v>-694</v>
       </c>
       <c r="L7" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>1554</v>
+        <v>0</v>
       </c>
       <c r="M7" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>6144</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -1065,11 +1065,11 @@
       </c>
       <c r="D8" s="2" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>16'b00</v>
+        <v>16'b000</v>
       </c>
       <c r="E8" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1001</v>
+        <v>100</v>
       </c>
       <c r="F8" s="2" t="str">
         <f t="shared" si="5"/>
@@ -1077,27 +1077,27 @@
       </c>
       <c r="G8" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 6] = 16'b0010010000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 6] = 16'b0001000000000000;</v>
       </c>
       <c r="H8" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="I8" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>9216</v>
+        <v>4096</v>
       </c>
       <c r="K8" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>4626</v>
+        <v>-1718</v>
       </c>
       <c r="L8" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>4626</v>
+        <v>0</v>
       </c>
       <c r="M8" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>9216</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -1139,7 +1139,7 @@
       </c>
       <c r="K9" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>-4590</v>
+        <v>-5814</v>
       </c>
       <c r="L9" s="2">
         <f t="shared" ca="1" si="7"/>
@@ -1162,11 +1162,11 @@
       </c>
       <c r="D10" s="2" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>16'b00</v>
+        <v>16'b000</v>
       </c>
       <c r="E10" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1000</v>
+        <v>111</v>
       </c>
       <c r="F10" s="2" t="str">
         <f t="shared" si="5"/>
@@ -1174,31 +1174,31 @@
       </c>
       <c r="G10" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 8] = 16'b0010000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 8] = 16'b0001110000000000;</v>
       </c>
       <c r="H10" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I10" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>8192</v>
+        <v>7168</v>
       </c>
       <c r="J10" s="2">
         <f ca="1">J11/2^B17</f>
-        <v>13.587890625</v>
+        <v>9.611328125</v>
       </c>
       <c r="K10" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>3602</v>
+        <v>1354</v>
       </c>
       <c r="L10" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>3602</v>
+        <v>1354</v>
       </c>
       <c r="M10" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>8192</v>
+        <v>7168</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -1217,7 +1217,7 @@
       </c>
       <c r="E11" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F11" s="2" t="str">
         <f t="shared" si="5"/>
@@ -1225,31 +1225,31 @@
       </c>
       <c r="G11" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 9] = 16'b0001110000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 9] = 16'b0001100000000000;</v>
       </c>
       <c r="H11" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I11" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>7168</v>
+        <v>6144</v>
       </c>
       <c r="J11" s="2">
         <f ca="1">SUM(L2:L13)</f>
-        <v>13914</v>
+        <v>9842</v>
       </c>
       <c r="K11" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>2578</v>
+        <v>330</v>
       </c>
       <c r="L11" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>2578</v>
+        <v>330</v>
       </c>
       <c r="M11" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>7168</v>
+        <v>6144</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -1264,11 +1264,11 @@
       </c>
       <c r="D12" s="2" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>16'b0000</v>
+        <v>16'b00000</v>
       </c>
       <c r="E12" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F12" s="2" t="str">
         <f t="shared" si="5"/>
@@ -1276,19 +1276,19 @@
       </c>
       <c r="G12" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[10] = 16'b0000100000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[10] = 16'b0000010000000000;</v>
       </c>
       <c r="H12" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I12" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>2048</v>
+        <v>1024</v>
       </c>
       <c r="K12" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>-2542</v>
+        <v>-4790</v>
       </c>
       <c r="L12" s="2">
         <f t="shared" ca="1" si="7"/>
@@ -1311,11 +1311,11 @@
       </c>
       <c r="D13" s="2" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>16'b0000</v>
+        <v>16'b000</v>
       </c>
       <c r="E13" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>11</v>
+        <v>100</v>
       </c>
       <c r="F13" s="2" t="str">
         <f t="shared" si="5"/>
@@ -1323,19 +1323,19 @@
       </c>
       <c r="G13" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[11] = 16'b0000110000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[11] = 16'b0001000000000000;</v>
       </c>
       <c r="H13" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I13" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>3072</v>
+        <v>4096</v>
       </c>
       <c r="K13" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>-1518</v>
+        <v>-1718</v>
       </c>
       <c r="L13" s="2">
         <f t="shared" ca="1" si="7"/>
@@ -1386,27 +1386,27 @@
       <c r="C17" s="8"/>
       <c r="G17" s="4" t="str">
         <f ca="1">_xlfn.CONCAT("notePosition_i = 10'b",REPT(0,B17-LEN(_xlfn.BASE(I17,2))),_xlfn.BASE(I17,2),";" )</f>
-        <v>notePosition_i = 10'b0111010101;</v>
+        <v>notePosition_i = 10'b0000000100;</v>
       </c>
       <c r="H17" s="2">
         <f ca="1">I17/2^10</f>
-        <v>0.4580078125</v>
+        <v>3.90625E-3</v>
       </c>
       <c r="I17" s="2">
         <f ca="1">RANDBETWEEN(0,1023)</f>
-        <v>469</v>
+        <v>4</v>
       </c>
       <c r="J17" s="2">
         <f ca="1">I17*24</f>
-        <v>11256</v>
+        <v>96</v>
       </c>
       <c r="K17" s="2">
         <f ca="1">IF(J21=3,24576-J17,8192-J17)</f>
-        <v>-3064</v>
+        <v>8096</v>
       </c>
       <c r="L17" s="2">
         <f ca="1">IF(J21=3,K23+170, K23)</f>
-        <v>-32</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
@@ -1448,15 +1448,15 @@
       </c>
       <c r="H20" s="2">
         <f ca="1">IF(J$21=1,G20,1)</f>
-        <v>1</v>
+        <v>21824</v>
       </c>
       <c r="J20" s="2" t="str">
         <f ca="1">_xlfn.CONCAT(REPT(0,3-LEN(DEC2BIN(2^_xlfn.FLOOR.MATH((J17+1)/8192)))),DEC2BIN(2^_xlfn.FLOOR.MATH((J17+1)/8192)))</f>
-        <v>010</v>
+        <v>001</v>
       </c>
       <c r="K20" s="2">
         <f ca="1">K17*H20*H21*H22</f>
-        <v>-133737472</v>
+        <v>176687104</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>24</v>
@@ -1475,19 +1475,19 @@
       </c>
       <c r="H21" s="2">
         <f ca="1">IF(J$21=2,G21,1)</f>
-        <v>43648</v>
+        <v>1</v>
       </c>
       <c r="J21" s="2">
         <f ca="1">LEN(DEC2BIN(2^_xlfn.FLOOR.MATH((J17+1)/8192)))</f>
-        <v>2</v>
-      </c>
-      <c r="K21" s="2" t="e">
+        <v>1</v>
+      </c>
+      <c r="K21" s="2" t="str">
         <f ca="1">_xlfn.BASE(K20,2,32)</f>
-        <v>#NUM!</v>
+        <v>00001010100010000000100000000000</v>
       </c>
       <c r="L21" s="2">
         <f ca="1">MOD(IF(L17&lt;0,L17+1023,L17), 1024)</f>
-        <v>991</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
@@ -1512,21 +1512,21 @@
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="K23" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(K20/2^(B17+B17+C15-3))</f>
-        <v>-32</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G26" s="4" t="str">
         <f ca="1">_xlfn.CONCAT("        noteAmplitude_i = 10'b",REPT(0,B17-LEN(_xlfn.BASE(I26,2))),_xlfn.BASE(I26,2),";" )</f>
-        <v xml:space="preserve">        noteAmplitude_i = 10'b0100011101;</v>
+        <v xml:space="preserve">        noteAmplitude_i = 10'b0101011101;</v>
       </c>
       <c r="H26" s="2">
         <f ca="1">I26/2^10</f>
-        <v>0.2783203125</v>
+        <v>0.3408203125</v>
       </c>
       <c r="I26" s="2">
         <f ca="1">RANDBETWEEN(0,1023)</f>
-        <v>285</v>
+        <v>349</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>28</v>
@@ -1558,35 +1558,35 @@
       </c>
       <c r="G27" s="4" t="str">
         <f ca="1">_xlfn.CONCAT("        noteAmplitudeFast_i = 10'b",REPT(0,B17-LEN(_xlfn.BASE(I27,2))),_xlfn.BASE(I27,2),";" )</f>
-        <v xml:space="preserve">        noteAmplitudeFast_i = 10'b0111111000;</v>
+        <v xml:space="preserve">        noteAmplitudeFast_i = 10'b0000100100;</v>
       </c>
       <c r="H27" s="2">
         <f t="shared" ref="H27:H28" ca="1" si="9">I27/2^10</f>
-        <v>0.4921875</v>
+        <v>3.515625E-2</v>
       </c>
       <c r="I27" s="2">
         <f ca="1">RANDBETWEEN(0,1023)</f>
-        <v>504</v>
+        <v>36</v>
       </c>
       <c r="J27" s="2">
         <f ca="1">I28*E31</f>
-        <v>5640</v>
+        <v>792</v>
       </c>
       <c r="K27" s="2">
         <f ca="1">IF(E33,I26,I27)</f>
-        <v>504</v>
+        <v>36</v>
       </c>
       <c r="L27" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(K33/2^(B17-8))</f>
-        <v>201</v>
+        <v>14</v>
       </c>
       <c r="M27" s="2">
         <f ca="1">$L$27</f>
-        <v>201</v>
+        <v>14</v>
       </c>
       <c r="N27" s="2">
         <f ca="1">$L$33</f>
-        <v>102</v>
+        <v>11</v>
       </c>
       <c r="O27" s="2">
         <f>0</f>
@@ -1594,21 +1594,21 @@
       </c>
       <c r="P27" s="2">
         <f ca="1">M27*2^16+N27*2^8+O27</f>
-        <v>13198848</v>
+        <v>920320</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G28" s="4" t="str">
         <f ca="1">_xlfn.CONCAT("        noteHue_i = 10'b",REPT(0,B17-LEN(_xlfn.BASE(I28,2))),_xlfn.BASE(I28,2),";" )</f>
-        <v xml:space="preserve">        noteHue_i = 10'b1110101100;</v>
+        <v xml:space="preserve">        noteHue_i = 10'b0010000100;</v>
       </c>
       <c r="H28" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>0.91796875</v>
+        <v>0.12890625</v>
       </c>
       <c r="I28" s="2">
         <f ca="1">RANDBETWEEN(0,1023)</f>
-        <v>940</v>
+        <v>132</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>29</v>
@@ -1621,11 +1621,11 @@
       </c>
       <c r="M28" s="2">
         <f ca="1">$L$35</f>
-        <v>98</v>
+        <v>3</v>
       </c>
       <c r="N28" s="2">
         <f ca="1">$L$27</f>
-        <v>201</v>
+        <v>14</v>
       </c>
       <c r="O28" s="2">
         <f>0</f>
@@ -1633,21 +1633,21 @@
       </c>
       <c r="P28" s="2">
         <f t="shared" ref="P28:P33" ca="1" si="10">M28*2^16+N28*2^8+O28</f>
-        <v>6473984</v>
+        <v>200192</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="J29" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(J27/2^10)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K29" s="2">
         <f ca="1">K27*E30</f>
-        <v>825552</v>
+        <v>58968</v>
       </c>
       <c r="L29" s="2">
         <f ca="1">K33*J31</f>
-        <v>419120</v>
+        <v>45144</v>
       </c>
       <c r="M29" s="2">
         <f>0</f>
@@ -1655,15 +1655,15 @@
       </c>
       <c r="N29" s="2">
         <f ca="1">$L$27</f>
-        <v>201</v>
+        <v>14</v>
       </c>
       <c r="O29" s="2">
         <f ca="1">$L$33</f>
-        <v>102</v>
+        <v>11</v>
       </c>
       <c r="P29" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>51558</v>
+        <v>3595</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
@@ -1688,15 +1688,15 @@
       </c>
       <c r="N30" s="2">
         <f ca="1">$L$35</f>
-        <v>98</v>
+        <v>3</v>
       </c>
       <c r="O30" s="2">
         <f ca="1">$L$27</f>
-        <v>201</v>
+        <v>14</v>
       </c>
       <c r="P30" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>25289</v>
+        <v>782</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
@@ -1708,19 +1708,19 @@
       </c>
       <c r="J31" s="2">
         <f ca="1">MOD(J27,2^10)</f>
-        <v>520</v>
+        <v>792</v>
       </c>
       <c r="K31" s="2">
         <f ca="1">IF(_xlfn.FLOOR.MATH(K29/2^10) &gt; 1023, 1023, _xlfn.FLOOR.MATH(K29/2^10))</f>
-        <v>806</v>
+        <v>57</v>
       </c>
       <c r="L31" s="2">
         <f ca="1">K33*(1023-J31)</f>
-        <v>405418</v>
+        <v>13167</v>
       </c>
       <c r="M31" s="2">
         <f ca="1">$L$33</f>
-        <v>102</v>
+        <v>11</v>
       </c>
       <c r="N31" s="2">
         <f>0</f>
@@ -1728,11 +1728,11 @@
       </c>
       <c r="O31" s="2">
         <f ca="1">$L$27</f>
-        <v>201</v>
+        <v>14</v>
       </c>
       <c r="P31" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>6684873</v>
+        <v>720910</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
@@ -1750,7 +1750,7 @@
       </c>
       <c r="M32" s="2">
         <f ca="1">$L$27</f>
-        <v>201</v>
+        <v>14</v>
       </c>
       <c r="N32" s="2">
         <f>0</f>
@@ -1758,11 +1758,11 @@
       </c>
       <c r="O32" s="2">
         <f ca="1">$L$35</f>
-        <v>98</v>
+        <v>3</v>
       </c>
       <c r="P32" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>13172834</v>
+        <v>917507</v>
       </c>
     </row>
     <row r="33" spans="5:16" x14ac:dyDescent="0.3">
@@ -1774,19 +1774,19 @@
       </c>
       <c r="K33" s="2">
         <f ca="1">IF(K31&gt;E32,E32,K31)</f>
-        <v>806</v>
+        <v>57</v>
       </c>
       <c r="L33" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(L29/2^(2*B17-8))</f>
-        <v>102</v>
+        <v>11</v>
       </c>
       <c r="M33" s="2">
         <f ca="1">$L$27</f>
-        <v>201</v>
+        <v>14</v>
       </c>
       <c r="N33" s="2">
         <f ca="1">$L$33</f>
-        <v>102</v>
+        <v>11</v>
       </c>
       <c r="O33" s="2">
         <f>0</f>
@@ -1794,7 +1794,7 @@
       </c>
       <c r="P33" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>13198848</v>
+        <v>920320</v>
       </c>
     </row>
     <row r="34" spans="5:16" x14ac:dyDescent="0.3">
@@ -1808,11 +1808,11 @@
     <row r="35" spans="5:16" x14ac:dyDescent="0.3">
       <c r="L35" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(L31/2^(2*B17-8))</f>
-        <v>98</v>
+        <v>3</v>
       </c>
       <c r="M35" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="M35" ca="1">_xlfn.BASE(_xlfn.SWITCH(J29,0,P27,1,P28,2,P29,3,P30,4,P31,5,P32,6,P33),16,6)</f>
-        <v>C90062</v>
+        <v>0E0B00</v>
       </c>
     </row>
     <row r="36" spans="5:16" x14ac:dyDescent="0.3">
@@ -1839,7 +1839,7 @@
       </c>
       <c r="I39" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(H52/B19)</f>
-        <v>278</v>
+        <v>196</v>
       </c>
       <c r="J39" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(H39/I$39)</f>
@@ -1847,91 +1847,91 @@
       </c>
       <c r="L39" s="2">
         <f ca="1">L27-L33-L35</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="5:16" x14ac:dyDescent="0.3">
       <c r="G40" s="4" t="str">
         <f t="shared" ref="G40:G50" ca="1" si="11">_xlfn.CONCAT(A3,B3,C3,B$16+B$17,"'b",_xlfn.BASE(L3,2,$B$16+$B$17),";")</f>
-        <v xml:space="preserve">            noteAmplitudes_i[ 1] = 16'b0000000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 1] = 16'b0000010101001010;</v>
       </c>
       <c r="H40" s="2">
         <f t="shared" ref="H40:H50" ca="1" si="12">L3</f>
-        <v>0</v>
+        <v>1354</v>
       </c>
       <c r="J40" s="2">
         <f t="shared" ref="J40:J50" ca="1" si="13">_xlfn.FLOOR.MATH(H40/I$39)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="5:16" x14ac:dyDescent="0.3">
       <c r="G41" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 2] = 16'b0000000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 2] = 16'b0000110101001010;</v>
       </c>
       <c r="H41" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>3402</v>
       </c>
       <c r="J41" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="5:16" x14ac:dyDescent="0.3">
       <c r="G42" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 3] = 16'b0000011000010010;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 3] = 16'b0000000000000000;</v>
       </c>
       <c r="H42" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>1554</v>
+        <v>0</v>
       </c>
       <c r="J42" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="5:16" x14ac:dyDescent="0.3">
       <c r="G43" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 4] = 16'b0000000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 4] = 16'b0000110101001010;</v>
       </c>
       <c r="H43" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>3402</v>
       </c>
       <c r="J43" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44" spans="5:16" x14ac:dyDescent="0.3">
       <c r="G44" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 5] = 16'b0000011000010010;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 5] = 16'b0000000000000000;</v>
       </c>
       <c r="H44" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>1554</v>
+        <v>0</v>
       </c>
       <c r="J44" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="5:16" x14ac:dyDescent="0.3">
       <c r="G45" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 6] = 16'b0001001000010010;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 6] = 16'b0000000000000000;</v>
       </c>
       <c r="H45" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>4626</v>
+        <v>0</v>
       </c>
       <c r="J45" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="5:16" x14ac:dyDescent="0.3">
@@ -1951,29 +1951,29 @@
     <row r="47" spans="5:16" x14ac:dyDescent="0.3">
       <c r="G47" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 8] = 16'b0000111000010010;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 8] = 16'b0000010101001010;</v>
       </c>
       <c r="H47" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>3602</v>
+        <v>1354</v>
       </c>
       <c r="J47" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="5:16" x14ac:dyDescent="0.3">
       <c r="G48" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 9] = 16'b0000101000010010;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 9] = 16'b0000000101001010;</v>
       </c>
       <c r="H48" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>2578</v>
+        <v>330</v>
       </c>
       <c r="J48" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.3">
@@ -2007,7 +2007,7 @@
     <row r="51" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G51" s="5" t="str">
         <f ca="1">_xlfn.CONCAT("            amplitudeSumNew_i = ",B16+B17+_xlfn.CEILING.MATH(IMLOG2(B19)),"'b",_xlfn.BASE(H52,2,B16+B17+_xlfn.CEILING.MATH(IMLOG2(B19))),";")</f>
-        <v xml:space="preserve">            amplitudeSumNew_i = 22'b0000000011011001011010;</v>
+        <v xml:space="preserve">            amplitudeSumNew_i = 22'b0000000010011001110010;</v>
       </c>
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.3">
@@ -2016,7 +2016,7 @@
       </c>
       <c r="H52" s="2">
         <f ca="1">SUM(H39:H50)</f>
-        <v>13914</v>
+        <v>9842</v>
       </c>
     </row>
     <row r="54" spans="1:25" x14ac:dyDescent="0.3">
@@ -2493,7 +2493,7 @@
         <v>2</v>
       </c>
       <c r="K73" s="2" cm="1">
-        <f t="array" aca="1" ref="K73" ca="1">_xlfn.SWITCH(J73,1,8*2^10 - I73, 2, 8*2^10 -I73, 3, 24*2^10 -I73)</f>
+        <f t="array" aca="1" ref="K73" ca="1">_xlfn.SWITCH(J73,1,8*2^10 - I73, 2, 8*2^10 -I73, 3, 24*2^B$17 -I73)</f>
         <v>-3688</v>
       </c>
       <c r="L73" s="2" cm="1">
@@ -2542,7 +2542,7 @@
         <v>1</v>
       </c>
       <c r="K74" s="2" cm="1">
-        <f t="array" aca="1" ref="K74" ca="1">_xlfn.SWITCH(J74,1,8*2^10 - I74, 2, 8*2^10 -I74, 3, 24*2^10 -I74)</f>
+        <f t="array" aca="1" ref="K74" ca="1">_xlfn.SWITCH(J74,1,8*2^10 - I74, 2, 8*2^10 -I74, 3, 24*2^B$17 -I74)</f>
         <v>1760</v>
       </c>
       <c r="L74" s="2" cm="1">
@@ -2591,7 +2591,7 @@
         <v>3</v>
       </c>
       <c r="K75" s="2" cm="1">
-        <f t="array" aca="1" ref="K75" ca="1">_xlfn.SWITCH(J75,1,8*2^10 - I75, 2, 8*2^10 -I75, 3, 24*2^10 -I75)</f>
+        <f t="array" aca="1" ref="K75" ca="1">_xlfn.SWITCH(J75,1,8*2^10 - I75, 2, 8*2^10 -I75, 3, 24*2^B$17 -I75)</f>
         <v>3840</v>
       </c>
       <c r="L75" s="2" cm="1">
@@ -2640,7 +2640,7 @@
         <v>3</v>
       </c>
       <c r="K76" s="2" cm="1">
-        <f t="array" aca="1" ref="K76" ca="1">_xlfn.SWITCH(J76,1,8*2^10 - I76, 2, 8*2^10 -I76, 3, 24*2^10 -I76)</f>
+        <f t="array" aca="1" ref="K76" ca="1">_xlfn.SWITCH(J76,1,8*2^10 - I76, 2, 8*2^10 -I76, 3, 24*2^B$17 -I76)</f>
         <v>1440</v>
       </c>
       <c r="L76" s="2" cm="1">
@@ -2689,7 +2689,7 @@
         <v>3</v>
       </c>
       <c r="K77" s="2" cm="1">
-        <f t="array" aca="1" ref="K77" ca="1">_xlfn.SWITCH(J77,1,8*2^10 - I77, 2, 8*2^10 -I77, 3, 24*2^10 -I77)</f>
+        <f t="array" aca="1" ref="K77" ca="1">_xlfn.SWITCH(J77,1,8*2^10 - I77, 2, 8*2^10 -I77, 3, 24*2^B$17 -I77)</f>
         <v>5496</v>
       </c>
       <c r="L77" s="2" cm="1">
@@ -2738,7 +2738,7 @@
         <v>2</v>
       </c>
       <c r="K78" s="2" cm="1">
-        <f t="array" aca="1" ref="K78" ca="1">_xlfn.SWITCH(J78,1,8*2^10 - I78, 2, 8*2^10 -I78, 3, 24*2^10 -I78)</f>
+        <f t="array" aca="1" ref="K78" ca="1">_xlfn.SWITCH(J78,1,8*2^10 - I78, 2, 8*2^10 -I78, 3, 24*2^B$17 -I78)</f>
         <v>-7504</v>
       </c>
       <c r="L78" s="2" cm="1">
@@ -2787,7 +2787,7 @@
         <v>2</v>
       </c>
       <c r="K79" s="2" cm="1">
-        <f t="array" aca="1" ref="K79" ca="1">_xlfn.SWITCH(J79,1,8*2^10 - I79, 2, 8*2^10 -I79, 3, 24*2^10 -I79)</f>
+        <f t="array" aca="1" ref="K79" ca="1">_xlfn.SWITCH(J79,1,8*2^10 - I79, 2, 8*2^10 -I79, 3, 24*2^B$17 -I79)</f>
         <v>-88</v>
       </c>
       <c r="L79" s="2" cm="1">
@@ -2836,7 +2836,7 @@
         <v>2</v>
       </c>
       <c r="K80" s="2" cm="1">
-        <f t="array" aca="1" ref="K80" ca="1">_xlfn.SWITCH(J80,1,8*2^10 - I80, 2, 8*2^10 -I80, 3, 24*2^10 -I80)</f>
+        <f t="array" aca="1" ref="K80" ca="1">_xlfn.SWITCH(J80,1,8*2^10 - I80, 2, 8*2^10 -I80, 3, 24*2^B$17 -I80)</f>
         <v>-5584</v>
       </c>
       <c r="L80" s="2" cm="1">
@@ -2885,7 +2885,7 @@
         <v>1</v>
       </c>
       <c r="K81" s="2" cm="1">
-        <f t="array" aca="1" ref="K81" ca="1">_xlfn.SWITCH(J81,1,8*2^10 - I81, 2, 8*2^10 -I81, 3, 24*2^10 -I81)</f>
+        <f t="array" aca="1" ref="K81" ca="1">_xlfn.SWITCH(J81,1,8*2^10 - I81, 2, 8*2^10 -I81, 3, 24*2^B$17 -I81)</f>
         <v>7232</v>
       </c>
       <c r="L81" s="2" cm="1">
@@ -2934,7 +2934,7 @@
         <v>3</v>
       </c>
       <c r="K82" s="2" cm="1">
-        <f t="array" aca="1" ref="K82" ca="1">_xlfn.SWITCH(J82,1,8*2^10 - I82, 2, 8*2^10 -I82, 3, 24*2^10 -I82)</f>
+        <f t="array" aca="1" ref="K82" ca="1">_xlfn.SWITCH(J82,1,8*2^10 - I82, 2, 8*2^10 -I82, 3, 24*2^B$17 -I82)</f>
         <v>4104</v>
       </c>
       <c r="L82" s="2" cm="1">
@@ -2983,7 +2983,7 @@
         <v>3</v>
       </c>
       <c r="K83" s="2" cm="1">
-        <f t="array" aca="1" ref="K83" ca="1">_xlfn.SWITCH(J83,1,8*2^10 - I83, 2, 8*2^10 -I83, 3, 24*2^10 -I83)</f>
+        <f t="array" aca="1" ref="K83" ca="1">_xlfn.SWITCH(J83,1,8*2^10 - I83, 2, 8*2^10 -I83, 3, 24*2^B$17 -I83)</f>
         <v>4104</v>
       </c>
       <c r="L83" s="2" cm="1">
@@ -3032,7 +3032,7 @@
         <v>1</v>
       </c>
       <c r="K84" s="2" cm="1">
-        <f t="array" aca="1" ref="K84" ca="1">_xlfn.SWITCH(J84,1,8*2^10 - I84, 2, 8*2^10 -I84, 3, 24*2^10 -I84)</f>
+        <f t="array" aca="1" ref="K84" ca="1">_xlfn.SWITCH(J84,1,8*2^10 - I84, 2, 8*2^10 -I84, 3, 24*2^B$17 -I84)</f>
         <v>8192</v>
       </c>
       <c r="L84" s="2" cm="1">
@@ -3185,7 +3185,7 @@
     </row>
     <row r="89" spans="6:25" x14ac:dyDescent="0.3">
       <c r="I89" s="2">
-        <f t="shared" ref="I89:I101" ca="1" si="25">O74*E$31</f>
+        <f t="shared" ref="I89:I99" ca="1" si="25">O74*E$31</f>
         <v>216</v>
       </c>
       <c r="J89" s="2">
@@ -3973,7 +3973,7 @@
     </row>
     <row r="103" spans="9:25" x14ac:dyDescent="0.3">
       <c r="J103" s="2">
-        <f t="shared" ref="J103:J118" ca="1" si="39">K60/I$102</f>
+        <f t="shared" ref="J103:J114" ca="1" si="39">K60/I$102</f>
         <v>21.832244822677595</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added a PLL to get past division timing requirements
</commit_message>
<xml_diff>
--- a/other/LinearVisualizer.xlsx
+++ b/other/LinearVisualizer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\CCHW\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E2924C-ACA5-4443-8016-4CF75D04D2A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D20D662-E280-40FC-8DBC-7CAFA127215B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{9DBF0F91-83D7-4F64-B04C-B7CB81DC62EF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9DBF0F91-83D7-4F64-B04C-B7CB81DC62EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -695,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A6626A4-8C87-4B90-BEEB-AEB487ACEA9E}">
   <dimension ref="A1:Y114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F73" sqref="F73"/>
+    <sheetView tabSelected="1" topLeftCell="L81" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y88" sqref="Y88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -788,11 +788,11 @@
       </c>
       <c r="J2" s="2">
         <f ca="1">SUM(H2:H13)</f>
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="K2" s="2">
         <f t="shared" ref="K2:K13" ca="1" si="2">I2-J$7</f>
-        <v>-1718</v>
+        <v>-3248</v>
       </c>
       <c r="L2" s="2">
         <f ca="1">IF(K2&gt;0,K2,0)</f>
@@ -815,11 +815,11 @@
       </c>
       <c r="D3" s="2" t="str">
         <f t="shared" ref="D3:D13" ca="1" si="3">_xlfn.CONCAT(B$16+B$17,"'b",REPT("0",B$16-LEN(E3)))</f>
-        <v>16'b000</v>
+        <v>16'b00000</v>
       </c>
       <c r="E3" s="2" t="str">
         <f t="shared" ref="E3:E13" ca="1" si="4">DEC2BIN(_xlfn.FLOOR.MATH(RAND()*10))</f>
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="F3" s="2" t="str">
         <f t="shared" ref="F3:F13" si="5">_xlfn.CONCAT(REPT("0",B$17),";")</f>
@@ -827,31 +827,31 @@
       </c>
       <c r="G3" s="4" t="str">
         <f t="shared" ref="G3:G13" ca="1" si="6">_xlfn.CONCAT(A3,B3,C3,D3,E3,F3)</f>
-        <v xml:space="preserve">            noteAmplitudes_i[ 1] = 16'b0001110000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 1] = 16'b0000010000000000;</v>
       </c>
       <c r="H3" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I3" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>7168</v>
+        <v>1024</v>
       </c>
       <c r="J3" s="2">
         <f ca="1">J2*2^B17</f>
-        <v>58368</v>
+        <v>73728</v>
       </c>
       <c r="K3" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1354</v>
+        <v>-6320</v>
       </c>
       <c r="L3" s="2">
         <f t="shared" ref="L3:L13" ca="1" si="7">IF(K3&gt;0,K3,0)</f>
-        <v>1354</v>
+        <v>0</v>
       </c>
       <c r="M3" s="2">
         <f t="shared" ref="M3:M13" ca="1" si="8">IF(K3&gt;0,I3,0)</f>
-        <v>7168</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -866,11 +866,11 @@
       </c>
       <c r="D4" s="2" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>16'b00</v>
+        <v>16'b000</v>
       </c>
       <c r="E4" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1001</v>
+        <v>111</v>
       </c>
       <c r="F4" s="2" t="str">
         <f t="shared" si="5"/>
@@ -878,27 +878,27 @@
       </c>
       <c r="G4" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 2] = 16'b0010010000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 2] = 16'b0001110000000000;</v>
       </c>
       <c r="H4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I4" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>9216</v>
+        <v>7168</v>
       </c>
       <c r="K4" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>3402</v>
+        <v>-176</v>
       </c>
       <c r="L4" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>3402</v>
+        <v>0</v>
       </c>
       <c r="M4" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>9216</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -913,11 +913,11 @@
       </c>
       <c r="D5" s="2" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>16'b00000</v>
+        <v>16'b00</v>
       </c>
       <c r="E5" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>1001</v>
       </c>
       <c r="F5" s="2" t="str">
         <f t="shared" si="5"/>
@@ -925,30 +925,30 @@
       </c>
       <c r="G5" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 3] = 16'b0000010000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 3] = 16'b0010010000000000;</v>
       </c>
       <c r="H5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="I5" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>1024</v>
+        <v>9216</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="K5" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>-4790</v>
+        <v>1872</v>
       </c>
       <c r="L5" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>1872</v>
       </c>
       <c r="M5" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>9216</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -967,7 +967,7 @@
       </c>
       <c r="E6" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="F6" s="2" t="str">
         <f t="shared" si="5"/>
@@ -975,31 +975,31 @@
       </c>
       <c r="G6" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 4] = 16'b0010010000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 4] = 16'b0010000000000000;</v>
       </c>
       <c r="H6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I6" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>9216</v>
+        <v>8192</v>
       </c>
       <c r="J6" s="3">
         <f ca="1">J2*B18</f>
-        <v>5.677734375</v>
+        <v>7.171875</v>
       </c>
       <c r="K6" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>3402</v>
+        <v>848</v>
       </c>
       <c r="L6" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>3402</v>
+        <v>848</v>
       </c>
       <c r="M6" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>9216</v>
+        <v>8192</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -1014,11 +1014,11 @@
       </c>
       <c r="D7" s="2" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>16'b000</v>
+        <v>16'b00</v>
       </c>
       <c r="E7" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>101</v>
+        <v>1000</v>
       </c>
       <c r="F7" s="2" t="str">
         <f t="shared" si="5"/>
@@ -1026,31 +1026,31 @@
       </c>
       <c r="G7" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 5] = 16'b0001010000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 5] = 16'b0010000000000000;</v>
       </c>
       <c r="H7" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I7" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>5120</v>
+        <v>8192</v>
       </c>
       <c r="J7" s="2">
         <f ca="1">J3 * BIN2DEC(C18) / 2^B17</f>
-        <v>5814</v>
+        <v>7344</v>
       </c>
       <c r="K7" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>-694</v>
+        <v>848</v>
       </c>
       <c r="L7" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>848</v>
       </c>
       <c r="M7" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>8192</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -1069,7 +1069,7 @@
       </c>
       <c r="E8" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="F8" s="2" t="str">
         <f t="shared" si="5"/>
@@ -1077,19 +1077,19 @@
       </c>
       <c r="G8" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 6] = 16'b0001000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 6] = 16'b0001100000000000;</v>
       </c>
       <c r="H8" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I8" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>4096</v>
+        <v>6144</v>
       </c>
       <c r="K8" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>-1718</v>
+        <v>-1200</v>
       </c>
       <c r="L8" s="2">
         <f t="shared" ca="1" si="7"/>
@@ -1112,11 +1112,11 @@
       </c>
       <c r="D9" s="2" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>16'b00000</v>
+        <v>16'b00</v>
       </c>
       <c r="E9" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="F9" s="2" t="str">
         <f t="shared" si="5"/>
@@ -1124,30 +1124,30 @@
       </c>
       <c r="G9" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 7] = 16'b0000000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 7] = 16'b0010000000000000;</v>
       </c>
       <c r="H9" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I9" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>8192</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="K9" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>-5814</v>
+        <v>848</v>
       </c>
       <c r="L9" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>848</v>
       </c>
       <c r="M9" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>8192</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -1166,7 +1166,7 @@
       </c>
       <c r="E10" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="F10" s="2" t="str">
         <f t="shared" si="5"/>
@@ -1174,31 +1174,31 @@
       </c>
       <c r="G10" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 8] = 16'b0001110000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 8] = 16'b0001000000000000;</v>
       </c>
       <c r="H10" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I10" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>7168</v>
+        <v>4096</v>
       </c>
       <c r="J10" s="2">
         <f ca="1">J11/2^B17</f>
-        <v>9.611328125</v>
+        <v>6.140625</v>
       </c>
       <c r="K10" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1354</v>
+        <v>-3248</v>
       </c>
       <c r="L10" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>1354</v>
+        <v>0</v>
       </c>
       <c r="M10" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>7168</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -1217,7 +1217,7 @@
       </c>
       <c r="E11" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F11" s="2" t="str">
         <f t="shared" si="5"/>
@@ -1225,31 +1225,31 @@
       </c>
       <c r="G11" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 9] = 16'b0001100000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 9] = 16'b0001110000000000;</v>
       </c>
       <c r="H11" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I11" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>6144</v>
+        <v>7168</v>
       </c>
       <c r="J11" s="2">
         <f ca="1">SUM(L2:L13)</f>
-        <v>9842</v>
+        <v>6288</v>
       </c>
       <c r="K11" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>330</v>
+        <v>-176</v>
       </c>
       <c r="L11" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>330</v>
+        <v>0</v>
       </c>
       <c r="M11" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>6144</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -1264,11 +1264,11 @@
       </c>
       <c r="D12" s="2" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>16'b00000</v>
+        <v>16'b00</v>
       </c>
       <c r="E12" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>1001</v>
       </c>
       <c r="F12" s="2" t="str">
         <f t="shared" si="5"/>
@@ -1276,27 +1276,27 @@
       </c>
       <c r="G12" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[10] = 16'b0000010000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[10] = 16'b0010010000000000;</v>
       </c>
       <c r="H12" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="I12" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>1024</v>
+        <v>9216</v>
       </c>
       <c r="K12" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>-4790</v>
+        <v>1872</v>
       </c>
       <c r="L12" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>1872</v>
       </c>
       <c r="M12" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>9216</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -1311,11 +1311,11 @@
       </c>
       <c r="D13" s="2" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>16'b000</v>
+        <v>16'b00000</v>
       </c>
       <c r="E13" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F13" s="2" t="str">
         <f t="shared" si="5"/>
@@ -1323,19 +1323,19 @@
       </c>
       <c r="G13" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[11] = 16'b0001000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[11] = 16'b0000010000000000;</v>
       </c>
       <c r="H13" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I13" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>4096</v>
+        <v>1024</v>
       </c>
       <c r="K13" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>-1718</v>
+        <v>-6320</v>
       </c>
       <c r="L13" s="2">
         <f t="shared" ca="1" si="7"/>
@@ -1386,27 +1386,27 @@
       <c r="C17" s="8"/>
       <c r="G17" s="4" t="str">
         <f ca="1">_xlfn.CONCAT("notePosition_i = 10'b",REPT(0,B17-LEN(_xlfn.BASE(I17,2))),_xlfn.BASE(I17,2),";" )</f>
-        <v>notePosition_i = 10'b0000000100;</v>
+        <v>notePosition_i = 10'b0110010010;</v>
       </c>
       <c r="H17" s="2">
         <f ca="1">I17/2^10</f>
-        <v>3.90625E-3</v>
+        <v>0.392578125</v>
       </c>
       <c r="I17" s="2">
         <f ca="1">RANDBETWEEN(0,1023)</f>
-        <v>4</v>
+        <v>402</v>
       </c>
       <c r="J17" s="2">
         <f ca="1">I17*24</f>
-        <v>96</v>
+        <v>9648</v>
       </c>
       <c r="K17" s="2">
         <f ca="1">IF(J21=3,24576-J17,8192-J17)</f>
-        <v>8096</v>
+        <v>-1456</v>
       </c>
       <c r="L17" s="2">
         <f ca="1">IF(J21=3,K23+170, K23)</f>
-        <v>42</v>
+        <v>-16</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
@@ -1448,15 +1448,15 @@
       </c>
       <c r="H20" s="2">
         <f ca="1">IF(J$21=1,G20,1)</f>
-        <v>21824</v>
+        <v>1</v>
       </c>
       <c r="J20" s="2" t="str">
         <f ca="1">_xlfn.CONCAT(REPT(0,3-LEN(DEC2BIN(2^_xlfn.FLOOR.MATH((J17+1)/8192)))),DEC2BIN(2^_xlfn.FLOOR.MATH((J17+1)/8192)))</f>
-        <v>001</v>
+        <v>010</v>
       </c>
       <c r="K20" s="2">
         <f ca="1">K17*H20*H21*H22</f>
-        <v>176687104</v>
+        <v>-63551488</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>24</v>
@@ -1475,19 +1475,19 @@
       </c>
       <c r="H21" s="2">
         <f ca="1">IF(J$21=2,G21,1)</f>
-        <v>1</v>
+        <v>43648</v>
       </c>
       <c r="J21" s="2">
         <f ca="1">LEN(DEC2BIN(2^_xlfn.FLOOR.MATH((J17+1)/8192)))</f>
-        <v>1</v>
-      </c>
-      <c r="K21" s="2" t="str">
+        <v>2</v>
+      </c>
+      <c r="K21" s="2" t="e">
         <f ca="1">_xlfn.BASE(K20,2,32)</f>
-        <v>00001010100010000000100000000000</v>
+        <v>#NUM!</v>
       </c>
       <c r="L21" s="2">
         <f ca="1">MOD(IF(L17&lt;0,L17+1023,L17), 1024)</f>
-        <v>42</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
@@ -1512,21 +1512,21 @@
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="K23" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(K20/2^(B17+B17+C15-3))</f>
-        <v>42</v>
+        <v>-16</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G26" s="4" t="str">
         <f ca="1">_xlfn.CONCAT("        noteAmplitude_i = 10'b",REPT(0,B17-LEN(_xlfn.BASE(I26,2))),_xlfn.BASE(I26,2),";" )</f>
-        <v xml:space="preserve">        noteAmplitude_i = 10'b0101011101;</v>
+        <v xml:space="preserve">        noteAmplitude_i = 10'b0011000101;</v>
       </c>
       <c r="H26" s="2">
         <f ca="1">I26/2^10</f>
-        <v>0.3408203125</v>
+        <v>0.1923828125</v>
       </c>
       <c r="I26" s="2">
         <f ca="1">RANDBETWEEN(0,1023)</f>
-        <v>349</v>
+        <v>197</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>28</v>
@@ -1558,35 +1558,35 @@
       </c>
       <c r="G27" s="4" t="str">
         <f ca="1">_xlfn.CONCAT("        noteAmplitudeFast_i = 10'b",REPT(0,B17-LEN(_xlfn.BASE(I27,2))),_xlfn.BASE(I27,2),";" )</f>
-        <v xml:space="preserve">        noteAmplitudeFast_i = 10'b0000100100;</v>
+        <v xml:space="preserve">        noteAmplitudeFast_i = 10'b1101110011;</v>
       </c>
       <c r="H27" s="2">
         <f t="shared" ref="H27:H28" ca="1" si="9">I27/2^10</f>
-        <v>3.515625E-2</v>
+        <v>0.8623046875</v>
       </c>
       <c r="I27" s="2">
         <f ca="1">RANDBETWEEN(0,1023)</f>
-        <v>36</v>
+        <v>883</v>
       </c>
       <c r="J27" s="2">
         <f ca="1">I28*E31</f>
-        <v>792</v>
+        <v>4260</v>
       </c>
       <c r="K27" s="2">
         <f ca="1">IF(E33,I26,I27)</f>
-        <v>36</v>
+        <v>883</v>
       </c>
       <c r="L27" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(K33/2^(B17-8))</f>
-        <v>14</v>
+        <v>255</v>
       </c>
       <c r="M27" s="2">
         <f ca="1">$L$27</f>
-        <v>14</v>
+        <v>255</v>
       </c>
       <c r="N27" s="2">
         <f ca="1">$L$33</f>
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="O27" s="2">
         <f>0</f>
@@ -1594,21 +1594,21 @@
       </c>
       <c r="P27" s="2">
         <f ca="1">M27*2^16+N27*2^8+O27</f>
-        <v>920320</v>
+        <v>16721920</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G28" s="4" t="str">
         <f ca="1">_xlfn.CONCAT("        noteHue_i = 10'b",REPT(0,B17-LEN(_xlfn.BASE(I28,2))),_xlfn.BASE(I28,2),";" )</f>
-        <v xml:space="preserve">        noteHue_i = 10'b0010000100;</v>
+        <v xml:space="preserve">        noteHue_i = 10'b1011000110;</v>
       </c>
       <c r="H28" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>0.12890625</v>
+        <v>0.693359375</v>
       </c>
       <c r="I28" s="2">
         <f ca="1">RANDBETWEEN(0,1023)</f>
-        <v>132</v>
+        <v>710</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>29</v>
@@ -1621,11 +1621,11 @@
       </c>
       <c r="M28" s="2">
         <f ca="1">$L$35</f>
-        <v>3</v>
+        <v>214</v>
       </c>
       <c r="N28" s="2">
         <f ca="1">$L$27</f>
-        <v>14</v>
+        <v>255</v>
       </c>
       <c r="O28" s="2">
         <f>0</f>
@@ -1633,21 +1633,21 @@
       </c>
       <c r="P28" s="2">
         <f t="shared" ref="P28:P33" ca="1" si="10">M28*2^16+N28*2^8+O28</f>
-        <v>200192</v>
+        <v>14089984</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="J29" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(J27/2^10)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K29" s="2">
         <f ca="1">K27*E30</f>
-        <v>58968</v>
+        <v>1446354</v>
       </c>
       <c r="L29" s="2">
         <f ca="1">K33*J31</f>
-        <v>45144</v>
+        <v>167772</v>
       </c>
       <c r="M29" s="2">
         <f>0</f>
@@ -1655,15 +1655,15 @@
       </c>
       <c r="N29" s="2">
         <f ca="1">$L$27</f>
-        <v>14</v>
+        <v>255</v>
       </c>
       <c r="O29" s="2">
         <f ca="1">$L$33</f>
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="P29" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>3595</v>
+        <v>65320</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
@@ -1688,15 +1688,15 @@
       </c>
       <c r="N30" s="2">
         <f ca="1">$L$35</f>
-        <v>3</v>
+        <v>214</v>
       </c>
       <c r="O30" s="2">
         <f ca="1">$L$27</f>
-        <v>14</v>
+        <v>255</v>
       </c>
       <c r="P30" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>782</v>
+        <v>55039</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
@@ -1708,19 +1708,19 @@
       </c>
       <c r="J31" s="2">
         <f ca="1">MOD(J27,2^10)</f>
-        <v>792</v>
+        <v>164</v>
       </c>
       <c r="K31" s="2">
         <f ca="1">IF(_xlfn.FLOOR.MATH(K29/2^10) &gt; 1023, 1023, _xlfn.FLOOR.MATH(K29/2^10))</f>
-        <v>57</v>
+        <v>1023</v>
       </c>
       <c r="L31" s="2">
         <f ca="1">K33*(1023-J31)</f>
-        <v>13167</v>
+        <v>878757</v>
       </c>
       <c r="M31" s="2">
         <f ca="1">$L$33</f>
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="N31" s="2">
         <f>0</f>
@@ -1728,11 +1728,11 @@
       </c>
       <c r="O31" s="2">
         <f ca="1">$L$27</f>
-        <v>14</v>
+        <v>255</v>
       </c>
       <c r="P31" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>720910</v>
+        <v>2621695</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
@@ -1750,7 +1750,7 @@
       </c>
       <c r="M32" s="2">
         <f ca="1">$L$27</f>
-        <v>14</v>
+        <v>255</v>
       </c>
       <c r="N32" s="2">
         <f>0</f>
@@ -1758,11 +1758,11 @@
       </c>
       <c r="O32" s="2">
         <f ca="1">$L$35</f>
-        <v>3</v>
+        <v>214</v>
       </c>
       <c r="P32" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>917507</v>
+        <v>16711894</v>
       </c>
     </row>
     <row r="33" spans="5:16" x14ac:dyDescent="0.3">
@@ -1774,19 +1774,19 @@
       </c>
       <c r="K33" s="2">
         <f ca="1">IF(K31&gt;E32,E32,K31)</f>
-        <v>57</v>
+        <v>1023</v>
       </c>
       <c r="L33" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(L29/2^(2*B17-8))</f>
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="M33" s="2">
         <f ca="1">$L$27</f>
-        <v>14</v>
+        <v>255</v>
       </c>
       <c r="N33" s="2">
         <f ca="1">$L$33</f>
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="O33" s="2">
         <f>0</f>
@@ -1794,7 +1794,7 @@
       </c>
       <c r="P33" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>920320</v>
+        <v>16721920</v>
       </c>
     </row>
     <row r="34" spans="5:16" x14ac:dyDescent="0.3">
@@ -1808,11 +1808,11 @@
     <row r="35" spans="5:16" x14ac:dyDescent="0.3">
       <c r="L35" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(L31/2^(2*B17-8))</f>
-        <v>3</v>
+        <v>214</v>
       </c>
       <c r="M35" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="M35" ca="1">_xlfn.BASE(_xlfn.SWITCH(J29,0,P27,1,P28,2,P29,3,P30,4,P31,5,P32,6,P33),16,6)</f>
-        <v>0E0B00</v>
+        <v>2800FF</v>
       </c>
     </row>
     <row r="36" spans="5:16" x14ac:dyDescent="0.3">
@@ -1839,7 +1839,7 @@
       </c>
       <c r="I39" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(H52/B19)</f>
-        <v>196</v>
+        <v>125</v>
       </c>
       <c r="J39" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(H39/I$39)</f>
@@ -1847,77 +1847,77 @@
       </c>
       <c r="L39" s="2">
         <f ca="1">L27-L33-L35</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="5:16" x14ac:dyDescent="0.3">
       <c r="G40" s="4" t="str">
         <f t="shared" ref="G40:G50" ca="1" si="11">_xlfn.CONCAT(A3,B3,C3,B$16+B$17,"'b",_xlfn.BASE(L3,2,$B$16+$B$17),";")</f>
-        <v xml:space="preserve">            noteAmplitudes_i[ 1] = 16'b0000010101001010;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 1] = 16'b0000000000000000;</v>
       </c>
       <c r="H40" s="2">
         <f t="shared" ref="H40:H50" ca="1" si="12">L3</f>
-        <v>1354</v>
+        <v>0</v>
       </c>
       <c r="J40" s="2">
         <f t="shared" ref="J40:J50" ca="1" si="13">_xlfn.FLOOR.MATH(H40/I$39)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="5:16" x14ac:dyDescent="0.3">
       <c r="G41" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 2] = 16'b0000110101001010;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 2] = 16'b0000000000000000;</v>
       </c>
       <c r="H41" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>3402</v>
+        <v>0</v>
       </c>
       <c r="J41" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="5:16" x14ac:dyDescent="0.3">
       <c r="G42" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 3] = 16'b0000000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 3] = 16'b0000011101010000;</v>
       </c>
       <c r="H42" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>1872</v>
       </c>
       <c r="J42" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="5:16" x14ac:dyDescent="0.3">
       <c r="G43" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 4] = 16'b0000110101001010;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 4] = 16'b0000001101010000;</v>
       </c>
       <c r="H43" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>3402</v>
+        <v>848</v>
       </c>
       <c r="J43" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="5:16" x14ac:dyDescent="0.3">
       <c r="G44" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 5] = 16'b0000000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 5] = 16'b0000001101010000;</v>
       </c>
       <c r="H44" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>848</v>
       </c>
       <c r="J44" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="5:16" x14ac:dyDescent="0.3">
@@ -1937,57 +1937,57 @@
     <row r="46" spans="5:16" x14ac:dyDescent="0.3">
       <c r="G46" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 7] = 16'b0000000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 7] = 16'b0000001101010000;</v>
       </c>
       <c r="H46" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>848</v>
       </c>
       <c r="J46" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="5:16" x14ac:dyDescent="0.3">
       <c r="G47" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 8] = 16'b0000010101001010;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 8] = 16'b0000000000000000;</v>
       </c>
       <c r="H47" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>1354</v>
+        <v>0</v>
       </c>
       <c r="J47" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="5:16" x14ac:dyDescent="0.3">
       <c r="G48" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 9] = 16'b0000000101001010;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 9] = 16'b0000000000000000;</v>
       </c>
       <c r="H48" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>330</v>
+        <v>0</v>
       </c>
       <c r="J48" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G49" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[10] = 16'b0000000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[10] = 16'b0000011101010000;</v>
       </c>
       <c r="H49" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>1872</v>
       </c>
       <c r="J49" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:25" x14ac:dyDescent="0.3">
@@ -2007,7 +2007,7 @@
     <row r="51" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G51" s="5" t="str">
         <f ca="1">_xlfn.CONCAT("            amplitudeSumNew_i = ",B16+B17+_xlfn.CEILING.MATH(IMLOG2(B19)),"'b",_xlfn.BASE(H52,2,B16+B17+_xlfn.CEILING.MATH(IMLOG2(B19))),";")</f>
-        <v xml:space="preserve">            amplitudeSumNew_i = 22'b0000000010011001110010;</v>
+        <v xml:space="preserve">            amplitudeSumNew_i = 22'b0000000001100010010000;</v>
       </c>
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.3">
@@ -2016,7 +2016,7 @@
       </c>
       <c r="H52" s="2">
         <f ca="1">SUM(H39:H50)</f>
-        <v>9842</v>
+        <v>6288</v>
       </c>
     </row>
     <row r="54" spans="1:25" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
adapted linear visualizer to work with Note struct
</commit_message>
<xml_diff>
--- a/other/LinearVisualizer.xlsx
+++ b/other/LinearVisualizer.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\CCHW\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B626433E-82C3-4F8F-803A-892CF8B0AFAD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{267BD6F9-C137-4E0A-8C41-295F70BBA74A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9DBF0F91-83D7-4F64-B04C-B7CB81DC62EF}"/>
   </bookViews>
@@ -695,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A6626A4-8C87-4B90-BEEB-AEB487ACEA9E}">
   <dimension ref="A1:Y114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H71" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H83" sqref="H83"/>
+    <sheetView tabSelected="1" topLeftCell="J79" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y90" sqref="Y90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -764,11 +764,11 @@
       </c>
       <c r="D2" s="2" t="str">
         <f ca="1">_xlfn.CONCAT(B$16+B$17,"'b",REPT("0",B$16-LEN(E2)))</f>
-        <v>16'b0000</v>
+        <v>16'b000</v>
       </c>
       <c r="E2" s="2" t="str">
         <f ca="1">DEC2BIN(_xlfn.FLOOR.MATH(RAND()*10))</f>
-        <v>11</v>
+        <v>101</v>
       </c>
       <c r="F2" s="2" t="str">
         <f>_xlfn.CONCAT(REPT("0",B$17),";")</f>
@@ -776,23 +776,23 @@
       </c>
       <c r="G2" s="4" t="str">
         <f ca="1">_xlfn.CONCAT(A2,B2,C2,D2,E2,F2)</f>
-        <v xml:space="preserve">            noteAmplitudes_i[ 0] = 16'b0000110000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 0] = 16'b0001010000000000;</v>
       </c>
       <c r="H2" s="2">
         <f t="shared" ref="H2:H13" ca="1" si="0">BIN2DEC(E2)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I2" s="2">
         <f t="shared" ref="I2:I13" ca="1" si="1">H2*2^B$17</f>
-        <v>3072</v>
+        <v>5120</v>
       </c>
       <c r="J2" s="2">
         <f ca="1">SUM(H2:H13)</f>
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="K2" s="2">
         <f t="shared" ref="K2:K13" ca="1" si="2">I2-J$7</f>
-        <v>-1620</v>
+        <v>-1000</v>
       </c>
       <c r="L2" s="2">
         <f ca="1">IF(K2&gt;0,K2,0)</f>
@@ -815,11 +815,11 @@
       </c>
       <c r="D3" s="2" t="str">
         <f t="shared" ref="D3:D13" ca="1" si="3">_xlfn.CONCAT(B$16+B$17,"'b",REPT("0",B$16-LEN(E3)))</f>
-        <v>16'b0000</v>
+        <v>16'b000</v>
       </c>
       <c r="E3" s="2" t="str">
         <f t="shared" ref="E3:E13" ca="1" si="4">DEC2BIN(_xlfn.FLOOR.MATH(RAND()*10))</f>
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="F3" s="2" t="str">
         <f t="shared" ref="F3:F13" si="5">_xlfn.CONCAT(REPT("0",B$17),";")</f>
@@ -827,31 +827,31 @@
       </c>
       <c r="G3" s="4" t="str">
         <f t="shared" ref="G3:G13" ca="1" si="6">_xlfn.CONCAT(A3,B3,C3,D3,E3,F3)</f>
-        <v xml:space="preserve">            noteAmplitudes_i[ 1] = 16'b0000110000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 1] = 16'b0001110000000000;</v>
       </c>
       <c r="H3" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I3" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>3072</v>
+        <v>7168</v>
       </c>
       <c r="J3" s="2">
         <f ca="1">J2*2^B17</f>
-        <v>47104</v>
+        <v>61440</v>
       </c>
       <c r="K3" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>-1620</v>
+        <v>1048</v>
       </c>
       <c r="L3" s="2">
         <f t="shared" ref="L3:L13" ca="1" si="7">IF(K3&gt;0,K3,0)</f>
-        <v>0</v>
+        <v>1048</v>
       </c>
       <c r="M3" s="2">
         <f t="shared" ref="M3:M13" ca="1" si="8">IF(K3&gt;0,I3,0)</f>
-        <v>0</v>
+        <v>7168</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -866,11 +866,11 @@
       </c>
       <c r="D4" s="2" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>16'b000</v>
+        <v>16'b00</v>
       </c>
       <c r="E4" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>110</v>
+        <v>1001</v>
       </c>
       <c r="F4" s="2" t="str">
         <f t="shared" si="5"/>
@@ -878,27 +878,27 @@
       </c>
       <c r="G4" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 2] = 16'b0001100000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 2] = 16'b0010010000000000;</v>
       </c>
       <c r="H4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="I4" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>6144</v>
+        <v>9216</v>
       </c>
       <c r="K4" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1452</v>
+        <v>3096</v>
       </c>
       <c r="L4" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>1452</v>
+        <v>3096</v>
       </c>
       <c r="M4" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>6144</v>
+        <v>9216</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -940,7 +940,7 @@
       </c>
       <c r="K5" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>-3668</v>
+        <v>-5096</v>
       </c>
       <c r="L5" s="2">
         <f t="shared" ca="1" si="7"/>
@@ -967,7 +967,7 @@
       </c>
       <c r="E6" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" s="2" t="str">
         <f t="shared" si="5"/>
@@ -975,23 +975,23 @@
       </c>
       <c r="G6" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 4] = 16'b0000110000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 4] = 16'b0000100000000000;</v>
       </c>
       <c r="H6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I6" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>3072</v>
+        <v>2048</v>
       </c>
       <c r="J6" s="3">
         <f ca="1">J2*B18</f>
-        <v>4.58203125</v>
+        <v>5.9765625</v>
       </c>
       <c r="K6" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>-1620</v>
+        <v>-4072</v>
       </c>
       <c r="L6" s="2">
         <f t="shared" ca="1" si="7"/>
@@ -1014,11 +1014,11 @@
       </c>
       <c r="D7" s="2" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>16'b000</v>
+        <v>16'b00000</v>
       </c>
       <c r="E7" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>110</v>
+        <v>1</v>
       </c>
       <c r="F7" s="2" t="str">
         <f t="shared" si="5"/>
@@ -1026,31 +1026,31 @@
       </c>
       <c r="G7" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 5] = 16'b0001100000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 5] = 16'b0000010000000000;</v>
       </c>
       <c r="H7" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I7" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>6144</v>
+        <v>1024</v>
       </c>
       <c r="J7" s="2">
         <f ca="1">J3 * BIN2DEC(C18) / 2^B17</f>
-        <v>4692</v>
+        <v>6120</v>
       </c>
       <c r="K7" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1452</v>
+        <v>-5096</v>
       </c>
       <c r="L7" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>1452</v>
+        <v>0</v>
       </c>
       <c r="M7" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>6144</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -1065,11 +1065,11 @@
       </c>
       <c r="D8" s="2" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>16'b0000</v>
+        <v>16'b000</v>
       </c>
       <c r="E8" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>11</v>
+        <v>110</v>
       </c>
       <c r="F8" s="2" t="str">
         <f t="shared" si="5"/>
@@ -1077,27 +1077,27 @@
       </c>
       <c r="G8" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 6] = 16'b0000110000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 6] = 16'b0001100000000000;</v>
       </c>
       <c r="H8" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I8" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>3072</v>
+        <v>6144</v>
       </c>
       <c r="K8" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>-1620</v>
+        <v>24</v>
       </c>
       <c r="L8" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="M8" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>6144</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -1116,7 +1116,7 @@
       </c>
       <c r="E9" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="F9" s="2" t="str">
         <f t="shared" si="5"/>
@@ -1124,30 +1124,30 @@
       </c>
       <c r="G9" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 7] = 16'b0001110000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 7] = 16'b0001000000000000;</v>
       </c>
       <c r="H9" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I9" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>7168</v>
+        <v>4096</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="K9" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>2476</v>
+        <v>-2024</v>
       </c>
       <c r="L9" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>2476</v>
+        <v>0</v>
       </c>
       <c r="M9" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>7168</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -1162,11 +1162,11 @@
       </c>
       <c r="D10" s="2" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>16'b00000</v>
+        <v>16'b00</v>
       </c>
       <c r="E10" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>1001</v>
       </c>
       <c r="F10" s="2" t="str">
         <f t="shared" si="5"/>
@@ -1174,31 +1174,31 @@
       </c>
       <c r="G10" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 8] = 16'b0000010000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 8] = 16'b0010010000000000;</v>
       </c>
       <c r="H10" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="I10" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>1024</v>
+        <v>9216</v>
       </c>
       <c r="J10" s="2">
         <f ca="1">J11/2^B17</f>
-        <v>9.08984375</v>
+        <v>9.1171875</v>
       </c>
       <c r="K10" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>-3668</v>
+        <v>3096</v>
       </c>
       <c r="L10" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>3096</v>
       </c>
       <c r="M10" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>9216</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -1217,7 +1217,7 @@
       </c>
       <c r="E11" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="F11" s="2" t="str">
         <f t="shared" si="5"/>
@@ -1225,31 +1225,31 @@
       </c>
       <c r="G11" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 9] = 16'b0001100000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 9] = 16'b0001010000000000;</v>
       </c>
       <c r="H11" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I11" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>6144</v>
+        <v>5120</v>
       </c>
       <c r="J11" s="2">
         <f ca="1">SUM(L2:L13)</f>
-        <v>9308</v>
+        <v>9336</v>
       </c>
       <c r="K11" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1452</v>
+        <v>-1000</v>
       </c>
       <c r="L11" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>1452</v>
+        <v>0</v>
       </c>
       <c r="M11" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>6144</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -1264,11 +1264,11 @@
       </c>
       <c r="D12" s="2" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>16'b000</v>
+        <v>16'b00</v>
       </c>
       <c r="E12" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>111</v>
+        <v>1000</v>
       </c>
       <c r="F12" s="2" t="str">
         <f t="shared" si="5"/>
@@ -1276,27 +1276,27 @@
       </c>
       <c r="G12" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[10] = 16'b0001110000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[10] = 16'b0010000000000000;</v>
       </c>
       <c r="H12" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I12" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>7168</v>
+        <v>8192</v>
       </c>
       <c r="K12" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>2476</v>
+        <v>2072</v>
       </c>
       <c r="L12" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>2476</v>
+        <v>2072</v>
       </c>
       <c r="M12" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>7168</v>
+        <v>8192</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -1311,11 +1311,11 @@
       </c>
       <c r="D13" s="2" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>16'b00000</v>
+        <v>16'b0000</v>
       </c>
       <c r="E13" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F13" s="2" t="str">
         <f t="shared" si="5"/>
@@ -1323,19 +1323,19 @@
       </c>
       <c r="G13" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[11] = 16'b0000000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[11] = 16'b0000110000000000;</v>
       </c>
       <c r="H13" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I13" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>3072</v>
       </c>
       <c r="K13" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>-4692</v>
+        <v>-3048</v>
       </c>
       <c r="L13" s="2">
         <f t="shared" ca="1" si="7"/>
@@ -1386,27 +1386,27 @@
       <c r="C17" s="8"/>
       <c r="G17" s="4" t="str">
         <f ca="1">_xlfn.CONCAT("notePosition_i = 10'b",REPT(0,B17-LEN(_xlfn.BASE(I17,2))),_xlfn.BASE(I17,2),";" )</f>
-        <v>notePosition_i = 10'b0101001111;</v>
+        <v>notePosition_i = 10'b0000011111;</v>
       </c>
       <c r="H17" s="2">
         <f ca="1">I17/2^10</f>
-        <v>0.3271484375</v>
+        <v>3.02734375E-2</v>
       </c>
       <c r="I17" s="2">
         <f ca="1">RANDBETWEEN(0,1023)</f>
-        <v>335</v>
+        <v>31</v>
       </c>
       <c r="J17" s="2">
         <f ca="1">I17*24</f>
-        <v>8040</v>
+        <v>744</v>
       </c>
       <c r="K17" s="2">
         <f ca="1">IF(J21=3,24576-J17,8192-J17)</f>
-        <v>152</v>
+        <v>7448</v>
       </c>
       <c r="L17" s="2">
         <f ca="1">IF(J21=3,K23+170, K23)</f>
-        <v>0</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
@@ -1456,7 +1456,7 @@
       </c>
       <c r="K20" s="2">
         <f ca="1">K17*H20*H21*H22</f>
-        <v>3317248</v>
+        <v>162545152</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>24</v>
@@ -1483,11 +1483,11 @@
       </c>
       <c r="K21" s="2" t="str">
         <f ca="1">_xlfn.BASE(K20,2,32)</f>
-        <v>00000000001100101001111000000000</v>
+        <v>00001001101100000011111000000000</v>
       </c>
       <c r="L21" s="2">
         <f ca="1">MOD(IF(L17&lt;0,L17+1023,L17), 1024)</f>
-        <v>0</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
@@ -1512,21 +1512,21 @@
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="K23" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(K20/2^(B17+B17+C15-3))</f>
-        <v>0</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G26" s="4" t="str">
         <f ca="1">_xlfn.CONCAT("        noteAmplitude_i = 10'b",REPT(0,B17-LEN(_xlfn.BASE(I26,2))),_xlfn.BASE(I26,2),";" )</f>
-        <v xml:space="preserve">        noteAmplitude_i = 10'b1011001000;</v>
+        <v xml:space="preserve">        noteAmplitude_i = 10'b0100101111;</v>
       </c>
       <c r="H26" s="2">
         <f ca="1">I26/2^10</f>
-        <v>0.6953125</v>
+        <v>0.2958984375</v>
       </c>
       <c r="I26" s="2">
         <f ca="1">RANDBETWEEN(0,1023)</f>
-        <v>712</v>
+        <v>303</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>28</v>
@@ -1558,23 +1558,23 @@
       </c>
       <c r="G27" s="4" t="str">
         <f ca="1">_xlfn.CONCAT("        noteAmplitudeFast_i = 10'b",REPT(0,B17-LEN(_xlfn.BASE(I27,2))),_xlfn.BASE(I27,2),";" )</f>
-        <v xml:space="preserve">        noteAmplitudeFast_i = 10'b1110000110;</v>
+        <v xml:space="preserve">        noteAmplitudeFast_i = 10'b1010101100;</v>
       </c>
       <c r="H27" s="2">
         <f t="shared" ref="H27:H28" ca="1" si="9">I27/2^10</f>
-        <v>0.880859375</v>
+        <v>0.66796875</v>
       </c>
       <c r="I27" s="2">
         <f ca="1">RANDBETWEEN(0,1023)</f>
-        <v>902</v>
+        <v>684</v>
       </c>
       <c r="J27" s="2">
         <f ca="1">I28*E31</f>
-        <v>2664</v>
+        <v>2028</v>
       </c>
       <c r="K27" s="2">
         <f ca="1">IF(E33,I26,I27)</f>
-        <v>902</v>
+        <v>684</v>
       </c>
       <c r="L27" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(K33/2^(B17-8))</f>
@@ -1586,7 +1586,7 @@
       </c>
       <c r="N27" s="2">
         <f ca="1">$L$33</f>
-        <v>153</v>
+        <v>250</v>
       </c>
       <c r="O27" s="2">
         <f>0</f>
@@ -1594,21 +1594,21 @@
       </c>
       <c r="P27" s="2">
         <f ca="1">M27*2^16+N27*2^8+O27</f>
-        <v>16750848</v>
+        <v>16775680</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G28" s="4" t="str">
         <f ca="1">_xlfn.CONCAT("        noteHue_i = 10'b",REPT(0,B17-LEN(_xlfn.BASE(I28,2))),_xlfn.BASE(I28,2),";" )</f>
-        <v xml:space="preserve">        noteHue_i = 10'b0110111100;</v>
+        <v xml:space="preserve">        noteHue_i = 10'b0101010010;</v>
       </c>
       <c r="H28" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>0.43359375</v>
+        <v>0.330078125</v>
       </c>
       <c r="I28" s="2">
         <f ca="1">RANDBETWEEN(0,1023)</f>
-        <v>444</v>
+        <v>338</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>29</v>
@@ -1621,7 +1621,7 @@
       </c>
       <c r="M28" s="2">
         <f ca="1">$L$35</f>
-        <v>101</v>
+        <v>4</v>
       </c>
       <c r="N28" s="2">
         <f ca="1">$L$27</f>
@@ -1633,21 +1633,21 @@
       </c>
       <c r="P28" s="2">
         <f t="shared" ref="P28:P33" ca="1" si="10">M28*2^16+N28*2^8+O28</f>
-        <v>6684416</v>
+        <v>327424</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="J29" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(J27/2^10)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K29" s="2">
         <f ca="1">K27*E30</f>
-        <v>1477476</v>
+        <v>1120392</v>
       </c>
       <c r="L29" s="2">
         <f ca="1">K33*J31</f>
-        <v>630168</v>
+        <v>1027092</v>
       </c>
       <c r="M29" s="2">
         <f>0</f>
@@ -1659,11 +1659,11 @@
       </c>
       <c r="O29" s="2">
         <f ca="1">$L$33</f>
-        <v>153</v>
+        <v>250</v>
       </c>
       <c r="P29" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>65433</v>
+        <v>65530</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
@@ -1688,7 +1688,7 @@
       </c>
       <c r="N30" s="2">
         <f ca="1">$L$35</f>
-        <v>101</v>
+        <v>4</v>
       </c>
       <c r="O30" s="2">
         <f ca="1">$L$27</f>
@@ -1696,7 +1696,7 @@
       </c>
       <c r="P30" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>26111</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
@@ -1708,7 +1708,7 @@
       </c>
       <c r="J31" s="2">
         <f ca="1">MOD(J27,2^10)</f>
-        <v>616</v>
+        <v>1004</v>
       </c>
       <c r="K31" s="2">
         <f ca="1">IF(_xlfn.FLOOR.MATH(K29/2^10) &gt; 1023, 1023, _xlfn.FLOOR.MATH(K29/2^10))</f>
@@ -1716,11 +1716,11 @@
       </c>
       <c r="L31" s="2">
         <f ca="1">K33*(1023-J31)</f>
-        <v>416361</v>
+        <v>19437</v>
       </c>
       <c r="M31" s="2">
         <f ca="1">$L$33</f>
-        <v>153</v>
+        <v>250</v>
       </c>
       <c r="N31" s="2">
         <f>0</f>
@@ -1732,7 +1732,7 @@
       </c>
       <c r="P31" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>10027263</v>
+        <v>16384255</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
@@ -1758,11 +1758,11 @@
       </c>
       <c r="O32" s="2">
         <f ca="1">$L$35</f>
-        <v>101</v>
+        <v>4</v>
       </c>
       <c r="P32" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>16711781</v>
+        <v>16711684</v>
       </c>
     </row>
     <row r="33" spans="5:16" x14ac:dyDescent="0.3">
@@ -1778,7 +1778,7 @@
       </c>
       <c r="L33" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(L29/2^(2*B17-8))</f>
-        <v>153</v>
+        <v>250</v>
       </c>
       <c r="M33" s="2">
         <f ca="1">$L$27</f>
@@ -1786,7 +1786,7 @@
       </c>
       <c r="N33" s="2">
         <f ca="1">$L$33</f>
-        <v>153</v>
+        <v>250</v>
       </c>
       <c r="O33" s="2">
         <f>0</f>
@@ -1794,7 +1794,7 @@
       </c>
       <c r="P33" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>16750848</v>
+        <v>16775680</v>
       </c>
     </row>
     <row r="34" spans="5:16" x14ac:dyDescent="0.3">
@@ -1808,11 +1808,11 @@
     <row r="35" spans="5:16" x14ac:dyDescent="0.3">
       <c r="L35" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(L31/2^(2*B17-8))</f>
-        <v>101</v>
+        <v>4</v>
       </c>
       <c r="M35" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="M35" ca="1">_xlfn.BASE(_xlfn.SWITCH(J29,0,P27,1,P28,2,P29,3,P30,4,P31,5,P32,6,P33),16,6)</f>
-        <v>00FF99</v>
+        <v>04FF00</v>
       </c>
     </row>
     <row r="36" spans="5:16" x14ac:dyDescent="0.3">
@@ -1853,29 +1853,29 @@
     <row r="40" spans="5:16" x14ac:dyDescent="0.3">
       <c r="G40" s="4" t="str">
         <f t="shared" ref="G40:G50" ca="1" si="11">_xlfn.CONCAT(A3,B3,C3,B$16+B$17,"'b",_xlfn.BASE(L3,2,$B$16+$B$17),";")</f>
-        <v xml:space="preserve">            noteAmplitudes_i[ 1] = 16'b0000000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 1] = 16'b0000010000011000;</v>
       </c>
       <c r="H40" s="2">
         <f t="shared" ref="H40:H50" ca="1" si="12">L3</f>
-        <v>0</v>
+        <v>1048</v>
       </c>
       <c r="J40" s="2">
         <f t="shared" ref="J40:J50" ca="1" si="13">_xlfn.FLOOR.MATH(H40/I$39)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="5:16" x14ac:dyDescent="0.3">
       <c r="G41" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 2] = 16'b0000010110101100;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 2] = 16'b0000110000011000;</v>
       </c>
       <c r="H41" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>1452</v>
+        <v>3096</v>
       </c>
       <c r="J41" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="5:16" x14ac:dyDescent="0.3">
@@ -1909,25 +1909,25 @@
     <row r="44" spans="5:16" x14ac:dyDescent="0.3">
       <c r="G44" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 5] = 16'b0000010110101100;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 5] = 16'b0000000000000000;</v>
       </c>
       <c r="H44" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>1452</v>
+        <v>0</v>
       </c>
       <c r="J44" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="5:16" x14ac:dyDescent="0.3">
       <c r="G45" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 6] = 16'b0000000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 6] = 16'b0000000000011000;</v>
       </c>
       <c r="H45" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="J45" s="2">
         <f t="shared" ca="1" si="13"/>
@@ -1937,57 +1937,57 @@
     <row r="46" spans="5:16" x14ac:dyDescent="0.3">
       <c r="G46" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 7] = 16'b0000100110101100;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 7] = 16'b0000000000000000;</v>
       </c>
       <c r="H46" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>2476</v>
+        <v>0</v>
       </c>
       <c r="J46" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="5:16" x14ac:dyDescent="0.3">
       <c r="G47" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 8] = 16'b0000000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 8] = 16'b0000110000011000;</v>
       </c>
       <c r="H47" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>3096</v>
       </c>
       <c r="J47" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="5:16" x14ac:dyDescent="0.3">
       <c r="G48" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 9] = 16'b0000010110101100;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 9] = 16'b0000000000000000;</v>
       </c>
       <c r="H48" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>1452</v>
+        <v>0</v>
       </c>
       <c r="J48" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G49" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[10] = 16'b0000100110101100;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[10] = 16'b0000100000011000;</v>
       </c>
       <c r="H49" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>2476</v>
+        <v>2072</v>
       </c>
       <c r="J49" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50" spans="1:25" x14ac:dyDescent="0.3">
@@ -2007,7 +2007,7 @@
     <row r="51" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G51" s="5" t="str">
         <f ca="1">_xlfn.CONCAT("            amplitudeSumNew_i = ",B16+B17+_xlfn.CEILING.MATH(IMLOG2(B19)),"'b",_xlfn.BASE(H52,2,B16+B17+_xlfn.CEILING.MATH(IMLOG2(B19))),";")</f>
-        <v xml:space="preserve">            amplitudeSumNew_i = 22'b0000000010010001011100;</v>
+        <v xml:space="preserve">            amplitudeSumNew_i = 22'b0000000010010001111000;</v>
       </c>
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.3">
@@ -2016,7 +2016,7 @@
       </c>
       <c r="H52" s="2">
         <f ca="1">SUM(H39:H50)</f>
-        <v>9308</v>
+        <v>9336</v>
       </c>
     </row>
     <row r="54" spans="1:25" x14ac:dyDescent="0.3">
@@ -3013,7 +3013,7 @@
     </row>
     <row r="84" spans="6:25" x14ac:dyDescent="0.3">
       <c r="F84" s="2">
-        <f t="shared" ca="1" si="14"/>
+        <f ca="1">H84/2^B$17</f>
         <v>0</v>
       </c>
       <c r="G84" s="6" t="s">
@@ -3178,54 +3178,58 @@
         <f ca="1">U88*2^16+V88*2^8+W88</f>
         <v>15663320</v>
       </c>
+      <c r="Y88" s="2" t="str">
+        <f t="shared" ref="Y88:Y99" ca="1" si="25">_xlfn.BASE(X88,16,6)</f>
+        <v>EF00D8</v>
+      </c>
     </row>
     <row r="89" spans="6:25" x14ac:dyDescent="0.3">
       <c r="I89" s="2">
-        <f t="shared" ref="I89:I99" ca="1" si="25">O74*E$31</f>
+        <f t="shared" ref="I89:I99" ca="1" si="26">O74*E$31</f>
         <v>216</v>
       </c>
       <c r="J89" s="2">
-        <f t="shared" ref="J89:J99" ca="1" si="26">_xlfn.FLOOR.MATH(I89/2^B$17)</f>
+        <f t="shared" ref="J89:J99" ca="1" si="27">_xlfn.FLOOR.MATH(I89/2^B$17)</f>
         <v>0</v>
       </c>
       <c r="K89" s="2">
-        <f t="shared" ref="K89:K99" ca="1" si="27">MOD(I89, 2^B$17)</f>
+        <f t="shared" ref="K89:K99" ca="1" si="28">MOD(I89, 2^B$17)</f>
         <v>216</v>
       </c>
       <c r="L89" s="2">
-        <f t="shared" ref="L89:L99" ca="1" si="28">IF(E34,K60,L60)</f>
+        <f t="shared" ref="L89:L99" ca="1" si="29">IF(E34,K60,L60)</f>
         <v>717</v>
       </c>
       <c r="M89" s="2">
-        <f t="shared" ref="M89:M99" ca="1" si="29">L89*E$30</f>
+        <f t="shared" ref="M89:M99" ca="1" si="30">L89*E$30</f>
         <v>1174446</v>
       </c>
       <c r="N89" s="2">
-        <f t="shared" ref="N89:N99" ca="1" si="30">IF(_xlfn.FLOOR.MATH(M89/2^B$17) &gt; 1023, 1023, _xlfn.FLOOR.MATH(M89/2^B$17))</f>
+        <f t="shared" ref="N89:N99" ca="1" si="31">IF(_xlfn.FLOOR.MATH(M89/2^B$17) &gt; 1023, 1023, _xlfn.FLOOR.MATH(M89/2^B$17))</f>
         <v>1023</v>
       </c>
       <c r="O89" s="2">
-        <f t="shared" ref="O89:O99" ca="1" si="31">IF(N89&gt;E$32,E$32,N89)</f>
+        <f t="shared" ref="O89:O99" ca="1" si="32">IF(N89&gt;E$32,E$32,N89)</f>
         <v>1023</v>
       </c>
       <c r="P89" s="2">
-        <f t="shared" ref="P89:P99" ca="1" si="32">_xlfn.FLOOR.MATH(O89/2^(B$17-8))</f>
+        <f t="shared" ref="P89:P99" ca="1" si="33">_xlfn.FLOOR.MATH(O89/2^(B$17-8))</f>
         <v>255</v>
       </c>
       <c r="Q89" s="2">
-        <f t="shared" ref="Q89:Q99" ca="1" si="33">O89*K89</f>
+        <f t="shared" ref="Q89:Q99" ca="1" si="34">O89*K89</f>
         <v>220968</v>
       </c>
       <c r="R89" s="2">
-        <f t="shared" ref="R89:R99" ca="1" si="34">O89*(2^(B$17) - 1 - K89)</f>
+        <f t="shared" ref="R89:R99" ca="1" si="35">O89*(2^(B$17) - 1 - K89)</f>
         <v>825561</v>
       </c>
       <c r="S89" s="2">
-        <f t="shared" ref="S89:S99" ca="1" si="35">_xlfn.FLOOR.MATH(Q89/2^(2*B$17-8))</f>
+        <f t="shared" ref="S89:S99" ca="1" si="36">_xlfn.FLOOR.MATH(Q89/2^(2*B$17-8))</f>
         <v>53</v>
       </c>
       <c r="T89" s="2">
-        <f t="shared" ref="T89:T99" ca="1" si="36">_xlfn.FLOOR.MATH(R89/2^(2*B$17-8))</f>
+        <f t="shared" ref="T89:T99" ca="1" si="37">_xlfn.FLOOR.MATH(R89/2^(2*B$17-8))</f>
         <v>201</v>
       </c>
       <c r="U89" s="2" cm="1">
@@ -3241,61 +3245,61 @@
         <v>0</v>
       </c>
       <c r="X89" s="2">
-        <f t="shared" ref="X89:X99" ca="1" si="37">U89*2^16+V89*2^8+W89</f>
+        <f t="shared" ref="X89:X99" ca="1" si="38">U89*2^16+V89*2^8+W89</f>
         <v>16725248</v>
       </c>
       <c r="Y89" s="2" t="str">
-        <f t="shared" ref="Y89:Y99" ca="1" si="38">_xlfn.BASE(X89,16,6)</f>
+        <f t="shared" ca="1" si="25"/>
         <v>FF3500</v>
       </c>
     </row>
     <row r="90" spans="6:25" x14ac:dyDescent="0.3">
       <c r="I90" s="2">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="26"/>
         <v>2454</v>
       </c>
       <c r="J90" s="2">
-        <f t="shared" ca="1" si="26"/>
+        <f t="shared" ca="1" si="27"/>
         <v>2</v>
       </c>
       <c r="K90" s="2">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="28"/>
         <v>406</v>
       </c>
       <c r="L90" s="2">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="29"/>
         <v>450</v>
       </c>
       <c r="M90" s="2">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="30"/>
         <v>737100</v>
       </c>
       <c r="N90" s="2">
-        <f t="shared" ca="1" si="30"/>
-        <v>719</v>
-      </c>
-      <c r="O90" s="2">
         <f t="shared" ca="1" si="31"/>
         <v>719</v>
       </c>
+      <c r="O90" s="2">
+        <f t="shared" ca="1" si="32"/>
+        <v>719</v>
+      </c>
       <c r="P90" s="2">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="33"/>
         <v>179</v>
       </c>
       <c r="Q90" s="2">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="34"/>
         <v>291914</v>
       </c>
       <c r="R90" s="2">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="35"/>
         <v>443623</v>
       </c>
       <c r="S90" s="2">
-        <f t="shared" ca="1" si="35"/>
+        <f t="shared" ca="1" si="36"/>
         <v>71</v>
       </c>
       <c r="T90" s="2">
-        <f t="shared" ca="1" si="36"/>
+        <f t="shared" ca="1" si="37"/>
         <v>108</v>
       </c>
       <c r="U90" s="2" cm="1">
@@ -3311,61 +3315,61 @@
         <v>71</v>
       </c>
       <c r="X90" s="2">
-        <f t="shared" ca="1" si="37"/>
+        <f t="shared" ca="1" si="38"/>
         <v>45895</v>
       </c>
       <c r="Y90" s="2" t="str">
-        <f t="shared" ca="1" si="38"/>
+        <f t="shared" ca="1" si="25"/>
         <v>00B347</v>
       </c>
     </row>
     <row r="91" spans="6:25" x14ac:dyDescent="0.3">
       <c r="I91" s="2">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="26"/>
         <v>1554</v>
       </c>
       <c r="J91" s="2">
-        <f t="shared" ca="1" si="26"/>
+        <f t="shared" ca="1" si="27"/>
         <v>1</v>
       </c>
       <c r="K91" s="2">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="28"/>
         <v>530</v>
       </c>
       <c r="L91" s="2">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="29"/>
         <v>0</v>
       </c>
       <c r="M91" s="2">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="30"/>
         <v>0</v>
       </c>
       <c r="N91" s="2">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>0</v>
       </c>
       <c r="O91" s="2">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="P91" s="2">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="33"/>
         <v>0</v>
       </c>
       <c r="Q91" s="2">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="34"/>
         <v>0</v>
       </c>
       <c r="R91" s="2">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="35"/>
         <v>0</v>
       </c>
       <c r="S91" s="2">
-        <f t="shared" ca="1" si="35"/>
+        <f t="shared" ca="1" si="36"/>
         <v>0</v>
       </c>
       <c r="T91" s="2">
-        <f t="shared" ca="1" si="36"/>
+        <f t="shared" ca="1" si="37"/>
         <v>0</v>
       </c>
       <c r="U91" s="2" cm="1">
@@ -3381,61 +3385,61 @@
         <v>0</v>
       </c>
       <c r="X91" s="2">
-        <f t="shared" ca="1" si="37"/>
+        <f t="shared" ca="1" si="38"/>
         <v>0</v>
       </c>
       <c r="Y91" s="2" t="str">
-        <f t="shared" ca="1" si="38"/>
+        <f t="shared" ca="1" si="25"/>
         <v>000000</v>
       </c>
     </row>
     <row r="92" spans="6:25" x14ac:dyDescent="0.3">
       <c r="I92" s="2">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="26"/>
         <v>3078</v>
       </c>
       <c r="J92" s="2">
-        <f t="shared" ca="1" si="26"/>
+        <f t="shared" ca="1" si="27"/>
         <v>3</v>
       </c>
       <c r="K92" s="2">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="28"/>
         <v>6</v>
       </c>
       <c r="L92" s="2">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="29"/>
         <v>0</v>
       </c>
       <c r="M92" s="2">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="30"/>
         <v>0</v>
       </c>
       <c r="N92" s="2">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>0</v>
       </c>
       <c r="O92" s="2">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="P92" s="2">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="33"/>
         <v>0</v>
       </c>
       <c r="Q92" s="2">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="34"/>
         <v>0</v>
       </c>
       <c r="R92" s="2">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="35"/>
         <v>0</v>
       </c>
       <c r="S92" s="2">
-        <f t="shared" ca="1" si="35"/>
+        <f t="shared" ca="1" si="36"/>
         <v>0</v>
       </c>
       <c r="T92" s="2">
-        <f t="shared" ca="1" si="36"/>
+        <f t="shared" ca="1" si="37"/>
         <v>0</v>
       </c>
       <c r="U92" s="2" cm="1">
@@ -3451,61 +3455,61 @@
         <v>0</v>
       </c>
       <c r="X92" s="2">
-        <f t="shared" ca="1" si="37"/>
+        <f t="shared" ca="1" si="38"/>
         <v>0</v>
       </c>
       <c r="Y92" s="2" t="str">
-        <f t="shared" ca="1" si="38"/>
+        <f t="shared" ca="1" si="25"/>
         <v>000000</v>
       </c>
     </row>
     <row r="93" spans="6:25" x14ac:dyDescent="0.3">
       <c r="I93" s="2">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="26"/>
         <v>4266</v>
       </c>
       <c r="J93" s="2">
-        <f t="shared" ca="1" si="26"/>
+        <f t="shared" ca="1" si="27"/>
         <v>4</v>
       </c>
       <c r="K93" s="2">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="28"/>
         <v>170</v>
       </c>
       <c r="L93" s="2">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="29"/>
         <v>0</v>
       </c>
       <c r="M93" s="2">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="30"/>
         <v>0</v>
       </c>
       <c r="N93" s="2">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>0</v>
       </c>
       <c r="O93" s="2">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="P93" s="2">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="33"/>
         <v>0</v>
       </c>
       <c r="Q93" s="2">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="34"/>
         <v>0</v>
       </c>
       <c r="R93" s="2">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="35"/>
         <v>0</v>
       </c>
       <c r="S93" s="2">
-        <f t="shared" ca="1" si="35"/>
+        <f t="shared" ca="1" si="36"/>
         <v>0</v>
       </c>
       <c r="T93" s="2">
-        <f t="shared" ca="1" si="36"/>
+        <f t="shared" ca="1" si="37"/>
         <v>0</v>
       </c>
       <c r="U93" s="2" cm="1">
@@ -3521,61 +3525,61 @@
         <v>0</v>
       </c>
       <c r="X93" s="2">
-        <f t="shared" ca="1" si="37"/>
+        <f t="shared" ca="1" si="38"/>
         <v>0</v>
       </c>
       <c r="Y93" s="2" t="str">
-        <f t="shared" ca="1" si="38"/>
+        <f t="shared" ca="1" si="25"/>
         <v>000000</v>
       </c>
     </row>
     <row r="94" spans="6:25" x14ac:dyDescent="0.3">
       <c r="I94" s="2">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="26"/>
         <v>6120</v>
       </c>
       <c r="J94" s="2">
-        <f t="shared" ca="1" si="26"/>
+        <f t="shared" ca="1" si="27"/>
         <v>5</v>
       </c>
       <c r="K94" s="2">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="28"/>
         <v>1000</v>
       </c>
       <c r="L94" s="2">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="29"/>
         <v>0</v>
       </c>
       <c r="M94" s="2">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="30"/>
         <v>0</v>
       </c>
       <c r="N94" s="2">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>0</v>
       </c>
       <c r="O94" s="2">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="P94" s="2">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="33"/>
         <v>0</v>
       </c>
       <c r="Q94" s="2">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="34"/>
         <v>0</v>
       </c>
       <c r="R94" s="2">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="35"/>
         <v>0</v>
       </c>
       <c r="S94" s="2">
-        <f t="shared" ca="1" si="35"/>
+        <f t="shared" ca="1" si="36"/>
         <v>0</v>
       </c>
       <c r="T94" s="2">
-        <f t="shared" ca="1" si="36"/>
+        <f t="shared" ca="1" si="37"/>
         <v>0</v>
       </c>
       <c r="U94" s="2" cm="1">
@@ -3591,61 +3595,61 @@
         <v>0</v>
       </c>
       <c r="X94" s="2">
-        <f t="shared" ca="1" si="37"/>
+        <f t="shared" ca="1" si="38"/>
         <v>0</v>
       </c>
       <c r="Y94" s="2" t="str">
-        <f t="shared" ca="1" si="38"/>
+        <f t="shared" ca="1" si="25"/>
         <v>000000</v>
       </c>
     </row>
     <row r="95" spans="6:25" x14ac:dyDescent="0.3">
       <c r="I95" s="2">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="26"/>
         <v>4746</v>
       </c>
       <c r="J95" s="2">
-        <f t="shared" ca="1" si="26"/>
+        <f t="shared" ca="1" si="27"/>
         <v>4</v>
       </c>
       <c r="K95" s="2">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="28"/>
         <v>650</v>
       </c>
       <c r="L95" s="2">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="29"/>
         <v>0</v>
       </c>
       <c r="M95" s="2">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="30"/>
         <v>0</v>
       </c>
       <c r="N95" s="2">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>0</v>
       </c>
       <c r="O95" s="2">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="P95" s="2">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="33"/>
         <v>0</v>
       </c>
       <c r="Q95" s="2">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="34"/>
         <v>0</v>
       </c>
       <c r="R95" s="2">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="35"/>
         <v>0</v>
       </c>
       <c r="S95" s="2">
-        <f t="shared" ca="1" si="35"/>
+        <f t="shared" ca="1" si="36"/>
         <v>0</v>
       </c>
       <c r="T95" s="2">
-        <f t="shared" ca="1" si="36"/>
+        <f t="shared" ca="1" si="37"/>
         <v>0</v>
       </c>
       <c r="U95" s="2" cm="1">
@@ -3661,61 +3665,61 @@
         <v>0</v>
       </c>
       <c r="X95" s="2">
-        <f t="shared" ca="1" si="37"/>
+        <f t="shared" ca="1" si="38"/>
         <v>0</v>
       </c>
       <c r="Y95" s="2" t="str">
-        <f t="shared" ca="1" si="38"/>
+        <f t="shared" ca="1" si="25"/>
         <v>000000</v>
       </c>
     </row>
     <row r="96" spans="6:25" x14ac:dyDescent="0.3">
       <c r="I96" s="2">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="26"/>
         <v>900</v>
       </c>
       <c r="J96" s="2">
-        <f t="shared" ca="1" si="26"/>
+        <f t="shared" ca="1" si="27"/>
         <v>0</v>
       </c>
       <c r="K96" s="2">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="28"/>
         <v>900</v>
       </c>
       <c r="L96" s="2">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="29"/>
         <v>0</v>
       </c>
       <c r="M96" s="2">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="30"/>
         <v>0</v>
       </c>
       <c r="N96" s="2">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>0</v>
       </c>
       <c r="O96" s="2">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="P96" s="2">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="33"/>
         <v>0</v>
       </c>
       <c r="Q96" s="2">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="34"/>
         <v>0</v>
       </c>
       <c r="R96" s="2">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="35"/>
         <v>0</v>
       </c>
       <c r="S96" s="2">
-        <f t="shared" ca="1" si="35"/>
+        <f t="shared" ca="1" si="36"/>
         <v>0</v>
       </c>
       <c r="T96" s="2">
-        <f t="shared" ca="1" si="36"/>
+        <f t="shared" ca="1" si="37"/>
         <v>0</v>
       </c>
       <c r="U96" s="2" cm="1">
@@ -3731,61 +3735,61 @@
         <v>0</v>
       </c>
       <c r="X96" s="2">
-        <f t="shared" ca="1" si="37"/>
+        <f t="shared" ca="1" si="38"/>
         <v>0</v>
       </c>
       <c r="Y96" s="2" t="str">
-        <f t="shared" ca="1" si="38"/>
+        <f t="shared" ca="1" si="25"/>
         <v>000000</v>
       </c>
     </row>
     <row r="97" spans="9:25" x14ac:dyDescent="0.3">
       <c r="I97" s="2">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="26"/>
         <v>2556</v>
       </c>
       <c r="J97" s="2">
-        <f t="shared" ca="1" si="26"/>
+        <f t="shared" ca="1" si="27"/>
         <v>2</v>
       </c>
       <c r="K97" s="2">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="28"/>
         <v>508</v>
       </c>
       <c r="L97" s="2">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="29"/>
         <v>0</v>
       </c>
       <c r="M97" s="2">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="30"/>
         <v>0</v>
       </c>
       <c r="N97" s="2">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>0</v>
       </c>
       <c r="O97" s="2">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="P97" s="2">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="33"/>
         <v>0</v>
       </c>
       <c r="Q97" s="2">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="34"/>
         <v>0</v>
       </c>
       <c r="R97" s="2">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="35"/>
         <v>0</v>
       </c>
       <c r="S97" s="2">
-        <f t="shared" ca="1" si="35"/>
+        <f t="shared" ca="1" si="36"/>
         <v>0</v>
       </c>
       <c r="T97" s="2">
-        <f t="shared" ca="1" si="36"/>
+        <f t="shared" ca="1" si="37"/>
         <v>0</v>
       </c>
       <c r="U97" s="2" cm="1">
@@ -3801,61 +3805,61 @@
         <v>0</v>
       </c>
       <c r="X97" s="2">
-        <f t="shared" ca="1" si="37"/>
+        <f t="shared" ca="1" si="38"/>
         <v>0</v>
       </c>
       <c r="Y97" s="2" t="str">
-        <f t="shared" ca="1" si="38"/>
+        <f t="shared" ca="1" si="25"/>
         <v>000000</v>
       </c>
     </row>
     <row r="98" spans="9:25" x14ac:dyDescent="0.3">
       <c r="I98" s="2">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="26"/>
         <v>2556</v>
       </c>
       <c r="J98" s="2">
-        <f t="shared" ca="1" si="26"/>
+        <f t="shared" ca="1" si="27"/>
         <v>2</v>
       </c>
       <c r="K98" s="2">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="28"/>
         <v>508</v>
       </c>
       <c r="L98" s="2">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="29"/>
         <v>0</v>
       </c>
       <c r="M98" s="2">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="30"/>
         <v>0</v>
       </c>
       <c r="N98" s="2">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>0</v>
       </c>
       <c r="O98" s="2">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="P98" s="2">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="33"/>
         <v>0</v>
       </c>
       <c r="Q98" s="2">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="34"/>
         <v>0</v>
       </c>
       <c r="R98" s="2">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="35"/>
         <v>0</v>
       </c>
       <c r="S98" s="2">
-        <f t="shared" ca="1" si="35"/>
+        <f t="shared" ca="1" si="36"/>
         <v>0</v>
       </c>
       <c r="T98" s="2">
-        <f t="shared" ca="1" si="36"/>
+        <f t="shared" ca="1" si="37"/>
         <v>0</v>
       </c>
       <c r="U98" s="2" cm="1">
@@ -3871,61 +3875,61 @@
         <v>0</v>
       </c>
       <c r="X98" s="2">
-        <f t="shared" ca="1" si="37"/>
+        <f t="shared" ca="1" si="38"/>
         <v>0</v>
       </c>
       <c r="Y98" s="2" t="str">
-        <f t="shared" ca="1" si="38"/>
+        <f t="shared" ca="1" si="25"/>
         <v>000000</v>
       </c>
     </row>
     <row r="99" spans="9:25" x14ac:dyDescent="0.3">
       <c r="I99" s="2">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="26"/>
         <v>1020</v>
       </c>
       <c r="J99" s="2">
-        <f t="shared" ca="1" si="26"/>
+        <f t="shared" ca="1" si="27"/>
         <v>0</v>
       </c>
       <c r="K99" s="2">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="28"/>
         <v>1020</v>
       </c>
       <c r="L99" s="2">
-        <f t="shared" ca="1" si="28"/>
+        <f t="shared" ca="1" si="29"/>
         <v>0</v>
       </c>
       <c r="M99" s="2">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ca="1" si="30"/>
         <v>0</v>
       </c>
       <c r="N99" s="2">
-        <f t="shared" ca="1" si="30"/>
+        <f t="shared" ca="1" si="31"/>
         <v>0</v>
       </c>
       <c r="O99" s="2">
-        <f t="shared" ca="1" si="31"/>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="P99" s="2">
-        <f t="shared" ca="1" si="32"/>
+        <f t="shared" ca="1" si="33"/>
         <v>0</v>
       </c>
       <c r="Q99" s="2">
-        <f t="shared" ca="1" si="33"/>
+        <f t="shared" ca="1" si="34"/>
         <v>0</v>
       </c>
       <c r="R99" s="2">
-        <f t="shared" ca="1" si="34"/>
+        <f t="shared" ca="1" si="35"/>
         <v>0</v>
       </c>
       <c r="S99" s="2">
-        <f t="shared" ca="1" si="35"/>
+        <f t="shared" ca="1" si="36"/>
         <v>0</v>
       </c>
       <c r="T99" s="2">
-        <f t="shared" ca="1" si="36"/>
+        <f t="shared" ca="1" si="37"/>
         <v>0</v>
       </c>
       <c r="U99" s="2" cm="1">
@@ -3941,11 +3945,11 @@
         <v>0</v>
       </c>
       <c r="X99" s="2">
-        <f t="shared" ca="1" si="37"/>
+        <f t="shared" ca="1" si="38"/>
         <v>0</v>
       </c>
       <c r="Y99" s="2" t="str">
-        <f t="shared" ca="1" si="38"/>
+        <f t="shared" ca="1" si="25"/>
         <v>000000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added basic value tests between Cait and Toliy systems
</commit_message>
<xml_diff>
--- a/other/LinearVisualizer.xlsx
+++ b/other/LinearVisualizer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\CCHW\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F8EB39-C507-4592-9428-943E106582EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D0BBD0-379B-49F3-AFF3-2C2BB0C5A201}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9DBF0F91-83D7-4F64-B04C-B7CB81DC62EF}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9DBF0F91-83D7-4F64-B04C-B7CB81DC62EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -218,18 +218,6 @@
     <t>positions</t>
   </si>
   <si>
-    <t>0000000111101111</t>
-  </si>
-  <si>
-    <t>0000000100001100</t>
-  </si>
-  <si>
-    <t>0000001101100000</t>
-  </si>
-  <si>
-    <t>0000001111000100</t>
-  </si>
-  <si>
     <t>0000001100011011</t>
   </si>
   <si>
@@ -297,6 +285,18 @@
   </si>
   <si>
     <t>The blue highlighted cells represent the parameter values for both sets of tests</t>
+  </si>
+  <si>
+    <t>1011111111100100</t>
+  </si>
+  <si>
+    <t>0110000001100100</t>
+  </si>
+  <si>
+    <t>1001111111100100</t>
+  </si>
+  <si>
+    <t>1010100001100100</t>
   </si>
 </sst>
 </file>
@@ -712,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A6626A4-8C87-4B90-BEEB-AEB487ACEA9E}">
   <dimension ref="A2:Y138"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:N2"/>
+    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H94" sqref="H94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -745,17 +745,17 @@
   <sheetData>
     <row r="2" spans="1:1" ht="46.2" x14ac:dyDescent="0.85">
       <c r="A2" s="12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="46.2" x14ac:dyDescent="0.85">
       <c r="A4" s="12" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="46.2" x14ac:dyDescent="0.85">
       <c r="A6" s="12" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
@@ -795,36 +795,36 @@
         <v>2</v>
       </c>
       <c r="D26" s="2" t="str">
-        <f ca="1">_xlfn.CONCAT(B$40+B$41,"'b",REPT("0",B$40-LEN(E26)))</f>
-        <v>16'b00000</v>
+        <f t="shared" ref="D26:D37" ca="1" si="0">_xlfn.CONCAT(B$40+B$41,"'b",REPT("0",B$40-LEN(E26)))</f>
+        <v>16'b000</v>
       </c>
       <c r="E26" s="2" t="str">
         <f ca="1">DEC2BIN(_xlfn.FLOOR.MATH(RAND()*10))</f>
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="F26" s="2" t="str">
-        <f>_xlfn.CONCAT(REPT("0",B$41),";")</f>
+        <f t="shared" ref="F26:F37" si="1">_xlfn.CONCAT(REPT("0",B$41),";")</f>
         <v>0000000000;</v>
       </c>
       <c r="G26" s="4" t="str">
         <f ca="1">_xlfn.CONCAT(A26,B26,C26,D26,E26,F26)</f>
-        <v xml:space="preserve">            noteAmplitudes_i[ 0] = 16'b0000000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 0] = 16'b0001010000000000;</v>
       </c>
       <c r="H26" s="2">
-        <f t="shared" ref="H26:H37" ca="1" si="0">BIN2DEC(E26)</f>
-        <v>0</v>
+        <f t="shared" ref="H26:H37" ca="1" si="2">BIN2DEC(E26)</f>
+        <v>5</v>
       </c>
       <c r="I26" s="2">
-        <f ca="1">H26*2^B$41</f>
-        <v>0</v>
+        <f t="shared" ref="I26:I37" ca="1" si="3">H26*2^B$41</f>
+        <v>5120</v>
       </c>
       <c r="J26" s="2">
         <f ca="1">SUM(H26:H37)</f>
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="K26" s="2">
-        <f ca="1">I26-J$31</f>
-        <v>-4080</v>
+        <f t="shared" ref="K26:K37" ca="1" si="4">I26-J$31</f>
+        <v>-286</v>
       </c>
       <c r="L26" s="2">
         <f ca="1">IF(K26&gt;0,K26,0)</f>
@@ -846,44 +846,44 @@
         <v>2</v>
       </c>
       <c r="D27" s="2" t="str">
-        <f ca="1">_xlfn.CONCAT(B$40+B$41,"'b",REPT("0",B$40-LEN(E27)))</f>
-        <v>16'b000</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>16'b0000</v>
       </c>
       <c r="E27" s="2" t="str">
-        <f t="shared" ref="E27:E37" ca="1" si="1">DEC2BIN(_xlfn.FLOOR.MATH(RAND()*10))</f>
-        <v>111</v>
+        <f t="shared" ref="E27:E37" ca="1" si="5">DEC2BIN(_xlfn.FLOOR.MATH(RAND()*10))</f>
+        <v>11</v>
       </c>
       <c r="F27" s="2" t="str">
-        <f>_xlfn.CONCAT(REPT("0",B$41),";")</f>
+        <f t="shared" si="1"/>
         <v>0000000000;</v>
       </c>
       <c r="G27" s="4" t="str">
-        <f t="shared" ref="G27:G37" ca="1" si="2">_xlfn.CONCAT(A27,B27,C27,D27,E27,F27)</f>
-        <v xml:space="preserve">            noteAmplitudes_i[ 1] = 16'b0001110000000000;</v>
+        <f t="shared" ref="G27:G37" ca="1" si="6">_xlfn.CONCAT(A27,B27,C27,D27,E27,F27)</f>
+        <v xml:space="preserve">            noteAmplitudes_i[ 1] = 16'b0000110000000000;</v>
       </c>
       <c r="H27" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
       </c>
       <c r="I27" s="2">
-        <f ca="1">H27*2^B$41</f>
-        <v>7168</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>3072</v>
       </c>
       <c r="J27" s="2">
         <f ca="1">J26*2^B41</f>
-        <v>40960</v>
+        <v>54272</v>
       </c>
       <c r="K27" s="2">
-        <f ca="1">I27-J$31</f>
-        <v>3088</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>-2334</v>
       </c>
       <c r="L27" s="2">
-        <f t="shared" ref="L27:L37" ca="1" si="3">IF(K27&gt;0,K27,0)</f>
-        <v>3088</v>
+        <f t="shared" ref="L27:L37" ca="1" si="7">IF(K27&gt;0,K27,0)</f>
+        <v>0</v>
       </c>
       <c r="M27" s="2">
-        <f t="shared" ref="M27:M37" ca="1" si="4">IF(K27&gt;0,I27,0)</f>
-        <v>7168</v>
+        <f t="shared" ref="M27:M37" ca="1" si="8">IF(K27&gt;0,I27,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
@@ -897,40 +897,40 @@
         <v>2</v>
       </c>
       <c r="D28" s="2" t="str">
-        <f ca="1">_xlfn.CONCAT(B$40+B$41,"'b",REPT("0",B$40-LEN(E28)))</f>
-        <v>16'b000</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>16'b00</v>
       </c>
       <c r="E28" s="2" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>111</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>1000</v>
       </c>
       <c r="F28" s="2" t="str">
-        <f>_xlfn.CONCAT(REPT("0",B$41),";")</f>
+        <f t="shared" si="1"/>
         <v>0000000000;</v>
       </c>
       <c r="G28" s="4" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v xml:space="preserve">            noteAmplitudes_i[ 2] = 16'b0010000000000000;</v>
+      </c>
+      <c r="H28" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 2] = 16'b0001110000000000;</v>
-      </c>
-      <c r="H28" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I28" s="2">
-        <f ca="1">H28*2^B$41</f>
-        <v>7168</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>8192</v>
       </c>
       <c r="K28" s="2">
-        <f ca="1">I28-J$31</f>
-        <v>3088</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>2786</v>
       </c>
       <c r="L28" s="2">
-        <f t="shared" ca="1" si="3"/>
-        <v>3088</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>2786</v>
       </c>
       <c r="M28" s="2">
-        <f t="shared" ca="1" si="4"/>
-        <v>7168</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>8192</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
@@ -944,42 +944,42 @@
         <v>2</v>
       </c>
       <c r="D29" s="2" t="str">
-        <f ca="1">_xlfn.CONCAT(B$40+B$41,"'b",REPT("0",B$40-LEN(E29)))</f>
-        <v>16'b00000</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>16'b000</v>
       </c>
       <c r="E29" s="2" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>101</v>
       </c>
       <c r="F29" s="2" t="str">
-        <f>_xlfn.CONCAT(REPT("0",B$41),";")</f>
+        <f t="shared" si="1"/>
         <v>0000000000;</v>
       </c>
       <c r="G29" s="4" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v xml:space="preserve">            noteAmplitudes_i[ 3] = 16'b0001010000000000;</v>
+      </c>
+      <c r="H29" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 3] = 16'b0000000000000000;</v>
-      </c>
-      <c r="H29" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I29" s="2">
-        <f ca="1">H29*2^B$41</f>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>5120</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>8</v>
       </c>
       <c r="K29" s="2">
-        <f ca="1">I29-J$31</f>
-        <v>-4080</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>-286</v>
       </c>
       <c r="L29" s="2">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
       <c r="M29" s="2">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -994,44 +994,44 @@
         <v>2</v>
       </c>
       <c r="D30" s="2" t="str">
-        <f ca="1">_xlfn.CONCAT(B$40+B$41,"'b",REPT("0",B$40-LEN(E30)))</f>
-        <v>16'b0000</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>16'b00</v>
       </c>
       <c r="E30" s="2" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>1000</v>
       </c>
       <c r="F30" s="2" t="str">
-        <f>_xlfn.CONCAT(REPT("0",B$41),";")</f>
+        <f t="shared" si="1"/>
         <v>0000000000;</v>
       </c>
       <c r="G30" s="4" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v xml:space="preserve">            noteAmplitudes_i[ 4] = 16'b0010000000000000;</v>
+      </c>
+      <c r="H30" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 4] = 16'b0000110000000000;</v>
-      </c>
-      <c r="H30" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="I30" s="2">
-        <f ca="1">H30*2^B$41</f>
-        <v>3072</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>8192</v>
       </c>
       <c r="J30" s="3">
         <f ca="1">J26*B42</f>
-        <v>3.984375</v>
+        <v>5.279296875</v>
       </c>
       <c r="K30" s="2">
-        <f ca="1">I30-J$31</f>
-        <v>-1008</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>2786</v>
       </c>
       <c r="L30" s="2">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>2786</v>
       </c>
       <c r="M30" s="2">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>8192</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
@@ -1045,44 +1045,44 @@
         <v>2</v>
       </c>
       <c r="D31" s="2" t="str">
-        <f ca="1">_xlfn.CONCAT(B$40+B$41,"'b",REPT("0",B$40-LEN(E31)))</f>
-        <v>16'b000</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>16'b00000</v>
       </c>
       <c r="E31" s="2" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>101</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
       </c>
       <c r="F31" s="2" t="str">
-        <f>_xlfn.CONCAT(REPT("0",B$41),";")</f>
+        <f t="shared" si="1"/>
         <v>0000000000;</v>
       </c>
       <c r="G31" s="4" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v xml:space="preserve">            noteAmplitudes_i[ 5] = 16'b0000000000000000;</v>
+      </c>
+      <c r="H31" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 5] = 16'b0001010000000000;</v>
-      </c>
-      <c r="H31" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I31" s="2">
-        <f ca="1">H31*2^B$41</f>
-        <v>5120</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="J31" s="2">
         <f ca="1">J27 * BIN2DEC(C42) / 2^B41</f>
-        <v>4080</v>
+        <v>5406</v>
       </c>
       <c r="K31" s="2">
-        <f ca="1">I31-J$31</f>
-        <v>1040</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>-5406</v>
       </c>
       <c r="L31" s="2">
-        <f t="shared" ca="1" si="3"/>
-        <v>1040</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0</v>
       </c>
       <c r="M31" s="2">
-        <f t="shared" ca="1" si="4"/>
-        <v>5120</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
@@ -1096,40 +1096,40 @@
         <v>2</v>
       </c>
       <c r="D32" s="2" t="str">
-        <f ca="1">_xlfn.CONCAT(B$40+B$41,"'b",REPT("0",B$40-LEN(E32)))</f>
-        <v>16'b000</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>16'b0000</v>
       </c>
       <c r="E32" s="2" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>110</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>11</v>
       </c>
       <c r="F32" s="2" t="str">
-        <f>_xlfn.CONCAT(REPT("0",B$41),";")</f>
+        <f t="shared" si="1"/>
         <v>0000000000;</v>
       </c>
       <c r="G32" s="4" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v xml:space="preserve">            noteAmplitudes_i[ 6] = 16'b0000110000000000;</v>
+      </c>
+      <c r="H32" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 6] = 16'b0001100000000000;</v>
-      </c>
-      <c r="H32" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I32" s="2">
-        <f ca="1">H32*2^B$41</f>
-        <v>6144</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>3072</v>
       </c>
       <c r="K32" s="2">
-        <f ca="1">I32-J$31</f>
-        <v>2064</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>-2334</v>
       </c>
       <c r="L32" s="2">
-        <f t="shared" ca="1" si="3"/>
-        <v>2064</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0</v>
       </c>
       <c r="M32" s="2">
-        <f t="shared" ca="1" si="4"/>
-        <v>6144</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
@@ -1143,43 +1143,43 @@
         <v>2</v>
       </c>
       <c r="D33" s="2" t="str">
-        <f ca="1">_xlfn.CONCAT(B$40+B$41,"'b",REPT("0",B$40-LEN(E33)))</f>
-        <v>16'b00000</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>16'b00</v>
       </c>
       <c r="E33" s="2" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>1001</v>
       </c>
       <c r="F33" s="2" t="str">
-        <f>_xlfn.CONCAT(REPT("0",B$41),";")</f>
+        <f t="shared" si="1"/>
         <v>0000000000;</v>
       </c>
       <c r="G33" s="4" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v xml:space="preserve">            noteAmplitudes_i[ 7] = 16'b0010010000000000;</v>
+      </c>
+      <c r="H33" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 7] = 16'b0000000000000000;</v>
-      </c>
-      <c r="H33" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="I33" s="2">
-        <f ca="1">H33*2^B$41</f>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>9216</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>13</v>
       </c>
       <c r="K33" s="2">
-        <f ca="1">I33-J$31</f>
-        <v>-4080</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>3810</v>
       </c>
       <c r="L33" s="2">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>3810</v>
       </c>
       <c r="M33" s="2">
-        <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>9216</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
@@ -1193,43 +1193,43 @@
         <v>2</v>
       </c>
       <c r="D34" s="2" t="str">
-        <f ca="1">_xlfn.CONCAT(B$40+B$41,"'b",REPT("0",B$40-LEN(E34)))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>16'b0000</v>
       </c>
       <c r="E34" s="2" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>11</v>
       </c>
       <c r="F34" s="2" t="str">
-        <f>_xlfn.CONCAT(REPT("0",B$41),";")</f>
+        <f t="shared" si="1"/>
         <v>0000000000;</v>
       </c>
       <c r="G34" s="4" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v xml:space="preserve">            noteAmplitudes_i[ 8] = 16'b0000110000000000;</v>
+      </c>
+      <c r="H34" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 8] = 16'b0000100000000000;</v>
-      </c>
-      <c r="H34" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I34" s="2">
-        <f ca="1">H34*2^B$41</f>
-        <v>2048</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>3072</v>
       </c>
       <c r="J34" s="2">
         <f ca="1">J35/2^B41</f>
-        <v>10.09375</v>
+        <v>9.162109375</v>
       </c>
       <c r="K34" s="2">
-        <f ca="1">I34-J$31</f>
-        <v>-2032</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>-2334</v>
       </c>
       <c r="L34" s="2">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
       <c r="M34" s="2">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -1244,44 +1244,44 @@
         <v>2</v>
       </c>
       <c r="D35" s="2" t="str">
-        <f ca="1">_xlfn.CONCAT(B$40+B$41,"'b",REPT("0",B$40-LEN(E35)))</f>
-        <v>16'b000</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>16'b00000</v>
       </c>
       <c r="E35" s="2" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>100</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>1</v>
       </c>
       <c r="F35" s="2" t="str">
-        <f>_xlfn.CONCAT(REPT("0",B$41),";")</f>
+        <f t="shared" si="1"/>
         <v>0000000000;</v>
       </c>
       <c r="G35" s="4" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v xml:space="preserve">            noteAmplitudes_i[ 9] = 16'b0000010000000000;</v>
+      </c>
+      <c r="H35" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 9] = 16'b0001000000000000;</v>
-      </c>
-      <c r="H35" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I35" s="2">
-        <f ca="1">H35*2^B$41</f>
-        <v>4096</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1024</v>
       </c>
       <c r="J35" s="2">
         <f ca="1">SUM(L26:L37)</f>
-        <v>10336</v>
+        <v>9382</v>
       </c>
       <c r="K35" s="2">
-        <f ca="1">I35-J$31</f>
-        <v>16</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>-4382</v>
       </c>
       <c r="L35" s="2">
-        <f t="shared" ca="1" si="3"/>
-        <v>16</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0</v>
       </c>
       <c r="M35" s="2">
-        <f t="shared" ca="1" si="4"/>
-        <v>4096</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
@@ -1295,40 +1295,40 @@
         <v>2</v>
       </c>
       <c r="D36" s="2" t="str">
-        <f ca="1">_xlfn.CONCAT(B$40+B$41,"'b",REPT("0",B$40-LEN(E36)))</f>
-        <v>16'b000</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>16'b0000</v>
       </c>
       <c r="E36" s="2" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>101</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>11</v>
       </c>
       <c r="F36" s="2" t="str">
-        <f>_xlfn.CONCAT(REPT("0",B$41),";")</f>
+        <f t="shared" si="1"/>
         <v>0000000000;</v>
       </c>
       <c r="G36" s="4" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v xml:space="preserve">            noteAmplitudes_i[10] = 16'b0000110000000000;</v>
+      </c>
+      <c r="H36" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v xml:space="preserve">            noteAmplitudes_i[10] = 16'b0001010000000000;</v>
-      </c>
-      <c r="H36" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I36" s="2">
-        <f ca="1">H36*2^B$41</f>
-        <v>5120</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>3072</v>
       </c>
       <c r="K36" s="2">
-        <f ca="1">I36-J$31</f>
-        <v>1040</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>-2334</v>
       </c>
       <c r="L36" s="2">
-        <f t="shared" ca="1" si="3"/>
-        <v>1040</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0</v>
       </c>
       <c r="M36" s="2">
-        <f t="shared" ca="1" si="4"/>
-        <v>5120</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
@@ -1342,39 +1342,39 @@
         <v>2</v>
       </c>
       <c r="D37" s="2" t="str">
-        <f ca="1">_xlfn.CONCAT(B$40+B$41,"'b",REPT("0",B$40-LEN(E37)))</f>
-        <v>16'b00000</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>16'b000</v>
       </c>
       <c r="E37" s="2" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>101</v>
       </c>
       <c r="F37" s="2" t="str">
-        <f>_xlfn.CONCAT(REPT("0",B$41),";")</f>
+        <f t="shared" si="1"/>
         <v>0000000000;</v>
       </c>
       <c r="G37" s="4" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v xml:space="preserve">            noteAmplitudes_i[11] = 16'b0001010000000000;</v>
+      </c>
+      <c r="H37" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v xml:space="preserve">            noteAmplitudes_i[11] = 16'b0000010000000000;</v>
-      </c>
-      <c r="H37" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I37" s="2">
-        <f ca="1">H37*2^B$41</f>
-        <v>1024</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>5120</v>
       </c>
       <c r="K37" s="2">
-        <f ca="1">I37-J$31</f>
-        <v>-3056</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>-286</v>
       </c>
       <c r="L37" s="2">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
       <c r="M37" s="2">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -1418,27 +1418,27 @@
       <c r="C41" s="8"/>
       <c r="G41" s="4" t="str">
         <f ca="1">_xlfn.CONCAT("notePosition_i = 10'b",REPT(0,B41-LEN(_xlfn.BASE(I41,2))),_xlfn.BASE(I41,2),";" )</f>
-        <v>notePosition_i = 10'b0000000010;</v>
+        <v>notePosition_i = 10'b0000010011;</v>
       </c>
       <c r="H41" s="2">
         <f ca="1">I41/2^10</f>
-        <v>1.953125E-3</v>
+        <v>1.85546875E-2</v>
       </c>
       <c r="I41" s="2">
         <f ca="1">RANDBETWEEN(0,1023)</f>
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="J41" s="2">
         <f ca="1">I41*24</f>
-        <v>48</v>
+        <v>456</v>
       </c>
       <c r="K41" s="2">
         <f ca="1">IF(J45=3,24576-J41,8192-J41)</f>
-        <v>8144</v>
+        <v>7736</v>
       </c>
       <c r="L41" s="2">
         <f ca="1">IF(J45=3,K47+170, K47)</f>
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
@@ -1488,7 +1488,7 @@
       </c>
       <c r="K44" s="2">
         <f ca="1">K41*H44*H45*H46</f>
-        <v>177734656</v>
+        <v>168830464</v>
       </c>
       <c r="L44" s="2" t="s">
         <v>24</v>
@@ -1515,11 +1515,11 @@
       </c>
       <c r="K45" s="2" t="str">
         <f ca="1">_xlfn.BASE(K44,2,32)</f>
-        <v>00001010100110000000010000000000</v>
+        <v>00001010000100000010011000000000</v>
       </c>
       <c r="L45" s="2">
         <f ca="1">MOD(IF(L41&lt;0,L41+1023,L41), 1024)</f>
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
@@ -1544,21 +1544,21 @@
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K47" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(K44/2^(B41+B41+C39-3))</f>
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="50" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G50" s="4" t="str">
         <f ca="1">_xlfn.CONCAT("        noteAmplitude_i = 10'b",REPT(0,B41-LEN(_xlfn.BASE(I50,2))),_xlfn.BASE(I50,2),";" )</f>
-        <v xml:space="preserve">        noteAmplitude_i = 10'b0110000001;</v>
+        <v xml:space="preserve">        noteAmplitude_i = 10'b1101101011;</v>
       </c>
       <c r="H50" s="2">
         <f ca="1">I50/2^10</f>
-        <v>0.3759765625</v>
+        <v>0.8544921875</v>
       </c>
       <c r="I50" s="2">
         <f ca="1">RANDBETWEEN(0,1023)</f>
-        <v>385</v>
+        <v>875</v>
       </c>
       <c r="J50" s="2" t="s">
         <v>28</v>
@@ -1590,23 +1590,23 @@
       </c>
       <c r="G51" s="4" t="str">
         <f ca="1">_xlfn.CONCAT("        noteAmplitudeFast_i = 10'b",REPT(0,B41-LEN(_xlfn.BASE(I51,2))),_xlfn.BASE(I51,2),";" )</f>
-        <v xml:space="preserve">        noteAmplitudeFast_i = 10'b1010001111;</v>
+        <v xml:space="preserve">        noteAmplitudeFast_i = 10'b1100100000;</v>
       </c>
       <c r="H51" s="2">
-        <f t="shared" ref="H51:H52" ca="1" si="5">I51/2^10</f>
-        <v>0.6396484375</v>
+        <f t="shared" ref="H51:H52" ca="1" si="9">I51/2^10</f>
+        <v>0.78125</v>
       </c>
       <c r="I51" s="2">
         <f ca="1">RANDBETWEEN(0,1023)</f>
-        <v>655</v>
+        <v>800</v>
       </c>
       <c r="J51" s="2">
         <f ca="1">I52*E55</f>
-        <v>3006</v>
+        <v>1380</v>
       </c>
       <c r="K51" s="2">
         <f ca="1">IF(E57,I50,I51)</f>
-        <v>655</v>
+        <v>800</v>
       </c>
       <c r="L51" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(K57/2^(B41-8))</f>
@@ -1618,7 +1618,7 @@
       </c>
       <c r="N51" s="2">
         <f ca="1">$L$57</f>
-        <v>239</v>
+        <v>88</v>
       </c>
       <c r="O51" s="2">
         <f>0</f>
@@ -1626,21 +1626,21 @@
       </c>
       <c r="P51" s="2">
         <f ca="1">M51*2^16+N51*2^8+O51</f>
-        <v>16772864</v>
+        <v>16734208</v>
       </c>
     </row>
     <row r="52" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G52" s="4" t="str">
         <f ca="1">_xlfn.CONCAT("        noteHue_i = 10'b",REPT(0,B41-LEN(_xlfn.BASE(I52,2))),_xlfn.BASE(I52,2),";" )</f>
-        <v xml:space="preserve">        noteHue_i = 10'b0111110101;</v>
+        <v xml:space="preserve">        noteHue_i = 10'b0011100110;</v>
       </c>
       <c r="H52" s="2">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.4892578125</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>0.224609375</v>
       </c>
       <c r="I52" s="2">
         <f ca="1">RANDBETWEEN(0,1023)</f>
-        <v>501</v>
+        <v>230</v>
       </c>
       <c r="J52" s="2" t="s">
         <v>29</v>
@@ -1653,7 +1653,7 @@
       </c>
       <c r="M52" s="2">
         <f ca="1">$L$59</f>
-        <v>16</v>
+        <v>166</v>
       </c>
       <c r="N52" s="2">
         <f ca="1">$L$51</f>
@@ -1664,22 +1664,22 @@
         <v>0</v>
       </c>
       <c r="P52" s="2">
-        <f t="shared" ref="P52:P57" ca="1" si="6">M52*2^16+N52*2^8+O52</f>
-        <v>1113856</v>
+        <f t="shared" ref="P52:P57" ca="1" si="10">M52*2^16+N52*2^8+O52</f>
+        <v>10944256</v>
       </c>
     </row>
     <row r="53" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J53" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(J51/2^10)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K53" s="2">
         <f ca="1">K51*E54</f>
-        <v>1072890</v>
+        <v>1310400</v>
       </c>
       <c r="L53" s="2">
         <f ca="1">K57*J55</f>
-        <v>980034</v>
+        <v>364188</v>
       </c>
       <c r="M53" s="2">
         <f>0</f>
@@ -1691,11 +1691,11 @@
       </c>
       <c r="O53" s="2">
         <f ca="1">$L$57</f>
-        <v>239</v>
+        <v>88</v>
       </c>
       <c r="P53" s="2">
-        <f t="shared" ca="1" si="6"/>
-        <v>65519</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>65368</v>
       </c>
     </row>
     <row r="54" spans="2:16" x14ac:dyDescent="0.3">
@@ -1720,15 +1720,15 @@
       </c>
       <c r="N54" s="2">
         <f ca="1">$L$59</f>
-        <v>16</v>
+        <v>166</v>
       </c>
       <c r="O54" s="2">
         <f ca="1">$L$51</f>
         <v>255</v>
       </c>
       <c r="P54" s="2">
-        <f t="shared" ca="1" si="6"/>
-        <v>4351</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>42751</v>
       </c>
     </row>
     <row r="55" spans="2:16" x14ac:dyDescent="0.3">
@@ -1740,7 +1740,7 @@
       </c>
       <c r="J55" s="2">
         <f ca="1">MOD(J51,2^10)</f>
-        <v>958</v>
+        <v>356</v>
       </c>
       <c r="K55" s="2">
         <f ca="1">IF(_xlfn.FLOOR.MATH(K53/2^10) &gt; 1023, 1023, _xlfn.FLOOR.MATH(K53/2^10))</f>
@@ -1748,11 +1748,11 @@
       </c>
       <c r="L55" s="2">
         <f ca="1">K57*(1023-J55)</f>
-        <v>66495</v>
+        <v>682341</v>
       </c>
       <c r="M55" s="2">
         <f ca="1">$L$57</f>
-        <v>239</v>
+        <v>88</v>
       </c>
       <c r="N55" s="2">
         <f>0</f>
@@ -1763,8 +1763,8 @@
         <v>255</v>
       </c>
       <c r="P55" s="2">
-        <f t="shared" ca="1" si="6"/>
-        <v>15663359</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>5767423</v>
       </c>
     </row>
     <row r="56" spans="2:16" x14ac:dyDescent="0.3">
@@ -1790,11 +1790,11 @@
       </c>
       <c r="O56" s="2">
         <f ca="1">$L$59</f>
-        <v>16</v>
+        <v>166</v>
       </c>
       <c r="P56" s="2">
-        <f t="shared" ca="1" si="6"/>
-        <v>16711696</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>16711846</v>
       </c>
     </row>
     <row r="57" spans="2:16" x14ac:dyDescent="0.3">
@@ -1810,7 +1810,7 @@
       </c>
       <c r="L57" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(L53/2^(2*B41-8))</f>
-        <v>239</v>
+        <v>88</v>
       </c>
       <c r="M57" s="2">
         <f ca="1">$L$51</f>
@@ -1818,15 +1818,15 @@
       </c>
       <c r="N57" s="2">
         <f ca="1">$L$57</f>
-        <v>239</v>
+        <v>88</v>
       </c>
       <c r="O57" s="2">
         <f>0</f>
         <v>0</v>
       </c>
       <c r="P57" s="2">
-        <f t="shared" ca="1" si="6"/>
-        <v>16772864</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>16734208</v>
       </c>
     </row>
     <row r="58" spans="2:16" x14ac:dyDescent="0.3">
@@ -1840,11 +1840,11 @@
     <row r="59" spans="2:16" x14ac:dyDescent="0.3">
       <c r="L59" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(L55/2^(2*B41-8))</f>
-        <v>16</v>
+        <v>166</v>
       </c>
       <c r="M59" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="M59" ca="1">_xlfn.BASE(_xlfn.SWITCH(J53,0,P51,1,P52,2,P53,3,P54,4,P55,5,P56,6,P57),16,6)</f>
-        <v>00FFEF</v>
+        <v>A6FF00</v>
       </c>
     </row>
     <row r="60" spans="2:16" x14ac:dyDescent="0.3">
@@ -1862,7 +1862,7 @@
     </row>
     <row r="63" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G63" s="4" t="str">
-        <f ca="1">_xlfn.CONCAT(A26,B26,C26,B$40+B$41,"'b",_xlfn.BASE(L26,2,$B$40+$B$41),";")</f>
+        <f t="shared" ref="G63:G74" ca="1" si="11">_xlfn.CONCAT(A26,B26,C26,B$40+B$41,"'b",_xlfn.BASE(L26,2,$B$40+$B$41),";")</f>
         <v xml:space="preserve">            noteAmplitudes_i[ 0] = 16'b0000000000000000;</v>
       </c>
       <c r="H63" s="2">
@@ -1871,175 +1871,175 @@
       </c>
       <c r="I63" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(H76/B43)</f>
-        <v>206</v>
+        <v>187</v>
       </c>
       <c r="J63" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(H63/I$63)</f>
+        <f t="shared" ref="J63:J74" ca="1" si="12">_xlfn.FLOOR.MATH(H63/I$63)</f>
         <v>0</v>
       </c>
       <c r="L63" s="2">
         <f ca="1">L51-L57-L59</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G64" s="4" t="str">
-        <f ca="1">_xlfn.CONCAT(A27,B27,C27,B$40+B$41,"'b",_xlfn.BASE(L27,2,$B$40+$B$41),";")</f>
-        <v xml:space="preserve">            noteAmplitudes_i[ 1] = 16'b0000110000010000;</v>
+        <f t="shared" ca="1" si="11"/>
+        <v xml:space="preserve">            noteAmplitudes_i[ 1] = 16'b0000000000000000;</v>
       </c>
       <c r="H64" s="2">
-        <f t="shared" ref="H64:H74" ca="1" si="7">L27</f>
-        <v>3088</v>
+        <f t="shared" ref="H64:H74" ca="1" si="13">L27</f>
+        <v>0</v>
       </c>
       <c r="J64" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(H64/I$63)</f>
-        <v>14</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G65" s="4" t="str">
-        <f ca="1">_xlfn.CONCAT(A28,B28,C28,B$40+B$41,"'b",_xlfn.BASE(L28,2,$B$40+$B$41),";")</f>
-        <v xml:space="preserve">            noteAmplitudes_i[ 2] = 16'b0000110000010000;</v>
+        <f t="shared" ca="1" si="11"/>
+        <v xml:space="preserve">            noteAmplitudes_i[ 2] = 16'b0000101011100010;</v>
       </c>
       <c r="H65" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>3088</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>2786</v>
       </c>
       <c r="J65" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(H65/I$63)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G66" s="4" t="str">
-        <f ca="1">_xlfn.CONCAT(A29,B29,C29,B$40+B$41,"'b",_xlfn.BASE(L29,2,$B$40+$B$41),";")</f>
+        <f t="shared" ca="1" si="11"/>
         <v xml:space="preserve">            noteAmplitudes_i[ 3] = 16'b0000000000000000;</v>
       </c>
       <c r="H66" s="2">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
       <c r="J66" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(H66/I$63)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G67" s="4" t="str">
-        <f ca="1">_xlfn.CONCAT(A30,B30,C30,B$40+B$41,"'b",_xlfn.BASE(L30,2,$B$40+$B$41),";")</f>
-        <v xml:space="preserve">            noteAmplitudes_i[ 4] = 16'b0000000000000000;</v>
+        <f t="shared" ca="1" si="11"/>
+        <v xml:space="preserve">            noteAmplitudes_i[ 4] = 16'b0000101011100010;</v>
       </c>
       <c r="H67" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>2786</v>
       </c>
       <c r="J67" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(H67/I$63)</f>
-        <v>0</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>14</v>
       </c>
     </row>
     <row r="68" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G68" s="4" t="str">
-        <f ca="1">_xlfn.CONCAT(A31,B31,C31,B$40+B$41,"'b",_xlfn.BASE(L31,2,$B$40+$B$41),";")</f>
-        <v xml:space="preserve">            noteAmplitudes_i[ 5] = 16'b0000010000010000;</v>
+        <f t="shared" ca="1" si="11"/>
+        <v xml:space="preserve">            noteAmplitudes_i[ 5] = 16'b0000000000000000;</v>
       </c>
       <c r="H68" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>1040</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>0</v>
       </c>
       <c r="J68" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(H68/I$63)</f>
-        <v>5</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G69" s="4" t="str">
-        <f ca="1">_xlfn.CONCAT(A32,B32,C32,B$40+B$41,"'b",_xlfn.BASE(L32,2,$B$40+$B$41),";")</f>
-        <v xml:space="preserve">            noteAmplitudes_i[ 6] = 16'b0000100000010000;</v>
+        <f t="shared" ca="1" si="11"/>
+        <v xml:space="preserve">            noteAmplitudes_i[ 6] = 16'b0000000000000000;</v>
       </c>
       <c r="H69" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>2064</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>0</v>
       </c>
       <c r="J69" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(H69/I$63)</f>
-        <v>10</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G70" s="4" t="str">
-        <f ca="1">_xlfn.CONCAT(A33,B33,C33,B$40+B$41,"'b",_xlfn.BASE(L33,2,$B$40+$B$41),";")</f>
-        <v xml:space="preserve">            noteAmplitudes_i[ 7] = 16'b0000000000000000;</v>
+        <f t="shared" ca="1" si="11"/>
+        <v xml:space="preserve">            noteAmplitudes_i[ 7] = 16'b0000111011100010;</v>
       </c>
       <c r="H70" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>3810</v>
       </c>
       <c r="J70" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(H70/I$63)</f>
-        <v>0</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>20</v>
       </c>
     </row>
     <row r="71" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G71" s="4" t="str">
-        <f ca="1">_xlfn.CONCAT(A34,B34,C34,B$40+B$41,"'b",_xlfn.BASE(L34,2,$B$40+$B$41),";")</f>
+        <f t="shared" ca="1" si="11"/>
         <v xml:space="preserve">            noteAmplitudes_i[ 8] = 16'b0000000000000000;</v>
       </c>
       <c r="H71" s="2">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
       <c r="J71" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(H71/I$63)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G72" s="4" t="str">
-        <f ca="1">_xlfn.CONCAT(A35,B35,C35,B$40+B$41,"'b",_xlfn.BASE(L35,2,$B$40+$B$41),";")</f>
-        <v xml:space="preserve">            noteAmplitudes_i[ 9] = 16'b0000000000010000;</v>
+        <f t="shared" ca="1" si="11"/>
+        <v xml:space="preserve">            noteAmplitudes_i[ 9] = 16'b0000000000000000;</v>
       </c>
       <c r="H72" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>16</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>0</v>
       </c>
       <c r="J72" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(H72/I$63)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G73" s="4" t="str">
-        <f ca="1">_xlfn.CONCAT(A36,B36,C36,B$40+B$41,"'b",_xlfn.BASE(L36,2,$B$40+$B$41),";")</f>
-        <v xml:space="preserve">            noteAmplitudes_i[10] = 16'b0000010000010000;</v>
+        <f t="shared" ca="1" si="11"/>
+        <v xml:space="preserve">            noteAmplitudes_i[10] = 16'b0000000000000000;</v>
       </c>
       <c r="H73" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>1040</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>0</v>
       </c>
       <c r="J73" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(H73/I$63)</f>
-        <v>5</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G74" s="4" t="str">
-        <f ca="1">_xlfn.CONCAT(A37,B37,C37,B$40+B$41,"'b",_xlfn.BASE(L37,2,$B$40+$B$41),";")</f>
+        <f t="shared" ca="1" si="11"/>
         <v xml:space="preserve">            noteAmplitudes_i[11] = 16'b0000000000000000;</v>
       </c>
       <c r="H74" s="2">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="13"/>
         <v>0</v>
       </c>
       <c r="J74" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(H74/I$63)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G75" s="5" t="str">
         <f ca="1">_xlfn.CONCAT("            amplitudeSumNew_i = ",B40+B41+_xlfn.CEILING.MATH(IMLOG2(B43)),"'b",_xlfn.BASE(H76,2,B40+B41+_xlfn.CEILING.MATH(IMLOG2(B43))),";")</f>
-        <v xml:space="preserve">            amplitudeSumNew_i = 22'b0000000010100001100000;</v>
+        <v xml:space="preserve">            amplitudeSumNew_i = 22'b0000000010010010100110;</v>
       </c>
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.3">
@@ -2048,7 +2048,7 @@
       </c>
       <c r="H76" s="2">
         <f ca="1">SUM(H63:H74)</f>
-        <v>10336</v>
+        <v>9382</v>
       </c>
     </row>
     <row r="78" spans="1:25" x14ac:dyDescent="0.3">
@@ -2137,7 +2137,7 @@
         <v>51</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J82" s="2" t="s">
         <v>10</v>
@@ -2151,11 +2151,11 @@
     </row>
     <row r="83" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F83" s="2">
-        <f ca="1">H83/2^B$41</f>
+        <f t="shared" ref="F83:F94" ca="1" si="14">H83/2^B$41</f>
         <v>0.5859375</v>
       </c>
       <c r="G83" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H83" s="2" cm="1">
         <f t="array" aca="1" ref="H83" ca="1">SUMPRODUCT(--MID(G83,LEN(G83)+1-ROW(INDIRECT("1:"&amp;LEN(G83))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G83)))-1)))</f>
@@ -2165,7 +2165,7 @@
         <v>9</v>
       </c>
       <c r="J83" s="2">
-        <f ca="1">H83-I$87</f>
+        <f t="shared" ref="J83:J94" ca="1" si="15">H83-I$87</f>
         <v>423.990234375</v>
       </c>
       <c r="K83" s="2">
@@ -2179,11 +2179,11 @@
     </row>
     <row r="84" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F84" s="2">
-        <f ca="1">H84/2^B$41</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0.7001953125</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="H84" s="2" cm="1">
         <f t="array" aca="1" ref="H84" ca="1">SUMPRODUCT(--MID(G84,LEN(G84)+1-ROW(INDIRECT("1:"&amp;LEN(G84))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G84)))-1)))</f>
@@ -2194,25 +2194,25 @@
         <v>1767</v>
       </c>
       <c r="J84" s="2">
-        <f ca="1">H84-I$87</f>
+        <f t="shared" ca="1" si="15"/>
         <v>540.990234375</v>
       </c>
       <c r="K84" s="2">
-        <f t="shared" ref="K84:K94" ca="1" si="8">IF(J84&lt;0, 0, J84)</f>
+        <f t="shared" ref="K84:K94" ca="1" si="16">IF(J84&lt;0, 0, J84)</f>
         <v>540.990234375</v>
       </c>
       <c r="L84" s="2">
-        <f t="shared" ref="L84:L94" ca="1" si="9">IF(K84=0,0,H84)</f>
+        <f t="shared" ref="L84:L94" ca="1" si="17">IF(K84=0,0,H84)</f>
         <v>717</v>
       </c>
     </row>
     <row r="85" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F85" s="2">
-        <f ca="1">H85/2^B$41</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0.439453125</v>
       </c>
       <c r="G85" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="H85" s="2" cm="1">
         <f t="array" aca="1" ref="H85" ca="1">SUMPRODUCT(--MID(G85,LEN(G85)+1-ROW(INDIRECT("1:"&amp;LEN(G85))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G85)))-1)))</f>
@@ -2223,53 +2223,53 @@
         <v>1.7255859375</v>
       </c>
       <c r="J85" s="2">
-        <f ca="1">H85-I$87</f>
+        <f t="shared" ca="1" si="15"/>
         <v>273.990234375</v>
       </c>
       <c r="K85" s="2">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="16"/>
         <v>273.990234375</v>
       </c>
       <c r="L85" s="2">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="17"/>
         <v>450</v>
       </c>
     </row>
     <row r="86" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F86" s="2">
-        <f ca="1">H86/2^B$41</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H86" s="2" cm="1">
         <f t="array" aca="1" ref="H86" ca="1">SUMPRODUCT(--MID(G86,LEN(G86)+1-ROW(INDIRECT("1:"&amp;LEN(G86))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G86)))-1)))</f>
         <v>0</v>
       </c>
       <c r="I86" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="J86" s="2">
-        <f ca="1">H86-I$87</f>
+        <f t="shared" ca="1" si="15"/>
         <v>-176.009765625</v>
       </c>
       <c r="K86" s="2">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="16"/>
         <v>0</v>
       </c>
       <c r="L86" s="2">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="17"/>
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F87" s="2">
-        <f ca="1">H87/2^B$41</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H87" s="2" cm="1">
         <f t="array" aca="1" ref="H87" ca="1">SUMPRODUCT(--MID(G87,LEN(G87)+1-ROW(INDIRECT("1:"&amp;LEN(G87))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G87)))-1)))</f>
@@ -2280,25 +2280,25 @@
         <v>176.009765625</v>
       </c>
       <c r="J87" s="2">
-        <f ca="1">H87-I$87</f>
+        <f t="shared" ca="1" si="15"/>
         <v>-176.009765625</v>
       </c>
       <c r="K87" s="2">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="16"/>
         <v>0</v>
       </c>
       <c r="L87" s="2">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="17"/>
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F88" s="2">
-        <f ca="1">H88/2^B$41</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
       <c r="G88" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H88" s="2" cm="1">
         <f t="array" aca="1" ref="H88" ca="1">SUMPRODUCT(--MID(G88,LEN(G88)+1-ROW(INDIRECT("1:"&amp;LEN(G88))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G88)))-1)))</f>
@@ -2309,25 +2309,25 @@
         <v>0.17188453674316406</v>
       </c>
       <c r="J88" s="2">
-        <f ca="1">H88-I$87</f>
+        <f t="shared" ca="1" si="15"/>
         <v>-176.009765625</v>
       </c>
       <c r="K88" s="2">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="16"/>
         <v>0</v>
       </c>
       <c r="L88" s="2">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="17"/>
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F89" s="2">
-        <f ca="1">H89/2^B$41</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
       <c r="G89" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H89" s="2" cm="1">
         <f t="array" aca="1" ref="H89" ca="1">SUMPRODUCT(--MID(G89,LEN(G89)+1-ROW(INDIRECT("1:"&amp;LEN(G89))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G89)))-1)))</f>
@@ -2337,25 +2337,25 @@
         <v>13</v>
       </c>
       <c r="J89" s="2">
-        <f ca="1">H89-I$87</f>
+        <f t="shared" ca="1" si="15"/>
         <v>-176.009765625</v>
       </c>
       <c r="K89" s="2">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="16"/>
         <v>0</v>
       </c>
       <c r="L89" s="2">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="17"/>
         <v>0</v>
       </c>
     </row>
     <row r="90" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F90" s="2">
-        <f ca="1">H90/2^B$41</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H90" s="2" cm="1">
         <f t="array" aca="1" ref="H90" ca="1">SUMPRODUCT(--MID(G90,LEN(G90)+1-ROW(INDIRECT("1:"&amp;LEN(G90))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G90)))-1)))</f>
@@ -2366,115 +2366,115 @@
         <v>1238.970703125</v>
       </c>
       <c r="J90" s="2">
-        <f ca="1">H90-I$87</f>
+        <f t="shared" ca="1" si="15"/>
         <v>-176.009765625</v>
       </c>
       <c r="K90" s="2">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="16"/>
         <v>0</v>
       </c>
       <c r="L90" s="2">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="17"/>
         <v>0</v>
       </c>
     </row>
     <row r="91" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F91" s="2">
-        <f ca="1">H91/2^B$41</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
       <c r="G91" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H91" s="2" cm="1">
         <f t="array" aca="1" ref="H91" ca="1">SUMPRODUCT(--MID(G91,LEN(G91)+1-ROW(INDIRECT("1:"&amp;LEN(G91))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G91)))-1)))</f>
         <v>0</v>
       </c>
       <c r="J91" s="2">
-        <f ca="1">H91-I$87</f>
+        <f t="shared" ca="1" si="15"/>
         <v>-176.009765625</v>
       </c>
       <c r="K91" s="2">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="16"/>
         <v>0</v>
       </c>
       <c r="L91" s="2">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="17"/>
         <v>0</v>
       </c>
     </row>
     <row r="92" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F92" s="2">
-        <f ca="1">H92/2^B$41</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
       <c r="G92" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H92" s="2" cm="1">
         <f t="array" aca="1" ref="H92" ca="1">SUMPRODUCT(--MID(G92,LEN(G92)+1-ROW(INDIRECT("1:"&amp;LEN(G92))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G92)))-1)))</f>
         <v>0</v>
       </c>
       <c r="J92" s="2">
-        <f ca="1">H92-I$87</f>
+        <f t="shared" ca="1" si="15"/>
         <v>-176.009765625</v>
       </c>
       <c r="K92" s="2">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="16"/>
         <v>0</v>
       </c>
       <c r="L92" s="2">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="17"/>
         <v>0</v>
       </c>
     </row>
     <row r="93" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F93" s="2">
-        <f ca="1">H93/2^B$41</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
       <c r="G93" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H93" s="2" cm="1">
         <f t="array" aca="1" ref="H93" ca="1">SUMPRODUCT(--MID(G93,LEN(G93)+1-ROW(INDIRECT("1:"&amp;LEN(G93))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G93)))-1)))</f>
         <v>0</v>
       </c>
       <c r="J93" s="2">
-        <f ca="1">H93-I$87</f>
+        <f t="shared" ca="1" si="15"/>
         <v>-176.009765625</v>
       </c>
       <c r="K93" s="2">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="16"/>
         <v>0</v>
       </c>
       <c r="L93" s="2">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="17"/>
         <v>0</v>
       </c>
     </row>
     <row r="94" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F94" s="2">
-        <f ca="1">H94/2^B$41</f>
+        <f t="shared" ca="1" si="14"/>
         <v>0</v>
       </c>
       <c r="G94" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H94" s="2" cm="1">
         <f t="array" aca="1" ref="H94" ca="1">SUMPRODUCT(--MID(G94,LEN(G94)+1-ROW(INDIRECT("1:"&amp;LEN(G94))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G94)))-1)))</f>
         <v>0</v>
       </c>
       <c r="J94" s="2">
-        <f ca="1">H94-I$87</f>
+        <f t="shared" ca="1" si="15"/>
         <v>-176.009765625</v>
       </c>
       <c r="K94" s="2">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="16"/>
         <v>0</v>
       </c>
       <c r="L94" s="2">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -2495,229 +2495,229 @@
         <v>17</v>
       </c>
       <c r="M96" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="N96" s="2" t="s">
         <v>23</v>
       </c>
       <c r="O96" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="97" spans="6:25" x14ac:dyDescent="0.3">
       <c r="F97" s="2">
         <f ca="1">H97/2^B$41</f>
-        <v>0.4833984375</v>
+        <v>47.97265625</v>
       </c>
       <c r="G97" s="6" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="H97" s="2" cm="1">
         <f t="array" aca="1" ref="H97" ca="1">SUMPRODUCT(--MID(G97,LEN(G97)+1-ROW(INDIRECT("1:"&amp;LEN(G97))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G97)))-1)))</f>
-        <v>495</v>
+        <v>49124</v>
       </c>
       <c r="I97" s="2">
-        <f ca="1">H97*B$39</f>
-        <v>11880</v>
-      </c>
-      <c r="J97" s="2">
+        <f t="shared" ref="I97:I108" ca="1" si="18">H97*B$39</f>
+        <v>1178976</v>
+      </c>
+      <c r="J97" s="2" t="e">
         <f ca="1">LEN(DEC2BIN(2^_xlfn.FLOOR.MATH((I97+1)/8192)))</f>
-        <v>2</v>
-      </c>
-      <c r="K97" s="2" cm="1">
+        <v>#NUM!</v>
+      </c>
+      <c r="K97" s="2" t="e" cm="1">
         <f t="array" aca="1" ref="K97" ca="1">_xlfn.SWITCH(J97,1,8*2^10 - I97, 2, 8*2^10 -I97, 3, 24*2^B$41 -I97)</f>
-        <v>-3688</v>
-      </c>
-      <c r="L97" s="2" cm="1">
+        <v>#NUM!</v>
+      </c>
+      <c r="L97" s="2" t="e" cm="1">
         <f t="array" aca="1" ref="L97" ca="1">_xlfn.SWITCH(J97,1,K97*G$44, 2, K97*G$45, 3, K97*G$46)</f>
-        <v>-160973824</v>
-      </c>
-      <c r="M97" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(L97/2^(B$41+B$41))</f>
-        <v>-154</v>
-      </c>
-      <c r="N97" s="2">
+        <v>#NUM!</v>
+      </c>
+      <c r="M97" s="2" t="e">
+        <f t="shared" ref="M97:M108" ca="1" si="19">_xlfn.FLOOR.MATH(L97/2^(B$41+B$41))</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="N97" s="2" t="e">
         <f ca="1">IF(J97=3,M97+170,M97)</f>
-        <v>-154</v>
-      </c>
-      <c r="O97" s="2">
+        <v>#NUM!</v>
+      </c>
+      <c r="O97" s="2" t="e">
         <f ca="1">MOD(N97,1024)</f>
-        <v>870</v>
-      </c>
-      <c r="P97" s="2">
-        <f ca="1">O97/2^B$41</f>
-        <v>0.849609375</v>
-      </c>
-      <c r="Q97" s="2">
+        <v>#NUM!</v>
+      </c>
+      <c r="P97" s="2" t="e">
+        <f t="shared" ref="P97:P108" ca="1" si="20">O97/2^B$41</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="Q97" s="2" t="e">
         <f ca="1">P97*360</f>
-        <v>305.859375</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="98" spans="6:25" x14ac:dyDescent="0.3">
       <c r="F98" s="2">
-        <f ca="1">H98/2^B$41</f>
-        <v>0.26171875</v>
+        <f t="shared" ref="F97:F108" ca="1" si="21">H98/2^B$41</f>
+        <v>24.09765625</v>
       </c>
       <c r="G98" s="6" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="H98" s="2" cm="1">
         <f t="array" aca="1" ref="H98" ca="1">SUMPRODUCT(--MID(G98,LEN(G98)+1-ROW(INDIRECT("1:"&amp;LEN(G98))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G98)))-1)))</f>
-        <v>268</v>
+        <v>24676</v>
       </c>
       <c r="I98" s="2">
-        <f ca="1">H98*B$39</f>
-        <v>6432</v>
-      </c>
-      <c r="J98" s="2">
-        <f t="shared" ref="J98:J108" ca="1" si="10">LEN(DEC2BIN(2^_xlfn.FLOOR.MATH((I98+1)/8192)))</f>
-        <v>1</v>
-      </c>
-      <c r="K98" s="2" cm="1">
+        <f t="shared" ca="1" si="18"/>
+        <v>592224</v>
+      </c>
+      <c r="J98" s="2" t="e">
+        <f t="shared" ref="J98:J108" ca="1" si="22">LEN(DEC2BIN(2^_xlfn.FLOOR.MATH((I98+1)/8192)))</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="K98" s="2" t="e" cm="1">
         <f t="array" aca="1" ref="K98" ca="1">_xlfn.SWITCH(J98,1,8*2^10 - I98, 2, 8*2^10 -I98, 3, 24*2^B$41 -I98)</f>
-        <v>1760</v>
-      </c>
-      <c r="L98" s="2" cm="1">
+        <v>#NUM!</v>
+      </c>
+      <c r="L98" s="2" t="e" cm="1">
         <f t="array" aca="1" ref="L98" ca="1">_xlfn.SWITCH(J98,1,K98*G$44, 2, K98*G$45, 3, K98*G$46)</f>
-        <v>38410240</v>
-      </c>
-      <c r="M98" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(L98/2^(B$41+B$41))</f>
-        <v>36</v>
-      </c>
-      <c r="N98" s="2">
-        <f t="shared" ref="N98:N108" ca="1" si="11">IF(J98=3,M98+170,M98)</f>
-        <v>36</v>
-      </c>
-      <c r="O98" s="2">
-        <f t="shared" ref="O98:O108" ca="1" si="12">MOD(N98,1024)</f>
-        <v>36</v>
-      </c>
-      <c r="P98" s="2">
-        <f ca="1">O98/2^B$41</f>
-        <v>3.515625E-2</v>
-      </c>
-      <c r="Q98" s="2">
-        <f t="shared" ref="Q98:Q108" ca="1" si="13">P98*360</f>
-        <v>12.65625</v>
+        <v>#NUM!</v>
+      </c>
+      <c r="M98" s="2" t="e">
+        <f t="shared" ca="1" si="19"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="N98" s="2" t="e">
+        <f t="shared" ref="N98:N108" ca="1" si="23">IF(J98=3,M98+170,M98)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="O98" s="2" t="e">
+        <f t="shared" ref="O98:O108" ca="1" si="24">MOD(N98,1024)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="P98" s="2" t="e">
+        <f t="shared" ca="1" si="20"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="Q98" s="2" t="e">
+        <f t="shared" ref="Q98:Q108" ca="1" si="25">P98*360</f>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="99" spans="6:25" x14ac:dyDescent="0.3">
       <c r="F99" s="2">
-        <f ca="1">H99/2^B$41</f>
-        <v>0.84375</v>
+        <f t="shared" ca="1" si="21"/>
+        <v>39.97265625</v>
       </c>
       <c r="G99" s="6" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="H99" s="2" cm="1">
         <f t="array" aca="1" ref="H99" ca="1">SUMPRODUCT(--MID(G99,LEN(G99)+1-ROW(INDIRECT("1:"&amp;LEN(G99))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G99)))-1)))</f>
-        <v>864</v>
+        <v>40932</v>
       </c>
       <c r="I99" s="2">
-        <f ca="1">H99*B$39</f>
-        <v>20736</v>
-      </c>
-      <c r="J99" s="2">
-        <f t="shared" ca="1" si="10"/>
-        <v>3</v>
-      </c>
-      <c r="K99" s="2" cm="1">
+        <f t="shared" ca="1" si="18"/>
+        <v>982368</v>
+      </c>
+      <c r="J99" s="2" t="e">
+        <f t="shared" ca="1" si="22"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="K99" s="2" t="e" cm="1">
         <f t="array" aca="1" ref="K99" ca="1">_xlfn.SWITCH(J99,1,8*2^10 - I99, 2, 8*2^10 -I99, 3, 24*2^B$41 -I99)</f>
-        <v>3840</v>
-      </c>
-      <c r="L99" s="2" cm="1">
+        <v>#NUM!</v>
+      </c>
+      <c r="L99" s="2" t="e" cm="1">
         <f t="array" aca="1" ref="L99" ca="1">_xlfn.SWITCH(J99,1,K99*G$44, 2, K99*G$45, 3, K99*G$46)</f>
-        <v>251412480</v>
-      </c>
-      <c r="M99" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(L99/2^(B$41+B$41))</f>
-        <v>239</v>
-      </c>
-      <c r="N99" s="2">
-        <f t="shared" ca="1" si="11"/>
-        <v>409</v>
-      </c>
-      <c r="O99" s="2">
-        <f t="shared" ca="1" si="12"/>
-        <v>409</v>
-      </c>
-      <c r="P99" s="2">
-        <f ca="1">O99/2^B$41</f>
-        <v>0.3994140625</v>
-      </c>
-      <c r="Q99" s="2">
-        <f t="shared" ca="1" si="13"/>
-        <v>143.7890625</v>
+        <v>#NUM!</v>
+      </c>
+      <c r="M99" s="2" t="e">
+        <f t="shared" ca="1" si="19"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="N99" s="2" t="e">
+        <f t="shared" ca="1" si="23"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="O99" s="2" t="e">
+        <f t="shared" ca="1" si="24"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P99" s="2" t="e">
+        <f t="shared" ca="1" si="20"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="Q99" s="2" t="e">
+        <f t="shared" ca="1" si="25"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="100" spans="6:25" x14ac:dyDescent="0.3">
       <c r="F100" s="2">
-        <f ca="1">H100/2^B$41</f>
-        <v>0.94140625</v>
+        <f t="shared" ca="1" si="21"/>
+        <v>42.09765625</v>
       </c>
       <c r="G100" s="6" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="H100" s="2" cm="1">
         <f t="array" aca="1" ref="H100" ca="1">SUMPRODUCT(--MID(G100,LEN(G100)+1-ROW(INDIRECT("1:"&amp;LEN(G100))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G100)))-1)))</f>
-        <v>964</v>
+        <v>43108</v>
       </c>
       <c r="I100" s="2">
-        <f ca="1">H100*B$39</f>
-        <v>23136</v>
-      </c>
-      <c r="J100" s="2">
-        <f t="shared" ca="1" si="10"/>
-        <v>3</v>
-      </c>
-      <c r="K100" s="2" cm="1">
+        <f t="shared" ca="1" si="18"/>
+        <v>1034592</v>
+      </c>
+      <c r="J100" s="2" t="e">
+        <f t="shared" ca="1" si="22"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="K100" s="2" t="e" cm="1">
         <f t="array" aca="1" ref="K100" ca="1">_xlfn.SWITCH(J100,1,8*2^10 - I100, 2, 8*2^10 -I100, 3, 24*2^B$41 -I100)</f>
-        <v>1440</v>
-      </c>
-      <c r="L100" s="2" cm="1">
+        <v>#NUM!</v>
+      </c>
+      <c r="L100" s="2" t="e" cm="1">
         <f t="array" aca="1" ref="L100" ca="1">_xlfn.SWITCH(J100,1,K100*G$44, 2, K100*G$45, 3, K100*G$46)</f>
-        <v>94279680</v>
-      </c>
-      <c r="M100" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(L100/2^(B$41+B$41))</f>
-        <v>89</v>
-      </c>
-      <c r="N100" s="2">
-        <f t="shared" ca="1" si="11"/>
-        <v>259</v>
-      </c>
-      <c r="O100" s="2">
-        <f t="shared" ca="1" si="12"/>
-        <v>259</v>
-      </c>
-      <c r="P100" s="2">
-        <f ca="1">O100/2^B$41</f>
-        <v>0.2529296875</v>
-      </c>
-      <c r="Q100" s="2">
-        <f t="shared" ca="1" si="13"/>
-        <v>91.0546875</v>
+        <v>#NUM!</v>
+      </c>
+      <c r="M100" s="2" t="e">
+        <f t="shared" ca="1" si="19"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="N100" s="2" t="e">
+        <f t="shared" ca="1" si="23"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="O100" s="2" t="e">
+        <f t="shared" ca="1" si="24"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="P100" s="2" t="e">
+        <f t="shared" ca="1" si="20"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="Q100" s="2" t="e">
+        <f t="shared" ca="1" si="25"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="101" spans="6:25" x14ac:dyDescent="0.3">
       <c r="F101" s="2">
-        <f ca="1">H101/2^B$41</f>
+        <f t="shared" ca="1" si="21"/>
         <v>0.7763671875</v>
       </c>
       <c r="G101" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H101" s="2" cm="1">
         <f t="array" aca="1" ref="H101" ca="1">SUMPRODUCT(--MID(G101,LEN(G101)+1-ROW(INDIRECT("1:"&amp;LEN(G101))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G101)))-1)))</f>
         <v>795</v>
       </c>
       <c r="I101" s="2">
-        <f ca="1">H101*B$39</f>
+        <f t="shared" ca="1" si="18"/>
         <v>19080</v>
       </c>
       <c r="J101" s="2">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="22"/>
         <v>3</v>
       </c>
       <c r="K101" s="2" cm="1">
@@ -2729,44 +2729,44 @@
         <v>359834112</v>
       </c>
       <c r="M101" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(L101/2^(B$41+B$41))</f>
+        <f t="shared" ca="1" si="19"/>
         <v>343</v>
       </c>
       <c r="N101" s="2">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="23"/>
         <v>513</v>
       </c>
       <c r="O101" s="2">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="24"/>
         <v>513</v>
       </c>
       <c r="P101" s="2">
-        <f ca="1">O101/2^B$41</f>
+        <f t="shared" ca="1" si="20"/>
         <v>0.5009765625</v>
       </c>
       <c r="Q101" s="2">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="25"/>
         <v>180.3515625</v>
       </c>
     </row>
     <row r="102" spans="6:25" x14ac:dyDescent="0.3">
       <c r="F102" s="2">
-        <f ca="1">H102/2^B$41</f>
+        <f t="shared" ca="1" si="21"/>
         <v>0.638671875</v>
       </c>
       <c r="G102" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="H102" s="2" cm="1">
         <f t="array" aca="1" ref="H102" ca="1">SUMPRODUCT(--MID(G102,LEN(G102)+1-ROW(INDIRECT("1:"&amp;LEN(G102))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G102)))-1)))</f>
         <v>654</v>
       </c>
       <c r="I102" s="2">
-        <f ca="1">H102*B$39</f>
+        <f t="shared" ca="1" si="18"/>
         <v>15696</v>
       </c>
       <c r="J102" s="2">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="22"/>
         <v>2</v>
       </c>
       <c r="K102" s="2" cm="1">
@@ -2778,44 +2778,44 @@
         <v>-327534592</v>
       </c>
       <c r="M102" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(L102/2^(B$41+B$41))</f>
+        <f t="shared" ca="1" si="19"/>
         <v>-313</v>
       </c>
       <c r="N102" s="2">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="23"/>
         <v>-313</v>
       </c>
       <c r="O102" s="2">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="24"/>
         <v>711</v>
       </c>
       <c r="P102" s="2">
-        <f ca="1">O102/2^B$41</f>
+        <f t="shared" ca="1" si="20"/>
         <v>0.6943359375</v>
       </c>
       <c r="Q102" s="2">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="25"/>
         <v>249.9609375</v>
       </c>
     </row>
     <row r="103" spans="6:25" x14ac:dyDescent="0.3">
       <c r="F103" s="2">
-        <f ca="1">H103/2^B$41</f>
+        <f t="shared" ca="1" si="21"/>
         <v>0.3369140625</v>
       </c>
       <c r="G103" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H103" s="2" cm="1">
         <f t="array" aca="1" ref="H103" ca="1">SUMPRODUCT(--MID(G103,LEN(G103)+1-ROW(INDIRECT("1:"&amp;LEN(G103))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G103)))-1)))</f>
         <v>345</v>
       </c>
       <c r="I103" s="2">
-        <f ca="1">H103*B$39</f>
+        <f t="shared" ca="1" si="18"/>
         <v>8280</v>
       </c>
       <c r="J103" s="2">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="22"/>
         <v>2</v>
       </c>
       <c r="K103" s="2" cm="1">
@@ -2827,44 +2827,44 @@
         <v>-3841024</v>
       </c>
       <c r="M103" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(L103/2^(B$41+B$41))</f>
+        <f t="shared" ca="1" si="19"/>
         <v>-4</v>
       </c>
       <c r="N103" s="2">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="23"/>
         <v>-4</v>
       </c>
       <c r="O103" s="2">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="24"/>
         <v>1020</v>
       </c>
       <c r="P103" s="2">
-        <f ca="1">O103/2^B$41</f>
+        <f t="shared" ca="1" si="20"/>
         <v>0.99609375</v>
       </c>
       <c r="Q103" s="2">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="25"/>
         <v>358.59375</v>
       </c>
     </row>
     <row r="104" spans="6:25" x14ac:dyDescent="0.3">
       <c r="F104" s="2">
-        <f ca="1">H104/2^B$41</f>
+        <f t="shared" ca="1" si="21"/>
         <v>0.560546875</v>
       </c>
       <c r="G104" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H104" s="2" cm="1">
         <f t="array" aca="1" ref="H104" ca="1">SUMPRODUCT(--MID(G104,LEN(G104)+1-ROW(INDIRECT("1:"&amp;LEN(G104))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G104)))-1)))</f>
         <v>574</v>
       </c>
       <c r="I104" s="2">
-        <f ca="1">H104*B$39</f>
+        <f t="shared" ca="1" si="18"/>
         <v>13776</v>
       </c>
       <c r="J104" s="2">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="22"/>
         <v>2</v>
       </c>
       <c r="K104" s="2" cm="1">
@@ -2876,44 +2876,44 @@
         <v>-243730432</v>
       </c>
       <c r="M104" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(L104/2^(B$41+B$41))</f>
+        <f t="shared" ca="1" si="19"/>
         <v>-233</v>
       </c>
       <c r="N104" s="2">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="23"/>
         <v>-233</v>
       </c>
       <c r="O104" s="2">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="24"/>
         <v>791</v>
       </c>
       <c r="P104" s="2">
-        <f ca="1">O104/2^B$41</f>
+        <f t="shared" ca="1" si="20"/>
         <v>0.7724609375</v>
       </c>
       <c r="Q104" s="2">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="25"/>
         <v>278.0859375</v>
       </c>
     </row>
     <row r="105" spans="6:25" x14ac:dyDescent="0.3">
       <c r="F105" s="2">
-        <f ca="1">H105/2^B$41</f>
+        <f t="shared" ca="1" si="21"/>
         <v>3.90625E-2</v>
       </c>
       <c r="G105" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H105" s="2" cm="1">
         <f t="array" aca="1" ref="H105" ca="1">SUMPRODUCT(--MID(G105,LEN(G105)+1-ROW(INDIRECT("1:"&amp;LEN(G105))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G105)))-1)))</f>
         <v>40</v>
       </c>
       <c r="I105" s="2">
-        <f ca="1">H105*B$39</f>
+        <f t="shared" ca="1" si="18"/>
         <v>960</v>
       </c>
       <c r="J105" s="2">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="22"/>
         <v>1</v>
       </c>
       <c r="K105" s="2" cm="1">
@@ -2925,44 +2925,44 @@
         <v>157831168</v>
       </c>
       <c r="M105" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(L105/2^(B$41+B$41))</f>
+        <f t="shared" ca="1" si="19"/>
         <v>150</v>
       </c>
       <c r="N105" s="2">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="23"/>
         <v>150</v>
       </c>
       <c r="O105" s="2">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="24"/>
         <v>150</v>
       </c>
       <c r="P105" s="2">
-        <f ca="1">O105/2^B$41</f>
+        <f t="shared" ca="1" si="20"/>
         <v>0.146484375</v>
       </c>
       <c r="Q105" s="2">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="25"/>
         <v>52.734375</v>
       </c>
     </row>
     <row r="106" spans="6:25" x14ac:dyDescent="0.3">
       <c r="F106" s="2">
-        <f ca="1">H106/2^B$41</f>
+        <f t="shared" ca="1" si="21"/>
         <v>0.8330078125</v>
       </c>
       <c r="G106" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H106" s="2" cm="1">
         <f t="array" aca="1" ref="H106" ca="1">SUMPRODUCT(--MID(G106,LEN(G106)+1-ROW(INDIRECT("1:"&amp;LEN(G106))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G106)))-1)))</f>
         <v>853</v>
       </c>
       <c r="I106" s="2">
-        <f ca="1">H106*B$39</f>
+        <f t="shared" ca="1" si="18"/>
         <v>20472</v>
       </c>
       <c r="J106" s="2">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="22"/>
         <v>3</v>
       </c>
       <c r="K106" s="2" cm="1">
@@ -2974,44 +2974,44 @@
         <v>268697088</v>
       </c>
       <c r="M106" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(L106/2^(B$41+B$41))</f>
+        <f t="shared" ca="1" si="19"/>
         <v>256</v>
       </c>
       <c r="N106" s="2">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="23"/>
         <v>426</v>
       </c>
       <c r="O106" s="2">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="24"/>
         <v>426</v>
       </c>
       <c r="P106" s="2">
-        <f ca="1">O106/2^B$41</f>
+        <f t="shared" ca="1" si="20"/>
         <v>0.416015625</v>
       </c>
       <c r="Q106" s="2">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="25"/>
         <v>149.765625</v>
       </c>
     </row>
     <row r="107" spans="6:25" x14ac:dyDescent="0.3">
       <c r="F107" s="2">
-        <f ca="1">H107/2^B$41</f>
+        <f t="shared" ca="1" si="21"/>
         <v>0.8330078125</v>
       </c>
       <c r="G107" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H107" s="2" cm="1">
         <f t="array" aca="1" ref="H107" ca="1">SUMPRODUCT(--MID(G107,LEN(G107)+1-ROW(INDIRECT("1:"&amp;LEN(G107))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G107)))-1)))</f>
         <v>853</v>
       </c>
       <c r="I107" s="2">
-        <f ca="1">H107*B$39</f>
+        <f t="shared" ca="1" si="18"/>
         <v>20472</v>
       </c>
       <c r="J107" s="2">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="22"/>
         <v>3</v>
       </c>
       <c r="K107" s="2" cm="1">
@@ -3023,44 +3023,44 @@
         <v>268697088</v>
       </c>
       <c r="M107" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(L107/2^(B$41+B$41))</f>
+        <f t="shared" ca="1" si="19"/>
         <v>256</v>
       </c>
       <c r="N107" s="2">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="23"/>
         <v>426</v>
       </c>
       <c r="O107" s="2">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="24"/>
         <v>426</v>
       </c>
       <c r="P107" s="2">
-        <f ca="1">O107/2^B$41</f>
+        <f t="shared" ca="1" si="20"/>
         <v>0.416015625</v>
       </c>
       <c r="Q107" s="2">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="25"/>
         <v>149.765625</v>
       </c>
     </row>
     <row r="108" spans="6:25" x14ac:dyDescent="0.3">
       <c r="F108" s="2">
-        <f ca="1">H108/2^B$41</f>
+        <f t="shared" ca="1" si="21"/>
         <v>0</v>
       </c>
       <c r="G108" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H108" s="2" cm="1">
         <f t="array" aca="1" ref="H108" ca="1">SUMPRODUCT(--MID(G108,LEN(G108)+1-ROW(INDIRECT("1:"&amp;LEN(G108))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G108)))-1)))</f>
         <v>0</v>
       </c>
       <c r="I108" s="2">
-        <f ca="1">H108*B$39</f>
+        <f t="shared" ca="1" si="18"/>
         <v>0</v>
       </c>
       <c r="J108" s="2">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ca="1" si="22"/>
         <v>1</v>
       </c>
       <c r="K108" s="2" cm="1">
@@ -3072,29 +3072,29 @@
         <v>178782208</v>
       </c>
       <c r="M108" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(L108/2^(B$41+B$41))</f>
+        <f t="shared" ca="1" si="19"/>
         <v>170</v>
       </c>
       <c r="N108" s="2">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="23"/>
         <v>170</v>
       </c>
       <c r="O108" s="2">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="24"/>
         <v>170</v>
       </c>
       <c r="P108" s="2">
-        <f ca="1">O108/2^B$41</f>
+        <f t="shared" ca="1" si="20"/>
         <v>0.166015625</v>
       </c>
       <c r="Q108" s="2">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="25"/>
         <v>59.765625</v>
       </c>
     </row>
     <row r="111" spans="6:25" x14ac:dyDescent="0.3">
       <c r="I111" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="J111" s="2" t="s">
         <v>29</v>
@@ -3130,348 +3130,348 @@
         <v>40</v>
       </c>
       <c r="U111" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="V111" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="W111" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="X111" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y111" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="V111" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="W111" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="X111" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="Y111" s="2" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="112" spans="6:25" x14ac:dyDescent="0.3">
-      <c r="I112" s="2">
-        <f ca="1">O97*E$55</f>
-        <v>5220</v>
-      </c>
-      <c r="J112" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(I112/2^B$41)</f>
-        <v>5</v>
-      </c>
-      <c r="K112" s="2">
-        <f ca="1">MOD(I112, 2^B$41)</f>
-        <v>100</v>
+      <c r="I112" s="2" t="e">
+        <f t="shared" ref="I112:I123" ca="1" si="26">O97*E$55</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="J112" s="2" t="e">
+        <f t="shared" ref="J112:J123" ca="1" si="27">_xlfn.FLOOR.MATH(I112/2^B$41)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="K112" s="2" t="e">
+        <f t="shared" ref="K112:K123" ca="1" si="28">MOD(I112, 2^B$41)</f>
+        <v>#NUM!</v>
       </c>
       <c r="L112" s="2">
         <f ca="1">IF(E57,K83,L83)</f>
         <v>600</v>
       </c>
       <c r="M112" s="2">
-        <f ca="1">L112*E$54</f>
+        <f t="shared" ref="M112:M123" ca="1" si="29">L112*E$54</f>
         <v>982800</v>
       </c>
       <c r="N112" s="2">
-        <f ca="1">IF(_xlfn.FLOOR.MATH(M112/2^B$41) &gt; 1023, 1023, _xlfn.FLOOR.MATH(M112/2^B$41))</f>
+        <f t="shared" ref="N112:N123" ca="1" si="30">IF(_xlfn.FLOOR.MATH(M112/2^B$41) &gt; 1023, 1023, _xlfn.FLOOR.MATH(M112/2^B$41))</f>
         <v>959</v>
       </c>
       <c r="O112" s="2">
-        <f ca="1">IF(N112&gt;E$56,E$56,N112)</f>
+        <f t="shared" ref="O112:O123" ca="1" si="31">IF(N112&gt;E$56,E$56,N112)</f>
         <v>959</v>
       </c>
       <c r="P112" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(O112/2^(B$41-8))</f>
+        <f t="shared" ref="P112:P123" ca="1" si="32">_xlfn.FLOOR.MATH(O112/2^(B$41-8))</f>
         <v>239</v>
       </c>
-      <c r="Q112" s="2">
+      <c r="Q112" s="2" t="e">
         <f ca="1">O112*K112</f>
-        <v>95900</v>
-      </c>
-      <c r="R112" s="2">
-        <f ca="1">O112*(2^(B$41) - 1 - K112)</f>
-        <v>885157</v>
-      </c>
-      <c r="S112" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(Q112/2^(2*B$41-8))</f>
-        <v>23</v>
-      </c>
-      <c r="T112" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(R112/2^(2*B$41-8))</f>
-        <v>216</v>
-      </c>
-      <c r="U112" s="2" cm="1">
+        <v>#NUM!</v>
+      </c>
+      <c r="R112" s="2" t="e">
+        <f t="shared" ref="R112:R123" ca="1" si="33">O112*(2^(B$41) - 1 - K112)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="S112" s="2" t="e">
+        <f t="shared" ref="S112:S123" ca="1" si="34">_xlfn.FLOOR.MATH(Q112/2^(2*B$41-8))</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="T112" s="2" t="e">
+        <f t="shared" ref="T112:T123" ca="1" si="35">_xlfn.FLOOR.MATH(R112/2^(2*B$41-8))</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="U112" s="2" t="e" cm="1">
         <f t="array" aca="1" ref="U112" ca="1">_xlfn.SWITCH(J112,0,P112,1,T112,2,0,3,0,4,S112,5,P112)</f>
-        <v>239</v>
-      </c>
-      <c r="V112" s="2" cm="1">
+        <v>#NUM!</v>
+      </c>
+      <c r="V112" s="2" t="e" cm="1">
         <f t="array" aca="1" ref="V112" ca="1">_xlfn.SWITCH(J112,0,S112,1,P112,2,P112,3,T112,4,0,5,0)</f>
-        <v>0</v>
-      </c>
-      <c r="W112" s="2" cm="1">
+        <v>#NUM!</v>
+      </c>
+      <c r="W112" s="2" t="e" cm="1">
         <f t="array" aca="1" ref="W112" ca="1">_xlfn.SWITCH(J112,0,0,1,0,2,S112,3,P112,4,P112,5,T112)</f>
-        <v>216</v>
-      </c>
-      <c r="X112" s="2">
+        <v>#NUM!</v>
+      </c>
+      <c r="X112" s="2" t="e">
         <f ca="1">U112*2^16+V112*2^8+W112</f>
-        <v>15663320</v>
-      </c>
-      <c r="Y112" s="2" t="str">
-        <f t="shared" ref="Y112:Y123" ca="1" si="14">_xlfn.BASE(X112,16,6)</f>
-        <v>EF00D8</v>
+        <v>#NUM!</v>
+      </c>
+      <c r="Y112" s="2" t="e">
+        <f t="shared" ref="Y112:Y123" ca="1" si="36">_xlfn.BASE(X112,16,6)</f>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="113" spans="9:25" x14ac:dyDescent="0.3">
-      <c r="I113" s="2">
-        <f ca="1">O98*E$55</f>
-        <v>216</v>
-      </c>
-      <c r="J113" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(I113/2^B$41)</f>
-        <v>0</v>
-      </c>
-      <c r="K113" s="2">
-        <f ca="1">MOD(I113, 2^B$41)</f>
-        <v>216</v>
+      <c r="I113" s="2" t="e">
+        <f t="shared" ca="1" si="26"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="J113" s="2" t="e">
+        <f t="shared" ca="1" si="27"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="K113" s="2" t="e">
+        <f t="shared" ca="1" si="28"/>
+        <v>#NUM!</v>
       </c>
       <c r="L113" s="2">
-        <f t="shared" ref="L113:L123" ca="1" si="15">IF(E58,K84,L84)</f>
+        <f t="shared" ref="L113:L123" ca="1" si="37">IF(E58,K84,L84)</f>
         <v>717</v>
       </c>
       <c r="M113" s="2">
-        <f ca="1">L113*E$54</f>
+        <f t="shared" ca="1" si="29"/>
         <v>1174446</v>
       </c>
       <c r="N113" s="2">
-        <f ca="1">IF(_xlfn.FLOOR.MATH(M113/2^B$41) &gt; 1023, 1023, _xlfn.FLOOR.MATH(M113/2^B$41))</f>
+        <f t="shared" ca="1" si="30"/>
         <v>1023</v>
       </c>
       <c r="O113" s="2">
-        <f ca="1">IF(N113&gt;E$56,E$56,N113)</f>
+        <f t="shared" ca="1" si="31"/>
         <v>1023</v>
       </c>
       <c r="P113" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(O113/2^(B$41-8))</f>
+        <f t="shared" ca="1" si="32"/>
         <v>255</v>
       </c>
-      <c r="Q113" s="2">
-        <f t="shared" ref="Q113:Q123" ca="1" si="16">O113*K113</f>
-        <v>220968</v>
-      </c>
-      <c r="R113" s="2">
-        <f ca="1">O113*(2^(B$41) - 1 - K113)</f>
-        <v>825561</v>
-      </c>
-      <c r="S113" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(Q113/2^(2*B$41-8))</f>
-        <v>53</v>
-      </c>
-      <c r="T113" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(R113/2^(2*B$41-8))</f>
-        <v>201</v>
-      </c>
-      <c r="U113" s="2" cm="1">
+      <c r="Q113" s="2" t="e">
+        <f t="shared" ref="Q113:Q123" ca="1" si="38">O113*K113</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="R113" s="2" t="e">
+        <f t="shared" ca="1" si="33"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="S113" s="2" t="e">
+        <f t="shared" ca="1" si="34"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="T113" s="2" t="e">
+        <f t="shared" ca="1" si="35"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="U113" s="2" t="e" cm="1">
         <f t="array" aca="1" ref="U113" ca="1">_xlfn.SWITCH(J113,0,P113,1,T113,2,0,3,0,4,S113,5,P113)</f>
-        <v>255</v>
-      </c>
-      <c r="V113" s="2" cm="1">
+        <v>#NUM!</v>
+      </c>
+      <c r="V113" s="2" t="e" cm="1">
         <f t="array" aca="1" ref="V113" ca="1">_xlfn.SWITCH(J113,0,S113,1,P113,2,P113,3,T113,4,0,5,0)</f>
-        <v>53</v>
-      </c>
-      <c r="W113" s="2" cm="1">
+        <v>#NUM!</v>
+      </c>
+      <c r="W113" s="2" t="e" cm="1">
         <f t="array" aca="1" ref="W113" ca="1">_xlfn.SWITCH(J113,0,0,1,0,2,S113,3,P113,4,P113,5,T113)</f>
-        <v>0</v>
-      </c>
-      <c r="X113" s="2">
-        <f t="shared" ref="X113:X123" ca="1" si="17">U113*2^16+V113*2^8+W113</f>
-        <v>16725248</v>
-      </c>
-      <c r="Y113" s="2" t="str">
-        <f t="shared" ca="1" si="14"/>
-        <v>FF3500</v>
+        <v>#NUM!</v>
+      </c>
+      <c r="X113" s="2" t="e">
+        <f t="shared" ref="X113:X123" ca="1" si="39">U113*2^16+V113*2^8+W113</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="Y113" s="2" t="e">
+        <f t="shared" ca="1" si="36"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="114" spans="9:25" x14ac:dyDescent="0.3">
-      <c r="I114" s="2">
-        <f ca="1">O99*E$55</f>
-        <v>2454</v>
-      </c>
-      <c r="J114" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(I114/2^B$41)</f>
-        <v>2</v>
-      </c>
-      <c r="K114" s="2">
-        <f ca="1">MOD(I114, 2^B$41)</f>
-        <v>406</v>
+      <c r="I114" s="2" t="e">
+        <f t="shared" ca="1" si="26"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="J114" s="2" t="e">
+        <f t="shared" ca="1" si="27"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="K114" s="2" t="e">
+        <f t="shared" ca="1" si="28"/>
+        <v>#NUM!</v>
       </c>
       <c r="L114" s="2">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="37"/>
         <v>450</v>
       </c>
       <c r="M114" s="2">
-        <f ca="1">L114*E$54</f>
+        <f t="shared" ca="1" si="29"/>
         <v>737100</v>
       </c>
       <c r="N114" s="2">
-        <f ca="1">IF(_xlfn.FLOOR.MATH(M114/2^B$41) &gt; 1023, 1023, _xlfn.FLOOR.MATH(M114/2^B$41))</f>
+        <f t="shared" ca="1" si="30"/>
         <v>719</v>
       </c>
       <c r="O114" s="2">
-        <f ca="1">IF(N114&gt;E$56,E$56,N114)</f>
+        <f t="shared" ca="1" si="31"/>
         <v>719</v>
       </c>
       <c r="P114" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(O114/2^(B$41-8))</f>
+        <f t="shared" ca="1" si="32"/>
         <v>179</v>
       </c>
-      <c r="Q114" s="2">
-        <f t="shared" ca="1" si="16"/>
-        <v>291914</v>
-      </c>
-      <c r="R114" s="2">
-        <f ca="1">O114*(2^(B$41) - 1 - K114)</f>
-        <v>443623</v>
-      </c>
-      <c r="S114" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(Q114/2^(2*B$41-8))</f>
-        <v>71</v>
-      </c>
-      <c r="T114" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(R114/2^(2*B$41-8))</f>
-        <v>108</v>
-      </c>
-      <c r="U114" s="2" cm="1">
+      <c r="Q114" s="2" t="e">
+        <f t="shared" ca="1" si="38"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="R114" s="2" t="e">
+        <f t="shared" ca="1" si="33"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="S114" s="2" t="e">
+        <f t="shared" ca="1" si="34"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="T114" s="2" t="e">
+        <f t="shared" ca="1" si="35"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="U114" s="2" t="e" cm="1">
         <f t="array" aca="1" ref="U114" ca="1">_xlfn.SWITCH(J114,0,P114,1,T114,2,0,3,0,4,S114,5,P114)</f>
-        <v>0</v>
-      </c>
-      <c r="V114" s="2" cm="1">
+        <v>#NUM!</v>
+      </c>
+      <c r="V114" s="2" t="e" cm="1">
         <f t="array" aca="1" ref="V114" ca="1">_xlfn.SWITCH(J114,0,S114,1,P114,2,P114,3,T114,4,0,5,0)</f>
-        <v>179</v>
-      </c>
-      <c r="W114" s="2" cm="1">
+        <v>#NUM!</v>
+      </c>
+      <c r="W114" s="2" t="e" cm="1">
         <f t="array" aca="1" ref="W114" ca="1">_xlfn.SWITCH(J114,0,0,1,0,2,S114,3,P114,4,P114,5,T114)</f>
-        <v>71</v>
-      </c>
-      <c r="X114" s="2">
-        <f t="shared" ca="1" si="17"/>
-        <v>45895</v>
-      </c>
-      <c r="Y114" s="2" t="str">
-        <f t="shared" ca="1" si="14"/>
-        <v>00B347</v>
+        <v>#NUM!</v>
+      </c>
+      <c r="X114" s="2" t="e">
+        <f t="shared" ca="1" si="39"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="Y114" s="2" t="e">
+        <f t="shared" ca="1" si="36"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="115" spans="9:25" x14ac:dyDescent="0.3">
-      <c r="I115" s="2">
-        <f ca="1">O100*E$55</f>
-        <v>1554</v>
-      </c>
-      <c r="J115" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(I115/2^B$41)</f>
-        <v>1</v>
-      </c>
-      <c r="K115" s="2">
-        <f ca="1">MOD(I115, 2^B$41)</f>
-        <v>530</v>
+      <c r="I115" s="2" t="e">
+        <f t="shared" ca="1" si="26"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="J115" s="2" t="e">
+        <f t="shared" ca="1" si="27"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="K115" s="2" t="e">
+        <f t="shared" ca="1" si="28"/>
+        <v>#NUM!</v>
       </c>
       <c r="L115" s="2">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="37"/>
         <v>0</v>
       </c>
       <c r="M115" s="2">
-        <f ca="1">L115*E$54</f>
+        <f t="shared" ca="1" si="29"/>
         <v>0</v>
       </c>
       <c r="N115" s="2">
-        <f ca="1">IF(_xlfn.FLOOR.MATH(M115/2^B$41) &gt; 1023, 1023, _xlfn.FLOOR.MATH(M115/2^B$41))</f>
+        <f t="shared" ca="1" si="30"/>
         <v>0</v>
       </c>
       <c r="O115" s="2">
-        <f ca="1">IF(N115&gt;E$56,E$56,N115)</f>
+        <f t="shared" ca="1" si="31"/>
         <v>0</v>
       </c>
       <c r="P115" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(O115/2^(B$41-8))</f>
-        <v>0</v>
-      </c>
-      <c r="Q115" s="2">
-        <f t="shared" ca="1" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="R115" s="2">
-        <f ca="1">O115*(2^(B$41) - 1 - K115)</f>
-        <v>0</v>
-      </c>
-      <c r="S115" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(Q115/2^(2*B$41-8))</f>
-        <v>0</v>
-      </c>
-      <c r="T115" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(R115/2^(2*B$41-8))</f>
-        <v>0</v>
-      </c>
-      <c r="U115" s="2" cm="1">
+        <f t="shared" ca="1" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="Q115" s="2" t="e">
+        <f t="shared" ca="1" si="38"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="R115" s="2" t="e">
+        <f t="shared" ca="1" si="33"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="S115" s="2" t="e">
+        <f t="shared" ca="1" si="34"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="T115" s="2" t="e">
+        <f t="shared" ca="1" si="35"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="U115" s="2" t="e" cm="1">
         <f t="array" aca="1" ref="U115" ca="1">_xlfn.SWITCH(J115,0,P115,1,T115,2,0,3,0,4,S115,5,P115)</f>
-        <v>0</v>
-      </c>
-      <c r="V115" s="2" cm="1">
+        <v>#NUM!</v>
+      </c>
+      <c r="V115" s="2" t="e" cm="1">
         <f t="array" aca="1" ref="V115" ca="1">_xlfn.SWITCH(J115,0,S115,1,P115,2,P115,3,T115,4,0,5,0)</f>
-        <v>0</v>
-      </c>
-      <c r="W115" s="2" cm="1">
+        <v>#NUM!</v>
+      </c>
+      <c r="W115" s="2" t="e" cm="1">
         <f t="array" aca="1" ref="W115" ca="1">_xlfn.SWITCH(J115,0,0,1,0,2,S115,3,P115,4,P115,5,T115)</f>
-        <v>0</v>
-      </c>
-      <c r="X115" s="2">
-        <f t="shared" ca="1" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="Y115" s="2" t="str">
-        <f t="shared" ca="1" si="14"/>
-        <v>000000</v>
+        <v>#NUM!</v>
+      </c>
+      <c r="X115" s="2" t="e">
+        <f t="shared" ca="1" si="39"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="Y115" s="2" t="e">
+        <f t="shared" ca="1" si="36"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="116" spans="9:25" x14ac:dyDescent="0.3">
       <c r="I116" s="2">
-        <f ca="1">O101*E$55</f>
+        <f t="shared" ca="1" si="26"/>
         <v>3078</v>
       </c>
       <c r="J116" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(I116/2^B$41)</f>
+        <f t="shared" ca="1" si="27"/>
         <v>3</v>
       </c>
       <c r="K116" s="2">
-        <f ca="1">MOD(I116, 2^B$41)</f>
+        <f t="shared" ca="1" si="28"/>
         <v>6</v>
       </c>
       <c r="L116" s="2">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="37"/>
         <v>0</v>
       </c>
       <c r="M116" s="2">
-        <f ca="1">L116*E$54</f>
+        <f t="shared" ca="1" si="29"/>
         <v>0</v>
       </c>
       <c r="N116" s="2">
-        <f ca="1">IF(_xlfn.FLOOR.MATH(M116/2^B$41) &gt; 1023, 1023, _xlfn.FLOOR.MATH(M116/2^B$41))</f>
+        <f t="shared" ca="1" si="30"/>
         <v>0</v>
       </c>
       <c r="O116" s="2">
-        <f ca="1">IF(N116&gt;E$56,E$56,N116)</f>
+        <f t="shared" ca="1" si="31"/>
         <v>0</v>
       </c>
       <c r="P116" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(O116/2^(B$41-8))</f>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="Q116" s="2">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="38"/>
         <v>0</v>
       </c>
       <c r="R116" s="2">
-        <f ca="1">O116*(2^(B$41) - 1 - K116)</f>
+        <f t="shared" ca="1" si="33"/>
         <v>0</v>
       </c>
       <c r="S116" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(Q116/2^(2*B$41-8))</f>
+        <f t="shared" ca="1" si="34"/>
         <v>0</v>
       </c>
       <c r="T116" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(R116/2^(2*B$41-8))</f>
+        <f t="shared" ca="1" si="35"/>
         <v>0</v>
       </c>
       <c r="U116" s="2" cm="1">
@@ -3487,61 +3487,61 @@
         <v>0</v>
       </c>
       <c r="X116" s="2">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="39"/>
         <v>0</v>
       </c>
       <c r="Y116" s="2" t="str">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="36"/>
         <v>000000</v>
       </c>
     </row>
     <row r="117" spans="9:25" x14ac:dyDescent="0.3">
       <c r="I117" s="2">
-        <f ca="1">O102*E$55</f>
+        <f t="shared" ca="1" si="26"/>
         <v>4266</v>
       </c>
       <c r="J117" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(I117/2^B$41)</f>
+        <f t="shared" ca="1" si="27"/>
         <v>4</v>
       </c>
       <c r="K117" s="2">
-        <f ca="1">MOD(I117, 2^B$41)</f>
+        <f t="shared" ca="1" si="28"/>
         <v>170</v>
       </c>
       <c r="L117" s="2">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="37"/>
         <v>0</v>
       </c>
       <c r="M117" s="2">
-        <f ca="1">L117*E$54</f>
+        <f t="shared" ca="1" si="29"/>
         <v>0</v>
       </c>
       <c r="N117" s="2">
-        <f ca="1">IF(_xlfn.FLOOR.MATH(M117/2^B$41) &gt; 1023, 1023, _xlfn.FLOOR.MATH(M117/2^B$41))</f>
+        <f t="shared" ca="1" si="30"/>
         <v>0</v>
       </c>
       <c r="O117" s="2">
-        <f ca="1">IF(N117&gt;E$56,E$56,N117)</f>
+        <f t="shared" ca="1" si="31"/>
         <v>0</v>
       </c>
       <c r="P117" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(O117/2^(B$41-8))</f>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="Q117" s="2">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="38"/>
         <v>0</v>
       </c>
       <c r="R117" s="2">
-        <f ca="1">O117*(2^(B$41) - 1 - K117)</f>
+        <f t="shared" ca="1" si="33"/>
         <v>0</v>
       </c>
       <c r="S117" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(Q117/2^(2*B$41-8))</f>
+        <f t="shared" ca="1" si="34"/>
         <v>0</v>
       </c>
       <c r="T117" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(R117/2^(2*B$41-8))</f>
+        <f t="shared" ca="1" si="35"/>
         <v>0</v>
       </c>
       <c r="U117" s="2" cm="1">
@@ -3557,61 +3557,61 @@
         <v>0</v>
       </c>
       <c r="X117" s="2">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="39"/>
         <v>0</v>
       </c>
       <c r="Y117" s="2" t="str">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="36"/>
         <v>000000</v>
       </c>
     </row>
     <row r="118" spans="9:25" x14ac:dyDescent="0.3">
       <c r="I118" s="2">
-        <f ca="1">O103*E$55</f>
+        <f t="shared" ca="1" si="26"/>
         <v>6120</v>
       </c>
       <c r="J118" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(I118/2^B$41)</f>
+        <f t="shared" ca="1" si="27"/>
         <v>5</v>
       </c>
       <c r="K118" s="2">
-        <f ca="1">MOD(I118, 2^B$41)</f>
+        <f t="shared" ca="1" si="28"/>
         <v>1000</v>
       </c>
       <c r="L118" s="2">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="37"/>
         <v>0</v>
       </c>
       <c r="M118" s="2">
-        <f ca="1">L118*E$54</f>
+        <f t="shared" ca="1" si="29"/>
         <v>0</v>
       </c>
       <c r="N118" s="2">
-        <f ca="1">IF(_xlfn.FLOOR.MATH(M118/2^B$41) &gt; 1023, 1023, _xlfn.FLOOR.MATH(M118/2^B$41))</f>
+        <f t="shared" ca="1" si="30"/>
         <v>0</v>
       </c>
       <c r="O118" s="2">
-        <f ca="1">IF(N118&gt;E$56,E$56,N118)</f>
+        <f t="shared" ca="1" si="31"/>
         <v>0</v>
       </c>
       <c r="P118" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(O118/2^(B$41-8))</f>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="Q118" s="2">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="38"/>
         <v>0</v>
       </c>
       <c r="R118" s="2">
-        <f ca="1">O118*(2^(B$41) - 1 - K118)</f>
+        <f t="shared" ca="1" si="33"/>
         <v>0</v>
       </c>
       <c r="S118" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(Q118/2^(2*B$41-8))</f>
+        <f t="shared" ca="1" si="34"/>
         <v>0</v>
       </c>
       <c r="T118" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(R118/2^(2*B$41-8))</f>
+        <f t="shared" ca="1" si="35"/>
         <v>0</v>
       </c>
       <c r="U118" s="2" cm="1">
@@ -3627,61 +3627,61 @@
         <v>0</v>
       </c>
       <c r="X118" s="2">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="39"/>
         <v>0</v>
       </c>
       <c r="Y118" s="2" t="str">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="36"/>
         <v>000000</v>
       </c>
     </row>
     <row r="119" spans="9:25" x14ac:dyDescent="0.3">
       <c r="I119" s="2">
-        <f ca="1">O104*E$55</f>
+        <f t="shared" ca="1" si="26"/>
         <v>4746</v>
       </c>
       <c r="J119" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(I119/2^B$41)</f>
+        <f t="shared" ca="1" si="27"/>
         <v>4</v>
       </c>
       <c r="K119" s="2">
-        <f ca="1">MOD(I119, 2^B$41)</f>
+        <f t="shared" ca="1" si="28"/>
         <v>650</v>
       </c>
       <c r="L119" s="2">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="37"/>
         <v>0</v>
       </c>
       <c r="M119" s="2">
-        <f ca="1">L119*E$54</f>
+        <f t="shared" ca="1" si="29"/>
         <v>0</v>
       </c>
       <c r="N119" s="2">
-        <f ca="1">IF(_xlfn.FLOOR.MATH(M119/2^B$41) &gt; 1023, 1023, _xlfn.FLOOR.MATH(M119/2^B$41))</f>
+        <f t="shared" ca="1" si="30"/>
         <v>0</v>
       </c>
       <c r="O119" s="2">
-        <f ca="1">IF(N119&gt;E$56,E$56,N119)</f>
+        <f t="shared" ca="1" si="31"/>
         <v>0</v>
       </c>
       <c r="P119" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(O119/2^(B$41-8))</f>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="Q119" s="2">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="38"/>
         <v>0</v>
       </c>
       <c r="R119" s="2">
-        <f ca="1">O119*(2^(B$41) - 1 - K119)</f>
+        <f t="shared" ca="1" si="33"/>
         <v>0</v>
       </c>
       <c r="S119" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(Q119/2^(2*B$41-8))</f>
+        <f t="shared" ca="1" si="34"/>
         <v>0</v>
       </c>
       <c r="T119" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(R119/2^(2*B$41-8))</f>
+        <f t="shared" ca="1" si="35"/>
         <v>0</v>
       </c>
       <c r="U119" s="2" cm="1">
@@ -3697,61 +3697,61 @@
         <v>0</v>
       </c>
       <c r="X119" s="2">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="39"/>
         <v>0</v>
       </c>
       <c r="Y119" s="2" t="str">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="36"/>
         <v>000000</v>
       </c>
     </row>
     <row r="120" spans="9:25" x14ac:dyDescent="0.3">
       <c r="I120" s="2">
-        <f ca="1">O105*E$55</f>
+        <f t="shared" ca="1" si="26"/>
         <v>900</v>
       </c>
       <c r="J120" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(I120/2^B$41)</f>
+        <f t="shared" ca="1" si="27"/>
         <v>0</v>
       </c>
       <c r="K120" s="2">
-        <f ca="1">MOD(I120, 2^B$41)</f>
+        <f t="shared" ca="1" si="28"/>
         <v>900</v>
       </c>
       <c r="L120" s="2">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="37"/>
         <v>0</v>
       </c>
       <c r="M120" s="2">
-        <f ca="1">L120*E$54</f>
+        <f t="shared" ca="1" si="29"/>
         <v>0</v>
       </c>
       <c r="N120" s="2">
-        <f ca="1">IF(_xlfn.FLOOR.MATH(M120/2^B$41) &gt; 1023, 1023, _xlfn.FLOOR.MATH(M120/2^B$41))</f>
+        <f t="shared" ca="1" si="30"/>
         <v>0</v>
       </c>
       <c r="O120" s="2">
-        <f ca="1">IF(N120&gt;E$56,E$56,N120)</f>
+        <f t="shared" ca="1" si="31"/>
         <v>0</v>
       </c>
       <c r="P120" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(O120/2^(B$41-8))</f>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="Q120" s="2">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="38"/>
         <v>0</v>
       </c>
       <c r="R120" s="2">
-        <f ca="1">O120*(2^(B$41) - 1 - K120)</f>
+        <f t="shared" ca="1" si="33"/>
         <v>0</v>
       </c>
       <c r="S120" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(Q120/2^(2*B$41-8))</f>
+        <f t="shared" ca="1" si="34"/>
         <v>0</v>
       </c>
       <c r="T120" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(R120/2^(2*B$41-8))</f>
+        <f t="shared" ca="1" si="35"/>
         <v>0</v>
       </c>
       <c r="U120" s="2" cm="1">
@@ -3767,61 +3767,61 @@
         <v>0</v>
       </c>
       <c r="X120" s="2">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="39"/>
         <v>0</v>
       </c>
       <c r="Y120" s="2" t="str">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="36"/>
         <v>000000</v>
       </c>
     </row>
     <row r="121" spans="9:25" x14ac:dyDescent="0.3">
       <c r="I121" s="2">
-        <f ca="1">O106*E$55</f>
+        <f t="shared" ca="1" si="26"/>
         <v>2556</v>
       </c>
       <c r="J121" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(I121/2^B$41)</f>
+        <f t="shared" ca="1" si="27"/>
         <v>2</v>
       </c>
       <c r="K121" s="2">
-        <f ca="1">MOD(I121, 2^B$41)</f>
+        <f t="shared" ca="1" si="28"/>
         <v>508</v>
       </c>
       <c r="L121" s="2">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="37"/>
         <v>0</v>
       </c>
       <c r="M121" s="2">
-        <f ca="1">L121*E$54</f>
+        <f t="shared" ca="1" si="29"/>
         <v>0</v>
       </c>
       <c r="N121" s="2">
-        <f ca="1">IF(_xlfn.FLOOR.MATH(M121/2^B$41) &gt; 1023, 1023, _xlfn.FLOOR.MATH(M121/2^B$41))</f>
+        <f t="shared" ca="1" si="30"/>
         <v>0</v>
       </c>
       <c r="O121" s="2">
-        <f ca="1">IF(N121&gt;E$56,E$56,N121)</f>
+        <f t="shared" ca="1" si="31"/>
         <v>0</v>
       </c>
       <c r="P121" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(O121/2^(B$41-8))</f>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="Q121" s="2">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="38"/>
         <v>0</v>
       </c>
       <c r="R121" s="2">
-        <f ca="1">O121*(2^(B$41) - 1 - K121)</f>
+        <f t="shared" ca="1" si="33"/>
         <v>0</v>
       </c>
       <c r="S121" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(Q121/2^(2*B$41-8))</f>
+        <f t="shared" ca="1" si="34"/>
         <v>0</v>
       </c>
       <c r="T121" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(R121/2^(2*B$41-8))</f>
+        <f t="shared" ca="1" si="35"/>
         <v>0</v>
       </c>
       <c r="U121" s="2" cm="1">
@@ -3837,61 +3837,61 @@
         <v>0</v>
       </c>
       <c r="X121" s="2">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="39"/>
         <v>0</v>
       </c>
       <c r="Y121" s="2" t="str">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="36"/>
         <v>000000</v>
       </c>
     </row>
     <row r="122" spans="9:25" x14ac:dyDescent="0.3">
       <c r="I122" s="2">
-        <f ca="1">O107*E$55</f>
+        <f t="shared" ca="1" si="26"/>
         <v>2556</v>
       </c>
       <c r="J122" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(I122/2^B$41)</f>
+        <f t="shared" ca="1" si="27"/>
         <v>2</v>
       </c>
       <c r="K122" s="2">
-        <f ca="1">MOD(I122, 2^B$41)</f>
+        <f t="shared" ca="1" si="28"/>
         <v>508</v>
       </c>
       <c r="L122" s="2">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="37"/>
         <v>0</v>
       </c>
       <c r="M122" s="2">
-        <f ca="1">L122*E$54</f>
+        <f t="shared" ca="1" si="29"/>
         <v>0</v>
       </c>
       <c r="N122" s="2">
-        <f ca="1">IF(_xlfn.FLOOR.MATH(M122/2^B$41) &gt; 1023, 1023, _xlfn.FLOOR.MATH(M122/2^B$41))</f>
+        <f t="shared" ca="1" si="30"/>
         <v>0</v>
       </c>
       <c r="O122" s="2">
-        <f ca="1">IF(N122&gt;E$56,E$56,N122)</f>
+        <f t="shared" ca="1" si="31"/>
         <v>0</v>
       </c>
       <c r="P122" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(O122/2^(B$41-8))</f>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="Q122" s="2">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="38"/>
         <v>0</v>
       </c>
       <c r="R122" s="2">
-        <f ca="1">O122*(2^(B$41) - 1 - K122)</f>
+        <f t="shared" ca="1" si="33"/>
         <v>0</v>
       </c>
       <c r="S122" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(Q122/2^(2*B$41-8))</f>
+        <f t="shared" ca="1" si="34"/>
         <v>0</v>
       </c>
       <c r="T122" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(R122/2^(2*B$41-8))</f>
+        <f t="shared" ca="1" si="35"/>
         <v>0</v>
       </c>
       <c r="U122" s="2" cm="1">
@@ -3907,61 +3907,61 @@
         <v>0</v>
       </c>
       <c r="X122" s="2">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="39"/>
         <v>0</v>
       </c>
       <c r="Y122" s="2" t="str">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="36"/>
         <v>000000</v>
       </c>
     </row>
     <row r="123" spans="9:25" x14ac:dyDescent="0.3">
       <c r="I123" s="2">
-        <f ca="1">O108*E$55</f>
+        <f t="shared" ca="1" si="26"/>
         <v>1020</v>
       </c>
       <c r="J123" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(I123/2^B$41)</f>
+        <f t="shared" ca="1" si="27"/>
         <v>0</v>
       </c>
       <c r="K123" s="2">
-        <f ca="1">MOD(I123, 2^B$41)</f>
+        <f t="shared" ca="1" si="28"/>
         <v>1020</v>
       </c>
       <c r="L123" s="2">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="37"/>
         <v>0</v>
       </c>
       <c r="M123" s="2">
-        <f ca="1">L123*E$54</f>
+        <f t="shared" ca="1" si="29"/>
         <v>0</v>
       </c>
       <c r="N123" s="2">
-        <f ca="1">IF(_xlfn.FLOOR.MATH(M123/2^B$41) &gt; 1023, 1023, _xlfn.FLOOR.MATH(M123/2^B$41))</f>
+        <f t="shared" ca="1" si="30"/>
         <v>0</v>
       </c>
       <c r="O123" s="2">
-        <f ca="1">IF(N123&gt;E$56,E$56,N123)</f>
+        <f t="shared" ca="1" si="31"/>
         <v>0</v>
       </c>
       <c r="P123" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(O123/2^(B$41-8))</f>
+        <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
       <c r="Q123" s="2">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="38"/>
         <v>0</v>
       </c>
       <c r="R123" s="2">
-        <f ca="1">O123*(2^(B$41) - 1 - K123)</f>
+        <f t="shared" ca="1" si="33"/>
         <v>0</v>
       </c>
       <c r="S123" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(Q123/2^(2*B$41-8))</f>
+        <f t="shared" ca="1" si="34"/>
         <v>0</v>
       </c>
       <c r="T123" s="2">
-        <f ca="1">_xlfn.FLOOR.MATH(R123/2^(2*B$41-8))</f>
+        <f t="shared" ca="1" si="35"/>
         <v>0</v>
       </c>
       <c r="U123" s="2" cm="1">
@@ -3977,11 +3977,11 @@
         <v>0</v>
       </c>
       <c r="X123" s="2">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="39"/>
         <v>0</v>
       </c>
       <c r="Y123" s="2" t="str">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="36"/>
         <v>000000</v>
       </c>
     </row>
@@ -3999,79 +3999,79 @@
         <v>24.779414062499999</v>
       </c>
       <c r="J126" s="2">
-        <f ca="1">K83/I$126</f>
+        <f t="shared" ref="J126:J138" ca="1" si="40">K83/I$126</f>
         <v>17.110583539448857</v>
       </c>
     </row>
     <row r="127" spans="9:25" x14ac:dyDescent="0.3">
       <c r="J127" s="2">
-        <f ca="1">K84/I$126</f>
+        <f t="shared" ca="1" si="40"/>
         <v>21.832244822677595</v>
       </c>
     </row>
     <row r="128" spans="9:25" x14ac:dyDescent="0.3">
       <c r="J128" s="2">
-        <f ca="1">K85/I$126</f>
+        <f t="shared" ca="1" si="40"/>
         <v>11.05717163787355</v>
       </c>
     </row>
     <row r="129" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J129" s="2">
-        <f ca="1">K86/I$126</f>
+        <f t="shared" ca="1" si="40"/>
         <v>0</v>
       </c>
     </row>
     <row r="130" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J130" s="2">
-        <f ca="1">K87/I$126</f>
+        <f t="shared" ca="1" si="40"/>
         <v>0</v>
       </c>
     </row>
     <row r="131" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J131" s="2">
-        <f ca="1">K88/I$126</f>
+        <f t="shared" ca="1" si="40"/>
         <v>0</v>
       </c>
     </row>
     <row r="132" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J132" s="2">
-        <f ca="1">K89/I$126</f>
+        <f t="shared" ca="1" si="40"/>
         <v>0</v>
       </c>
     </row>
     <row r="133" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J133" s="2">
-        <f ca="1">K90/I$126</f>
+        <f t="shared" ca="1" si="40"/>
         <v>0</v>
       </c>
     </row>
     <row r="134" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J134" s="2">
-        <f ca="1">K91/I$126</f>
+        <f t="shared" ca="1" si="40"/>
         <v>0</v>
       </c>
     </row>
     <row r="135" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J135" s="2">
-        <f ca="1">K92/I$126</f>
+        <f t="shared" ca="1" si="40"/>
         <v>0</v>
       </c>
     </row>
     <row r="136" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J136" s="2">
-        <f ca="1">K93/I$126</f>
+        <f t="shared" ca="1" si="40"/>
         <v>0</v>
       </c>
     </row>
     <row r="137" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J137" s="2">
-        <f ca="1">K94/I$126</f>
+        <f t="shared" ca="1" si="40"/>
         <v>0</v>
       </c>
     </row>
     <row r="138" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J138" s="2">
-        <f ca="1">K95/I$126</f>
+        <f t="shared" ca="1" si="40"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated LV to work with 11 decimal bits
</commit_message>
<xml_diff>
--- a/other/LinearVisualizer.xlsx
+++ b/other/LinearVisualizer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\CCHW\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D0BBD0-379B-49F3-AFF3-2C2BB0C5A201}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009C1BE5-C8E6-4B7D-ABF3-BFE4CA678746}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9DBF0F91-83D7-4F64-B04C-B7CB81DC62EF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9DBF0F91-83D7-4F64-B04C-B7CB81DC62EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -372,7 +372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -396,6 +396,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -712,8 +713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A6626A4-8C87-4B90-BEEB-AEB487ACEA9E}">
   <dimension ref="A2:Y138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H94" sqref="H94"/>
+    <sheetView tabSelected="1" topLeftCell="C91" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -796,35 +797,35 @@
       </c>
       <c r="D26" s="2" t="str">
         <f t="shared" ref="D26:D37" ca="1" si="0">_xlfn.CONCAT(B$40+B$41,"'b",REPT("0",B$40-LEN(E26)))</f>
-        <v>16'b000</v>
+        <v>16'b0000</v>
       </c>
       <c r="E26" s="2" t="str">
         <f ca="1">DEC2BIN(_xlfn.FLOOR.MATH(RAND()*10))</f>
-        <v>101</v>
+        <v>1</v>
       </c>
       <c r="F26" s="2" t="str">
         <f t="shared" ref="F26:F37" si="1">_xlfn.CONCAT(REPT("0",B$41),";")</f>
-        <v>0000000000;</v>
+        <v>00000000000;</v>
       </c>
       <c r="G26" s="4" t="str">
         <f ca="1">_xlfn.CONCAT(A26,B26,C26,D26,E26,F26)</f>
-        <v xml:space="preserve">            noteAmplitudes_i[ 0] = 16'b0001010000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 0] = 16'b0000100000000000;</v>
       </c>
       <c r="H26" s="2">
         <f t="shared" ref="H26:H37" ca="1" si="2">BIN2DEC(E26)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I26" s="2">
         <f t="shared" ref="I26:I37" ca="1" si="3">H26*2^B$41</f>
-        <v>5120</v>
+        <v>2048</v>
       </c>
       <c r="J26" s="2">
         <f ca="1">SUM(H26:H37)</f>
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="K26" s="2">
         <f t="shared" ref="K26:K37" ca="1" si="4">I26-J$31</f>
-        <v>-286</v>
+        <v>-10047</v>
       </c>
       <c r="L26" s="2">
         <f ca="1">IF(K26&gt;0,K26,0)</f>
@@ -851,31 +852,31 @@
       </c>
       <c r="E27" s="2" t="str">
         <f t="shared" ref="E27:E37" ca="1" si="5">DEC2BIN(_xlfn.FLOOR.MATH(RAND()*10))</f>
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F27" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0000000000;</v>
+        <v>00000000000;</v>
       </c>
       <c r="G27" s="4" t="str">
         <f t="shared" ref="G27:G37" ca="1" si="6">_xlfn.CONCAT(A27,B27,C27,D27,E27,F27)</f>
-        <v xml:space="preserve">            noteAmplitudes_i[ 1] = 16'b0000110000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 1] = 16'b0000100000000000;</v>
       </c>
       <c r="H27" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I27" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>3072</v>
+        <v>2048</v>
       </c>
       <c r="J27" s="2">
         <f ca="1">J26*2^B41</f>
-        <v>54272</v>
+        <v>120832</v>
       </c>
       <c r="K27" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>-2334</v>
+        <v>-10047</v>
       </c>
       <c r="L27" s="2">
         <f t="shared" ref="L27:L37" ca="1" si="7">IF(K27&gt;0,K27,0)</f>
@@ -902,35 +903,35 @@
       </c>
       <c r="E28" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>1000</v>
+        <v>101</v>
       </c>
       <c r="F28" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0000000000;</v>
+        <v>00000000000;</v>
       </c>
       <c r="G28" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 2] = 16'b0010000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 2] = 16'b0010100000000000;</v>
       </c>
       <c r="H28" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I28" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>8192</v>
+        <v>10240</v>
       </c>
       <c r="K28" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>2786</v>
+        <v>-1855</v>
       </c>
       <c r="L28" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>2786</v>
+        <v>0</v>
       </c>
       <c r="M28" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>8192</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
@@ -945,42 +946,42 @@
       </c>
       <c r="D29" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16'b000</v>
+        <v>16'b00</v>
       </c>
       <c r="E29" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="F29" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0000000000;</v>
+        <v>00000000000;</v>
       </c>
       <c r="G29" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 3] = 16'b0001010000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 3] = 16'b0011000000000000;</v>
       </c>
       <c r="H29" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I29" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>5120</v>
+        <v>12288</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>8</v>
       </c>
       <c r="K29" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>-286</v>
+        <v>193</v>
       </c>
       <c r="L29" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>193</v>
       </c>
       <c r="M29" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>12288</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
@@ -995,43 +996,43 @@
       </c>
       <c r="D30" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16'b00</v>
+        <v>16'b0000</v>
       </c>
       <c r="E30" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="F30" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0000000000;</v>
+        <v>00000000000;</v>
       </c>
       <c r="G30" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 4] = 16'b0010000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 4] = 16'b0000100000000000;</v>
       </c>
       <c r="H30" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="I30" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>8192</v>
+        <v>2048</v>
       </c>
       <c r="J30" s="3">
         <f ca="1">J26*B42</f>
-        <v>5.279296875</v>
+        <v>5.876953125</v>
       </c>
       <c r="K30" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>2786</v>
+        <v>-10047</v>
       </c>
       <c r="L30" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>2786</v>
+        <v>0</v>
       </c>
       <c r="M30" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>8192</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
@@ -1046,43 +1047,43 @@
       </c>
       <c r="D31" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16'b00000</v>
+        <v>16'b0</v>
       </c>
       <c r="E31" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="F31" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0000000000;</v>
+        <v>00000000000;</v>
       </c>
       <c r="G31" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 5] = 16'b0000000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 5] = 16'b0100000000000000;</v>
       </c>
       <c r="H31" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I31" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>16384</v>
       </c>
       <c r="J31" s="2">
         <f ca="1">J27 * BIN2DEC(C42) / 2^B41</f>
-        <v>5406</v>
+        <v>12095</v>
       </c>
       <c r="K31" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>-5406</v>
+        <v>4289</v>
       </c>
       <c r="L31" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>4289</v>
       </c>
       <c r="M31" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>16384</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
@@ -1097,39 +1098,39 @@
       </c>
       <c r="D32" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16'b0000</v>
+        <v>16'b0</v>
       </c>
       <c r="E32" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>11</v>
+        <v>1000</v>
       </c>
       <c r="F32" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0000000000;</v>
+        <v>00000000000;</v>
       </c>
       <c r="G32" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 6] = 16'b0000110000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 6] = 16'b0100000000000000;</v>
       </c>
       <c r="H32" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="I32" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>3072</v>
+        <v>16384</v>
       </c>
       <c r="K32" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>-2334</v>
+        <v>4289</v>
       </c>
       <c r="L32" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>4289</v>
       </c>
       <c r="M32" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>16384</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
@@ -1144,42 +1145,42 @@
       </c>
       <c r="D33" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16'b00</v>
+        <v>16'b0</v>
       </c>
       <c r="E33" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="F33" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0000000000;</v>
+        <v>00000000000;</v>
       </c>
       <c r="G33" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 7] = 16'b0010010000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 7] = 16'b0100000000000000;</v>
       </c>
       <c r="H33" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I33" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>9216</v>
+        <v>16384</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>13</v>
       </c>
       <c r="K33" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>3810</v>
+        <v>4289</v>
       </c>
       <c r="L33" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>3810</v>
+        <v>4289</v>
       </c>
       <c r="M33" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>9216</v>
+        <v>16384</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
@@ -1194,43 +1195,43 @@
       </c>
       <c r="D34" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16'b0000</v>
+        <v>16'b00</v>
       </c>
       <c r="E34" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>11</v>
+        <v>110</v>
       </c>
       <c r="F34" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0000000000;</v>
+        <v>00000000000;</v>
       </c>
       <c r="G34" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 8] = 16'b0000110000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 8] = 16'b0011000000000000;</v>
       </c>
       <c r="H34" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I34" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>3072</v>
+        <v>12288</v>
       </c>
       <c r="J34" s="2">
         <f ca="1">J35/2^B41</f>
-        <v>9.162109375</v>
+        <v>7.65966796875</v>
       </c>
       <c r="K34" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>-2334</v>
+        <v>193</v>
       </c>
       <c r="L34" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>193</v>
       </c>
       <c r="M34" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>12288</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
@@ -1245,43 +1246,43 @@
       </c>
       <c r="D35" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16'b00000</v>
+        <v>16'b00</v>
       </c>
       <c r="E35" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="F35" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0000000000;</v>
+        <v>00000000000;</v>
       </c>
       <c r="G35" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 9] = 16'b0000010000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 9] = 16'b0011100000000000;</v>
       </c>
       <c r="H35" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I35" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>1024</v>
+        <v>14336</v>
       </c>
       <c r="J35" s="2">
         <f ca="1">SUM(L26:L37)</f>
-        <v>9382</v>
+        <v>15687</v>
       </c>
       <c r="K35" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>-4382</v>
+        <v>2241</v>
       </c>
       <c r="L35" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>2241</v>
       </c>
       <c r="M35" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>14336</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
@@ -1296,31 +1297,31 @@
       </c>
       <c r="D36" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16'b0000</v>
+        <v>16'b000</v>
       </c>
       <c r="E36" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F36" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0000000000;</v>
+        <v>00000000000;</v>
       </c>
       <c r="G36" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[10] = 16'b0000110000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[10] = 16'b0001000000000000;</v>
       </c>
       <c r="H36" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I36" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>3072</v>
+        <v>4096</v>
       </c>
       <c r="K36" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>-2334</v>
+        <v>-7999</v>
       </c>
       <c r="L36" s="2">
         <f t="shared" ca="1" si="7"/>
@@ -1343,39 +1344,39 @@
       </c>
       <c r="D37" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16'b000</v>
+        <v>16'b00</v>
       </c>
       <c r="E37" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="F37" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0000000000;</v>
+        <v>00000000000;</v>
       </c>
       <c r="G37" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[11] = 16'b0001010000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[11] = 16'b0011000000000000;</v>
       </c>
       <c r="H37" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I37" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>5120</v>
+        <v>12288</v>
       </c>
       <c r="K37" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>-286</v>
+        <v>193</v>
       </c>
       <c r="L37" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>193</v>
       </c>
       <c r="M37" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>12288</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
@@ -1395,7 +1396,7 @@
         <v>0</v>
       </c>
       <c r="B40" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C40" s="8"/>
       <c r="J40" s="2" t="s">
@@ -1413,32 +1414,32 @@
         <v>1</v>
       </c>
       <c r="B41" s="8">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C41" s="8"/>
       <c r="G41" s="4" t="str">
         <f ca="1">_xlfn.CONCAT("notePosition_i = 10'b",REPT(0,B41-LEN(_xlfn.BASE(I41,2))),_xlfn.BASE(I41,2),";" )</f>
-        <v>notePosition_i = 10'b0000010011;</v>
+        <v>notePosition_i = 10'b01111011000;</v>
       </c>
       <c r="H41" s="2">
         <f ca="1">I41/2^10</f>
-        <v>1.85546875E-2</v>
+        <v>0.9609375</v>
       </c>
       <c r="I41" s="2">
         <f ca="1">RANDBETWEEN(0,1023)</f>
-        <v>19</v>
+        <v>984</v>
       </c>
       <c r="J41" s="2">
         <f ca="1">I41*24</f>
-        <v>456</v>
+        <v>23616</v>
       </c>
       <c r="K41" s="2">
         <f ca="1">IF(J45=3,24576-J41,8192-J41)</f>
-        <v>7736</v>
+        <v>960</v>
       </c>
       <c r="L41" s="2">
         <f ca="1">IF(J45=3,K47+170, K47)</f>
-        <v>40</v>
+        <v>177</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
@@ -1449,7 +1450,7 @@
         <v>9.9609375E-2</v>
       </c>
       <c r="C42" s="10">
-        <v>1100110</v>
+        <v>11001101</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
@@ -1470,25 +1471,25 @@
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E44" s="8">
         <f>_xlfn.FLOOR.MATH(IMLOG2(G44))</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F44" s="8" t="s">
         <v>18</v>
       </c>
       <c r="G44" s="11">
-        <v>21824</v>
+        <v>43648</v>
       </c>
       <c r="H44" s="2">
         <f ca="1">IF(J$45=1,G44,1)</f>
-        <v>21824</v>
+        <v>1</v>
       </c>
       <c r="J44" s="2" t="str">
         <f ca="1">_xlfn.CONCAT(REPT(0,3-LEN(DEC2BIN(2^_xlfn.FLOOR.MATH((J41+1)/8192)))),DEC2BIN(2^_xlfn.FLOOR.MATH((J41+1)/8192)))</f>
-        <v>001</v>
+        <v>100</v>
       </c>
       <c r="K44" s="2">
         <f ca="1">K41*H44*H45*H46</f>
-        <v>168830464</v>
+        <v>125706240</v>
       </c>
       <c r="L44" s="2" t="s">
         <v>24</v>
@@ -1497,13 +1498,13 @@
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E45" s="8">
         <f>_xlfn.FLOOR.MATH(IMLOG2(G45))</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F45" s="8" t="s">
         <v>19</v>
       </c>
       <c r="G45" s="11">
-        <v>43648</v>
+        <v>87296</v>
       </c>
       <c r="H45" s="2">
         <f ca="1">IF(J$45=2,G45,1)</f>
@@ -1511,31 +1512,31 @@
       </c>
       <c r="J45" s="2">
         <f ca="1">LEN(DEC2BIN(2^_xlfn.FLOOR.MATH((J41+1)/8192)))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K45" s="2" t="str">
         <f ca="1">_xlfn.BASE(K44,2,32)</f>
-        <v>00001010000100000010011000000000</v>
+        <v>00000111011111100010000000000000</v>
       </c>
       <c r="L45" s="2">
         <f ca="1">MOD(IF(L41&lt;0,L41+1023,L41), 1024)</f>
-        <v>40</v>
+        <v>177</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E46" s="8">
         <f>_xlfn.FLOOR.MATH(IMLOG2(G46))</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F46" s="8" t="s">
         <v>20</v>
       </c>
       <c r="G46" s="11">
-        <v>65472</v>
+        <v>130944</v>
       </c>
       <c r="H46" s="2">
         <f ca="1">IF(J$45=3,G46,1)</f>
-        <v>1</v>
+        <v>130944</v>
       </c>
       <c r="K46" s="2" t="s">
         <v>21</v>
@@ -1544,21 +1545,21 @@
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K47" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(K44/2^(B41+B41+C39-3))</f>
-        <v>40</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G50" s="4" t="str">
         <f ca="1">_xlfn.CONCAT("        noteAmplitude_i = 10'b",REPT(0,B41-LEN(_xlfn.BASE(I50,2))),_xlfn.BASE(I50,2),";" )</f>
-        <v xml:space="preserve">        noteAmplitude_i = 10'b1101101011;</v>
+        <v xml:space="preserve">        noteAmplitude_i = 10'b00010010110;</v>
       </c>
       <c r="H50" s="2">
         <f ca="1">I50/2^10</f>
-        <v>0.8544921875</v>
+        <v>0.146484375</v>
       </c>
       <c r="I50" s="2">
         <f ca="1">RANDBETWEEN(0,1023)</f>
-        <v>875</v>
+        <v>150</v>
       </c>
       <c r="J50" s="2" t="s">
         <v>28</v>
@@ -1582,43 +1583,43 @@
     <row r="51" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B51" s="2">
         <f>LEN(C42)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C51" s="2">
         <f>2^B51</f>
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="G51" s="4" t="str">
         <f ca="1">_xlfn.CONCAT("        noteAmplitudeFast_i = 10'b",REPT(0,B41-LEN(_xlfn.BASE(I51,2))),_xlfn.BASE(I51,2),";" )</f>
-        <v xml:space="preserve">        noteAmplitudeFast_i = 10'b1100100000;</v>
+        <v xml:space="preserve">        noteAmplitudeFast_i = 10'b00101010011;</v>
       </c>
       <c r="H51" s="2">
         <f t="shared" ref="H51:H52" ca="1" si="9">I51/2^10</f>
-        <v>0.78125</v>
+        <v>0.3310546875</v>
       </c>
       <c r="I51" s="2">
         <f ca="1">RANDBETWEEN(0,1023)</f>
-        <v>800</v>
+        <v>339</v>
       </c>
       <c r="J51" s="2">
         <f ca="1">I52*E55</f>
-        <v>1380</v>
+        <v>10320</v>
       </c>
       <c r="K51" s="2">
         <f ca="1">IF(E57,I50,I51)</f>
-        <v>800</v>
+        <v>339</v>
       </c>
       <c r="L51" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(K57/2^(B41-8))</f>
-        <v>255</v>
+        <v>127</v>
       </c>
       <c r="M51" s="2">
         <f ca="1">$L$51</f>
-        <v>255</v>
+        <v>127</v>
       </c>
       <c r="N51" s="2">
         <f ca="1">$L$57</f>
-        <v>88</v>
+        <v>4</v>
       </c>
       <c r="O51" s="2">
         <f>0</f>
@@ -1626,21 +1627,21 @@
       </c>
       <c r="P51" s="2">
         <f ca="1">M51*2^16+N51*2^8+O51</f>
-        <v>16734208</v>
+        <v>8324096</v>
       </c>
     </row>
     <row r="52" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G52" s="4" t="str">
         <f ca="1">_xlfn.CONCAT("        noteHue_i = 10'b",REPT(0,B41-LEN(_xlfn.BASE(I52,2))),_xlfn.BASE(I52,2),";" )</f>
-        <v xml:space="preserve">        noteHue_i = 10'b0011100110;</v>
+        <v xml:space="preserve">        noteHue_i = 10'b01101011100;</v>
       </c>
       <c r="H52" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>0.224609375</v>
+        <v>0.83984375</v>
       </c>
       <c r="I52" s="2">
         <f ca="1">RANDBETWEEN(0,1023)</f>
-        <v>230</v>
+        <v>860</v>
       </c>
       <c r="J52" s="2" t="s">
         <v>29</v>
@@ -1653,11 +1654,11 @@
       </c>
       <c r="M52" s="2">
         <f ca="1">$L$59</f>
-        <v>166</v>
+        <v>58</v>
       </c>
       <c r="N52" s="2">
         <f ca="1">$L$51</f>
-        <v>255</v>
+        <v>127</v>
       </c>
       <c r="O52" s="2">
         <f>0</f>
@@ -1665,21 +1666,21 @@
       </c>
       <c r="P52" s="2">
         <f t="shared" ref="P52:P57" ca="1" si="10">M52*2^16+N52*2^8+O52</f>
-        <v>10944256</v>
+        <v>3833600</v>
       </c>
     </row>
     <row r="53" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J53" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(J51/2^10)</f>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K53" s="2">
         <f ca="1">K51*E54</f>
-        <v>1310400</v>
+        <v>1110903</v>
       </c>
       <c r="L53" s="2">
         <f ca="1">K57*J55</f>
-        <v>364188</v>
+        <v>81840</v>
       </c>
       <c r="M53" s="2">
         <f>0</f>
@@ -1687,20 +1688,20 @@
       </c>
       <c r="N53" s="2">
         <f ca="1">$L$51</f>
-        <v>255</v>
+        <v>127</v>
       </c>
       <c r="O53" s="2">
         <f ca="1">$L$57</f>
-        <v>88</v>
+        <v>4</v>
       </c>
       <c r="P53" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>65368</v>
+        <v>32516</v>
       </c>
     </row>
     <row r="54" spans="2:16" x14ac:dyDescent="0.3">
       <c r="E54" s="8">
-        <v>1638</v>
+        <v>3277</v>
       </c>
       <c r="F54" s="8" t="s">
         <v>26</v>
@@ -1720,27 +1721,27 @@
       </c>
       <c r="N54" s="2">
         <f ca="1">$L$59</f>
-        <v>166</v>
+        <v>58</v>
       </c>
       <c r="O54" s="2">
         <f ca="1">$L$51</f>
-        <v>255</v>
+        <v>127</v>
       </c>
       <c r="P54" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>42751</v>
+        <v>14975</v>
       </c>
     </row>
     <row r="55" spans="2:16" x14ac:dyDescent="0.3">
       <c r="E55" s="8">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F55" s="8" t="s">
         <v>25</v>
       </c>
       <c r="J55" s="2">
         <f ca="1">MOD(J51,2^10)</f>
-        <v>356</v>
+        <v>80</v>
       </c>
       <c r="K55" s="2">
         <f ca="1">IF(_xlfn.FLOOR.MATH(K53/2^10) &gt; 1023, 1023, _xlfn.FLOOR.MATH(K53/2^10))</f>
@@ -1748,11 +1749,11 @@
       </c>
       <c r="L55" s="2">
         <f ca="1">K57*(1023-J55)</f>
-        <v>682341</v>
+        <v>964689</v>
       </c>
       <c r="M55" s="2">
         <f ca="1">$L$57</f>
-        <v>88</v>
+        <v>4</v>
       </c>
       <c r="N55" s="2">
         <f>0</f>
@@ -1760,16 +1761,16 @@
       </c>
       <c r="O55" s="2">
         <f ca="1">$L$51</f>
-        <v>255</v>
+        <v>127</v>
       </c>
       <c r="P55" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>5767423</v>
+        <v>262271</v>
       </c>
     </row>
     <row r="56" spans="2:16" x14ac:dyDescent="0.3">
       <c r="E56" s="8">
-        <v>1023</v>
+        <v>2047</v>
       </c>
       <c r="F56" s="8" t="s">
         <v>27</v>
@@ -1782,7 +1783,7 @@
       </c>
       <c r="M56" s="2">
         <f ca="1">$L$51</f>
-        <v>255</v>
+        <v>127</v>
       </c>
       <c r="N56" s="2">
         <f>0</f>
@@ -1790,11 +1791,11 @@
       </c>
       <c r="O56" s="2">
         <f ca="1">$L$59</f>
-        <v>166</v>
+        <v>58</v>
       </c>
       <c r="P56" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>16711846</v>
+        <v>8323130</v>
       </c>
     </row>
     <row r="57" spans="2:16" x14ac:dyDescent="0.3">
@@ -1810,15 +1811,15 @@
       </c>
       <c r="L57" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(L53/2^(2*B41-8))</f>
-        <v>88</v>
+        <v>4</v>
       </c>
       <c r="M57" s="2">
         <f ca="1">$L$51</f>
-        <v>255</v>
+        <v>127</v>
       </c>
       <c r="N57" s="2">
         <f ca="1">$L$57</f>
-        <v>88</v>
+        <v>4</v>
       </c>
       <c r="O57" s="2">
         <f>0</f>
@@ -1826,7 +1827,7 @@
       </c>
       <c r="P57" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>16734208</v>
+        <v>8324096</v>
       </c>
     </row>
     <row r="58" spans="2:16" x14ac:dyDescent="0.3">
@@ -1840,11 +1841,11 @@
     <row r="59" spans="2:16" x14ac:dyDescent="0.3">
       <c r="L59" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(L55/2^(2*B41-8))</f>
-        <v>166</v>
-      </c>
-      <c r="M59" s="2" t="str" cm="1">
+        <v>58</v>
+      </c>
+      <c r="M59" s="2" t="e" cm="1">
         <f t="array" aca="1" ref="M59" ca="1">_xlfn.BASE(_xlfn.SWITCH(J53,0,P51,1,P52,2,P53,3,P54,4,P55,5,P56,6,P57),16,6)</f>
-        <v>A6FF00</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="60" spans="2:16" x14ac:dyDescent="0.3">
@@ -1871,7 +1872,7 @@
       </c>
       <c r="I63" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(H76/B43)</f>
-        <v>187</v>
+        <v>313</v>
       </c>
       <c r="J63" s="2">
         <f t="shared" ref="J63:J74" ca="1" si="12">_xlfn.FLOOR.MATH(H63/I$63)</f>
@@ -1879,7 +1880,7 @@
       </c>
       <c r="L63" s="2">
         <f ca="1">L51-L57-L59</f>
-        <v>1</v>
+        <v>65</v>
       </c>
     </row>
     <row r="64" spans="2:16" x14ac:dyDescent="0.3">
@@ -1899,25 +1900,25 @@
     <row r="65" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G65" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 2] = 16'b0000101011100010;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 2] = 16'b0000000000000000;</v>
       </c>
       <c r="H65" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>2786</v>
+        <v>0</v>
       </c>
       <c r="J65" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G66" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 3] = 16'b0000000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 3] = 16'b0000000011000001;</v>
       </c>
       <c r="H66" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>193</v>
       </c>
       <c r="J66" s="2">
         <f t="shared" ca="1" si="12"/>
@@ -1927,67 +1928,67 @@
     <row r="67" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G67" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 4] = 16'b0000101011100010;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 4] = 16'b0000000000000000;</v>
       </c>
       <c r="H67" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>2786</v>
+        <v>0</v>
       </c>
       <c r="J67" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G68" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 5] = 16'b0000000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 5] = 16'b0001000011000001;</v>
       </c>
       <c r="H68" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>4289</v>
       </c>
       <c r="J68" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G69" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 6] = 16'b0000000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 6] = 16'b0001000011000001;</v>
       </c>
       <c r="H69" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>4289</v>
       </c>
       <c r="J69" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="70" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G70" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 7] = 16'b0000111011100010;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 7] = 16'b0001000011000001;</v>
       </c>
       <c r="H70" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>3810</v>
+        <v>4289</v>
       </c>
       <c r="J70" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="71" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G71" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 8] = 16'b0000000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 8] = 16'b0000000011000001;</v>
       </c>
       <c r="H71" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>193</v>
       </c>
       <c r="J71" s="2">
         <f t="shared" ca="1" si="12"/>
@@ -1997,15 +1998,15 @@
     <row r="72" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G72" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 9] = 16'b0000000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 9] = 16'b0000100011000001;</v>
       </c>
       <c r="H72" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>2241</v>
       </c>
       <c r="J72" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="73" spans="1:25" x14ac:dyDescent="0.3">
@@ -2025,11 +2026,11 @@
     <row r="74" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G74" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[11] = 16'b0000000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[11] = 16'b0000000011000001;</v>
       </c>
       <c r="H74" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>193</v>
       </c>
       <c r="J74" s="2">
         <f t="shared" ca="1" si="12"/>
@@ -2039,7 +2040,7 @@
     <row r="75" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G75" s="5" t="str">
         <f ca="1">_xlfn.CONCAT("            amplitudeSumNew_i = ",B40+B41+_xlfn.CEILING.MATH(IMLOG2(B43)),"'b",_xlfn.BASE(H76,2,B40+B41+_xlfn.CEILING.MATH(IMLOG2(B43))),";")</f>
-        <v xml:space="preserve">            amplitudeSumNew_i = 22'b0000000010010010100110;</v>
+        <v xml:space="preserve">            amplitudeSumNew_i = 22'b0000000011110101000111;</v>
       </c>
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.3">
@@ -2048,7 +2049,7 @@
       </c>
       <c r="H76" s="2">
         <f ca="1">SUM(H63:H74)</f>
-        <v>9382</v>
+        <v>15687</v>
       </c>
     </row>
     <row r="78" spans="1:25" x14ac:dyDescent="0.3">
@@ -2152,7 +2153,7 @@
     <row r="83" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F83" s="2">
         <f t="shared" ref="F83:F94" ca="1" si="14">H83/2^B$41</f>
-        <v>0.5859375</v>
+        <v>0.29296875</v>
       </c>
       <c r="G83" s="6" t="s">
         <v>60</v>
@@ -2166,11 +2167,11 @@
       </c>
       <c r="J83" s="2">
         <f t="shared" ref="J83:J94" ca="1" si="15">H83-I$87</f>
-        <v>423.990234375</v>
+        <v>423.12744140625</v>
       </c>
       <c r="K83" s="2">
         <f ca="1">IF(J83&lt;0, 0, J83)</f>
-        <v>423.990234375</v>
+        <v>423.12744140625</v>
       </c>
       <c r="L83" s="2">
         <f ca="1">IF(K83=0,0,H83)</f>
@@ -2180,7 +2181,7 @@
     <row r="84" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F84" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>0.7001953125</v>
+        <v>0.35009765625</v>
       </c>
       <c r="G84" s="6" t="s">
         <v>61</v>
@@ -2195,11 +2196,11 @@
       </c>
       <c r="J84" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>540.990234375</v>
+        <v>540.12744140625</v>
       </c>
       <c r="K84" s="2">
         <f t="shared" ref="K84:K94" ca="1" si="16">IF(J84&lt;0, 0, J84)</f>
-        <v>540.990234375</v>
+        <v>540.12744140625</v>
       </c>
       <c r="L84" s="2">
         <f t="shared" ref="L84:L94" ca="1" si="17">IF(K84=0,0,H84)</f>
@@ -2209,7 +2210,7 @@
     <row r="85" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F85" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>0.439453125</v>
+        <v>0.2197265625</v>
       </c>
       <c r="G85" s="6" t="s">
         <v>62</v>
@@ -2220,15 +2221,15 @@
       </c>
       <c r="I85" s="2">
         <f ca="1">I84/2^B41</f>
-        <v>1.7255859375</v>
+        <v>0.86279296875</v>
       </c>
       <c r="J85" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>273.990234375</v>
+        <v>273.12744140625</v>
       </c>
       <c r="K85" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>273.990234375</v>
+        <v>273.12744140625</v>
       </c>
       <c r="L85" s="2">
         <f t="shared" ca="1" si="17"/>
@@ -2252,7 +2253,7 @@
       </c>
       <c r="J86" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>-176.009765625</v>
+        <v>-176.87255859375</v>
       </c>
       <c r="K86" s="2">
         <f t="shared" ca="1" si="16"/>
@@ -2277,11 +2278,11 @@
       </c>
       <c r="I87" s="2">
         <f ca="1">I84*BIN2DEC(C42)/2^B41</f>
-        <v>176.009765625</v>
+        <v>176.87255859375</v>
       </c>
       <c r="J87" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>-176.009765625</v>
+        <v>-176.87255859375</v>
       </c>
       <c r="K87" s="2">
         <f t="shared" ca="1" si="16"/>
@@ -2306,11 +2307,11 @@
       </c>
       <c r="I88" s="2">
         <f ca="1">I85*B42</f>
-        <v>0.17188453674316406</v>
+        <v>8.5942268371582031E-2</v>
       </c>
       <c r="J88" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>-176.009765625</v>
+        <v>-176.87255859375</v>
       </c>
       <c r="K88" s="2">
         <f t="shared" ca="1" si="16"/>
@@ -2338,7 +2339,7 @@
       </c>
       <c r="J89" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>-176.009765625</v>
+        <v>-176.87255859375</v>
       </c>
       <c r="K89" s="2">
         <f t="shared" ca="1" si="16"/>
@@ -2363,11 +2364,11 @@
       </c>
       <c r="I90" s="2">
         <f ca="1">SUM(K83:K94)</f>
-        <v>1238.970703125</v>
+        <v>1236.38232421875</v>
       </c>
       <c r="J90" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>-176.009765625</v>
+        <v>-176.87255859375</v>
       </c>
       <c r="K90" s="2">
         <f t="shared" ca="1" si="16"/>
@@ -2392,7 +2393,7 @@
       </c>
       <c r="J91" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>-176.009765625</v>
+        <v>-176.87255859375</v>
       </c>
       <c r="K91" s="2">
         <f t="shared" ca="1" si="16"/>
@@ -2401,6 +2402,10 @@
       <c r="L91" s="2">
         <f t="shared" ca="1" si="17"/>
         <v>0</v>
+      </c>
+      <c r="N91" s="2">
+        <f ca="1">K98/2^11</f>
+        <v>-4.048828125</v>
       </c>
     </row>
     <row r="92" spans="6:15" x14ac:dyDescent="0.3">
@@ -2417,7 +2422,7 @@
       </c>
       <c r="J92" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>-176.009765625</v>
+        <v>-176.87255859375</v>
       </c>
       <c r="K92" s="2">
         <f t="shared" ca="1" si="16"/>
@@ -2442,7 +2447,7 @@
       </c>
       <c r="J93" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>-176.009765625</v>
+        <v>-176.87255859375</v>
       </c>
       <c r="K93" s="2">
         <f t="shared" ca="1" si="16"/>
@@ -2467,7 +2472,7 @@
       </c>
       <c r="J94" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>-176.009765625</v>
+        <v>-176.87255859375</v>
       </c>
       <c r="K94" s="2">
         <f t="shared" ca="1" si="16"/>
@@ -2504,10 +2509,10 @@
         <v>66</v>
       </c>
     </row>
-    <row r="97" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="97" spans="5:25" x14ac:dyDescent="0.3">
       <c r="F97" s="2">
         <f ca="1">H97/2^B$41</f>
-        <v>47.97265625</v>
+        <v>23.986328125</v>
       </c>
       <c r="G97" s="6" t="s">
         <v>76</v>
@@ -2517,46 +2522,46 @@
         <v>49124</v>
       </c>
       <c r="I97" s="2">
-        <f t="shared" ref="I97:I108" ca="1" si="18">H97*B$39</f>
-        <v>1178976</v>
-      </c>
-      <c r="J97" s="2" t="e">
-        <f ca="1">LEN(DEC2BIN(2^_xlfn.FLOOR.MATH((I97+1)/8192)))</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="K97" s="2" t="e" cm="1">
-        <f t="array" aca="1" ref="K97" ca="1">_xlfn.SWITCH(J97,1,8*2^10 - I97, 2, 8*2^10 -I97, 3, 24*2^B$41 -I97)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L97" s="2" t="e" cm="1">
+        <f ca="1">H97</f>
+        <v>49124</v>
+      </c>
+      <c r="J97" s="2">
+        <f ca="1">IF(F97&lt;8,1,IF(F97&lt;16,2,3))</f>
+        <v>3</v>
+      </c>
+      <c r="K97" s="2" cm="1">
+        <f t="array" aca="1" ref="K97" ca="1">_xlfn.SWITCH(J97,1,8*2^B$41 - I97, 2, 8*2^B$41 -I97, 3, 24*2^B$41 -I97)</f>
+        <v>28</v>
+      </c>
+      <c r="L97" s="2" cm="1">
         <f t="array" aca="1" ref="L97" ca="1">_xlfn.SWITCH(J97,1,K97*G$44, 2, K97*G$45, 3, K97*G$46)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M97" s="2" t="e">
-        <f t="shared" ref="M97:M108" ca="1" si="19">_xlfn.FLOOR.MATH(L97/2^(B$41+B$41))</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N97" s="2" t="e">
+        <v>3666432</v>
+      </c>
+      <c r="M97" s="2">
+        <f t="shared" ref="M97:M109" ca="1" si="18">_xlfn.FLOOR.MATH(L97/2^(B$41+B$41))</f>
+        <v>0</v>
+      </c>
+      <c r="N97" s="2">
         <f ca="1">IF(J97=3,M97+170,M97)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="O97" s="2" t="e">
+        <v>170</v>
+      </c>
+      <c r="O97" s="2">
         <f ca="1">MOD(N97,1024)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="P97" s="2" t="e">
-        <f t="shared" ref="P97:P108" ca="1" si="20">O97/2^B$41</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="Q97" s="2" t="e">
+        <v>170</v>
+      </c>
+      <c r="P97" s="2">
+        <f ca="1">O97/2^(B$41-1)</f>
+        <v>0.166015625</v>
+      </c>
+      <c r="Q97" s="13">
         <f ca="1">P97*360</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="98" spans="6:25" x14ac:dyDescent="0.3">
+        <v>59.765625</v>
+      </c>
+    </row>
+    <row r="98" spans="5:25" x14ac:dyDescent="0.3">
       <c r="F98" s="2">
-        <f t="shared" ref="F97:F108" ca="1" si="21">H98/2^B$41</f>
-        <v>24.09765625</v>
+        <f t="shared" ref="F98:F109" ca="1" si="19">H98/2^B$41</f>
+        <v>12.048828125</v>
       </c>
       <c r="G98" s="6" t="s">
         <v>77</v>
@@ -2566,46 +2571,46 @@
         <v>24676</v>
       </c>
       <c r="I98" s="2">
+        <f t="shared" ref="I98:I109" ca="1" si="20">H98</f>
+        <v>24676</v>
+      </c>
+      <c r="J98" s="2">
+        <f t="shared" ref="J98:J109" ca="1" si="21">IF(F98&lt;8,1,IF(F98&lt;16,2,3))</f>
+        <v>2</v>
+      </c>
+      <c r="K98" s="2" cm="1">
+        <f t="array" aca="1" ref="K98" ca="1">_xlfn.SWITCH(J98,1,8*2^B$41 - I98, 2, 8*2^B$41 -I98, 3, 24*2^B$41 -I98)</f>
+        <v>-8292</v>
+      </c>
+      <c r="L98" s="2" cm="1">
+        <f t="array" aca="1" ref="L98" ca="1">_xlfn.SWITCH(J98,1,K98*G$44, 2, K98*G$45, 3, K98*G$46)</f>
+        <v>-723858432</v>
+      </c>
+      <c r="M98" s="2">
         <f t="shared" ca="1" si="18"/>
-        <v>592224</v>
-      </c>
-      <c r="J98" s="2" t="e">
-        <f t="shared" ref="J98:J108" ca="1" si="22">LEN(DEC2BIN(2^_xlfn.FLOOR.MATH((I98+1)/8192)))</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="K98" s="2" t="e" cm="1">
-        <f t="array" aca="1" ref="K98" ca="1">_xlfn.SWITCH(J98,1,8*2^10 - I98, 2, 8*2^10 -I98, 3, 24*2^B$41 -I98)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L98" s="2" t="e" cm="1">
-        <f t="array" aca="1" ref="L98" ca="1">_xlfn.SWITCH(J98,1,K98*G$44, 2, K98*G$45, 3, K98*G$46)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M98" s="2" t="e">
+        <v>-173</v>
+      </c>
+      <c r="N98" s="2">
+        <f t="shared" ref="N98:N109" ca="1" si="22">IF(J98=3,M98+170,M98)</f>
+        <v>-173</v>
+      </c>
+      <c r="O98" s="2">
+        <f t="shared" ref="O98:O108" ca="1" si="23">MOD(N98,1024)</f>
+        <v>851</v>
+      </c>
+      <c r="P98" s="2">
+        <f t="shared" ref="P98:P109" ca="1" si="24">O98/2^(B$41-1)</f>
+        <v>0.8310546875</v>
+      </c>
+      <c r="Q98" s="13">
+        <f t="shared" ref="Q98:Q109" ca="1" si="25">P98*360</f>
+        <v>299.1796875</v>
+      </c>
+    </row>
+    <row r="99" spans="5:25" x14ac:dyDescent="0.3">
+      <c r="F99" s="2">
         <f t="shared" ca="1" si="19"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N98" s="2" t="e">
-        <f t="shared" ref="N98:N108" ca="1" si="23">IF(J98=3,M98+170,M98)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="O98" s="2" t="e">
-        <f t="shared" ref="O98:O108" ca="1" si="24">MOD(N98,1024)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="P98" s="2" t="e">
-        <f t="shared" ca="1" si="20"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="Q98" s="2" t="e">
-        <f t="shared" ref="Q98:Q108" ca="1" si="25">P98*360</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="99" spans="6:25" x14ac:dyDescent="0.3">
-      <c r="F99" s="2">
-        <f t="shared" ca="1" si="21"/>
-        <v>39.97265625</v>
+        <v>19.986328125</v>
       </c>
       <c r="G99" s="6" t="s">
         <v>78</v>
@@ -2615,46 +2620,46 @@
         <v>40932</v>
       </c>
       <c r="I99" s="2">
+        <f t="shared" ca="1" si="20"/>
+        <v>40932</v>
+      </c>
+      <c r="J99" s="2">
+        <f t="shared" ca="1" si="21"/>
+        <v>3</v>
+      </c>
+      <c r="K99" s="2" cm="1">
+        <f t="array" aca="1" ref="K99" ca="1">_xlfn.SWITCH(J99,1,8*2^B$41 - I99, 2, 8*2^B$41 -I99, 3, 24*2^B$41 -I99)</f>
+        <v>8220</v>
+      </c>
+      <c r="L99" s="2" cm="1">
+        <f t="array" aca="1" ref="L99" ca="1">_xlfn.SWITCH(J99,1,K99*G$44, 2, K99*G$45, 3, K99*G$46)</f>
+        <v>1076359680</v>
+      </c>
+      <c r="M99" s="2">
         <f t="shared" ca="1" si="18"/>
-        <v>982368</v>
-      </c>
-      <c r="J99" s="2" t="e">
+        <v>256</v>
+      </c>
+      <c r="N99" s="2">
         <f t="shared" ca="1" si="22"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="K99" s="2" t="e" cm="1">
-        <f t="array" aca="1" ref="K99" ca="1">_xlfn.SWITCH(J99,1,8*2^10 - I99, 2, 8*2^10 -I99, 3, 24*2^B$41 -I99)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L99" s="2" t="e" cm="1">
-        <f t="array" aca="1" ref="L99" ca="1">_xlfn.SWITCH(J99,1,K99*G$44, 2, K99*G$45, 3, K99*G$46)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M99" s="2" t="e">
+        <v>426</v>
+      </c>
+      <c r="O99" s="2">
+        <f t="shared" ca="1" si="23"/>
+        <v>426</v>
+      </c>
+      <c r="P99" s="2">
+        <f t="shared" ca="1" si="24"/>
+        <v>0.416015625</v>
+      </c>
+      <c r="Q99" s="13">
+        <f t="shared" ca="1" si="25"/>
+        <v>149.765625</v>
+      </c>
+    </row>
+    <row r="100" spans="5:25" x14ac:dyDescent="0.3">
+      <c r="F100" s="2">
         <f t="shared" ca="1" si="19"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N99" s="2" t="e">
-        <f t="shared" ca="1" si="23"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="O99" s="2" t="e">
-        <f t="shared" ca="1" si="24"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="P99" s="2" t="e">
-        <f t="shared" ca="1" si="20"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="Q99" s="2" t="e">
-        <f t="shared" ca="1" si="25"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="100" spans="6:25" x14ac:dyDescent="0.3">
-      <c r="F100" s="2">
-        <f t="shared" ca="1" si="21"/>
-        <v>42.09765625</v>
+        <v>21.048828125</v>
       </c>
       <c r="G100" s="6" t="s">
         <v>79</v>
@@ -2664,46 +2669,46 @@
         <v>43108</v>
       </c>
       <c r="I100" s="2">
+        <f t="shared" ca="1" si="20"/>
+        <v>43108</v>
+      </c>
+      <c r="J100" s="2">
+        <f t="shared" ca="1" si="21"/>
+        <v>3</v>
+      </c>
+      <c r="K100" s="2" cm="1">
+        <f t="array" aca="1" ref="K100" ca="1">_xlfn.SWITCH(J100,1,8*2^B$41 - I100, 2, 8*2^B$41 -I100, 3, 24*2^B$41 -I100)</f>
+        <v>6044</v>
+      </c>
+      <c r="L100" s="2" cm="1">
+        <f t="array" aca="1" ref="L100" ca="1">_xlfn.SWITCH(J100,1,K100*G$44, 2, K100*G$45, 3, K100*G$46)</f>
+        <v>791425536</v>
+      </c>
+      <c r="M100" s="2">
         <f t="shared" ca="1" si="18"/>
-        <v>1034592</v>
-      </c>
-      <c r="J100" s="2" t="e">
+        <v>188</v>
+      </c>
+      <c r="N100" s="2">
         <f t="shared" ca="1" si="22"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="K100" s="2" t="e" cm="1">
-        <f t="array" aca="1" ref="K100" ca="1">_xlfn.SWITCH(J100,1,8*2^10 - I100, 2, 8*2^10 -I100, 3, 24*2^B$41 -I100)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L100" s="2" t="e" cm="1">
-        <f t="array" aca="1" ref="L100" ca="1">_xlfn.SWITCH(J100,1,K100*G$44, 2, K100*G$45, 3, K100*G$46)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M100" s="2" t="e">
+        <v>358</v>
+      </c>
+      <c r="O100" s="2">
+        <f t="shared" ca="1" si="23"/>
+        <v>358</v>
+      </c>
+      <c r="P100" s="2">
+        <f t="shared" ca="1" si="24"/>
+        <v>0.349609375</v>
+      </c>
+      <c r="Q100" s="13">
+        <f t="shared" ca="1" si="25"/>
+        <v>125.859375</v>
+      </c>
+    </row>
+    <row r="101" spans="5:25" x14ac:dyDescent="0.3">
+      <c r="F101" s="2">
         <f t="shared" ca="1" si="19"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N100" s="2" t="e">
-        <f t="shared" ca="1" si="23"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="O100" s="2" t="e">
-        <f t="shared" ca="1" si="24"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="P100" s="2" t="e">
-        <f t="shared" ca="1" si="20"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="Q100" s="2" t="e">
-        <f t="shared" ca="1" si="25"/>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="101" spans="6:25" x14ac:dyDescent="0.3">
-      <c r="F101" s="2">
-        <f t="shared" ca="1" si="21"/>
-        <v>0.7763671875</v>
+        <v>0.38818359375</v>
       </c>
       <c r="G101" s="6" t="s">
         <v>53</v>
@@ -2713,46 +2718,46 @@
         <v>795</v>
       </c>
       <c r="I101" s="2">
-        <f t="shared" ca="1" si="18"/>
-        <v>19080</v>
+        <f t="shared" ca="1" si="20"/>
+        <v>795</v>
       </c>
       <c r="J101" s="2">
-        <f t="shared" ca="1" si="22"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="21"/>
+        <v>1</v>
       </c>
       <c r="K101" s="2" cm="1">
-        <f t="array" aca="1" ref="K101" ca="1">_xlfn.SWITCH(J101,1,8*2^10 - I101, 2, 8*2^10 -I101, 3, 24*2^B$41 -I101)</f>
-        <v>5496</v>
+        <f t="array" aca="1" ref="K101" ca="1">_xlfn.SWITCH(J101,1,8*2^B$41 - I101, 2, 8*2^B$41 -I101, 3, 24*2^B$41 -I101)</f>
+        <v>15589</v>
       </c>
       <c r="L101" s="2" cm="1">
         <f t="array" aca="1" ref="L101" ca="1">_xlfn.SWITCH(J101,1,K101*G$44, 2, K101*G$45, 3, K101*G$46)</f>
-        <v>359834112</v>
+        <v>680428672</v>
       </c>
       <c r="M101" s="2">
+        <f t="shared" ca="1" si="18"/>
+        <v>162</v>
+      </c>
+      <c r="N101" s="2">
+        <f t="shared" ca="1" si="22"/>
+        <v>162</v>
+      </c>
+      <c r="O101" s="2">
+        <f t="shared" ca="1" si="23"/>
+        <v>162</v>
+      </c>
+      <c r="P101" s="2">
+        <f t="shared" ca="1" si="24"/>
+        <v>0.158203125</v>
+      </c>
+      <c r="Q101" s="13">
+        <f t="shared" ca="1" si="25"/>
+        <v>56.953125</v>
+      </c>
+    </row>
+    <row r="102" spans="5:25" x14ac:dyDescent="0.3">
+      <c r="F102" s="2">
         <f t="shared" ca="1" si="19"/>
-        <v>343</v>
-      </c>
-      <c r="N101" s="2">
-        <f t="shared" ca="1" si="23"/>
-        <v>513</v>
-      </c>
-      <c r="O101" s="2">
-        <f t="shared" ca="1" si="24"/>
-        <v>513</v>
-      </c>
-      <c r="P101" s="2">
-        <f t="shared" ca="1" si="20"/>
-        <v>0.5009765625</v>
-      </c>
-      <c r="Q101" s="2">
-        <f t="shared" ca="1" si="25"/>
-        <v>180.3515625</v>
-      </c>
-    </row>
-    <row r="102" spans="6:25" x14ac:dyDescent="0.3">
-      <c r="F102" s="2">
-        <f t="shared" ca="1" si="21"/>
-        <v>0.638671875</v>
+        <v>0.3193359375</v>
       </c>
       <c r="G102" s="6" t="s">
         <v>54</v>
@@ -2762,46 +2767,46 @@
         <v>654</v>
       </c>
       <c r="I102" s="2">
-        <f t="shared" ca="1" si="18"/>
-        <v>15696</v>
+        <f t="shared" ca="1" si="20"/>
+        <v>654</v>
       </c>
       <c r="J102" s="2">
-        <f t="shared" ca="1" si="22"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="21"/>
+        <v>1</v>
       </c>
       <c r="K102" s="2" cm="1">
-        <f t="array" aca="1" ref="K102" ca="1">_xlfn.SWITCH(J102,1,8*2^10 - I102, 2, 8*2^10 -I102, 3, 24*2^B$41 -I102)</f>
-        <v>-7504</v>
+        <f t="array" aca="1" ref="K102" ca="1">_xlfn.SWITCH(J102,1,8*2^B$41 - I102, 2, 8*2^B$41 -I102, 3, 24*2^B$41 -I102)</f>
+        <v>15730</v>
       </c>
       <c r="L102" s="2" cm="1">
         <f t="array" aca="1" ref="L102" ca="1">_xlfn.SWITCH(J102,1,K102*G$44, 2, K102*G$45, 3, K102*G$46)</f>
-        <v>-327534592</v>
+        <v>686583040</v>
       </c>
       <c r="M102" s="2">
+        <f t="shared" ca="1" si="18"/>
+        <v>163</v>
+      </c>
+      <c r="N102" s="2">
+        <f t="shared" ca="1" si="22"/>
+        <v>163</v>
+      </c>
+      <c r="O102" s="2">
+        <f t="shared" ca="1" si="23"/>
+        <v>163</v>
+      </c>
+      <c r="P102" s="2">
+        <f t="shared" ca="1" si="24"/>
+        <v>0.1591796875</v>
+      </c>
+      <c r="Q102" s="13">
+        <f t="shared" ca="1" si="25"/>
+        <v>57.3046875</v>
+      </c>
+    </row>
+    <row r="103" spans="5:25" x14ac:dyDescent="0.3">
+      <c r="F103" s="2">
         <f t="shared" ca="1" si="19"/>
-        <v>-313</v>
-      </c>
-      <c r="N102" s="2">
-        <f t="shared" ca="1" si="23"/>
-        <v>-313</v>
-      </c>
-      <c r="O102" s="2">
-        <f t="shared" ca="1" si="24"/>
-        <v>711</v>
-      </c>
-      <c r="P102" s="2">
-        <f t="shared" ca="1" si="20"/>
-        <v>0.6943359375</v>
-      </c>
-      <c r="Q102" s="2">
-        <f t="shared" ca="1" si="25"/>
-        <v>249.9609375</v>
-      </c>
-    </row>
-    <row r="103" spans="6:25" x14ac:dyDescent="0.3">
-      <c r="F103" s="2">
-        <f t="shared" ca="1" si="21"/>
-        <v>0.3369140625</v>
+        <v>0.16845703125</v>
       </c>
       <c r="G103" s="6" t="s">
         <v>55</v>
@@ -2811,46 +2816,46 @@
         <v>345</v>
       </c>
       <c r="I103" s="2">
-        <f t="shared" ca="1" si="18"/>
-        <v>8280</v>
+        <f t="shared" ca="1" si="20"/>
+        <v>345</v>
       </c>
       <c r="J103" s="2">
-        <f t="shared" ca="1" si="22"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="21"/>
+        <v>1</v>
       </c>
       <c r="K103" s="2" cm="1">
-        <f t="array" aca="1" ref="K103" ca="1">_xlfn.SWITCH(J103,1,8*2^10 - I103, 2, 8*2^10 -I103, 3, 24*2^B$41 -I103)</f>
-        <v>-88</v>
+        <f t="array" aca="1" ref="K103" ca="1">_xlfn.SWITCH(J103,1,8*2^B$41 - I103, 2, 8*2^B$41 -I103, 3, 24*2^B$41 -I103)</f>
+        <v>16039</v>
       </c>
       <c r="L103" s="2" cm="1">
         <f t="array" aca="1" ref="L103" ca="1">_xlfn.SWITCH(J103,1,K103*G$44, 2, K103*G$45, 3, K103*G$46)</f>
-        <v>-3841024</v>
+        <v>700070272</v>
       </c>
       <c r="M103" s="2">
+        <f t="shared" ca="1" si="18"/>
+        <v>166</v>
+      </c>
+      <c r="N103" s="2">
+        <f t="shared" ca="1" si="22"/>
+        <v>166</v>
+      </c>
+      <c r="O103" s="2">
+        <f t="shared" ca="1" si="23"/>
+        <v>166</v>
+      </c>
+      <c r="P103" s="2">
+        <f t="shared" ca="1" si="24"/>
+        <v>0.162109375</v>
+      </c>
+      <c r="Q103" s="13">
+        <f t="shared" ca="1" si="25"/>
+        <v>58.359375</v>
+      </c>
+    </row>
+    <row r="104" spans="5:25" x14ac:dyDescent="0.3">
+      <c r="F104" s="2">
         <f t="shared" ca="1" si="19"/>
-        <v>-4</v>
-      </c>
-      <c r="N103" s="2">
-        <f t="shared" ca="1" si="23"/>
-        <v>-4</v>
-      </c>
-      <c r="O103" s="2">
-        <f t="shared" ca="1" si="24"/>
-        <v>1020</v>
-      </c>
-      <c r="P103" s="2">
-        <f t="shared" ca="1" si="20"/>
-        <v>0.99609375</v>
-      </c>
-      <c r="Q103" s="2">
-        <f t="shared" ca="1" si="25"/>
-        <v>358.59375</v>
-      </c>
-    </row>
-    <row r="104" spans="6:25" x14ac:dyDescent="0.3">
-      <c r="F104" s="2">
-        <f t="shared" ca="1" si="21"/>
-        <v>0.560546875</v>
+        <v>0.2802734375</v>
       </c>
       <c r="G104" s="6" t="s">
         <v>56</v>
@@ -2860,46 +2865,46 @@
         <v>574</v>
       </c>
       <c r="I104" s="2">
-        <f t="shared" ca="1" si="18"/>
-        <v>13776</v>
+        <f t="shared" ca="1" si="20"/>
+        <v>574</v>
       </c>
       <c r="J104" s="2">
-        <f t="shared" ca="1" si="22"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="21"/>
+        <v>1</v>
       </c>
       <c r="K104" s="2" cm="1">
-        <f t="array" aca="1" ref="K104" ca="1">_xlfn.SWITCH(J104,1,8*2^10 - I104, 2, 8*2^10 -I104, 3, 24*2^B$41 -I104)</f>
-        <v>-5584</v>
+        <f t="array" aca="1" ref="K104" ca="1">_xlfn.SWITCH(J104,1,8*2^B$41 - I104, 2, 8*2^B$41 -I104, 3, 24*2^B$41 -I104)</f>
+        <v>15810</v>
       </c>
       <c r="L104" s="2" cm="1">
         <f t="array" aca="1" ref="L104" ca="1">_xlfn.SWITCH(J104,1,K104*G$44, 2, K104*G$45, 3, K104*G$46)</f>
-        <v>-243730432</v>
+        <v>690074880</v>
       </c>
       <c r="M104" s="2">
+        <f t="shared" ca="1" si="18"/>
+        <v>164</v>
+      </c>
+      <c r="N104" s="2">
+        <f t="shared" ca="1" si="22"/>
+        <v>164</v>
+      </c>
+      <c r="O104" s="2">
+        <f t="shared" ca="1" si="23"/>
+        <v>164</v>
+      </c>
+      <c r="P104" s="2">
+        <f t="shared" ca="1" si="24"/>
+        <v>0.16015625</v>
+      </c>
+      <c r="Q104" s="13">
+        <f t="shared" ca="1" si="25"/>
+        <v>57.65625</v>
+      </c>
+    </row>
+    <row r="105" spans="5:25" x14ac:dyDescent="0.3">
+      <c r="F105" s="2">
         <f t="shared" ca="1" si="19"/>
-        <v>-233</v>
-      </c>
-      <c r="N104" s="2">
-        <f t="shared" ca="1" si="23"/>
-        <v>-233</v>
-      </c>
-      <c r="O104" s="2">
-        <f t="shared" ca="1" si="24"/>
-        <v>791</v>
-      </c>
-      <c r="P104" s="2">
-        <f t="shared" ca="1" si="20"/>
-        <v>0.7724609375</v>
-      </c>
-      <c r="Q104" s="2">
-        <f t="shared" ca="1" si="25"/>
-        <v>278.0859375</v>
-      </c>
-    </row>
-    <row r="105" spans="6:25" x14ac:dyDescent="0.3">
-      <c r="F105" s="2">
-        <f t="shared" ca="1" si="21"/>
-        <v>3.90625E-2</v>
+        <v>1.953125E-2</v>
       </c>
       <c r="G105" s="6" t="s">
         <v>57</v>
@@ -2909,46 +2914,46 @@
         <v>40</v>
       </c>
       <c r="I105" s="2">
-        <f t="shared" ca="1" si="18"/>
-        <v>960</v>
+        <f t="shared" ca="1" si="20"/>
+        <v>40</v>
       </c>
       <c r="J105" s="2">
-        <f t="shared" ca="1" si="22"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1</v>
       </c>
       <c r="K105" s="2" cm="1">
-        <f t="array" aca="1" ref="K105" ca="1">_xlfn.SWITCH(J105,1,8*2^10 - I105, 2, 8*2^10 -I105, 3, 24*2^B$41 -I105)</f>
-        <v>7232</v>
+        <f t="array" aca="1" ref="K105" ca="1">_xlfn.SWITCH(J105,1,8*2^B$41 - I105, 2, 8*2^B$41 -I105, 3, 24*2^B$41 -I105)</f>
+        <v>16344</v>
       </c>
       <c r="L105" s="2" cm="1">
         <f t="array" aca="1" ref="L105" ca="1">_xlfn.SWITCH(J105,1,K105*G$44, 2, K105*G$45, 3, K105*G$46)</f>
-        <v>157831168</v>
+        <v>713382912</v>
       </c>
       <c r="M105" s="2">
+        <f t="shared" ca="1" si="18"/>
+        <v>170</v>
+      </c>
+      <c r="N105" s="2">
+        <f t="shared" ca="1" si="22"/>
+        <v>170</v>
+      </c>
+      <c r="O105" s="2">
+        <f t="shared" ca="1" si="23"/>
+        <v>170</v>
+      </c>
+      <c r="P105" s="2">
+        <f t="shared" ca="1" si="24"/>
+        <v>0.166015625</v>
+      </c>
+      <c r="Q105" s="13">
+        <f t="shared" ca="1" si="25"/>
+        <v>59.765625</v>
+      </c>
+    </row>
+    <row r="106" spans="5:25" x14ac:dyDescent="0.3">
+      <c r="F106" s="2">
         <f t="shared" ca="1" si="19"/>
-        <v>150</v>
-      </c>
-      <c r="N105" s="2">
-        <f t="shared" ca="1" si="23"/>
-        <v>150</v>
-      </c>
-      <c r="O105" s="2">
-        <f t="shared" ca="1" si="24"/>
-        <v>150</v>
-      </c>
-      <c r="P105" s="2">
-        <f t="shared" ca="1" si="20"/>
-        <v>0.146484375</v>
-      </c>
-      <c r="Q105" s="2">
-        <f t="shared" ca="1" si="25"/>
-        <v>52.734375</v>
-      </c>
-    </row>
-    <row r="106" spans="6:25" x14ac:dyDescent="0.3">
-      <c r="F106" s="2">
-        <f t="shared" ca="1" si="21"/>
-        <v>0.8330078125</v>
+        <v>0.41650390625</v>
       </c>
       <c r="G106" s="6" t="s">
         <v>58</v>
@@ -2958,46 +2963,46 @@
         <v>853</v>
       </c>
       <c r="I106" s="2">
-        <f t="shared" ca="1" si="18"/>
-        <v>20472</v>
+        <f t="shared" ca="1" si="20"/>
+        <v>853</v>
       </c>
       <c r="J106" s="2">
-        <f t="shared" ca="1" si="22"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="21"/>
+        <v>1</v>
       </c>
       <c r="K106" s="2" cm="1">
-        <f t="array" aca="1" ref="K106" ca="1">_xlfn.SWITCH(J106,1,8*2^10 - I106, 2, 8*2^10 -I106, 3, 24*2^B$41 -I106)</f>
-        <v>4104</v>
+        <f t="array" aca="1" ref="K106" ca="1">_xlfn.SWITCH(J106,1,8*2^B$41 - I106, 2, 8*2^B$41 -I106, 3, 24*2^B$41 -I106)</f>
+        <v>15531</v>
       </c>
       <c r="L106" s="2" cm="1">
         <f t="array" aca="1" ref="L106" ca="1">_xlfn.SWITCH(J106,1,K106*G$44, 2, K106*G$45, 3, K106*G$46)</f>
-        <v>268697088</v>
+        <v>677897088</v>
       </c>
       <c r="M106" s="2">
+        <f t="shared" ca="1" si="18"/>
+        <v>161</v>
+      </c>
+      <c r="N106" s="2">
+        <f t="shared" ca="1" si="22"/>
+        <v>161</v>
+      </c>
+      <c r="O106" s="2">
+        <f t="shared" ca="1" si="23"/>
+        <v>161</v>
+      </c>
+      <c r="P106" s="2">
+        <f t="shared" ca="1" si="24"/>
+        <v>0.1572265625</v>
+      </c>
+      <c r="Q106" s="13">
+        <f t="shared" ca="1" si="25"/>
+        <v>56.6015625</v>
+      </c>
+    </row>
+    <row r="107" spans="5:25" x14ac:dyDescent="0.3">
+      <c r="F107" s="2">
         <f t="shared" ca="1" si="19"/>
-        <v>256</v>
-      </c>
-      <c r="N106" s="2">
-        <f t="shared" ca="1" si="23"/>
-        <v>426</v>
-      </c>
-      <c r="O106" s="2">
-        <f t="shared" ca="1" si="24"/>
-        <v>426</v>
-      </c>
-      <c r="P106" s="2">
-        <f t="shared" ca="1" si="20"/>
-        <v>0.416015625</v>
-      </c>
-      <c r="Q106" s="2">
-        <f t="shared" ca="1" si="25"/>
-        <v>149.765625</v>
-      </c>
-    </row>
-    <row r="107" spans="6:25" x14ac:dyDescent="0.3">
-      <c r="F107" s="2">
-        <f t="shared" ca="1" si="21"/>
-        <v>0.8330078125</v>
+        <v>0.41650390625</v>
       </c>
       <c r="G107" s="6" t="s">
         <v>58</v>
@@ -3007,45 +3012,45 @@
         <v>853</v>
       </c>
       <c r="I107" s="2">
-        <f t="shared" ca="1" si="18"/>
-        <v>20472</v>
+        <f t="shared" ca="1" si="20"/>
+        <v>853</v>
       </c>
       <c r="J107" s="2">
-        <f t="shared" ca="1" si="22"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="21"/>
+        <v>1</v>
       </c>
       <c r="K107" s="2" cm="1">
-        <f t="array" aca="1" ref="K107" ca="1">_xlfn.SWITCH(J107,1,8*2^10 - I107, 2, 8*2^10 -I107, 3, 24*2^B$41 -I107)</f>
-        <v>4104</v>
+        <f t="array" aca="1" ref="K107" ca="1">_xlfn.SWITCH(J107,1,8*2^B$41 - I107, 2, 8*2^B$41 -I107, 3, 24*2^B$41 -I107)</f>
+        <v>15531</v>
       </c>
       <c r="L107" s="2" cm="1">
         <f t="array" aca="1" ref="L107" ca="1">_xlfn.SWITCH(J107,1,K107*G$44, 2, K107*G$45, 3, K107*G$46)</f>
-        <v>268697088</v>
+        <v>677897088</v>
       </c>
       <c r="M107" s="2">
+        <f t="shared" ca="1" si="18"/>
+        <v>161</v>
+      </c>
+      <c r="N107" s="2">
+        <f t="shared" ca="1" si="22"/>
+        <v>161</v>
+      </c>
+      <c r="O107" s="2">
+        <f t="shared" ca="1" si="23"/>
+        <v>161</v>
+      </c>
+      <c r="P107" s="2">
+        <f t="shared" ca="1" si="24"/>
+        <v>0.1572265625</v>
+      </c>
+      <c r="Q107" s="13">
+        <f t="shared" ca="1" si="25"/>
+        <v>56.6015625</v>
+      </c>
+    </row>
+    <row r="108" spans="5:25" x14ac:dyDescent="0.3">
+      <c r="F108" s="2">
         <f t="shared" ca="1" si="19"/>
-        <v>256</v>
-      </c>
-      <c r="N107" s="2">
-        <f t="shared" ca="1" si="23"/>
-        <v>426</v>
-      </c>
-      <c r="O107" s="2">
-        <f t="shared" ca="1" si="24"/>
-        <v>426</v>
-      </c>
-      <c r="P107" s="2">
-        <f t="shared" ca="1" si="20"/>
-        <v>0.416015625</v>
-      </c>
-      <c r="Q107" s="2">
-        <f t="shared" ca="1" si="25"/>
-        <v>149.765625</v>
-      </c>
-    </row>
-    <row r="108" spans="6:25" x14ac:dyDescent="0.3">
-      <c r="F108" s="2">
-        <f t="shared" ca="1" si="21"/>
         <v>0</v>
       </c>
       <c r="G108" s="6" t="s">
@@ -3056,43 +3061,92 @@
         <v>0</v>
       </c>
       <c r="I108" s="2">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="20"/>
         <v>0</v>
       </c>
       <c r="J108" s="2">
-        <f t="shared" ca="1" si="22"/>
+        <f t="shared" ca="1" si="21"/>
         <v>1</v>
       </c>
       <c r="K108" s="2" cm="1">
-        <f t="array" aca="1" ref="K108" ca="1">_xlfn.SWITCH(J108,1,8*2^10 - I108, 2, 8*2^10 -I108, 3, 24*2^B$41 -I108)</f>
-        <v>8192</v>
+        <f t="array" aca="1" ref="K108" ca="1">_xlfn.SWITCH(J108,1,8*2^B$41 - I108, 2, 8*2^B$41 -I108, 3, 24*2^B$41 -I108)</f>
+        <v>16384</v>
       </c>
       <c r="L108" s="2" cm="1">
         <f t="array" aca="1" ref="L108" ca="1">_xlfn.SWITCH(J108,1,K108*G$44, 2, K108*G$45, 3, K108*G$46)</f>
-        <v>178782208</v>
+        <v>715128832</v>
       </c>
       <c r="M108" s="2">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="18"/>
         <v>170</v>
       </c>
       <c r="N108" s="2">
+        <f t="shared" ca="1" si="22"/>
+        <v>170</v>
+      </c>
+      <c r="O108" s="2">
         <f t="shared" ca="1" si="23"/>
         <v>170</v>
       </c>
-      <c r="O108" s="2">
+      <c r="P108" s="2">
         <f t="shared" ca="1" si="24"/>
-        <v>170</v>
-      </c>
-      <c r="P108" s="2">
-        <f t="shared" ca="1" si="20"/>
         <v>0.166015625</v>
       </c>
-      <c r="Q108" s="2">
+      <c r="Q108" s="13">
         <f t="shared" ca="1" si="25"/>
         <v>59.765625</v>
       </c>
     </row>
-    <row r="111" spans="6:25" x14ac:dyDescent="0.3">
+    <row r="109" spans="5:25" x14ac:dyDescent="0.3">
+      <c r="E109" s="13">
+        <f>Q109</f>
+        <v>126.9140625</v>
+      </c>
+      <c r="F109" s="2">
+        <v>21</v>
+      </c>
+      <c r="H109" s="2">
+        <f>F109*2^B41</f>
+        <v>43008</v>
+      </c>
+      <c r="I109" s="2">
+        <f t="shared" si="20"/>
+        <v>43008</v>
+      </c>
+      <c r="J109" s="2">
+        <f t="shared" si="21"/>
+        <v>3</v>
+      </c>
+      <c r="K109" s="2" cm="1">
+        <f t="array" ref="K109">_xlfn.SWITCH(J109,1,8*2^B$41 - I109, 2, 8*2^B$41 -I109, 3, 24*2^B$41 -I109)</f>
+        <v>6144</v>
+      </c>
+      <c r="L109" s="2" cm="1">
+        <f t="array" ref="L109">_xlfn.SWITCH(J109,1,K109*G$44, 2, K109*G$45, 3, K109*G$46)</f>
+        <v>804519936</v>
+      </c>
+      <c r="M109" s="2">
+        <f t="shared" si="18"/>
+        <v>191</v>
+      </c>
+      <c r="N109" s="2">
+        <f t="shared" si="22"/>
+        <v>361</v>
+      </c>
+      <c r="O109" s="2">
+        <f>MOD(N109,1024)</f>
+        <v>361</v>
+      </c>
+      <c r="P109" s="2">
+        <f t="shared" si="24"/>
+        <v>0.3525390625</v>
+      </c>
+      <c r="Q109" s="13">
+        <f t="shared" si="25"/>
+        <v>126.9140625</v>
+      </c>
+    </row>
+    <row r="111" spans="5:25" x14ac:dyDescent="0.3">
       <c r="I111" s="2" t="s">
         <v>67</v>
       </c>
@@ -3145,18 +3199,18 @@
         <v>72</v>
       </c>
     </row>
-    <row r="112" spans="6:25" x14ac:dyDescent="0.3">
-      <c r="I112" s="2" t="e">
+    <row r="112" spans="5:25" x14ac:dyDescent="0.3">
+      <c r="I112" s="2">
         <f t="shared" ref="I112:I123" ca="1" si="26">O97*E$55</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="J112" s="2" t="e">
+        <v>2040</v>
+      </c>
+      <c r="J112" s="2">
         <f t="shared" ref="J112:J123" ca="1" si="27">_xlfn.FLOOR.MATH(I112/2^B$41)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="K112" s="2" t="e">
+        <v>0</v>
+      </c>
+      <c r="K112" s="2">
         <f t="shared" ref="K112:K123" ca="1" si="28">MOD(I112, 2^B$41)</f>
-        <v>#NUM!</v>
+        <v>2040</v>
       </c>
       <c r="L112" s="2">
         <f ca="1">IF(E57,K83,L83)</f>
@@ -3164,69 +3218,69 @@
       </c>
       <c r="M112" s="2">
         <f t="shared" ref="M112:M123" ca="1" si="29">L112*E$54</f>
-        <v>982800</v>
+        <v>1966200</v>
       </c>
       <c r="N112" s="2">
         <f t="shared" ref="N112:N123" ca="1" si="30">IF(_xlfn.FLOOR.MATH(M112/2^B$41) &gt; 1023, 1023, _xlfn.FLOOR.MATH(M112/2^B$41))</f>
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="O112" s="2">
         <f t="shared" ref="O112:O123" ca="1" si="31">IF(N112&gt;E$56,E$56,N112)</f>
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="P112" s="2">
         <f t="shared" ref="P112:P123" ca="1" si="32">_xlfn.FLOOR.MATH(O112/2^(B$41-8))</f>
-        <v>239</v>
-      </c>
-      <c r="Q112" s="2" t="e">
+        <v>120</v>
+      </c>
+      <c r="Q112" s="2">
         <f ca="1">O112*K112</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="R112" s="2" t="e">
+        <v>1958400</v>
+      </c>
+      <c r="R112" s="2">
         <f t="shared" ref="R112:R123" ca="1" si="33">O112*(2^(B$41) - 1 - K112)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="S112" s="2" t="e">
+        <v>6720</v>
+      </c>
+      <c r="S112" s="2">
         <f t="shared" ref="S112:S123" ca="1" si="34">_xlfn.FLOOR.MATH(Q112/2^(2*B$41-8))</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="T112" s="2" t="e">
+        <v>119</v>
+      </c>
+      <c r="T112" s="2">
         <f t="shared" ref="T112:T123" ca="1" si="35">_xlfn.FLOOR.MATH(R112/2^(2*B$41-8))</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="U112" s="2" t="e" cm="1">
+        <v>0</v>
+      </c>
+      <c r="U112" s="2" cm="1">
         <f t="array" aca="1" ref="U112" ca="1">_xlfn.SWITCH(J112,0,P112,1,T112,2,0,3,0,4,S112,5,P112)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="V112" s="2" t="e" cm="1">
+        <v>120</v>
+      </c>
+      <c r="V112" s="2" cm="1">
         <f t="array" aca="1" ref="V112" ca="1">_xlfn.SWITCH(J112,0,S112,1,P112,2,P112,3,T112,4,0,5,0)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="W112" s="2" t="e" cm="1">
+        <v>119</v>
+      </c>
+      <c r="W112" s="2" cm="1">
         <f t="array" aca="1" ref="W112" ca="1">_xlfn.SWITCH(J112,0,0,1,0,2,S112,3,P112,4,P112,5,T112)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="X112" s="2" t="e">
+        <v>0</v>
+      </c>
+      <c r="X112" s="2">
         <f ca="1">U112*2^16+V112*2^8+W112</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="Y112" s="2" t="e">
+        <v>7894784</v>
+      </c>
+      <c r="Y112" s="2" t="str">
         <f t="shared" ref="Y112:Y123" ca="1" si="36">_xlfn.BASE(X112,16,6)</f>
-        <v>#NUM!</v>
+        <v>787700</v>
       </c>
     </row>
     <row r="113" spans="9:25" x14ac:dyDescent="0.3">
-      <c r="I113" s="2" t="e">
+      <c r="I113" s="2">
         <f t="shared" ca="1" si="26"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="J113" s="2" t="e">
+        <v>10212</v>
+      </c>
+      <c r="J113" s="2">
         <f t="shared" ca="1" si="27"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="K113" s="2" t="e">
+        <v>4</v>
+      </c>
+      <c r="K113" s="2">
         <f t="shared" ca="1" si="28"/>
-        <v>#NUM!</v>
+        <v>2020</v>
       </c>
       <c r="L113" s="2">
         <f t="shared" ref="L113:L123" ca="1" si="37">IF(E58,K84,L84)</f>
@@ -3234,7 +3288,7 @@
       </c>
       <c r="M113" s="2">
         <f t="shared" ca="1" si="29"/>
-        <v>1174446</v>
+        <v>2349609</v>
       </c>
       <c r="N113" s="2">
         <f t="shared" ca="1" si="30"/>
@@ -3246,57 +3300,57 @@
       </c>
       <c r="P113" s="2">
         <f t="shared" ca="1" si="32"/>
-        <v>255</v>
-      </c>
-      <c r="Q113" s="2" t="e">
+        <v>127</v>
+      </c>
+      <c r="Q113" s="2">
         <f t="shared" ref="Q113:Q123" ca="1" si="38">O113*K113</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="R113" s="2" t="e">
+        <v>2066460</v>
+      </c>
+      <c r="R113" s="2">
         <f t="shared" ca="1" si="33"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="S113" s="2" t="e">
+        <v>27621</v>
+      </c>
+      <c r="S113" s="2">
         <f t="shared" ca="1" si="34"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="T113" s="2" t="e">
+        <v>126</v>
+      </c>
+      <c r="T113" s="2">
         <f t="shared" ca="1" si="35"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="U113" s="2" t="e" cm="1">
+        <v>1</v>
+      </c>
+      <c r="U113" s="2" cm="1">
         <f t="array" aca="1" ref="U113" ca="1">_xlfn.SWITCH(J113,0,P113,1,T113,2,0,3,0,4,S113,5,P113)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="V113" s="2" t="e" cm="1">
+        <v>126</v>
+      </c>
+      <c r="V113" s="2" cm="1">
         <f t="array" aca="1" ref="V113" ca="1">_xlfn.SWITCH(J113,0,S113,1,P113,2,P113,3,T113,4,0,5,0)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="W113" s="2" t="e" cm="1">
+        <v>0</v>
+      </c>
+      <c r="W113" s="2" cm="1">
         <f t="array" aca="1" ref="W113" ca="1">_xlfn.SWITCH(J113,0,0,1,0,2,S113,3,P113,4,P113,5,T113)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="X113" s="2" t="e">
+        <v>127</v>
+      </c>
+      <c r="X113" s="2">
         <f t="shared" ref="X113:X123" ca="1" si="39">U113*2^16+V113*2^8+W113</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="Y113" s="2" t="e">
+        <v>8257663</v>
+      </c>
+      <c r="Y113" s="2" t="str">
         <f t="shared" ca="1" si="36"/>
-        <v>#NUM!</v>
+        <v>7E007F</v>
       </c>
     </row>
     <row r="114" spans="9:25" x14ac:dyDescent="0.3">
-      <c r="I114" s="2" t="e">
+      <c r="I114" s="2">
         <f t="shared" ca="1" si="26"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="J114" s="2" t="e">
+        <v>5112</v>
+      </c>
+      <c r="J114" s="2">
         <f t="shared" ca="1" si="27"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="K114" s="2" t="e">
+        <v>2</v>
+      </c>
+      <c r="K114" s="2">
         <f t="shared" ca="1" si="28"/>
-        <v>#NUM!</v>
+        <v>1016</v>
       </c>
       <c r="L114" s="2">
         <f t="shared" ca="1" si="37"/>
@@ -3304,69 +3358,69 @@
       </c>
       <c r="M114" s="2">
         <f t="shared" ca="1" si="29"/>
-        <v>737100</v>
+        <v>1474650</v>
       </c>
       <c r="N114" s="2">
         <f t="shared" ca="1" si="30"/>
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="O114" s="2">
         <f t="shared" ca="1" si="31"/>
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="P114" s="2">
         <f t="shared" ca="1" si="32"/>
-        <v>179</v>
-      </c>
-      <c r="Q114" s="2" t="e">
+        <v>90</v>
+      </c>
+      <c r="Q114" s="2">
         <f t="shared" ca="1" si="38"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="R114" s="2" t="e">
+        <v>731520</v>
+      </c>
+      <c r="R114" s="2">
         <f t="shared" ca="1" si="33"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="S114" s="2" t="e">
+        <v>742320</v>
+      </c>
+      <c r="S114" s="2">
         <f t="shared" ca="1" si="34"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="T114" s="2" t="e">
+        <v>44</v>
+      </c>
+      <c r="T114" s="2">
         <f t="shared" ca="1" si="35"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="U114" s="2" t="e" cm="1">
+        <v>45</v>
+      </c>
+      <c r="U114" s="2" cm="1">
         <f t="array" aca="1" ref="U114" ca="1">_xlfn.SWITCH(J114,0,P114,1,T114,2,0,3,0,4,S114,5,P114)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="V114" s="2" t="e" cm="1">
+        <v>0</v>
+      </c>
+      <c r="V114" s="2" cm="1">
         <f t="array" aca="1" ref="V114" ca="1">_xlfn.SWITCH(J114,0,S114,1,P114,2,P114,3,T114,4,0,5,0)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="W114" s="2" t="e" cm="1">
+        <v>90</v>
+      </c>
+      <c r="W114" s="2" cm="1">
         <f t="array" aca="1" ref="W114" ca="1">_xlfn.SWITCH(J114,0,0,1,0,2,S114,3,P114,4,P114,5,T114)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="X114" s="2" t="e">
+        <v>44</v>
+      </c>
+      <c r="X114" s="2">
         <f t="shared" ca="1" si="39"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="Y114" s="2" t="e">
+        <v>23084</v>
+      </c>
+      <c r="Y114" s="2" t="str">
         <f t="shared" ca="1" si="36"/>
-        <v>#NUM!</v>
+        <v>005A2C</v>
       </c>
     </row>
     <row r="115" spans="9:25" x14ac:dyDescent="0.3">
-      <c r="I115" s="2" t="e">
+      <c r="I115" s="2">
         <f t="shared" ca="1" si="26"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="J115" s="2" t="e">
+        <v>4296</v>
+      </c>
+      <c r="J115" s="2">
         <f t="shared" ca="1" si="27"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="K115" s="2" t="e">
+        <v>2</v>
+      </c>
+      <c r="K115" s="2">
         <f t="shared" ca="1" si="28"/>
-        <v>#NUM!</v>
+        <v>200</v>
       </c>
       <c r="L115" s="2">
         <f t="shared" ca="1" si="37"/>
@@ -3388,55 +3442,55 @@
         <f t="shared" ca="1" si="32"/>
         <v>0</v>
       </c>
-      <c r="Q115" s="2" t="e">
+      <c r="Q115" s="2">
         <f t="shared" ca="1" si="38"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="R115" s="2" t="e">
+        <v>0</v>
+      </c>
+      <c r="R115" s="2">
         <f t="shared" ca="1" si="33"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="S115" s="2" t="e">
+        <v>0</v>
+      </c>
+      <c r="S115" s="2">
         <f t="shared" ca="1" si="34"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="T115" s="2" t="e">
+        <v>0</v>
+      </c>
+      <c r="T115" s="2">
         <f t="shared" ca="1" si="35"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="U115" s="2" t="e" cm="1">
+        <v>0</v>
+      </c>
+      <c r="U115" s="2" cm="1">
         <f t="array" aca="1" ref="U115" ca="1">_xlfn.SWITCH(J115,0,P115,1,T115,2,0,3,0,4,S115,5,P115)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="V115" s="2" t="e" cm="1">
+        <v>0</v>
+      </c>
+      <c r="V115" s="2" cm="1">
         <f t="array" aca="1" ref="V115" ca="1">_xlfn.SWITCH(J115,0,S115,1,P115,2,P115,3,T115,4,0,5,0)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="W115" s="2" t="e" cm="1">
+        <v>0</v>
+      </c>
+      <c r="W115" s="2" cm="1">
         <f t="array" aca="1" ref="W115" ca="1">_xlfn.SWITCH(J115,0,0,1,0,2,S115,3,P115,4,P115,5,T115)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="X115" s="2" t="e">
+        <v>0</v>
+      </c>
+      <c r="X115" s="2">
         <f t="shared" ca="1" si="39"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="Y115" s="2" t="e">
+        <v>0</v>
+      </c>
+      <c r="Y115" s="2" t="str">
         <f t="shared" ca="1" si="36"/>
-        <v>#NUM!</v>
+        <v>000000</v>
       </c>
     </row>
     <row r="116" spans="9:25" x14ac:dyDescent="0.3">
       <c r="I116" s="2">
         <f t="shared" ca="1" si="26"/>
-        <v>3078</v>
+        <v>1944</v>
       </c>
       <c r="J116" s="2">
         <f t="shared" ca="1" si="27"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K116" s="2">
         <f t="shared" ca="1" si="28"/>
-        <v>6</v>
+        <v>1944</v>
       </c>
       <c r="L116" s="2">
         <f t="shared" ca="1" si="37"/>
@@ -3498,15 +3552,15 @@
     <row r="117" spans="9:25" x14ac:dyDescent="0.3">
       <c r="I117" s="2">
         <f t="shared" ca="1" si="26"/>
-        <v>4266</v>
+        <v>1956</v>
       </c>
       <c r="J117" s="2">
         <f t="shared" ca="1" si="27"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K117" s="2">
         <f t="shared" ca="1" si="28"/>
-        <v>170</v>
+        <v>1956</v>
       </c>
       <c r="L117" s="2">
         <f t="shared" ca="1" si="37"/>
@@ -3568,15 +3622,15 @@
     <row r="118" spans="9:25" x14ac:dyDescent="0.3">
       <c r="I118" s="2">
         <f t="shared" ca="1" si="26"/>
-        <v>6120</v>
+        <v>1992</v>
       </c>
       <c r="J118" s="2">
         <f t="shared" ca="1" si="27"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K118" s="2">
         <f t="shared" ca="1" si="28"/>
-        <v>1000</v>
+        <v>1992</v>
       </c>
       <c r="L118" s="2">
         <f t="shared" ca="1" si="37"/>
@@ -3638,15 +3692,15 @@
     <row r="119" spans="9:25" x14ac:dyDescent="0.3">
       <c r="I119" s="2">
         <f t="shared" ca="1" si="26"/>
-        <v>4746</v>
+        <v>1968</v>
       </c>
       <c r="J119" s="2">
         <f t="shared" ca="1" si="27"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K119" s="2">
         <f t="shared" ca="1" si="28"/>
-        <v>650</v>
+        <v>1968</v>
       </c>
       <c r="L119" s="2">
         <f t="shared" ca="1" si="37"/>
@@ -3708,7 +3762,7 @@
     <row r="120" spans="9:25" x14ac:dyDescent="0.3">
       <c r="I120" s="2">
         <f t="shared" ca="1" si="26"/>
-        <v>900</v>
+        <v>2040</v>
       </c>
       <c r="J120" s="2">
         <f t="shared" ca="1" si="27"/>
@@ -3716,7 +3770,7 @@
       </c>
       <c r="K120" s="2">
         <f t="shared" ca="1" si="28"/>
-        <v>900</v>
+        <v>2040</v>
       </c>
       <c r="L120" s="2">
         <f t="shared" ca="1" si="37"/>
@@ -3778,15 +3832,15 @@
     <row r="121" spans="9:25" x14ac:dyDescent="0.3">
       <c r="I121" s="2">
         <f t="shared" ca="1" si="26"/>
-        <v>2556</v>
+        <v>1932</v>
       </c>
       <c r="J121" s="2">
         <f t="shared" ca="1" si="27"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K121" s="2">
         <f t="shared" ca="1" si="28"/>
-        <v>508</v>
+        <v>1932</v>
       </c>
       <c r="L121" s="2">
         <f t="shared" ca="1" si="37"/>
@@ -3848,15 +3902,15 @@
     <row r="122" spans="9:25" x14ac:dyDescent="0.3">
       <c r="I122" s="2">
         <f t="shared" ca="1" si="26"/>
-        <v>2556</v>
+        <v>1932</v>
       </c>
       <c r="J122" s="2">
         <f t="shared" ca="1" si="27"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K122" s="2">
         <f t="shared" ca="1" si="28"/>
-        <v>508</v>
+        <v>1932</v>
       </c>
       <c r="L122" s="2">
         <f t="shared" ca="1" si="37"/>
@@ -3918,7 +3972,7 @@
     <row r="123" spans="9:25" x14ac:dyDescent="0.3">
       <c r="I123" s="2">
         <f t="shared" ca="1" si="26"/>
-        <v>1020</v>
+        <v>2040</v>
       </c>
       <c r="J123" s="2">
         <f t="shared" ca="1" si="27"/>
@@ -3926,7 +3980,7 @@
       </c>
       <c r="K123" s="2">
         <f t="shared" ca="1" si="28"/>
-        <v>1020</v>
+        <v>2040</v>
       </c>
       <c r="L123" s="2">
         <f t="shared" ca="1" si="37"/>
@@ -3996,23 +4050,23 @@
     <row r="126" spans="9:25" x14ac:dyDescent="0.3">
       <c r="I126" s="2">
         <f ca="1">I90/B43</f>
-        <v>24.779414062499999</v>
+        <v>24.727646484375001</v>
       </c>
       <c r="J126" s="2">
         <f t="shared" ref="J126:J138" ca="1" si="40">K83/I$126</f>
-        <v>17.110583539448857</v>
+        <v>17.111512883913857</v>
       </c>
     </row>
     <row r="127" spans="9:25" x14ac:dyDescent="0.3">
       <c r="J127" s="2">
         <f t="shared" ca="1" si="40"/>
-        <v>21.832244822677595</v>
+        <v>21.84305901281579</v>
       </c>
     </row>
     <row r="128" spans="9:25" x14ac:dyDescent="0.3">
       <c r="J128" s="2">
         <f t="shared" ca="1" si="40"/>
-        <v>11.05717163787355</v>
+        <v>11.045428103270353</v>
       </c>
     </row>
     <row r="129" spans="10:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Fixed LV components to be full updated to new D and W
</commit_message>
<xml_diff>
--- a/other/LinearVisualizer.xlsx
+++ b/other/LinearVisualizer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\CCHW\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009C1BE5-C8E6-4B7D-ABF3-BFE4CA678746}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D601CDB-AFA0-4D17-BCFC-7314BB194C23}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9DBF0F91-83D7-4F64-B04C-B7CB81DC62EF}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9DBF0F91-83D7-4F64-B04C-B7CB81DC62EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="78">
   <si>
     <t>W</t>
   </si>
@@ -239,15 +239,6 @@
     <t>0000000000000000</t>
   </si>
   <si>
-    <t>0000001001011000</t>
-  </si>
-  <si>
-    <t>0000001011001101</t>
-  </si>
-  <si>
-    <t>0000000111000010</t>
-  </si>
-  <si>
     <t>value</t>
   </si>
   <si>
@@ -297,6 +288,9 @@
   </si>
   <si>
     <t>1010100001100100</t>
+  </si>
+  <si>
+    <t>1111111111111111</t>
   </si>
 </sst>
 </file>
@@ -713,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A6626A4-8C87-4B90-BEEB-AEB487ACEA9E}">
   <dimension ref="A2:Y138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C91" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView tabSelected="1" topLeftCell="H69" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T123" sqref="T123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -746,17 +740,17 @@
   <sheetData>
     <row r="2" spans="1:1" ht="46.2" x14ac:dyDescent="0.85">
       <c r="A2" s="12" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="46.2" x14ac:dyDescent="0.85">
       <c r="A4" s="12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="46.2" x14ac:dyDescent="0.85">
       <c r="A6" s="12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
@@ -797,11 +791,11 @@
       </c>
       <c r="D26" s="2" t="str">
         <f t="shared" ref="D26:D37" ca="1" si="0">_xlfn.CONCAT(B$40+B$41,"'b",REPT("0",B$40-LEN(E26)))</f>
-        <v>16'b0000</v>
+        <v>16'b00</v>
       </c>
       <c r="E26" s="2" t="str">
         <f ca="1">DEC2BIN(_xlfn.FLOOR.MATH(RAND()*10))</f>
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F26" s="2" t="str">
         <f t="shared" ref="F26:F37" si="1">_xlfn.CONCAT(REPT("0",B$41),";")</f>
@@ -809,23 +803,23 @@
       </c>
       <c r="G26" s="4" t="str">
         <f ca="1">_xlfn.CONCAT(A26,B26,C26,D26,E26,F26)</f>
-        <v xml:space="preserve">            noteAmplitudes_i[ 0] = 16'b0000100000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 0] = 16'b0010000000000000;</v>
       </c>
       <c r="H26" s="2">
         <f t="shared" ref="H26:H37" ca="1" si="2">BIN2DEC(E26)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I26" s="2">
         <f t="shared" ref="I26:I37" ca="1" si="3">H26*2^B$41</f>
-        <v>2048</v>
+        <v>8192</v>
       </c>
       <c r="J26" s="2">
         <f ca="1">SUM(H26:H37)</f>
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K26" s="2">
         <f t="shared" ref="K26:K37" ca="1" si="4">I26-J$31</f>
-        <v>-10047</v>
+        <v>-3698</v>
       </c>
       <c r="L26" s="2">
         <f ca="1">IF(K26&gt;0,K26,0)</f>
@@ -872,11 +866,11 @@
       </c>
       <c r="J27" s="2">
         <f ca="1">J26*2^B41</f>
-        <v>120832</v>
+        <v>118784</v>
       </c>
       <c r="K27" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>-10047</v>
+        <v>-9842</v>
       </c>
       <c r="L27" s="2">
         <f t="shared" ref="L27:L37" ca="1" si="7">IF(K27&gt;0,K27,0)</f>
@@ -903,7 +897,7 @@
       </c>
       <c r="E28" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="F28" s="2" t="str">
         <f t="shared" si="1"/>
@@ -911,27 +905,27 @@
       </c>
       <c r="G28" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 2] = 16'b0010100000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 2] = 16'b0011000000000000;</v>
       </c>
       <c r="H28" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I28" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>10240</v>
+        <v>12288</v>
       </c>
       <c r="K28" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>-1855</v>
+        <v>398</v>
       </c>
       <c r="L28" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>398</v>
       </c>
       <c r="M28" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>12288</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
@@ -950,7 +944,7 @@
       </c>
       <c r="E29" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="F29" s="2" t="str">
         <f t="shared" si="1"/>
@@ -958,30 +952,30 @@
       </c>
       <c r="G29" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 3] = 16'b0011000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 3] = 16'b0010000000000000;</v>
       </c>
       <c r="H29" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I29" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>12288</v>
+        <v>8192</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>8</v>
       </c>
       <c r="K29" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>193</v>
+        <v>-3698</v>
       </c>
       <c r="L29" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>193</v>
+        <v>0</v>
       </c>
       <c r="M29" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>12288</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
@@ -996,11 +990,11 @@
       </c>
       <c r="D30" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16'b0000</v>
+        <v>16'b000</v>
       </c>
       <c r="E30" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F30" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1008,23 +1002,23 @@
       </c>
       <c r="G30" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 4] = 16'b0000100000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 4] = 16'b0001000000000000;</v>
       </c>
       <c r="H30" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I30" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>2048</v>
+        <v>4096</v>
       </c>
       <c r="J30" s="3">
         <f ca="1">J26*B42</f>
-        <v>5.876953125</v>
+        <v>5.77734375</v>
       </c>
       <c r="K30" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>-10047</v>
+        <v>-7794</v>
       </c>
       <c r="L30" s="2">
         <f t="shared" ca="1" si="7"/>
@@ -1051,7 +1045,7 @@
       </c>
       <c r="E31" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="F31" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1059,31 +1053,31 @@
       </c>
       <c r="G31" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 5] = 16'b0100000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 5] = 16'b0100100000000000;</v>
       </c>
       <c r="H31" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I31" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>16384</v>
+        <v>18432</v>
       </c>
       <c r="J31" s="2">
         <f ca="1">J27 * BIN2DEC(C42) / 2^B41</f>
-        <v>12095</v>
+        <v>11890</v>
       </c>
       <c r="K31" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>4289</v>
+        <v>6542</v>
       </c>
       <c r="L31" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>4289</v>
+        <v>6542</v>
       </c>
       <c r="M31" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>16384</v>
+        <v>18432</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
@@ -1098,11 +1092,11 @@
       </c>
       <c r="D32" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16'b0</v>
+        <v>16'b00</v>
       </c>
       <c r="E32" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>1000</v>
+        <v>101</v>
       </c>
       <c r="F32" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1110,27 +1104,27 @@
       </c>
       <c r="G32" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 6] = 16'b0100000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 6] = 16'b0010100000000000;</v>
       </c>
       <c r="H32" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I32" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>16384</v>
+        <v>10240</v>
       </c>
       <c r="K32" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>4289</v>
+        <v>-1650</v>
       </c>
       <c r="L32" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>4289</v>
+        <v>0</v>
       </c>
       <c r="M32" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>16384</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
@@ -1145,11 +1139,11 @@
       </c>
       <c r="D33" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16'b0</v>
+        <v>16'b00</v>
       </c>
       <c r="E33" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>1000</v>
+        <v>110</v>
       </c>
       <c r="F33" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1157,30 +1151,30 @@
       </c>
       <c r="G33" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 7] = 16'b0100000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 7] = 16'b0011000000000000;</v>
       </c>
       <c r="H33" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I33" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>16384</v>
+        <v>12288</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>13</v>
       </c>
       <c r="K33" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>4289</v>
+        <v>398</v>
       </c>
       <c r="L33" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>4289</v>
+        <v>398</v>
       </c>
       <c r="M33" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>16384</v>
+        <v>12288</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
@@ -1199,7 +1193,7 @@
       </c>
       <c r="E34" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="F34" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1207,31 +1201,31 @@
       </c>
       <c r="G34" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 8] = 16'b0011000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 8] = 16'b0010100000000000;</v>
       </c>
       <c r="H34" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I34" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>12288</v>
+        <v>10240</v>
       </c>
       <c r="J34" s="2">
         <f ca="1">J35/2^B41</f>
-        <v>7.65966796875</v>
+        <v>6.9716796875</v>
       </c>
       <c r="K34" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>193</v>
+        <v>-1650</v>
       </c>
       <c r="L34" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>193</v>
+        <v>0</v>
       </c>
       <c r="M34" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>12288</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
@@ -1270,15 +1264,15 @@
       </c>
       <c r="J35" s="2">
         <f ca="1">SUM(L26:L37)</f>
-        <v>15687</v>
+        <v>14278</v>
       </c>
       <c r="K35" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>2241</v>
+        <v>2446</v>
       </c>
       <c r="L35" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>2241</v>
+        <v>2446</v>
       </c>
       <c r="M35" s="2">
         <f t="shared" ca="1" si="8"/>
@@ -1297,11 +1291,11 @@
       </c>
       <c r="D36" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16'b000</v>
+        <v>16'b0000</v>
       </c>
       <c r="E36" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F36" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1309,19 +1303,19 @@
       </c>
       <c r="G36" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[10] = 16'b0001000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[10] = 16'b0000100000000000;</v>
       </c>
       <c r="H36" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I36" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>4096</v>
+        <v>2048</v>
       </c>
       <c r="K36" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>-7999</v>
+        <v>-9842</v>
       </c>
       <c r="L36" s="2">
         <f t="shared" ca="1" si="7"/>
@@ -1344,11 +1338,11 @@
       </c>
       <c r="D37" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16'b00</v>
+        <v>16'b0</v>
       </c>
       <c r="E37" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>110</v>
+        <v>1000</v>
       </c>
       <c r="F37" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1356,27 +1350,27 @@
       </c>
       <c r="G37" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[11] = 16'b0011000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[11] = 16'b0100000000000000;</v>
       </c>
       <c r="H37" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I37" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>12288</v>
+        <v>16384</v>
       </c>
       <c r="K37" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>193</v>
+        <v>4494</v>
       </c>
       <c r="L37" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>193</v>
+        <v>4494</v>
       </c>
       <c r="M37" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>12288</v>
+        <v>16384</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
@@ -1419,27 +1413,27 @@
       <c r="C41" s="8"/>
       <c r="G41" s="4" t="str">
         <f ca="1">_xlfn.CONCAT("notePosition_i = 10'b",REPT(0,B41-LEN(_xlfn.BASE(I41,2))),_xlfn.BASE(I41,2),";" )</f>
-        <v>notePosition_i = 10'b01111011000;</v>
+        <v>notePosition_i = 10'b01000110001;</v>
       </c>
       <c r="H41" s="2">
         <f ca="1">I41/2^10</f>
-        <v>0.9609375</v>
+        <v>0.5478515625</v>
       </c>
       <c r="I41" s="2">
         <f ca="1">RANDBETWEEN(0,1023)</f>
-        <v>984</v>
+        <v>561</v>
       </c>
       <c r="J41" s="2">
         <f ca="1">I41*24</f>
-        <v>23616</v>
+        <v>13464</v>
       </c>
       <c r="K41" s="2">
         <f ca="1">IF(J45=3,24576-J41,8192-J41)</f>
-        <v>960</v>
+        <v>-5272</v>
       </c>
       <c r="L41" s="2">
         <f ca="1">IF(J45=3,K47+170, K47)</f>
-        <v>177</v>
+        <v>-28</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
@@ -1451,6 +1445,10 @@
       </c>
       <c r="C42" s="10">
         <v>11001101</v>
+      </c>
+      <c r="D42" s="2">
+        <f>BIN2DEC(C42)</f>
+        <v>205</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
@@ -1485,11 +1483,11 @@
       </c>
       <c r="J44" s="2" t="str">
         <f ca="1">_xlfn.CONCAT(REPT(0,3-LEN(DEC2BIN(2^_xlfn.FLOOR.MATH((J41+1)/8192)))),DEC2BIN(2^_xlfn.FLOOR.MATH((J41+1)/8192)))</f>
-        <v>100</v>
+        <v>010</v>
       </c>
       <c r="K44" s="2">
         <f ca="1">K41*H44*H45*H46</f>
-        <v>125706240</v>
+        <v>-460224512</v>
       </c>
       <c r="L44" s="2" t="s">
         <v>24</v>
@@ -1508,19 +1506,19 @@
       </c>
       <c r="H45" s="2">
         <f ca="1">IF(J$45=2,G45,1)</f>
-        <v>1</v>
+        <v>87296</v>
       </c>
       <c r="J45" s="2">
         <f ca="1">LEN(DEC2BIN(2^_xlfn.FLOOR.MATH((J41+1)/8192)))</f>
-        <v>3</v>
-      </c>
-      <c r="K45" s="2" t="str">
+        <v>2</v>
+      </c>
+      <c r="K45" s="2" t="e">
         <f ca="1">_xlfn.BASE(K44,2,32)</f>
-        <v>00000111011111100010000000000000</v>
+        <v>#NUM!</v>
       </c>
       <c r="L45" s="2">
         <f ca="1">MOD(IF(L41&lt;0,L41+1023,L41), 1024)</f>
-        <v>177</v>
+        <v>995</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
@@ -1536,7 +1534,7 @@
       </c>
       <c r="H46" s="2">
         <f ca="1">IF(J$45=3,G46,1)</f>
-        <v>130944</v>
+        <v>1</v>
       </c>
       <c r="K46" s="2" t="s">
         <v>21</v>
@@ -1545,21 +1543,21 @@
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K47" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(K44/2^(B41+B41+C39-3))</f>
-        <v>7</v>
+        <v>-28</v>
       </c>
     </row>
     <row r="50" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G50" s="4" t="str">
         <f ca="1">_xlfn.CONCAT("        noteAmplitude_i = 10'b",REPT(0,B41-LEN(_xlfn.BASE(I50,2))),_xlfn.BASE(I50,2),";" )</f>
-        <v xml:space="preserve">        noteAmplitude_i = 10'b00010010110;</v>
+        <v xml:space="preserve">        noteAmplitude_i = 10'b01100100101;</v>
       </c>
       <c r="H50" s="2">
         <f ca="1">I50/2^10</f>
-        <v>0.146484375</v>
+        <v>0.7861328125</v>
       </c>
       <c r="I50" s="2">
         <f ca="1">RANDBETWEEN(0,1023)</f>
-        <v>150</v>
+        <v>805</v>
       </c>
       <c r="J50" s="2" t="s">
         <v>28</v>
@@ -1591,23 +1589,23 @@
       </c>
       <c r="G51" s="4" t="str">
         <f ca="1">_xlfn.CONCAT("        noteAmplitudeFast_i = 10'b",REPT(0,B41-LEN(_xlfn.BASE(I51,2))),_xlfn.BASE(I51,2),";" )</f>
-        <v xml:space="preserve">        noteAmplitudeFast_i = 10'b00101010011;</v>
+        <v xml:space="preserve">        noteAmplitudeFast_i = 10'b01000011001;</v>
       </c>
       <c r="H51" s="2">
         <f t="shared" ref="H51:H52" ca="1" si="9">I51/2^10</f>
-        <v>0.3310546875</v>
+        <v>0.5244140625</v>
       </c>
       <c r="I51" s="2">
         <f ca="1">RANDBETWEEN(0,1023)</f>
-        <v>339</v>
+        <v>537</v>
       </c>
       <c r="J51" s="2">
         <f ca="1">I52*E55</f>
-        <v>10320</v>
+        <v>1560</v>
       </c>
       <c r="K51" s="2">
         <f ca="1">IF(E57,I50,I51)</f>
-        <v>339</v>
+        <v>537</v>
       </c>
       <c r="L51" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(K57/2^(B41-8))</f>
@@ -1619,7 +1617,7 @@
       </c>
       <c r="N51" s="2">
         <f ca="1">$L$57</f>
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="O51" s="2">
         <f>0</f>
@@ -1627,21 +1625,21 @@
       </c>
       <c r="P51" s="2">
         <f ca="1">M51*2^16+N51*2^8+O51</f>
-        <v>8324096</v>
+        <v>8331520</v>
       </c>
     </row>
     <row r="52" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G52" s="4" t="str">
         <f ca="1">_xlfn.CONCAT("        noteHue_i = 10'b",REPT(0,B41-LEN(_xlfn.BASE(I52,2))),_xlfn.BASE(I52,2),";" )</f>
-        <v xml:space="preserve">        noteHue_i = 10'b01101011100;</v>
+        <v xml:space="preserve">        noteHue_i = 10'b00010000010;</v>
       </c>
       <c r="H52" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>0.83984375</v>
+        <v>0.126953125</v>
       </c>
       <c r="I52" s="2">
         <f ca="1">RANDBETWEEN(0,1023)</f>
-        <v>860</v>
+        <v>130</v>
       </c>
       <c r="J52" s="2" t="s">
         <v>29</v>
@@ -1654,7 +1652,7 @@
       </c>
       <c r="M52" s="2">
         <f ca="1">$L$59</f>
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="N52" s="2">
         <f ca="1">$L$51</f>
@@ -1666,21 +1664,21 @@
       </c>
       <c r="P52" s="2">
         <f t="shared" ref="P52:P57" ca="1" si="10">M52*2^16+N52*2^8+O52</f>
-        <v>3833600</v>
+        <v>1998592</v>
       </c>
     </row>
     <row r="53" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J53" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(J51/2^10)</f>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="K53" s="2">
         <f ca="1">K51*E54</f>
-        <v>1110903</v>
+        <v>1759749</v>
       </c>
       <c r="L53" s="2">
         <f ca="1">K57*J55</f>
-        <v>81840</v>
+        <v>548328</v>
       </c>
       <c r="M53" s="2">
         <f>0</f>
@@ -1692,11 +1690,11 @@
       </c>
       <c r="O53" s="2">
         <f ca="1">$L$57</f>
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="P53" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>32516</v>
+        <v>32545</v>
       </c>
     </row>
     <row r="54" spans="2:16" x14ac:dyDescent="0.3">
@@ -1721,7 +1719,7 @@
       </c>
       <c r="N54" s="2">
         <f ca="1">$L$59</f>
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="O54" s="2">
         <f ca="1">$L$51</f>
@@ -1729,7 +1727,7 @@
       </c>
       <c r="P54" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>14975</v>
+        <v>7807</v>
       </c>
     </row>
     <row r="55" spans="2:16" x14ac:dyDescent="0.3">
@@ -1741,7 +1739,7 @@
       </c>
       <c r="J55" s="2">
         <f ca="1">MOD(J51,2^10)</f>
-        <v>80</v>
+        <v>536</v>
       </c>
       <c r="K55" s="2">
         <f ca="1">IF(_xlfn.FLOOR.MATH(K53/2^10) &gt; 1023, 1023, _xlfn.FLOOR.MATH(K53/2^10))</f>
@@ -1749,11 +1747,11 @@
       </c>
       <c r="L55" s="2">
         <f ca="1">K57*(1023-J55)</f>
-        <v>964689</v>
+        <v>498201</v>
       </c>
       <c r="M55" s="2">
         <f ca="1">$L$57</f>
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="N55" s="2">
         <f>0</f>
@@ -1765,7 +1763,7 @@
       </c>
       <c r="P55" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>262271</v>
+        <v>2162815</v>
       </c>
     </row>
     <row r="56" spans="2:16" x14ac:dyDescent="0.3">
@@ -1791,11 +1789,11 @@
       </c>
       <c r="O56" s="2">
         <f ca="1">$L$59</f>
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="P56" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>8323130</v>
+        <v>8323102</v>
       </c>
     </row>
     <row r="57" spans="2:16" x14ac:dyDescent="0.3">
@@ -1811,7 +1809,7 @@
       </c>
       <c r="L57" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(L53/2^(2*B41-8))</f>
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="M57" s="2">
         <f ca="1">$L$51</f>
@@ -1819,7 +1817,7 @@
       </c>
       <c r="N57" s="2">
         <f ca="1">$L$57</f>
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="O57" s="2">
         <f>0</f>
@@ -1827,7 +1825,7 @@
       </c>
       <c r="P57" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>8324096</v>
+        <v>8331520</v>
       </c>
     </row>
     <row r="58" spans="2:16" x14ac:dyDescent="0.3">
@@ -1841,11 +1839,11 @@
     <row r="59" spans="2:16" x14ac:dyDescent="0.3">
       <c r="L59" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(L55/2^(2*B41-8))</f>
-        <v>58</v>
-      </c>
-      <c r="M59" s="2" t="e" cm="1">
+        <v>30</v>
+      </c>
+      <c r="M59" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="M59" ca="1">_xlfn.BASE(_xlfn.SWITCH(J53,0,P51,1,P52,2,P53,3,P54,4,P55,5,P56,6,P57),16,6)</f>
-        <v>#N/A</v>
+        <v>1E7F00</v>
       </c>
     </row>
     <row r="60" spans="2:16" x14ac:dyDescent="0.3">
@@ -1872,7 +1870,7 @@
       </c>
       <c r="I63" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(H76/B43)</f>
-        <v>313</v>
+        <v>285</v>
       </c>
       <c r="J63" s="2">
         <f t="shared" ref="J63:J74" ca="1" si="12">_xlfn.FLOOR.MATH(H63/I$63)</f>
@@ -1880,7 +1878,7 @@
       </c>
       <c r="L63" s="2">
         <f ca="1">L51-L57-L59</f>
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="64" spans="2:16" x14ac:dyDescent="0.3">
@@ -1900,25 +1898,25 @@
     <row r="65" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G65" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 2] = 16'b0000000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 2] = 16'b0000000110001110;</v>
       </c>
       <c r="H65" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>398</v>
       </c>
       <c r="J65" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G66" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 3] = 16'b0000000011000001;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 3] = 16'b0000000000000000;</v>
       </c>
       <c r="H66" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>193</v>
+        <v>0</v>
       </c>
       <c r="J66" s="2">
         <f t="shared" ca="1" si="12"/>
@@ -1942,53 +1940,53 @@
     <row r="68" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G68" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 5] = 16'b0001000011000001;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 5] = 16'b0001100110001110;</v>
       </c>
       <c r="H68" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>4289</v>
+        <v>6542</v>
       </c>
       <c r="J68" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G69" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 6] = 16'b0001000011000001;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 6] = 16'b0000000000000000;</v>
       </c>
       <c r="H69" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>4289</v>
+        <v>0</v>
       </c>
       <c r="J69" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G70" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 7] = 16'b0001000011000001;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 7] = 16'b0000000110001110;</v>
       </c>
       <c r="H70" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>4289</v>
+        <v>398</v>
       </c>
       <c r="J70" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G71" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 8] = 16'b0000000011000001;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 8] = 16'b0000000000000000;</v>
       </c>
       <c r="H71" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>193</v>
+        <v>0</v>
       </c>
       <c r="J71" s="2">
         <f t="shared" ca="1" si="12"/>
@@ -1998,15 +1996,15 @@
     <row r="72" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G72" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 9] = 16'b0000100011000001;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 9] = 16'b0000100110001110;</v>
       </c>
       <c r="H72" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>2241</v>
+        <v>2446</v>
       </c>
       <c r="J72" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73" spans="1:25" x14ac:dyDescent="0.3">
@@ -2026,21 +2024,21 @@
     <row r="74" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G74" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[11] = 16'b0000000011000001;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[11] = 16'b0001000110001110;</v>
       </c>
       <c r="H74" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>193</v>
+        <v>4494</v>
       </c>
       <c r="J74" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="75" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G75" s="5" t="str">
         <f ca="1">_xlfn.CONCAT("            amplitudeSumNew_i = ",B40+B41+_xlfn.CEILING.MATH(IMLOG2(B43)),"'b",_xlfn.BASE(H76,2,B40+B41+_xlfn.CEILING.MATH(IMLOG2(B43))),";")</f>
-        <v xml:space="preserve">            amplitudeSumNew_i = 22'b0000000011110101000111;</v>
+        <v xml:space="preserve">            amplitudeSumNew_i = 22'b0000000011011111000110;</v>
       </c>
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.3">
@@ -2049,7 +2047,7 @@
       </c>
       <c r="H76" s="2">
         <f ca="1">SUM(H63:H74)</f>
-        <v>15687</v>
+        <v>14278</v>
       </c>
     </row>
     <row r="78" spans="1:25" x14ac:dyDescent="0.3">
@@ -2138,7 +2136,7 @@
         <v>51</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J82" s="2" t="s">
         <v>10</v>
@@ -2153,115 +2151,115 @@
     <row r="83" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F83" s="2">
         <f t="shared" ref="F83:F94" ca="1" si="14">H83/2^B$41</f>
-        <v>0.29296875</v>
+        <v>31.99951171875</v>
       </c>
       <c r="G83" s="6" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="H83" s="2" cm="1">
         <f t="array" aca="1" ref="H83" ca="1">SUMPRODUCT(--MID(G83,LEN(G83)+1-ROW(INDIRECT("1:"&amp;LEN(G83))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G83)))-1)))</f>
-        <v>600</v>
+        <v>65535</v>
       </c>
       <c r="I83" s="2" t="s">
         <v>9</v>
       </c>
       <c r="J83" s="2">
         <f t="shared" ref="J83:J94" ca="1" si="15">H83-I$87</f>
-        <v>423.12744140625</v>
+        <v>39296</v>
       </c>
       <c r="K83" s="2">
         <f ca="1">IF(J83&lt;0, 0, J83)</f>
-        <v>423.12744140625</v>
+        <v>39296</v>
       </c>
       <c r="L83" s="2">
         <f ca="1">IF(K83=0,0,H83)</f>
-        <v>600</v>
+        <v>65535</v>
       </c>
     </row>
     <row r="84" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F84" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>0.35009765625</v>
+        <v>31.99951171875</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="H84" s="2" cm="1">
         <f t="array" aca="1" ref="H84" ca="1">SUMPRODUCT(--MID(G84,LEN(G84)+1-ROW(INDIRECT("1:"&amp;LEN(G84))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G84)))-1)))</f>
-        <v>717</v>
+        <v>65535</v>
       </c>
       <c r="I84" s="2">
         <f ca="1">SUM(H83:H94)</f>
-        <v>1767</v>
+        <v>262140</v>
       </c>
       <c r="J84" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>540.12744140625</v>
+        <v>39296</v>
       </c>
       <c r="K84" s="2">
         <f t="shared" ref="K84:K94" ca="1" si="16">IF(J84&lt;0, 0, J84)</f>
-        <v>540.12744140625</v>
+        <v>39296</v>
       </c>
       <c r="L84" s="2">
         <f t="shared" ref="L84:L94" ca="1" si="17">IF(K84=0,0,H84)</f>
-        <v>717</v>
+        <v>65535</v>
       </c>
     </row>
     <row r="85" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F85" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>0.2197265625</v>
+        <v>31.99951171875</v>
       </c>
       <c r="G85" s="6" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="H85" s="2" cm="1">
         <f t="array" aca="1" ref="H85" ca="1">SUMPRODUCT(--MID(G85,LEN(G85)+1-ROW(INDIRECT("1:"&amp;LEN(G85))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G85)))-1)))</f>
-        <v>450</v>
+        <v>65535</v>
       </c>
       <c r="I85" s="2">
         <f ca="1">I84/2^B41</f>
-        <v>0.86279296875</v>
+        <v>127.998046875</v>
       </c>
       <c r="J85" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>273.12744140625</v>
+        <v>39296</v>
       </c>
       <c r="K85" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>273.12744140625</v>
+        <v>39296</v>
       </c>
       <c r="L85" s="2">
         <f t="shared" ca="1" si="17"/>
-        <v>450</v>
+        <v>65535</v>
       </c>
     </row>
     <row r="86" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F86" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>0</v>
+        <v>31.99951171875</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="H86" s="2" cm="1">
         <f t="array" aca="1" ref="H86" ca="1">SUMPRODUCT(--MID(G86,LEN(G86)+1-ROW(INDIRECT("1:"&amp;LEN(G86))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G86)))-1)))</f>
-        <v>0</v>
+        <v>65535</v>
       </c>
       <c r="I86" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="J86" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>-176.87255859375</v>
+        <v>39296</v>
       </c>
       <c r="K86" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>39296</v>
       </c>
       <c r="L86" s="2">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>65535</v>
       </c>
     </row>
     <row r="87" spans="6:15" x14ac:dyDescent="0.3">
@@ -2277,12 +2275,12 @@
         <v>0</v>
       </c>
       <c r="I87" s="2">
-        <f ca="1">I84*BIN2DEC(C42)/2^B41</f>
-        <v>176.87255859375</v>
+        <f ca="1">_xlfn.FLOOR.MATH(I84*D42/2^B41)</f>
+        <v>26239</v>
       </c>
       <c r="J87" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>-176.87255859375</v>
+        <v>-26239</v>
       </c>
       <c r="K87" s="2">
         <f t="shared" ca="1" si="16"/>
@@ -2307,11 +2305,11 @@
       </c>
       <c r="I88" s="2">
         <f ca="1">I85*B42</f>
-        <v>8.5942268371582031E-2</v>
+        <v>12.749805450439453</v>
       </c>
       <c r="J88" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>-176.87255859375</v>
+        <v>-26239</v>
       </c>
       <c r="K88" s="2">
         <f t="shared" ca="1" si="16"/>
@@ -2339,7 +2337,7 @@
       </c>
       <c r="J89" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>-176.87255859375</v>
+        <v>-26239</v>
       </c>
       <c r="K89" s="2">
         <f t="shared" ca="1" si="16"/>
@@ -2364,11 +2362,11 @@
       </c>
       <c r="I90" s="2">
         <f ca="1">SUM(K83:K94)</f>
-        <v>1236.38232421875</v>
+        <v>157184</v>
       </c>
       <c r="J90" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>-176.87255859375</v>
+        <v>-26239</v>
       </c>
       <c r="K90" s="2">
         <f t="shared" ca="1" si="16"/>
@@ -2393,7 +2391,7 @@
       </c>
       <c r="J91" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>-176.87255859375</v>
+        <v>-26239</v>
       </c>
       <c r="K91" s="2">
         <f t="shared" ca="1" si="16"/>
@@ -2422,7 +2420,7 @@
       </c>
       <c r="J92" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>-176.87255859375</v>
+        <v>-26239</v>
       </c>
       <c r="K92" s="2">
         <f t="shared" ca="1" si="16"/>
@@ -2447,7 +2445,7 @@
       </c>
       <c r="J93" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>-176.87255859375</v>
+        <v>-26239</v>
       </c>
       <c r="K93" s="2">
         <f t="shared" ca="1" si="16"/>
@@ -2472,7 +2470,7 @@
       </c>
       <c r="J94" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>-176.87255859375</v>
+        <v>-26239</v>
       </c>
       <c r="K94" s="2">
         <f t="shared" ca="1" si="16"/>
@@ -2500,13 +2498,13 @@
         <v>17</v>
       </c>
       <c r="M96" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N96" s="2" t="s">
         <v>23</v>
       </c>
       <c r="O96" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="97" spans="5:25" x14ac:dyDescent="0.3">
@@ -2515,7 +2513,7 @@
         <v>23.986328125</v>
       </c>
       <c r="G97" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H97" s="2" cm="1">
         <f t="array" aca="1" ref="H97" ca="1">SUMPRODUCT(--MID(G97,LEN(G97)+1-ROW(INDIRECT("1:"&amp;LEN(G97))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G97)))-1)))</f>
@@ -2560,11 +2558,11 @@
     </row>
     <row r="98" spans="5:25" x14ac:dyDescent="0.3">
       <c r="F98" s="2">
-        <f t="shared" ref="F98:F109" ca="1" si="19">H98/2^B$41</f>
+        <f t="shared" ref="F98:F108" ca="1" si="19">H98/2^B$41</f>
         <v>12.048828125</v>
       </c>
       <c r="G98" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H98" s="2" cm="1">
         <f t="array" aca="1" ref="H98" ca="1">SUMPRODUCT(--MID(G98,LEN(G98)+1-ROW(INDIRECT("1:"&amp;LEN(G98))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G98)))-1)))</f>
@@ -2613,7 +2611,7 @@
         <v>19.986328125</v>
       </c>
       <c r="G99" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H99" s="2" cm="1">
         <f t="array" aca="1" ref="H99" ca="1">SUMPRODUCT(--MID(G99,LEN(G99)+1-ROW(INDIRECT("1:"&amp;LEN(G99))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G99)))-1)))</f>
@@ -2662,7 +2660,7 @@
         <v>21.048828125</v>
       </c>
       <c r="G100" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H100" s="2" cm="1">
         <f t="array" aca="1" ref="H100" ca="1">SUMPRODUCT(--MID(G100,LEN(G100)+1-ROW(INDIRECT("1:"&amp;LEN(G100))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(G100)))-1)))</f>
@@ -3148,7 +3146,7 @@
     </row>
     <row r="111" spans="5:25" x14ac:dyDescent="0.3">
       <c r="I111" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J111" s="2" t="s">
         <v>29</v>
@@ -3184,19 +3182,19 @@
         <v>40</v>
       </c>
       <c r="U111" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="V111" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="W111" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="X111" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="V111" s="2" t="s">
+      <c r="Y111" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="W111" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="X111" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="Y111" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="112" spans="5:25" x14ac:dyDescent="0.3">
@@ -3214,47 +3212,47 @@
       </c>
       <c r="L112" s="2">
         <f ca="1">IF(E57,K83,L83)</f>
-        <v>600</v>
+        <v>65535</v>
       </c>
       <c r="M112" s="2">
-        <f t="shared" ref="M112:M123" ca="1" si="29">L112*E$54</f>
-        <v>1966200</v>
+        <f ca="1">L112*E$54</f>
+        <v>214758195</v>
       </c>
       <c r="N112" s="2">
-        <f t="shared" ref="N112:N123" ca="1" si="30">IF(_xlfn.FLOOR.MATH(M112/2^B$41) &gt; 1023, 1023, _xlfn.FLOOR.MATH(M112/2^B$41))</f>
-        <v>960</v>
+        <f t="shared" ref="N112:N123" ca="1" si="29">IF(_xlfn.FLOOR.MATH(M112/2^B$41) &gt; 1023, 1023, _xlfn.FLOOR.MATH(M112/2^B$41))</f>
+        <v>1023</v>
       </c>
       <c r="O112" s="2">
-        <f t="shared" ref="O112:O123" ca="1" si="31">IF(N112&gt;E$56,E$56,N112)</f>
-        <v>960</v>
+        <f t="shared" ref="O112:O123" ca="1" si="30">IF(N112&gt;E$56,E$56,N112)</f>
+        <v>1023</v>
       </c>
       <c r="P112" s="2">
-        <f t="shared" ref="P112:P123" ca="1" si="32">_xlfn.FLOOR.MATH(O112/2^(B$41-8))</f>
-        <v>120</v>
+        <f ca="1">_xlfn.FLOOR.MATH(O112/2^(B$41-9))</f>
+        <v>255</v>
       </c>
       <c r="Q112" s="2">
         <f ca="1">O112*K112</f>
-        <v>1958400</v>
+        <v>2086920</v>
       </c>
       <c r="R112" s="2">
-        <f t="shared" ref="R112:R123" ca="1" si="33">O112*(2^(B$41) - 1 - K112)</f>
-        <v>6720</v>
+        <f t="shared" ref="R112:R123" ca="1" si="31">O112*(2^(B$41) - 1 - K112)</f>
+        <v>7161</v>
       </c>
       <c r="S112" s="2">
-        <f t="shared" ref="S112:S123" ca="1" si="34">_xlfn.FLOOR.MATH(Q112/2^(2*B$41-8))</f>
-        <v>119</v>
+        <f ca="1">_xlfn.FLOOR.MATH(Q112/2^(2*B$41-9))</f>
+        <v>254</v>
       </c>
       <c r="T112" s="2">
-        <f t="shared" ref="T112:T123" ca="1" si="35">_xlfn.FLOOR.MATH(R112/2^(2*B$41-8))</f>
+        <f t="shared" ref="T112:T123" ca="1" si="32">_xlfn.FLOOR.MATH(R112/2^(2*B$41-8))</f>
         <v>0</v>
       </c>
       <c r="U112" s="2" cm="1">
         <f t="array" aca="1" ref="U112" ca="1">_xlfn.SWITCH(J112,0,P112,1,T112,2,0,3,0,4,S112,5,P112)</f>
-        <v>120</v>
+        <v>255</v>
       </c>
       <c r="V112" s="2" cm="1">
         <f t="array" aca="1" ref="V112" ca="1">_xlfn.SWITCH(J112,0,S112,1,P112,2,P112,3,T112,4,0,5,0)</f>
-        <v>119</v>
+        <v>254</v>
       </c>
       <c r="W112" s="2" cm="1">
         <f t="array" aca="1" ref="W112" ca="1">_xlfn.SWITCH(J112,0,0,1,0,2,S112,3,P112,4,P112,5,T112)</f>
@@ -3262,11 +3260,11 @@
       </c>
       <c r="X112" s="2">
         <f ca="1">U112*2^16+V112*2^8+W112</f>
-        <v>7894784</v>
+        <v>16776704</v>
       </c>
       <c r="Y112" s="2" t="str">
-        <f t="shared" ref="Y112:Y123" ca="1" si="36">_xlfn.BASE(X112,16,6)</f>
-        <v>787700</v>
+        <f t="shared" ref="Y112:Y123" ca="1" si="33">_xlfn.BASE(X112,16,6)</f>
+        <v>FFFE00</v>
       </c>
     </row>
     <row r="113" spans="9:25" x14ac:dyDescent="0.3">
@@ -3283,44 +3281,44 @@
         <v>2020</v>
       </c>
       <c r="L113" s="2">
-        <f t="shared" ref="L113:L123" ca="1" si="37">IF(E58,K84,L84)</f>
-        <v>717</v>
+        <f t="shared" ref="L113:L123" ca="1" si="34">IF(E58,K84,L84)</f>
+        <v>65535</v>
       </c>
       <c r="M113" s="2">
+        <f t="shared" ref="M112:M123" ca="1" si="35">L113*E$54</f>
+        <v>214758195</v>
+      </c>
+      <c r="N113" s="2">
         <f t="shared" ca="1" si="29"/>
-        <v>2349609</v>
-      </c>
-      <c r="N113" s="2">
+        <v>1023</v>
+      </c>
+      <c r="O113" s="2">
         <f t="shared" ca="1" si="30"/>
         <v>1023</v>
       </c>
-      <c r="O113" s="2">
+      <c r="P113" s="2">
+        <f t="shared" ref="P113:P123" ca="1" si="36">_xlfn.FLOOR.MATH(O113/2^(B$41-9))</f>
+        <v>255</v>
+      </c>
+      <c r="Q113" s="2">
+        <f t="shared" ref="Q113:Q123" ca="1" si="37">O113*K113</f>
+        <v>2066460</v>
+      </c>
+      <c r="R113" s="2">
         <f t="shared" ca="1" si="31"/>
-        <v>1023</v>
-      </c>
-      <c r="P113" s="2">
+        <v>27621</v>
+      </c>
+      <c r="S113" s="2">
+        <f t="shared" ref="S113:S123" ca="1" si="38">_xlfn.FLOOR.MATH(Q113/2^(2*B$41-9))</f>
+        <v>252</v>
+      </c>
+      <c r="T113" s="2">
         <f t="shared" ca="1" si="32"/>
-        <v>127</v>
-      </c>
-      <c r="Q113" s="2">
-        <f t="shared" ref="Q113:Q123" ca="1" si="38">O113*K113</f>
-        <v>2066460</v>
-      </c>
-      <c r="R113" s="2">
-        <f t="shared" ca="1" si="33"/>
-        <v>27621</v>
-      </c>
-      <c r="S113" s="2">
-        <f t="shared" ca="1" si="34"/>
-        <v>126</v>
-      </c>
-      <c r="T113" s="2">
-        <f t="shared" ca="1" si="35"/>
         <v>1</v>
       </c>
       <c r="U113" s="2" cm="1">
         <f t="array" aca="1" ref="U113" ca="1">_xlfn.SWITCH(J113,0,P113,1,T113,2,0,3,0,4,S113,5,P113)</f>
-        <v>126</v>
+        <v>252</v>
       </c>
       <c r="V113" s="2" cm="1">
         <f t="array" aca="1" ref="V113" ca="1">_xlfn.SWITCH(J113,0,S113,1,P113,2,P113,3,T113,4,0,5,0)</f>
@@ -3328,15 +3326,15 @@
       </c>
       <c r="W113" s="2" cm="1">
         <f t="array" aca="1" ref="W113" ca="1">_xlfn.SWITCH(J113,0,0,1,0,2,S113,3,P113,4,P113,5,T113)</f>
-        <v>127</v>
+        <v>255</v>
       </c>
       <c r="X113" s="2">
         <f t="shared" ref="X113:X123" ca="1" si="39">U113*2^16+V113*2^8+W113</f>
-        <v>8257663</v>
+        <v>16515327</v>
       </c>
       <c r="Y113" s="2" t="str">
-        <f t="shared" ca="1" si="36"/>
-        <v>7E007F</v>
+        <f t="shared" ca="1" si="33"/>
+        <v>FC00FF</v>
       </c>
     </row>
     <row r="114" spans="9:25" x14ac:dyDescent="0.3">
@@ -3353,40 +3351,40 @@
         <v>1016</v>
       </c>
       <c r="L114" s="2">
+        <f t="shared" ca="1" si="34"/>
+        <v>65535</v>
+      </c>
+      <c r="M114" s="2">
+        <f t="shared" ca="1" si="35"/>
+        <v>214758195</v>
+      </c>
+      <c r="N114" s="2">
+        <f t="shared" ca="1" si="29"/>
+        <v>1023</v>
+      </c>
+      <c r="O114" s="2">
+        <f t="shared" ca="1" si="30"/>
+        <v>1023</v>
+      </c>
+      <c r="P114" s="2">
+        <f t="shared" ca="1" si="36"/>
+        <v>255</v>
+      </c>
+      <c r="Q114" s="2">
         <f t="shared" ca="1" si="37"/>
-        <v>450</v>
-      </c>
-      <c r="M114" s="2">
-        <f t="shared" ca="1" si="29"/>
-        <v>1474650</v>
-      </c>
-      <c r="N114" s="2">
-        <f t="shared" ca="1" si="30"/>
-        <v>720</v>
-      </c>
-      <c r="O114" s="2">
+        <v>1039368</v>
+      </c>
+      <c r="R114" s="2">
         <f t="shared" ca="1" si="31"/>
-        <v>720</v>
-      </c>
-      <c r="P114" s="2">
+        <v>1054713</v>
+      </c>
+      <c r="S114" s="2">
+        <f t="shared" ca="1" si="38"/>
+        <v>126</v>
+      </c>
+      <c r="T114" s="2">
         <f t="shared" ca="1" si="32"/>
-        <v>90</v>
-      </c>
-      <c r="Q114" s="2">
-        <f t="shared" ca="1" si="38"/>
-        <v>731520</v>
-      </c>
-      <c r="R114" s="2">
-        <f t="shared" ca="1" si="33"/>
-        <v>742320</v>
-      </c>
-      <c r="S114" s="2">
-        <f t="shared" ca="1" si="34"/>
-        <v>44</v>
-      </c>
-      <c r="T114" s="2">
-        <f t="shared" ca="1" si="35"/>
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="U114" s="2" cm="1">
         <f t="array" aca="1" ref="U114" ca="1">_xlfn.SWITCH(J114,0,P114,1,T114,2,0,3,0,4,S114,5,P114)</f>
@@ -3394,19 +3392,19 @@
       </c>
       <c r="V114" s="2" cm="1">
         <f t="array" aca="1" ref="V114" ca="1">_xlfn.SWITCH(J114,0,S114,1,P114,2,P114,3,T114,4,0,5,0)</f>
-        <v>90</v>
+        <v>255</v>
       </c>
       <c r="W114" s="2" cm="1">
         <f t="array" aca="1" ref="W114" ca="1">_xlfn.SWITCH(J114,0,0,1,0,2,S114,3,P114,4,P114,5,T114)</f>
-        <v>44</v>
+        <v>126</v>
       </c>
       <c r="X114" s="2">
         <f t="shared" ca="1" si="39"/>
-        <v>23084</v>
+        <v>65406</v>
       </c>
       <c r="Y114" s="2" t="str">
-        <f t="shared" ca="1" si="36"/>
-        <v>005A2C</v>
+        <f t="shared" ca="1" si="33"/>
+        <v>00FF7E</v>
       </c>
     </row>
     <row r="115" spans="9:25" x14ac:dyDescent="0.3">
@@ -3423,40 +3421,40 @@
         <v>200</v>
       </c>
       <c r="L115" s="2">
+        <f t="shared" ca="1" si="34"/>
+        <v>65535</v>
+      </c>
+      <c r="M115" s="2">
+        <f t="shared" ca="1" si="35"/>
+        <v>214758195</v>
+      </c>
+      <c r="N115" s="2">
+        <f t="shared" ca="1" si="29"/>
+        <v>1023</v>
+      </c>
+      <c r="O115" s="2">
+        <f t="shared" ca="1" si="30"/>
+        <v>1023</v>
+      </c>
+      <c r="P115" s="2">
+        <f t="shared" ca="1" si="36"/>
+        <v>255</v>
+      </c>
+      <c r="Q115" s="2">
         <f t="shared" ca="1" si="37"/>
-        <v>0</v>
-      </c>
-      <c r="M115" s="2">
-        <f t="shared" ca="1" si="29"/>
-        <v>0</v>
-      </c>
-      <c r="N115" s="2">
-        <f t="shared" ca="1" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="O115" s="2">
+        <v>204600</v>
+      </c>
+      <c r="R115" s="2">
         <f t="shared" ca="1" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="P115" s="2">
+        <v>1889481</v>
+      </c>
+      <c r="S115" s="2">
+        <f t="shared" ca="1" si="38"/>
+        <v>24</v>
+      </c>
+      <c r="T115" s="2">
         <f t="shared" ca="1" si="32"/>
-        <v>0</v>
-      </c>
-      <c r="Q115" s="2">
-        <f t="shared" ca="1" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="R115" s="2">
-        <f t="shared" ca="1" si="33"/>
-        <v>0</v>
-      </c>
-      <c r="S115" s="2">
-        <f t="shared" ca="1" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="T115" s="2">
-        <f t="shared" ca="1" si="35"/>
-        <v>0</v>
+        <v>115</v>
       </c>
       <c r="U115" s="2" cm="1">
         <f t="array" aca="1" ref="U115" ca="1">_xlfn.SWITCH(J115,0,P115,1,T115,2,0,3,0,4,S115,5,P115)</f>
@@ -3464,19 +3462,19 @@
       </c>
       <c r="V115" s="2" cm="1">
         <f t="array" aca="1" ref="V115" ca="1">_xlfn.SWITCH(J115,0,S115,1,P115,2,P115,3,T115,4,0,5,0)</f>
-        <v>0</v>
+        <v>255</v>
       </c>
       <c r="W115" s="2" cm="1">
         <f t="array" aca="1" ref="W115" ca="1">_xlfn.SWITCH(J115,0,0,1,0,2,S115,3,P115,4,P115,5,T115)</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="X115" s="2">
         <f t="shared" ca="1" si="39"/>
-        <v>0</v>
+        <v>65304</v>
       </c>
       <c r="Y115" s="2" t="str">
-        <f t="shared" ca="1" si="36"/>
-        <v>000000</v>
+        <f t="shared" ca="1" si="33"/>
+        <v>00FF18</v>
       </c>
     </row>
     <row r="116" spans="9:25" x14ac:dyDescent="0.3">
@@ -3493,39 +3491,39 @@
         <v>1944</v>
       </c>
       <c r="L116" s="2">
+        <f t="shared" ca="1" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="M116" s="2">
+        <f t="shared" ca="1" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="N116" s="2">
+        <f t="shared" ca="1" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="O116" s="2">
+        <f t="shared" ca="1" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="P116" s="2">
+        <f t="shared" ca="1" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="Q116" s="2">
         <f t="shared" ca="1" si="37"/>
         <v>0</v>
       </c>
-      <c r="M116" s="2">
-        <f t="shared" ca="1" si="29"/>
-        <v>0</v>
-      </c>
-      <c r="N116" s="2">
-        <f t="shared" ca="1" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="O116" s="2">
+      <c r="R116" s="2">
         <f t="shared" ca="1" si="31"/>
         <v>0</v>
       </c>
-      <c r="P116" s="2">
+      <c r="S116" s="2">
+        <f t="shared" ca="1" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="T116" s="2">
         <f t="shared" ca="1" si="32"/>
-        <v>0</v>
-      </c>
-      <c r="Q116" s="2">
-        <f t="shared" ca="1" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="R116" s="2">
-        <f t="shared" ca="1" si="33"/>
-        <v>0</v>
-      </c>
-      <c r="S116" s="2">
-        <f t="shared" ca="1" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="T116" s="2">
-        <f t="shared" ca="1" si="35"/>
         <v>0</v>
       </c>
       <c r="U116" s="2" cm="1">
@@ -3545,7 +3543,7 @@
         <v>0</v>
       </c>
       <c r="Y116" s="2" t="str">
-        <f t="shared" ca="1" si="36"/>
+        <f t="shared" ca="1" si="33"/>
         <v>000000</v>
       </c>
     </row>
@@ -3563,39 +3561,39 @@
         <v>1956</v>
       </c>
       <c r="L117" s="2">
+        <f t="shared" ca="1" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="M117" s="2">
+        <f t="shared" ca="1" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="N117" s="2">
+        <f t="shared" ca="1" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="O117" s="2">
+        <f t="shared" ca="1" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="P117" s="2">
+        <f t="shared" ca="1" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="Q117" s="2">
         <f t="shared" ca="1" si="37"/>
         <v>0</v>
       </c>
-      <c r="M117" s="2">
-        <f t="shared" ca="1" si="29"/>
-        <v>0</v>
-      </c>
-      <c r="N117" s="2">
-        <f t="shared" ca="1" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="O117" s="2">
+      <c r="R117" s="2">
         <f t="shared" ca="1" si="31"/>
         <v>0</v>
       </c>
-      <c r="P117" s="2">
+      <c r="S117" s="2">
+        <f t="shared" ca="1" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="T117" s="2">
         <f t="shared" ca="1" si="32"/>
-        <v>0</v>
-      </c>
-      <c r="Q117" s="2">
-        <f t="shared" ca="1" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="R117" s="2">
-        <f t="shared" ca="1" si="33"/>
-        <v>0</v>
-      </c>
-      <c r="S117" s="2">
-        <f t="shared" ca="1" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="T117" s="2">
-        <f t="shared" ca="1" si="35"/>
         <v>0</v>
       </c>
       <c r="U117" s="2" cm="1">
@@ -3615,7 +3613,7 @@
         <v>0</v>
       </c>
       <c r="Y117" s="2" t="str">
-        <f t="shared" ca="1" si="36"/>
+        <f t="shared" ca="1" si="33"/>
         <v>000000</v>
       </c>
     </row>
@@ -3633,39 +3631,39 @@
         <v>1992</v>
       </c>
       <c r="L118" s="2">
+        <f t="shared" ca="1" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="M118" s="2">
+        <f t="shared" ca="1" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="N118" s="2">
+        <f t="shared" ca="1" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="O118" s="2">
+        <f t="shared" ca="1" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="P118" s="2">
+        <f t="shared" ca="1" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="Q118" s="2">
         <f t="shared" ca="1" si="37"/>
         <v>0</v>
       </c>
-      <c r="M118" s="2">
-        <f t="shared" ca="1" si="29"/>
-        <v>0</v>
-      </c>
-      <c r="N118" s="2">
-        <f t="shared" ca="1" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="O118" s="2">
+      <c r="R118" s="2">
         <f t="shared" ca="1" si="31"/>
         <v>0</v>
       </c>
-      <c r="P118" s="2">
+      <c r="S118" s="2">
+        <f t="shared" ca="1" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="T118" s="2">
         <f t="shared" ca="1" si="32"/>
-        <v>0</v>
-      </c>
-      <c r="Q118" s="2">
-        <f t="shared" ca="1" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="R118" s="2">
-        <f t="shared" ca="1" si="33"/>
-        <v>0</v>
-      </c>
-      <c r="S118" s="2">
-        <f t="shared" ca="1" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="T118" s="2">
-        <f t="shared" ca="1" si="35"/>
         <v>0</v>
       </c>
       <c r="U118" s="2" cm="1">
@@ -3685,7 +3683,7 @@
         <v>0</v>
       </c>
       <c r="Y118" s="2" t="str">
-        <f t="shared" ca="1" si="36"/>
+        <f t="shared" ca="1" si="33"/>
         <v>000000</v>
       </c>
     </row>
@@ -3703,39 +3701,39 @@
         <v>1968</v>
       </c>
       <c r="L119" s="2">
+        <f t="shared" ca="1" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="M119" s="2">
+        <f t="shared" ca="1" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="N119" s="2">
+        <f t="shared" ca="1" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="O119" s="2">
+        <f t="shared" ca="1" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="P119" s="2">
+        <f t="shared" ca="1" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="Q119" s="2">
         <f t="shared" ca="1" si="37"/>
         <v>0</v>
       </c>
-      <c r="M119" s="2">
-        <f t="shared" ca="1" si="29"/>
-        <v>0</v>
-      </c>
-      <c r="N119" s="2">
-        <f t="shared" ca="1" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="O119" s="2">
+      <c r="R119" s="2">
         <f t="shared" ca="1" si="31"/>
         <v>0</v>
       </c>
-      <c r="P119" s="2">
+      <c r="S119" s="2">
+        <f t="shared" ca="1" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="T119" s="2">
         <f t="shared" ca="1" si="32"/>
-        <v>0</v>
-      </c>
-      <c r="Q119" s="2">
-        <f t="shared" ca="1" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="R119" s="2">
-        <f t="shared" ca="1" si="33"/>
-        <v>0</v>
-      </c>
-      <c r="S119" s="2">
-        <f t="shared" ca="1" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="T119" s="2">
-        <f t="shared" ca="1" si="35"/>
         <v>0</v>
       </c>
       <c r="U119" s="2" cm="1">
@@ -3755,7 +3753,7 @@
         <v>0</v>
       </c>
       <c r="Y119" s="2" t="str">
-        <f t="shared" ca="1" si="36"/>
+        <f t="shared" ca="1" si="33"/>
         <v>000000</v>
       </c>
     </row>
@@ -3773,39 +3771,39 @@
         <v>2040</v>
       </c>
       <c r="L120" s="2">
+        <f t="shared" ca="1" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="M120" s="2">
+        <f t="shared" ca="1" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="N120" s="2">
+        <f t="shared" ca="1" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="O120" s="2">
+        <f t="shared" ca="1" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="P120" s="2">
+        <f t="shared" ca="1" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="Q120" s="2">
         <f t="shared" ca="1" si="37"/>
         <v>0</v>
       </c>
-      <c r="M120" s="2">
-        <f t="shared" ca="1" si="29"/>
-        <v>0</v>
-      </c>
-      <c r="N120" s="2">
-        <f t="shared" ca="1" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="O120" s="2">
+      <c r="R120" s="2">
         <f t="shared" ca="1" si="31"/>
         <v>0</v>
       </c>
-      <c r="P120" s="2">
+      <c r="S120" s="2">
+        <f t="shared" ca="1" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="T120" s="2">
         <f t="shared" ca="1" si="32"/>
-        <v>0</v>
-      </c>
-      <c r="Q120" s="2">
-        <f t="shared" ca="1" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="R120" s="2">
-        <f t="shared" ca="1" si="33"/>
-        <v>0</v>
-      </c>
-      <c r="S120" s="2">
-        <f t="shared" ca="1" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="T120" s="2">
-        <f t="shared" ca="1" si="35"/>
         <v>0</v>
       </c>
       <c r="U120" s="2" cm="1">
@@ -3825,7 +3823,7 @@
         <v>0</v>
       </c>
       <c r="Y120" s="2" t="str">
-        <f t="shared" ca="1" si="36"/>
+        <f t="shared" ca="1" si="33"/>
         <v>000000</v>
       </c>
     </row>
@@ -3843,39 +3841,39 @@
         <v>1932</v>
       </c>
       <c r="L121" s="2">
+        <f t="shared" ca="1" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="M121" s="2">
+        <f t="shared" ca="1" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="N121" s="2">
+        <f t="shared" ca="1" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="O121" s="2">
+        <f t="shared" ca="1" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="P121" s="2">
+        <f t="shared" ca="1" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="Q121" s="2">
         <f t="shared" ca="1" si="37"/>
         <v>0</v>
       </c>
-      <c r="M121" s="2">
-        <f t="shared" ca="1" si="29"/>
-        <v>0</v>
-      </c>
-      <c r="N121" s="2">
-        <f t="shared" ca="1" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="O121" s="2">
+      <c r="R121" s="2">
         <f t="shared" ca="1" si="31"/>
         <v>0</v>
       </c>
-      <c r="P121" s="2">
+      <c r="S121" s="2">
+        <f t="shared" ca="1" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="T121" s="2">
         <f t="shared" ca="1" si="32"/>
-        <v>0</v>
-      </c>
-      <c r="Q121" s="2">
-        <f t="shared" ca="1" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="R121" s="2">
-        <f t="shared" ca="1" si="33"/>
-        <v>0</v>
-      </c>
-      <c r="S121" s="2">
-        <f t="shared" ca="1" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="T121" s="2">
-        <f t="shared" ca="1" si="35"/>
         <v>0</v>
       </c>
       <c r="U121" s="2" cm="1">
@@ -3895,7 +3893,7 @@
         <v>0</v>
       </c>
       <c r="Y121" s="2" t="str">
-        <f t="shared" ca="1" si="36"/>
+        <f t="shared" ca="1" si="33"/>
         <v>000000</v>
       </c>
     </row>
@@ -3913,39 +3911,39 @@
         <v>1932</v>
       </c>
       <c r="L122" s="2">
+        <f t="shared" ca="1" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="M122" s="2">
+        <f t="shared" ca="1" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="N122" s="2">
+        <f t="shared" ca="1" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="O122" s="2">
+        <f t="shared" ca="1" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="P122" s="2">
+        <f t="shared" ca="1" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="Q122" s="2">
         <f t="shared" ca="1" si="37"/>
         <v>0</v>
       </c>
-      <c r="M122" s="2">
-        <f t="shared" ca="1" si="29"/>
-        <v>0</v>
-      </c>
-      <c r="N122" s="2">
-        <f t="shared" ca="1" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="O122" s="2">
+      <c r="R122" s="2">
         <f t="shared" ca="1" si="31"/>
         <v>0</v>
       </c>
-      <c r="P122" s="2">
+      <c r="S122" s="2">
+        <f t="shared" ca="1" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="T122" s="2">
         <f t="shared" ca="1" si="32"/>
-        <v>0</v>
-      </c>
-      <c r="Q122" s="2">
-        <f t="shared" ca="1" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="R122" s="2">
-        <f t="shared" ca="1" si="33"/>
-        <v>0</v>
-      </c>
-      <c r="S122" s="2">
-        <f t="shared" ca="1" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="T122" s="2">
-        <f t="shared" ca="1" si="35"/>
         <v>0</v>
       </c>
       <c r="U122" s="2" cm="1">
@@ -3965,7 +3963,7 @@
         <v>0</v>
       </c>
       <c r="Y122" s="2" t="str">
-        <f t="shared" ca="1" si="36"/>
+        <f t="shared" ca="1" si="33"/>
         <v>000000</v>
       </c>
     </row>
@@ -3983,39 +3981,39 @@
         <v>2040</v>
       </c>
       <c r="L123" s="2">
+        <f t="shared" ca="1" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="M123" s="2">
+        <f t="shared" ca="1" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="N123" s="2">
+        <f t="shared" ca="1" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="O123" s="2">
+        <f t="shared" ca="1" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="P123" s="2">
+        <f t="shared" ca="1" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="Q123" s="2">
         <f t="shared" ca="1" si="37"/>
         <v>0</v>
       </c>
-      <c r="M123" s="2">
-        <f t="shared" ca="1" si="29"/>
-        <v>0</v>
-      </c>
-      <c r="N123" s="2">
-        <f t="shared" ca="1" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="O123" s="2">
+      <c r="R123" s="2">
         <f t="shared" ca="1" si="31"/>
         <v>0</v>
       </c>
-      <c r="P123" s="2">
+      <c r="S123" s="2">
+        <f t="shared" ca="1" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="T123" s="2">
         <f t="shared" ca="1" si="32"/>
-        <v>0</v>
-      </c>
-      <c r="Q123" s="2">
-        <f t="shared" ca="1" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="R123" s="2">
-        <f t="shared" ca="1" si="33"/>
-        <v>0</v>
-      </c>
-      <c r="S123" s="2">
-        <f t="shared" ca="1" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="T123" s="2">
-        <f t="shared" ca="1" si="35"/>
         <v>0</v>
       </c>
       <c r="U123" s="2" cm="1">
@@ -4035,7 +4033,7 @@
         <v>0</v>
       </c>
       <c r="Y123" s="2" t="str">
-        <f t="shared" ca="1" si="36"/>
+        <f t="shared" ca="1" si="33"/>
         <v>000000</v>
       </c>
     </row>
@@ -4050,29 +4048,29 @@
     <row r="126" spans="9:25" x14ac:dyDescent="0.3">
       <c r="I126" s="2">
         <f ca="1">I90/B43</f>
-        <v>24.727646484375001</v>
+        <v>3143.68</v>
       </c>
       <c r="J126" s="2">
         <f t="shared" ref="J126:J138" ca="1" si="40">K83/I$126</f>
-        <v>17.111512883913857</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="127" spans="9:25" x14ac:dyDescent="0.3">
       <c r="J127" s="2">
         <f t="shared" ca="1" si="40"/>
-        <v>21.84305901281579</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="128" spans="9:25" x14ac:dyDescent="0.3">
       <c r="J128" s="2">
         <f t="shared" ca="1" si="40"/>
-        <v>11.045428103270353</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="129" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J129" s="2">
         <f t="shared" ca="1" si="40"/>
-        <v>0</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="130" spans="10:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
updated README with script info
</commit_message>
<xml_diff>
--- a/other/LinearVisualizer.xlsx
+++ b/other/LinearVisualizer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\CCHW\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D601CDB-AFA0-4D17-BCFC-7314BB194C23}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B1A192B-9ABB-4F7C-A530-CB00F3692B08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9DBF0F91-83D7-4F64-B04C-B7CB81DC62EF}"/>
   </bookViews>
@@ -707,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A6626A4-8C87-4B90-BEEB-AEB487ACEA9E}">
   <dimension ref="A2:Y138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H69" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T123" sqref="T123"/>
+    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="G108" sqref="G108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -791,11 +791,11 @@
       </c>
       <c r="D26" s="2" t="str">
         <f t="shared" ref="D26:D37" ca="1" si="0">_xlfn.CONCAT(B$40+B$41,"'b",REPT("0",B$40-LEN(E26)))</f>
-        <v>16'b00</v>
+        <v>16'b000</v>
       </c>
       <c r="E26" s="2" t="str">
         <f ca="1">DEC2BIN(_xlfn.FLOOR.MATH(RAND()*10))</f>
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F26" s="2" t="str">
         <f t="shared" ref="F26:F37" si="1">_xlfn.CONCAT(REPT("0",B$41),";")</f>
@@ -803,23 +803,23 @@
       </c>
       <c r="G26" s="4" t="str">
         <f ca="1">_xlfn.CONCAT(A26,B26,C26,D26,E26,F26)</f>
-        <v xml:space="preserve">            noteAmplitudes_i[ 0] = 16'b0010000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 0] = 16'b0001000000000000;</v>
       </c>
       <c r="H26" s="2">
         <f t="shared" ref="H26:H37" ca="1" si="2">BIN2DEC(E26)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I26" s="2">
         <f t="shared" ref="I26:I37" ca="1" si="3">H26*2^B$41</f>
-        <v>8192</v>
+        <v>4096</v>
       </c>
       <c r="J26" s="2">
         <f ca="1">SUM(H26:H37)</f>
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="K26" s="2">
         <f t="shared" ref="K26:K37" ca="1" si="4">I26-J$31</f>
-        <v>-3698</v>
+        <v>-6359</v>
       </c>
       <c r="L26" s="2">
         <f ca="1">IF(K26&gt;0,K26,0)</f>
@@ -842,11 +842,11 @@
       </c>
       <c r="D27" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16'b0000</v>
+        <v>16'b0</v>
       </c>
       <c r="E27" s="2" t="str">
         <f t="shared" ref="E27:E37" ca="1" si="5">DEC2BIN(_xlfn.FLOOR.MATH(RAND()*10))</f>
-        <v>1</v>
+        <v>1001</v>
       </c>
       <c r="F27" s="2" t="str">
         <f t="shared" si="1"/>
@@ -854,31 +854,31 @@
       </c>
       <c r="G27" s="4" t="str">
         <f t="shared" ref="G27:G37" ca="1" si="6">_xlfn.CONCAT(A27,B27,C27,D27,E27,F27)</f>
-        <v xml:space="preserve">            noteAmplitudes_i[ 1] = 16'b0000100000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 1] = 16'b0100100000000000;</v>
       </c>
       <c r="H27" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="I27" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>2048</v>
+        <v>18432</v>
       </c>
       <c r="J27" s="2">
         <f ca="1">J26*2^B41</f>
-        <v>118784</v>
+        <v>104448</v>
       </c>
       <c r="K27" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>-9842</v>
+        <v>7977</v>
       </c>
       <c r="L27" s="2">
         <f t="shared" ref="L27:L37" ca="1" si="7">IF(K27&gt;0,K27,0)</f>
-        <v>0</v>
+        <v>7977</v>
       </c>
       <c r="M27" s="2">
         <f t="shared" ref="M27:M37" ca="1" si="8">IF(K27&gt;0,I27,0)</f>
-        <v>0</v>
+        <v>18432</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
@@ -893,11 +893,11 @@
       </c>
       <c r="D28" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16'b00</v>
+        <v>16'b0000</v>
       </c>
       <c r="E28" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="F28" s="2" t="str">
         <f t="shared" si="1"/>
@@ -905,27 +905,27 @@
       </c>
       <c r="G28" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 2] = 16'b0011000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 2] = 16'b0000000000000000;</v>
       </c>
       <c r="H28" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I28" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>12288</v>
+        <v>0</v>
       </c>
       <c r="K28" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>398</v>
+        <v>-10455</v>
       </c>
       <c r="L28" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>398</v>
+        <v>0</v>
       </c>
       <c r="M28" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>12288</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
@@ -940,11 +940,11 @@
       </c>
       <c r="D29" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16'b00</v>
+        <v>16'b0000</v>
       </c>
       <c r="E29" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F29" s="2" t="str">
         <f t="shared" si="1"/>
@@ -952,22 +952,22 @@
       </c>
       <c r="G29" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 3] = 16'b0010000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 3] = 16'b0000100000000000;</v>
       </c>
       <c r="H29" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I29" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>8192</v>
+        <v>2048</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>8</v>
       </c>
       <c r="K29" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>-3698</v>
+        <v>-8407</v>
       </c>
       <c r="L29" s="2">
         <f t="shared" ca="1" si="7"/>
@@ -990,11 +990,11 @@
       </c>
       <c r="D30" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16'b000</v>
+        <v>16'b00</v>
       </c>
       <c r="E30" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>10</v>
+        <v>101</v>
       </c>
       <c r="F30" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1002,23 +1002,23 @@
       </c>
       <c r="G30" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 4] = 16'b0001000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 4] = 16'b0010100000000000;</v>
       </c>
       <c r="H30" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I30" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>4096</v>
+        <v>10240</v>
       </c>
       <c r="J30" s="3">
         <f ca="1">J26*B42</f>
-        <v>5.77734375</v>
+        <v>5.080078125</v>
       </c>
       <c r="K30" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>-7794</v>
+        <v>-215</v>
       </c>
       <c r="L30" s="2">
         <f t="shared" ca="1" si="7"/>
@@ -1041,11 +1041,11 @@
       </c>
       <c r="D31" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16'b0</v>
+        <v>16'b00</v>
       </c>
       <c r="E31" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>1001</v>
+        <v>100</v>
       </c>
       <c r="F31" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1053,31 +1053,31 @@
       </c>
       <c r="G31" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 5] = 16'b0100100000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 5] = 16'b0010000000000000;</v>
       </c>
       <c r="H31" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="I31" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>18432</v>
+        <v>8192</v>
       </c>
       <c r="J31" s="2">
         <f ca="1">J27 * BIN2DEC(C42) / 2^B41</f>
-        <v>11890</v>
+        <v>10455</v>
       </c>
       <c r="K31" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>6542</v>
+        <v>-2263</v>
       </c>
       <c r="L31" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>6542</v>
+        <v>0</v>
       </c>
       <c r="M31" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>18432</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
@@ -1092,11 +1092,11 @@
       </c>
       <c r="D32" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16'b00</v>
+        <v>16'b0</v>
       </c>
       <c r="E32" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>101</v>
+        <v>1001</v>
       </c>
       <c r="F32" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1104,27 +1104,27 @@
       </c>
       <c r="G32" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 6] = 16'b0010100000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 6] = 16'b0100100000000000;</v>
       </c>
       <c r="H32" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I32" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>10240</v>
+        <v>18432</v>
       </c>
       <c r="K32" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>-1650</v>
+        <v>7977</v>
       </c>
       <c r="L32" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>7977</v>
       </c>
       <c r="M32" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <v>18432</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
@@ -1166,11 +1166,11 @@
       </c>
       <c r="K33" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>398</v>
+        <v>1833</v>
       </c>
       <c r="L33" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>398</v>
+        <v>1833</v>
       </c>
       <c r="M33" s="2">
         <f t="shared" ca="1" si="8"/>
@@ -1189,11 +1189,11 @@
       </c>
       <c r="D34" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16'b00</v>
+        <v>16'b0000</v>
       </c>
       <c r="E34" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>101</v>
+        <v>0</v>
       </c>
       <c r="F34" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1201,23 +1201,23 @@
       </c>
       <c r="G34" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 8] = 16'b0010100000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 8] = 16'b0000000000000000;</v>
       </c>
       <c r="H34" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I34" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>10240</v>
+        <v>0</v>
       </c>
       <c r="J34" s="2">
         <f ca="1">J35/2^B41</f>
-        <v>6.9716796875</v>
+        <v>12.580078125</v>
       </c>
       <c r="K34" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>-1650</v>
+        <v>-10455</v>
       </c>
       <c r="L34" s="2">
         <f t="shared" ca="1" si="7"/>
@@ -1240,11 +1240,11 @@
       </c>
       <c r="D35" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16'b00</v>
+        <v>16'b000</v>
       </c>
       <c r="E35" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>111</v>
+        <v>11</v>
       </c>
       <c r="F35" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1252,31 +1252,31 @@
       </c>
       <c r="G35" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 9] = 16'b0011100000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 9] = 16'b0001100000000000;</v>
       </c>
       <c r="H35" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I35" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>14336</v>
+        <v>6144</v>
       </c>
       <c r="J35" s="2">
         <f ca="1">SUM(L26:L37)</f>
-        <v>14278</v>
+        <v>25764</v>
       </c>
       <c r="K35" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>2446</v>
+        <v>-4311</v>
       </c>
       <c r="L35" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>2446</v>
+        <v>0</v>
       </c>
       <c r="M35" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>14336</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
@@ -1291,11 +1291,11 @@
       </c>
       <c r="D36" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16'b0000</v>
+        <v>16'b000</v>
       </c>
       <c r="E36" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F36" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1303,19 +1303,19 @@
       </c>
       <c r="G36" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[10] = 16'b0000100000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[10] = 16'b0001100000000000;</v>
       </c>
       <c r="H36" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I36" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>2048</v>
+        <v>6144</v>
       </c>
       <c r="K36" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>-9842</v>
+        <v>-4311</v>
       </c>
       <c r="L36" s="2">
         <f t="shared" ca="1" si="7"/>
@@ -1342,7 +1342,7 @@
       </c>
       <c r="E37" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="F37" s="2" t="str">
         <f t="shared" si="1"/>
@@ -1350,27 +1350,27 @@
       </c>
       <c r="G37" s="4" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v xml:space="preserve">            noteAmplitudes_i[11] = 16'b0100000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[11] = 16'b0100100000000000;</v>
       </c>
       <c r="H37" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I37" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>16384</v>
+        <v>18432</v>
       </c>
       <c r="K37" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>4494</v>
+        <v>7977</v>
       </c>
       <c r="L37" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>4494</v>
+        <v>7977</v>
       </c>
       <c r="M37" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>16384</v>
+        <v>18432</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
@@ -1413,27 +1413,27 @@
       <c r="C41" s="8"/>
       <c r="G41" s="4" t="str">
         <f ca="1">_xlfn.CONCAT("notePosition_i = 10'b",REPT(0,B41-LEN(_xlfn.BASE(I41,2))),_xlfn.BASE(I41,2),";" )</f>
-        <v>notePosition_i = 10'b01000110001;</v>
+        <v>notePosition_i = 10'b01101100001;</v>
       </c>
       <c r="H41" s="2">
         <f ca="1">I41/2^10</f>
-        <v>0.5478515625</v>
+        <v>0.8447265625</v>
       </c>
       <c r="I41" s="2">
         <f ca="1">RANDBETWEEN(0,1023)</f>
-        <v>561</v>
+        <v>865</v>
       </c>
       <c r="J41" s="2">
         <f ca="1">I41*24</f>
-        <v>13464</v>
+        <v>20760</v>
       </c>
       <c r="K41" s="2">
         <f ca="1">IF(J45=3,24576-J41,8192-J41)</f>
-        <v>-5272</v>
+        <v>3816</v>
       </c>
       <c r="L41" s="2">
         <f ca="1">IF(J45=3,K47+170, K47)</f>
-        <v>-28</v>
+        <v>199</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
@@ -1483,11 +1483,11 @@
       </c>
       <c r="J44" s="2" t="str">
         <f ca="1">_xlfn.CONCAT(REPT(0,3-LEN(DEC2BIN(2^_xlfn.FLOOR.MATH((J41+1)/8192)))),DEC2BIN(2^_xlfn.FLOOR.MATH((J41+1)/8192)))</f>
-        <v>010</v>
+        <v>100</v>
       </c>
       <c r="K44" s="2">
         <f ca="1">K41*H44*H45*H46</f>
-        <v>-460224512</v>
+        <v>499682304</v>
       </c>
       <c r="L44" s="2" t="s">
         <v>24</v>
@@ -1506,19 +1506,19 @@
       </c>
       <c r="H45" s="2">
         <f ca="1">IF(J$45=2,G45,1)</f>
-        <v>87296</v>
+        <v>1</v>
       </c>
       <c r="J45" s="2">
         <f ca="1">LEN(DEC2BIN(2^_xlfn.FLOOR.MATH((J41+1)/8192)))</f>
-        <v>2</v>
-      </c>
-      <c r="K45" s="2" t="e">
+        <v>3</v>
+      </c>
+      <c r="K45" s="2" t="str">
         <f ca="1">_xlfn.BASE(K44,2,32)</f>
-        <v>#NUM!</v>
+        <v>00011101110010001000110000000000</v>
       </c>
       <c r="L45" s="2">
         <f ca="1">MOD(IF(L41&lt;0,L41+1023,L41), 1024)</f>
-        <v>995</v>
+        <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
@@ -1534,7 +1534,7 @@
       </c>
       <c r="H46" s="2">
         <f ca="1">IF(J$45=3,G46,1)</f>
-        <v>1</v>
+        <v>130944</v>
       </c>
       <c r="K46" s="2" t="s">
         <v>21</v>
@@ -1543,21 +1543,21 @@
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K47" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(K44/2^(B41+B41+C39-3))</f>
-        <v>-28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="50" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G50" s="4" t="str">
         <f ca="1">_xlfn.CONCAT("        noteAmplitude_i = 10'b",REPT(0,B41-LEN(_xlfn.BASE(I50,2))),_xlfn.BASE(I50,2),";" )</f>
-        <v xml:space="preserve">        noteAmplitude_i = 10'b01100100101;</v>
+        <v xml:space="preserve">        noteAmplitude_i = 10'b00000000111;</v>
       </c>
       <c r="H50" s="2">
         <f ca="1">I50/2^10</f>
-        <v>0.7861328125</v>
+        <v>6.8359375E-3</v>
       </c>
       <c r="I50" s="2">
         <f ca="1">RANDBETWEEN(0,1023)</f>
-        <v>805</v>
+        <v>7</v>
       </c>
       <c r="J50" s="2" t="s">
         <v>28</v>
@@ -1589,35 +1589,35 @@
       </c>
       <c r="G51" s="4" t="str">
         <f ca="1">_xlfn.CONCAT("        noteAmplitudeFast_i = 10'b",REPT(0,B41-LEN(_xlfn.BASE(I51,2))),_xlfn.BASE(I51,2),";" )</f>
-        <v xml:space="preserve">        noteAmplitudeFast_i = 10'b01000011001;</v>
+        <v xml:space="preserve">        noteAmplitudeFast_i = 10'b00011011001;</v>
       </c>
       <c r="H51" s="2">
         <f t="shared" ref="H51:H52" ca="1" si="9">I51/2^10</f>
-        <v>0.5244140625</v>
+        <v>0.2119140625</v>
       </c>
       <c r="I51" s="2">
         <f ca="1">RANDBETWEEN(0,1023)</f>
-        <v>537</v>
+        <v>217</v>
       </c>
       <c r="J51" s="2">
         <f ca="1">I52*E55</f>
-        <v>1560</v>
+        <v>7860</v>
       </c>
       <c r="K51" s="2">
         <f ca="1">IF(E57,I50,I51)</f>
-        <v>537</v>
+        <v>217</v>
       </c>
       <c r="L51" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(K57/2^(B41-8))</f>
-        <v>127</v>
+        <v>86</v>
       </c>
       <c r="M51" s="2">
         <f ca="1">$L$51</f>
-        <v>127</v>
+        <v>86</v>
       </c>
       <c r="N51" s="2">
         <f ca="1">$L$57</f>
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="O51" s="2">
         <f>0</f>
@@ -1625,21 +1625,21 @@
       </c>
       <c r="P51" s="2">
         <f ca="1">M51*2^16+N51*2^8+O51</f>
-        <v>8331520</v>
+        <v>5643520</v>
       </c>
     </row>
     <row r="52" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G52" s="4" t="str">
         <f ca="1">_xlfn.CONCAT("        noteHue_i = 10'b",REPT(0,B41-LEN(_xlfn.BASE(I52,2))),_xlfn.BASE(I52,2),";" )</f>
-        <v xml:space="preserve">        noteHue_i = 10'b00010000010;</v>
+        <v xml:space="preserve">        noteHue_i = 10'b01010001111;</v>
       </c>
       <c r="H52" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>0.126953125</v>
+        <v>0.6396484375</v>
       </c>
       <c r="I52" s="2">
         <f ca="1">RANDBETWEEN(0,1023)</f>
-        <v>130</v>
+        <v>655</v>
       </c>
       <c r="J52" s="2" t="s">
         <v>29</v>
@@ -1652,11 +1652,11 @@
       </c>
       <c r="M52" s="2">
         <f ca="1">$L$59</f>
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="N52" s="2">
         <f ca="1">$L$51</f>
-        <v>127</v>
+        <v>86</v>
       </c>
       <c r="O52" s="2">
         <f>0</f>
@@ -1664,21 +1664,21 @@
       </c>
       <c r="P52" s="2">
         <f t="shared" ref="P52:P57" ca="1" si="10">M52*2^16+N52*2^8+O52</f>
-        <v>1998592</v>
+        <v>939520</v>
       </c>
     </row>
     <row r="53" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J53" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(J51/2^10)</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="K53" s="2">
         <f ca="1">K51*E54</f>
-        <v>1759749</v>
+        <v>711109</v>
       </c>
       <c r="L53" s="2">
         <f ca="1">K57*J55</f>
-        <v>548328</v>
+        <v>480248</v>
       </c>
       <c r="M53" s="2">
         <f>0</f>
@@ -1686,15 +1686,15 @@
       </c>
       <c r="N53" s="2">
         <f ca="1">$L$51</f>
-        <v>127</v>
+        <v>86</v>
       </c>
       <c r="O53" s="2">
         <f ca="1">$L$57</f>
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="P53" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>32545</v>
+        <v>22045</v>
       </c>
     </row>
     <row r="54" spans="2:16" x14ac:dyDescent="0.3">
@@ -1719,15 +1719,15 @@
       </c>
       <c r="N54" s="2">
         <f ca="1">$L$59</f>
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="O54" s="2">
         <f ca="1">$L$51</f>
-        <v>127</v>
+        <v>86</v>
       </c>
       <c r="P54" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>7807</v>
+        <v>3670</v>
       </c>
     </row>
     <row r="55" spans="2:16" x14ac:dyDescent="0.3">
@@ -1739,19 +1739,19 @@
       </c>
       <c r="J55" s="2">
         <f ca="1">MOD(J51,2^10)</f>
-        <v>536</v>
+        <v>692</v>
       </c>
       <c r="K55" s="2">
         <f ca="1">IF(_xlfn.FLOOR.MATH(K53/2^10) &gt; 1023, 1023, _xlfn.FLOOR.MATH(K53/2^10))</f>
-        <v>1023</v>
+        <v>694</v>
       </c>
       <c r="L55" s="2">
         <f ca="1">K57*(1023-J55)</f>
-        <v>498201</v>
+        <v>229714</v>
       </c>
       <c r="M55" s="2">
         <f ca="1">$L$57</f>
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="N55" s="2">
         <f>0</f>
@@ -1759,11 +1759,11 @@
       </c>
       <c r="O55" s="2">
         <f ca="1">$L$51</f>
-        <v>127</v>
+        <v>86</v>
       </c>
       <c r="P55" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>2162815</v>
+        <v>1900630</v>
       </c>
     </row>
     <row r="56" spans="2:16" x14ac:dyDescent="0.3">
@@ -1781,7 +1781,7 @@
       </c>
       <c r="M56" s="2">
         <f ca="1">$L$51</f>
-        <v>127</v>
+        <v>86</v>
       </c>
       <c r="N56" s="2">
         <f>0</f>
@@ -1789,11 +1789,11 @@
       </c>
       <c r="O56" s="2">
         <f ca="1">$L$59</f>
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="P56" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>8323102</v>
+        <v>5636110</v>
       </c>
     </row>
     <row r="57" spans="2:16" x14ac:dyDescent="0.3">
@@ -1805,19 +1805,19 @@
       </c>
       <c r="K57" s="2">
         <f ca="1">IF(K55&gt;E56,E56,K55)</f>
-        <v>1023</v>
+        <v>694</v>
       </c>
       <c r="L57" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(L53/2^(2*B41-8))</f>
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="M57" s="2">
         <f ca="1">$L$51</f>
-        <v>127</v>
+        <v>86</v>
       </c>
       <c r="N57" s="2">
         <f ca="1">$L$57</f>
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="O57" s="2">
         <f>0</f>
@@ -1825,7 +1825,7 @@
       </c>
       <c r="P57" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>8331520</v>
+        <v>5643520</v>
       </c>
     </row>
     <row r="58" spans="2:16" x14ac:dyDescent="0.3">
@@ -1839,11 +1839,11 @@
     <row r="59" spans="2:16" x14ac:dyDescent="0.3">
       <c r="L59" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(L55/2^(2*B41-8))</f>
-        <v>30</v>
-      </c>
-      <c r="M59" s="2" t="str" cm="1">
+        <v>14</v>
+      </c>
+      <c r="M59" s="2" t="e" cm="1">
         <f t="array" aca="1" ref="M59" ca="1">_xlfn.BASE(_xlfn.SWITCH(J53,0,P51,1,P52,2,P53,3,P54,4,P55,5,P56,6,P57),16,6)</f>
-        <v>1E7F00</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="60" spans="2:16" x14ac:dyDescent="0.3">
@@ -1870,7 +1870,7 @@
       </c>
       <c r="I63" s="2">
         <f ca="1">_xlfn.FLOOR.MATH(H76/B43)</f>
-        <v>285</v>
+        <v>515</v>
       </c>
       <c r="J63" s="2">
         <f t="shared" ref="J63:J74" ca="1" si="12">_xlfn.FLOOR.MATH(H63/I$63)</f>
@@ -1878,35 +1878,35 @@
       </c>
       <c r="L63" s="2">
         <f ca="1">L51-L57-L59</f>
-        <v>64</v>
+        <v>43</v>
       </c>
     </row>
     <row r="64" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G64" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 1] = 16'b0000000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 1] = 16'b0001111100101001;</v>
       </c>
       <c r="H64" s="2">
         <f t="shared" ref="H64:H74" ca="1" si="13">L27</f>
-        <v>0</v>
+        <v>7977</v>
       </c>
       <c r="J64" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="65" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G65" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 2] = 16'b0000000110001110;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 2] = 16'b0000000000000000;</v>
       </c>
       <c r="H65" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>398</v>
+        <v>0</v>
       </c>
       <c r="J65" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:25" x14ac:dyDescent="0.3">
@@ -1940,43 +1940,43 @@
     <row r="68" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G68" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 5] = 16'b0001100110001110;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 5] = 16'b0000000000000000;</v>
       </c>
       <c r="H68" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>6542</v>
+        <v>0</v>
       </c>
       <c r="J68" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G69" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 6] = 16'b0000000000000000;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 6] = 16'b0001111100101001;</v>
       </c>
       <c r="H69" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>7977</v>
       </c>
       <c r="J69" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="70" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G70" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 7] = 16'b0000000110001110;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 7] = 16'b0000011100101001;</v>
       </c>
       <c r="H70" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>398</v>
+        <v>1833</v>
       </c>
       <c r="J70" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71" spans="1:25" x14ac:dyDescent="0.3">
@@ -1996,15 +1996,15 @@
     <row r="72" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G72" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[ 9] = 16'b0000100110001110;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[ 9] = 16'b0000000000000000;</v>
       </c>
       <c r="H72" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>2446</v>
+        <v>0</v>
       </c>
       <c r="J72" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:25" x14ac:dyDescent="0.3">
@@ -2024,11 +2024,11 @@
     <row r="74" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G74" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v xml:space="preserve">            noteAmplitudes_i[11] = 16'b0001000110001110;</v>
+        <v xml:space="preserve">            noteAmplitudes_i[11] = 16'b0001111100101001;</v>
       </c>
       <c r="H74" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>4494</v>
+        <v>7977</v>
       </c>
       <c r="J74" s="2">
         <f t="shared" ca="1" si="12"/>
@@ -2038,7 +2038,7 @@
     <row r="75" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G75" s="5" t="str">
         <f ca="1">_xlfn.CONCAT("            amplitudeSumNew_i = ",B40+B41+_xlfn.CEILING.MATH(IMLOG2(B43)),"'b",_xlfn.BASE(H76,2,B40+B41+_xlfn.CEILING.MATH(IMLOG2(B43))),";")</f>
-        <v xml:space="preserve">            amplitudeSumNew_i = 22'b0000000011011111000110;</v>
+        <v xml:space="preserve">            amplitudeSumNew_i = 22'b0000000110010010100100;</v>
       </c>
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.3">
@@ -2047,7 +2047,7 @@
       </c>
       <c r="H76" s="2">
         <f ca="1">SUM(H63:H74)</f>
-        <v>14278</v>
+        <v>25764</v>
       </c>
     </row>
     <row r="78" spans="1:25" x14ac:dyDescent="0.3">
@@ -3285,7 +3285,7 @@
         <v>65535</v>
       </c>
       <c r="M113" s="2">
-        <f t="shared" ref="M112:M123" ca="1" si="35">L113*E$54</f>
+        <f t="shared" ref="M113:M123" ca="1" si="35">L113*E$54</f>
         <v>214758195</v>
       </c>
       <c r="N113" s="2">

</xml_diff>